<commit_message>
Added maps and resampled villages to exclude Leroro and Emjindini Trust
</commit_message>
<xml_diff>
--- a/sampling/hea_selected_villages.xlsx
+++ b/sampling/hea_selected_villages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="-1260" windowWidth="24720" windowHeight="15180" tabRatio="500"/>
+    <workbookView xWindow="360" yWindow="0" windowWidth="24720" windowHeight="17040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="275">
   <si>
     <t>wkt_geom</t>
   </si>
@@ -439,6 +439,411 @@
   </si>
   <si>
     <t>Buyisonto</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.4907964320000815 -25.15075875199994471, 28.4897451270000488 -25.15089239299993551, 28.48823289800003522 -25.15108462399990685, 28.48670032100005756 -25.15142532099991968, 28.48676020900006733 -25.15084141799991713, 28.48687998300004764 -25.15016768599992147, 28.48699976000006018 -25.14925440399991885, 28.48707461500004001 -25.14864055799995768, 28.48713824700007535 -25.14842159399995936, 28.48725053600009005 -25.14716395799990778, 28.48725287200005596 -25.14714579299993602, 28.4873515970000426 -25.14637793699995427, 28.48744142700007842 -25.1455694569999082, 28.48750880100004679 -25.14494063799992318, 28.48760986000008089 -25.14446902599991063, 28.48765477500006682 -25.1440423289999444, 28.48769969200003516 -25.14332367999992357, 28.48760986000008089 -25.14322261799992475, 28.48772215000008146 -25.14291943999996093, 28.48800209800004168 -25.14285950899994759, 28.48836573000005146 -25.14284652199996017, 28.48859949200004849 -25.14285950899994759, 28.48884624100008978 -25.14279457499992532, 28.48920987300004981 -25.14276860099994337, 28.48956051800007927 -25.14278158799993079, 28.48972934600004692 -25.14279457499992532, 28.49001505600006112 -25.14272964099990304, 28.49021239500007141 -25.14270390099994756, 28.49043575300003894 -25.14382362299994256, 28.49066288000005542 -25.14529020899993483, 28.49079266600006122 -25.14601701199995887, 28.49099383500004024 -25.14734083299993017, 28.49109117600005092 -25.14798976399992725, 28.49066936900004521 -25.14804167799991674, 28.49068234700007451 -25.14841156999995064, 28.49071479400004137 -25.14963805099995753, 28.4907964320000815 -25.15075875199994471)))</t>
+  </si>
+  <si>
+    <t>demog_sas.49096</t>
+  </si>
+  <si>
+    <t>Phaphamang</t>
+  </si>
+  <si>
+    <t>Phake</t>
+  </si>
+  <si>
+    <t>MP316</t>
+  </si>
+  <si>
+    <t>Dr JS Moroka</t>
+  </si>
+  <si>
+    <t>DC31</t>
+  </si>
+  <si>
+    <t>Nkangala</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.96872778700003437 -25.19659764199991514, 28.96856567300005736 -25.2003533939999329, 28.96853268900008516 -25.20130988899995828, 28.96586858300008771 -25.20125330599995905, 28.96330493000004935 -25.20126177499992082, 28.96331370100006097 -25.2002808289999507, 28.96340245200007857 -25.19684911499990676, 28.96342217500006555 -25.19641521999994893, 28.96342181400007121 -25.19640081999995118, 28.96335034300005518 -25.19640135999992481, 28.96334766700005048 -25.19635528799994972, 28.96337971200006223 -25.19613453399995606, 28.96346624000005576 -25.19504432899992707, 28.96349463700005344 -25.19504543699991927, 28.96742689100005563 -25.19519326499994349, 28.96798864300006926 -25.19541500999989836, 28.96798864300006926 -25.19597676099994032, 28.968772135000048 -25.19603589099995133, 28.96872778700003437 -25.19659764199991514)))</t>
+  </si>
+  <si>
+    <t>demog_sas.51255</t>
+  </si>
+  <si>
+    <t>Pieterskraal B</t>
+  </si>
+  <si>
+    <t>Pieterskraal</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.76231299900007699 -25.11305114999993293, 28.76224775000008549 -25.1130664619999493, 28.76159308300004014 -25.11328004299992145, 28.76143102700007148 -25.11333291299990833, 28.76035944000005529 -25.11362832199995765, 28.75937473900006225 -25.11387739399992824, 28.75900982100006331 -25.11401061799995205, 28.75881288000005043 -25.11412646499991652, 28.75848271500007058 -25.1142365199999027, 28.75825681300005954 -25.11423072799993506, 28.75768916300006239 -25.11414384299990843, 28.75664483600008126 -25.11398859299992736, 28.75664490600007994 -25.11398821699992823, 28.75673867400007921 -25.11348659499992664, 28.75717577100004974 -25.11082030199991877, 28.75732875500006003 -25.11040505899995878, 28.75761001300008957 -25.10794201299995976, 28.75968908200007945 -25.1076731989999189, 28.75977650100008987 -25.10784803799992915, 28.7598639210000897 -25.10832884499990314, 28.75992948500004331 -25.10843811899991707, 28.7603447280000637 -25.10843811899991707, 28.76047585700007758 -25.10902820099994415, 28.76120367100008934 -25.1088841539999521, 28.76134069500005452 -25.10930808299992023, 28.76158104700004969 -25.11022769199990989, 28.7616849340000762 -25.11059959399995023, 28.76186934700007214 -25.11139625899994243, 28.76231299900007699 -25.11305114999993293)))</t>
+  </si>
+  <si>
+    <t>demog_sas.51005</t>
+  </si>
+  <si>
+    <t>Loding SP</t>
+  </si>
+  <si>
+    <t>Loding</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.12677272800004857 -25.24929171499991654, 29.12662827000008292 -25.24986793199991908, 29.12610481000007212 -25.25173231399992346, 29.12569394200005135 -25.25164336399990361, 29.12308680500007085 -25.25107282699991984, 29.12275459400007094 -25.2522355659999107, 29.12133290600008095 -25.25196162699996094, 29.12129995100008273 -25.24915369099994678, 29.12128938600005768 -25.24809264999993275, 29.121288679000088 -25.24802159999995865, 29.12670920800007934 -25.24927583499993133, 29.12677272800004857 -25.24929171499991654)))</t>
+  </si>
+  <si>
+    <t>demog_sas.60340</t>
+  </si>
+  <si>
+    <t>Phukukane SP</t>
+  </si>
+  <si>
+    <t>Phukukane</t>
+  </si>
+  <si>
+    <t>LIM472</t>
+  </si>
+  <si>
+    <t>Elias Motsoaledi</t>
+  </si>
+  <si>
+    <t>DC47</t>
+  </si>
+  <si>
+    <t>Greater Sekhukhune</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.91806747200007521 -25.12076359899992894, 28.91808162500007029 -25.12081454999989916, 28.91772697000004655 -25.12112283699991977, 28.91728336900007434 -25.1214723409999614, 28.91704006000009031 -25.12163454599993528, 28.9170359140000528 -25.1216373099999295, 28.91688009500006729 -25.12174118899991981, 28.91661124800004146 -25.12191594099994063, 28.91644769000004089 -25.12203139299992927, 28.91638272500006224 -25.12207725099995059, 28.91601977800008072 -25.1222923319999154, 28.91580469800004494 -25.12241331299992453, 28.91515061800004105 -25.12274785199992166, 28.91317865400003484 -25.12001743999991632, 28.91379718400008869 -25.11965924399993355, 28.91305655500007887 -25.11859772599990492, 28.91258487800007515 -25.11796567999994068, 28.91233960700003536 -25.11764376199994331, 28.9135146940000709 -25.11701236599992626, 28.91499196800004157 -25.11618656099994951, 28.91447813400003497 -25.11545251199993345, 28.91605633900007888 -25.1145808289999195, 28.91735927600007017 -25.11392018599991971, 28.91802909500006535 -25.113543985999911, 28.91841447100006235 -25.11312190599994665, 28.91856128100004852 -25.11291086699992547, 28.9188181980000536 -25.11286498899994513, 28.91960730100003829 -25.11283746299994846, 28.9201094820000435 -25.11277380599995013, 28.92009038500004081 -25.11283203199991476, 28.91984749400006294 -25.11354100599993089, 28.91949957300005281 -25.11440096399991617, 28.91924355300005445 -25.11509024399992995, 28.91920416600004273 -25.11512963099994522, 28.919112263000045 -25.11528061599994999, 28.91907943800003977 -25.11539877899992135, 28.91902692300004674 -25.1155891499999484, 28.91901379400007954 -25.11574670199991033, 28.91901379400007954 -25.11578608799993617, 28.91875121100008528 -25.11657383699991897, 28.91836390300005633 -25.11774233199992068, 28.91829825400003529 -25.11782766999990102, 28.91825230300008798 -25.11798521999992317, 28.91821291600007626 -25.1181427699999027, 28.91819978800004165 -25.11824780299992099, 28.91751050800008116 -25.1200727529999277, 28.91771400900006483 -25.12033533599992907, 28.91784530000006725 -25.12045349899995017, 28.91797659200005555 -25.12062417699991101, 28.91804880200004391 -25.12069638699995622, 28.91806747200007521 -25.12076359899992894)))</t>
+  </si>
+  <si>
+    <t>demog_sas.51128</t>
+  </si>
+  <si>
+    <t>Allemansdrift C</t>
+  </si>
+  <si>
+    <t>Allemansdrift</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.54302568500008874 -25.10442044199993106, 28.54294102100004693 -25.10452049999992141, 28.54235606100008127 -25.10525939599995127, 28.54247151200008048 -25.1053286679999168, 28.54205588500008162 -25.10566732699993153, 28.54165564900006302 -25.1059982909999313, 28.54115535600004705 -25.10637543499990443, 28.54087057400005278 -25.10656015899991189, 28.54052421800008688 -25.10676027699992119, 28.54023943500004634 -25.10687572899990982, 28.53995465200006265 -25.10698348399995439, 28.53965447600006655 -25.10706814899992878, 28.53943896500004485 -25.10712202799993165, 28.53912339500004691 -25.10717590499990237, 28.53882321900004726 -25.10720669199992017, 28.53848455900003955 -25.10722978299992292, 28.53804584000004851 -25.10722978299992292, 28.53763536300004944 -25.10717953699991867, 28.53728709400008157 -25.10710068499992076, 28.53680740400005433 -25.10699554699993996, 28.53645256300006849 -25.10690355099995941, 28.53534204600003932 -25.10669327599993039, 28.53457979700004898 -25.10652242699995895, 28.53374526600003946 -25.10634500899993427, 28.53310786900004814 -25.10623329799994963, 28.53263475000005656 -25.1061478739999302, 28.53199078100004726 -25.10607559199991101, 28.53137309700008473 -25.10602959399994916, 28.53081455200004157 -25.105990166999959, 28.53016401200005703 -25.10594416999990131, 28.52917268200008039 -25.10587844599990248, 28.52916973800006417 -25.10576367299995937, 28.52915037400003939 -25.10513431199990464, 28.52979910000004793 -25.10520208999992064, 28.52977973500008702 -25.10391431899995496, 28.52970227700006944 -25.10321718099993049, 28.53022512900008678 -25.10330432299992154, 28.53051560300008305 -25.10317845099990564, 28.53062211100007062 -25.10293638899992175, 28.53080607800006874 -25.10174544399990282, 28.53112560100003847 -25.10174544399990282, 28.53109655300005087 -25.1011741779999511, 28.53318796900003917 -25.1011257649999493, 28.53305241500004286 -25.10052544999990687, 28.53308146100004805 -25.10051576899991232, 28.53304273200006946 -25.09988640699992857, 28.53306845500003774 -25.09955974099995046, 28.53314458100004458 -25.09959803799995726, 28.53348721400004706 -25.09983909799990442, 28.53384436600003937 -25.10007166299993742, 28.53391092500004333 -25.10011416399993323, 28.53418906100006325 -25.10029176899990944, 28.53443408400005055 -25.10044542699995773, 28.53489601000006815 -25.10073213899994471, 28.53537286400006678 -25.10016135999995868, 28.53600190200006281 -25.09946862099991449, 28.53648761500005193 -25.0989112449999574, 28.53664683300008065 -25.09870850999993763, 28.54115392100004911 -25.10178217799995082, 28.54109539600005974 -25.10185742599992409, 28.54097392100004527 -25.10195388999994748, 28.54259466300004533 -25.10326591899990945, 28.54254848100003983 -25.1033351899999353, 28.54246670300005562 -25.10351919199990789, 28.5422502290000466 -25.10402573999990139, 28.54302568500008874 -25.10442044199993106)))</t>
+  </si>
+  <si>
+    <t>demog_sas.50977</t>
+  </si>
+  <si>
+    <t>Mmamethlake SP</t>
+  </si>
+  <si>
+    <t>Mmamethlake</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.10432595100008157 -25.04480215299992096, 29.10471700400006512 -25.04543385299990277, 29.10492757000008623 -25.04594522899992626, 29.10522837900003879 -25.04624603799993565, 29.10573975500005517 -25.04666716999992104, 29.10625113200006808 -25.04702814199992744, 29.10679258800007929 -25.04732895099994039, 29.10715355800005 -25.04759967899991935, 29.10769501500004708 -25.04793056899995918, 29.10823647200004416 -25.04838178299991114, 29.10883809000006295 -25.04892323999990822, 29.10841695700008813 -25.04913380699991876, 29.10805598800004645 -25.04943461499993518, 29.10772509600008107 -25.04991591099991766, 29.10766493400006993 -25.05051753099991174, 29.10754461100004065 -25.05105898599992997, 29.10736412400007112 -25.05169068499992946, 29.10718364000007696 -25.0518711709999593, 29.10709339700008513 -25.05214189899993116, 29.10688283000007459 -25.05262319499991008, 29.1065820210000652 -25.05304432699995232, 29.10634137300008106 -25.05349554099990428, 29.105829998000047 -25.05439796899991833, 29.10558117900006891 -25.05481341999990264, 29.10533145500005148 -25.05514676299992516, 29.10258087800008298 -25.05374645899991037, 29.10058736700005966 -25.05225089399993976, 29.09937169400006951 -25.05080789899994897, 29.09962866500006839 -25.0504520919999436, 29.09919379200004741 -25.04973059399992508, 29.0993222750000804 -25.04947362399991917, 29.09836357500006443 -25.04877189499995893, 29.0985711290000495 -25.04839631999993443, 29.09842619300007982 -25.04825138399991147, 29.09870124400003988 -25.04790130399993586, 29.0989671770000804 -25.0475595099999282, 29.09923044300006723 -25.04723548999993099, 29.09911347300004536 -25.04705167999992454, 29.09917365800004063 -25.0467818379999585, 29.0994456230000651 -25.04644080399992845, 29.09957081200008133 -25.04625949599994783, 29.09969622600004868 -25.04579764299996114, 29.1001215030000786 -25.04557487799991122, 29.10060753500004793 -25.04567613499995105, 29.10089105500008699 -25.04561538099994777, 29.10157960100008268 -25.04523060499991516, 29.10175083400008944 -25.04508098799993476, 29.1020098470000903 -25.04499033399991959, 29.10226886000004143 -25.04500760099995205, 29.10279120200004854 -25.04504645299994081, 29.10310608300005697 -25.04517239399990558, 29.10334147000008898 -25.04525085599993517, 29.1033739930000479 -25.04519510299991225, 29.10345934200006468 -25.04510513499991475, 29.10352098100008789 -25.0449783689999208, 29.10357913000007102 -25.0447969419999481, 29.10358654200007678 -25.04476050399995657, 29.10359657500004005 -25.04464575299994067, 29.10361983500007454 -25.04455852799992499, 29.10363495400008915 -25.04445851099995934, 29.10364363600007209 -25.04440550199990412, 29.10367100700005594 -25.04430266799994342, 29.10368728900004953 -25.04423405299991146, 29.10367682300005754 -25.0441793919999327, 29.10364309400006277 -25.04408751499994423, 29.10362681300006571 -25.04401773599994385, 29.10360833400005731 -25.04380559699990272, 29.10357071700007836 -25.04364454299991749, 29.1035642330000428 -25.04356999299994868, 29.10358172100006868 -25.04334267099994804, 29.10390481900003934 -25.04380948199991508, 29.10432595100008157 -25.04480215299992096)))</t>
+  </si>
+  <si>
+    <t>demog_sas.62471</t>
+  </si>
+  <si>
+    <t>Matlala Ramoshebo SP</t>
+  </si>
+  <si>
+    <t>Matlala Ramoshebo</t>
+  </si>
+  <si>
+    <t>LIM471</t>
+  </si>
+  <si>
+    <t>Ephraim Mogale</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.82293753200008268 -25.27798374999991893, 28.8233697670000879 -25.27811120399991651, 28.82375180100007128 -25.27822958299992706, 28.82422391200003986 -25.27839364399994793, 28.82353269500003989 -25.2803762289999554, 28.82330956300006264 -25.28094800699994948, 28.82302915900004336 -25.28174045299994077, 28.82384405200008359 -25.28198637199994891, 28.82382748800006311 -25.28206919399992003, 28.82363975800006983 -25.2826544709999439, 28.82351828500003776 -25.28297471699994503, 28.82348515600006067 -25.28311827599992512, 28.82339681200005188 -25.2833060059999184, 28.82330294700005524 -25.28357655899992906, 28.82307660900005075 -25.28411738999994895, 28.82285203700007514 -25.2849230489999286, 28.82274990600006959 -25.28526657999992722, 28.82274062100004031 -25.28542441999991652, 28.82270348300005125 -25.28562867999994523, 28.82266598900008958 -25.28567148399991993, 28.82248344200008106 -25.28577144999991688, 28.82196622700007538 -25.28563236699994832, 28.82157070800008114 -25.28551066899990474, 28.82158809300005586 -25.28545851299992364, 28.82120561400006409 -25.28534550799992076, 28.82080575000009048 -25.2852368509999188, 28.82035373000007894 -25.28510211199994728, 28.82034068800004434 -25.28505864899995004, 28.82030157300004802 -25.28501083699995888, 28.82026680200004876 -25.28494998799993709, 28.82043196300008958 -25.28446754399993424, 28.81962354100005186 -25.2842241469999216, 28.81910632600005329 -25.28406333299994913, 28.81859345600008737 -25.28391990399995848, 28.81846741100008913 -25.28385905399994726, 28.8188107730000489 -25.28288981699995475, 28.81860214800007824 -25.28287242999994078, 28.81828486500006292 -25.28277681299994128, 28.81798931200006564 -25.28271596299993007, 28.81796092000007548 -25.28270260499994038, 28.8177769760000615 -25.28263600499991526, 28.8179831200000649 -25.28209051799990448, 28.81837637800003904 -25.28112640099993769, 28.81850957600005358 -25.2807965719999288, 28.81885526400003528 -25.27990222799991216, 28.81916289300005118 -25.27907448399992063, 28.81940709400004152 -25.27847508299993251, 28.81966715100008969 -25.27778370799995855, 28.81983523700006344 -25.27738727999991752, 28.82025069600007683 -25.27636290799995678, 28.82120420000006789 -25.27721605599992927, 28.82161420200003477 -25.27754849099994772, 28.8216640690000645 -25.27758173299991995, 28.82182474500007174 -25.27764267899993555, 28.82244965800003911 -25.27782602399992129, 28.82274021900008165 -25.27792556799994372, 28.82293753200008268 -25.27798374999991893)))</t>
+  </si>
+  <si>
+    <t>demog_sas.51268</t>
+  </si>
+  <si>
+    <t>Kameelpoort SP</t>
+  </si>
+  <si>
+    <t>Kameelpoort</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.15858167100003939 -25.19794360599991023, 29.15849683700008654 -25.19801475699995663, 29.15832966600004283 -25.19820978999990757, 29.1582553670000415 -25.19828408799992303, 29.1582553670000415 -25.19867415299995983, 29.15839467700004661 -25.19994650799992542, 29.15852469800006475 -25.20097739499993494, 29.15864813100006359 -25.20176735999990569, 29.1583622530000639 -25.20198322799990365, 29.15781869400007054 -25.20227803999995686, 29.15770813800008909 -25.20170684099991831, 29.15575501000006398 -25.20213984599990908, 29.15436958400004741 -25.20247135699991858, 29.15436164100004035 -25.20196140899992088, 29.15433279700004832 -25.20083069899993689, 29.15433856600003537 -25.20018457999992734, 29.15430972000007159 -25.20005189499994458, 29.15320063400008976 -25.19919698099994321, 29.1538627030000761 -25.19855650099992772, 29.15462450700004737 -25.19790134999993469, 29.15524918700004164 -25.19728428999991721, 29.15613288000008652 -25.19652248399995997, 29.15697751800007964 -25.19572079299990719, 29.15746283000004269 -25.19625434099992844, 29.15830177200007611 -25.19721034399992732, 29.15844809900005075 -25.19744446699991158, 29.15858167100003939 -25.19794360599991023)))</t>
+  </si>
+  <si>
+    <t>demog_sas.61945</t>
+  </si>
+  <si>
+    <t>Mpheleng SP</t>
+  </si>
+  <si>
+    <t>Mpheleng</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.26194776200008718 -25.32509195699992688, 29.26199131300006684 -25.32548501299993049, 29.26243375200004948 -25.32571508199992749, 29.26294698200007716 -25.3260336389999452, 29.26338942100005625 -25.3260336389999452, 29.26386725500004005 -25.32622831199995517, 29.26415041500007774 -25.32652916999996151, 29.26438048300008177 -25.32690081899994539, 29.26453976200008356 -25.32734325699993505, 29.26473483600005565 -25.32736985799994045, 29.26409309800004976 -25.32915665599995236, 29.26381325700004155 -25.3294098469999085, 29.2635200890000533 -25.32975631699991936, 29.26342680900006243 -25.33006280999995852, 29.26340015700003505 -25.33043593099995761, 29.26321359600007099 -25.33103559299991048, 29.26306701300006807 -25.3315019949999396, 29.2629204280000863 -25.33184846599993989, 29.2629470800000604 -25.3322882169999275, 29.2629470800000604 -25.33248810399993189, 29.26272054200006778 -25.33267466599994577, 29.26256063400006724 -25.33340758299993567, 29.26209423000005572 -25.33415382699990914, 29.26152122100006281 -25.33491339699992295, 29.26056176500008732 -25.33620599899996151, 29.2604609830000868 -25.3364609169999575, 29.26010868800005582 -25.33735201699994377, 29.25948237500006144 -25.33840475299990658, 29.25882941300005768 -25.33927092899995159, 29.2584562920000657 -25.34021706099991889, 29.25798988800005063 -25.34168289599995205, 29.2579075850000514 -25.34261174599992827, 29.25772730300008106 -25.34370376999993368, 29.25737476700004436 -25.34520508799994332, 29.25737872700005582 -25.34523296599991227, 29.25701027200005555 -25.34507665199992843, 29.25663015300006009 -25.34475501299993994, 29.25633775400007153 -25.34465267299992774, 29.25608360800003993 -25.34307014199992736, 29.25521911900005989 -25.34282314499995437, 29.25402904300005957 -25.34239651399991544, 29.25410763300004646 -25.34226178799992013, 29.2545965170000386 -25.34146854699991991, 29.25505779800005257 -25.34098420299994814, 29.25548448200004259 -25.34036147499995195, 29.25579584700005498 -25.33961189199993669, 29.2561187430000551 -25.33823958299990409, 29.25503473300005552 -25.33802047199992913, 29.25474643300004018 -25.33799740799992151, 29.25348944300003495 -25.33780136499990476, 29.25308582200005958 -25.33766298099993719, 29.25297050200003923 -25.33714404099992734, 29.25164003100007903 -25.33699676099990938, 29.25172207400004254 -25.33605782499995485, 29.25190439200008541 -25.33541971299990792, 29.25196132700006046 -25.33521673299992472, 29.25199006300004712 -25.33511428199994953, 29.25229545200005177 -25.33383165499992629, 29.25255441200004825 -25.3327620339999271, 29.25257640700004913 -25.33267118199995949, 29.25320474200004028 -25.33055064599994921, 29.25356204700005591 -25.32947186499990266, 29.25372008500005094 -25.32870915899991715, 29.2539330930000574 -25.32725933199992951, 29.25436598000004906 -25.32598128399990856, 29.25474389600003988 -25.32488188799993623, 29.25493430100004844 -25.32386058599990974, 29.25515916000006555 -25.32388200199994799, 29.25538401900007912 -25.32392483199992839, 29.25570524700004071 -25.32404261499993581, 29.25618708700005755 -25.32409615399990344, 29.25655114500005993 -25.32417110599993748, 29.25675458900008152 -25.32425676599990538, 29.25688308000007964 -25.32437454999995907, 29.25706510900004886 -25.32455657999992127, 29.25728996800006243 -25.32459940899991935, 29.25762190200003943 -25.32446020999992697, 29.25784676100005299 -25.32419251999990095, 29.25805020500007458 -25.32396766199991944, 29.25830718800006025 -25.32383916999992834, 29.25869266000006519 -25.32387129299991102, 29.25892822800005533 -25.32395695399992519, 29.25924945400004162 -25.32408544599991629, 29.25955997400006936 -25.32425676599990538, 29.2598490780000553 -25.32436384199991153, 29.26003110700008847 -25.32435313499991025, 29.26044870200007963 -25.32450303999991092, 29.26074851400005628 -25.32455657999992127, 29.26106974100008529 -25.32464223899996014, 29.26111257100006924 -25.32473860699991519, 29.26110186400006796 -25.32496346599992876, 29.26124106300005678 -25.32509195699992688, 29.2614980440000636 -25.32498488199991016, 29.26194776200008718 -25.32509195699992688)))</t>
+  </si>
+  <si>
+    <t>demog_sas.57452</t>
+  </si>
+  <si>
+    <t>Thabakhubedu SP</t>
+  </si>
+  <si>
+    <t>Thabakhubedu</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.86861646900007372 -24.95652935799995475, 28.86859281300007751 -24.9565361169999278, 28.8679349350000507 -24.95674490499993681, 28.86725736000005327 -24.95697732899992616, 28.86680827000003546 -24.95713096599990877, 28.86641039100004491 -24.95727278299995078, 28.86603986700004043 -24.95742909799992049, 28.865654030000087 -24.95759187299995574, 28.86482281900003954 -24.95790308499994126, 28.86414846600007422 -24.9581140539999069, 28.86413135000003649 -24.9581181289999563, 28.86374342500005241 -24.9582615689999443, 28.86320766800008641 -24.95839550799991002, 28.86292403300006981 -24.95846641699995416, 28.86215979100006734 -24.95858065999993869, 28.86102918700004238 -24.95871065899990526, 28.8602727840000739 -24.95881290599993463, 28.85973864300007108 -24.95893160499991836, 28.8589706400000523 -24.95917934699991747, 28.85753373000005695 -24.95967483299995138, 28.85706400800006577 -24.95984752599991907, 28.85584908000004134 -24.96029418899991015, 28.85462756200007561 -24.96068507599994746, 28.85461036600008811 -24.96069057899995869, 28.85460149000005003 -24.96069271399994705, 28.85408339800005706 -24.96084448199991357, 28.85316196800005173 -24.96109908799991217, 28.85280733800004782 -24.9611960819999581, 28.85219507100003966 -24.96137794199995597, 28.85197380600004635 -24.96147493499995562, 28.85164342500007706 -24.96166588999994929, 28.85133729100004985 -24.96191746499994224, 28.85122301000006928 -24.96203138399994259, 28.85117072900004587 -24.96153143799995178, 28.85106608400008099 -24.96043848099992601, 28.85091493000004448 -24.9594617959999141, 28.85087423500004888 -24.95916530299990654, 28.85082772700008036 -24.95901996299994607, 28.85075796300003503 -24.95887462299992876, 28.85041496100006952 -24.95828744899995399, 28.85001382300004025 -24.95775841199991874, 28.84954873500004169 -24.95729913699994995, 28.84955353800006606 -24.957168607999904, 28.84964466200005972 -24.95675587199991696, 28.84978938700004392 -24.95621984999991128, 28.84990195200003882 -24.95558198399993444, 28.84993947300006312 -24.95522820899992666, 28.85003059700005679 -24.95432233299993641, 28.85009491900007106 -24.95406504199991105, 28.8501270810000392 -24.95392567699991559, 28.8501860420000753 -24.95331461199992873, 28.85024500600007968 -24.95282683199991425, 28.85028788800008215 -24.95228544999991982, 28.85034685100004026 -24.95197455799990394, 28.85041117300005453 -24.95173334799994791, 28.85051837600008184 -24.95148677899993572, 28.85067382300007921 -24.95124556799993343, 28.85074350600007165 -24.95113836399991669, 28.8507649480000623 -24.951074040999913, 28.8507649480000623 -24.95095075599994061, 28.8507649480000623 -24.95069346599990467, 28.85078638800007411 -24.95044153599991432, 28.85082926900008715 -24.95017352499991148, 28.85096863500007203 -24.94967502399993009, 28.85104903800004195 -24.94930516999994552, 28.85104903800004195 -24.94919260499995062, 28.85100615700008575 -24.9490532389999089, 28.85087751100007836 -24.94889243299991222, 28.85079373000007763 -24.94870172199995295, 28.85116687700008242 -24.94862704699994538, 28.85194720900005905 -24.9485515309999073, 28.85253455800005895 -24.94848440599992045, 28.85282823100004634 -24.94841727999994418, 28.85347431300004928 -24.94826624799992487, 28.85447280400006775 -24.94804809099991871, 28.85481682100004264 -24.9479138399999556, 28.85512727500008623 -24.94778797999993003, 28.85532865200008246 -24.94776280799993629, 28.85560554400007049 -24.94764533799991568, 28.8558656560000486 -24.94756143199992948, 28.8563187520000497 -24.94748591599994825, 28.85681380200009016 -24.94740200899991578, 28.85725352100007512 -24.94731881999990719, 28.85743471200004251 -24.94728453899995202, 28.85765286900004867 -24.94720063399995524, 28.85811435700009042 -24.94708316299994522, 28.85882756300009078 -24.9469321309999259, 28.85925548800008755 -24.9468146609999053, 28.8599938680000605 -24.94654615999991165, 28.8604050110000685 -24.94635317399990981, 28.86095040500003961 -24.94611823499991488, 28.86149580000005699 -24.94583295199993245, 28.86184820700003684 -24.94567352999990817, 28.8622425700000349 -24.94546376299990698, 28.86251107100008539 -24.94533790299993825, 28.86276279100007969 -24.9451952609999239, 28.8629389950000359 -24.94512813599993706, 28.8632830110000782 -24.94503583699992078, 28.86386196900008372 -24.94486802499994837, 28.86431506600007424 -24.94473377399992842, 28.86451644200008104 -24.94468342999994093, 28.86456678600006853 -24.94480928999990965, 28.8646758650000379 -24.94506100999990394, 28.86486045900005593 -24.9454469809999182, 28.86499470900008646 -24.94574065599994128, 28.86510378900004525 -24.94604271899993364, 28.86517930500008333 -24.94639512799994918, 28.86527999300005831 -24.94674753499992903, 28.86536390000009078 -24.94699925699995902, 28.86554010400004699 -24.94725097699995331, 28.86562401100007946 -24.9473432739999339, 28.86570581100005484 -24.94754607299995541, 28.86578211500005864 -24.94794032299995479, 28.86594744800004264 -24.9485507739999548, 28.86606190600008404 -24.94897045899995192, 28.86630279500008101 -24.94886778799991589, 28.86679262100005872 -24.94873199499994598, 28.86737459200008971 -24.94860105099991188, 28.86748570800006064 -24.94857425299994702, 28.86764998300003526 -24.94896045899992032, 28.86788263300007884 -24.94961963599990895, 28.86803773300005105 -24.95004616199992142, 28.8679380260000471 -24.95019572299992205, 28.86777738600005705 -24.95046714799991605, 28.86772753300004979 -24.95056685499992, 28.8676776790000531 -24.95070533799992063, 28.86772199300008879 -24.95094352799992521, 28.86781062300008216 -24.95115402099992252, 28.8681872950000411 -24.95152515399990989, 28.86835333600004105 -24.95166483999992124, 28.86780348800004958 -24.9520333499999083, 28.86764919600005896 -24.95217661999993197, 28.86764919600005896 -24.95230886799993186, 28.86779246600008264 -24.95267255499993553, 28.86795777700007193 -24.95312440699990475, 28.86812309000004007 -24.95354319699993084, 28.86818921400004001 -24.95391790299993318, 28.86825596600004928 -24.95447133499993697, 28.86828737300004377 -24.95477285299995174, 28.86825596600004928 -24.95502411699993672, 28.86828109100008533 -24.95519372099994371, 28.86843185100008213 -24.95568368799990822, 28.86861646900007372 -24.95652935799995475)))</t>
+  </si>
+  <si>
+    <t>Lefiswane SP</t>
+  </si>
+  <si>
+    <t>Lefiswane</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.71032430100007105 -25.02230495799994969, 28.71043479000007892 -25.02240181999991364, 28.71061720900007685 -25.0224914829999534, 28.71077180100007809 -25.02258732999990798, 28.71095112800009019 -25.02272646199992323, 28.71124794400003566 -25.0229830859999538, 28.71151075100004846 -25.02320260599992707, 28.71191269000007651 -25.02354580099995474, 28.71207655800003522 -25.02366019899994853, 28.71194051800006264 -25.02385189299991453, 28.71152002600007336 -25.02449808799991615, 28.7113252400000647 -25.0247578019999537, 28.71127205000004778 -25.02486549999991894, 28.7114134480000871 -25.02506741099995224, 28.71022163600008525 -25.02565151699991475, 28.7099148330000844 -25.0257990189999191, 28.7097319320000679 -25.0259465189999446, 28.70946052900006862 -25.02617072099991447, 28.70907702500005598 -25.02630642299993724, 28.70854012000006605 -25.02650112499992474, 28.70797371500003692 -25.02679612799994402, 28.70776131300004863 -25.02690822899995737, 28.70756027500004848 -25.0270636849999164, 28.70700921900004232 -25.02657703899990338, 28.70664399700007152 -25.02621181499995373, 28.70618078700005071 -25.02571297499991942, 28.70589573500006964 -25.02543683099992222, 28.70566261100003658 -25.0251934069999038, 28.70522891800004572 -25.02503851699992765, 28.70473327000007657 -25.02494558299991922, 28.70395882000008214 -25.02448091199994451, 28.70337023600006887 -25.02423308799990309, 28.70321534500004645 -25.02479069299994308, 28.70309143300005417 -25.02541025399995078, 28.70290556600008358 -25.02602981399991222, 28.70302947800007587 -25.02649448399995435, 28.70271969800006673 -25.02664937499991993, 28.70225502700003517 -25.02708306599993193, 28.70191426800005274 -25.02754773799995291, 28.70138764200004289 -25.02791947399992978, 28.70123275100007731 -25.02819827799993391, 28.7009849270000359 -25.02850805699995362, 28.70086101400005418 -25.02878685999991148, 28.70089199300008431 -25.0290966389999312, 28.70102553000003809 -25.03045156899992207, 28.7004636110000888 -25.02978429099994173, 28.69991638900006592 -25.02914189899991015, 28.69929779100004907 -25.02828537799990727, 28.69901228300005869 -25.02757160999993857, 28.69856022900006565 -25.02638199699993038, 28.69801300800008903 -25.02535892899993542, 28.69777508500004615 -25.02464516399993499, 28.697735132000048 -25.02452529999993658, 28.69734682500006784 -25.02336037999992868, 28.69706507900008319 -25.02252257299994653, 28.69748919300008083 -25.02235800699992296, 28.69816359100008185 -25.0221041149999337, 28.69901253900007987 -25.02169947599992383, 28.69935370500007821 -25.02155666299995573, 28.69963933200006068 -25.02151699199993118, 28.70001223400004164 -25.02155666299995573, 28.7001074430000358 -25.02150905799993552, 28.70028604100008351 -25.02106164299993907, 28.70037154500005272 -25.02087204599990855, 28.70048307300004353 -25.02074192999992874, 28.70070984600005204 -25.02061924899993528, 28.70088244500004748 -25.02059689899994055, 28.70112899700006892 -25.02057034799992152, 28.70139451400007147 -25.02058551999994052, 28.70191417000006595 -25.02061586499991108, 28.70239210100004357 -25.02065758899993853, 28.70258175700007541 -25.02068414099994698, 28.70267658400007349 -25.02054000199990469, 28.70279417000006106 -25.02026310499991268, 28.70296486000006553 -25.01995586499992896, 28.70304451500004461 -25.01986103799993089, 28.703222791000087 -25.01970551999994541, 28.70322658400004912 -25.01956896899991989, 28.70321899800006804 -25.01930345099992792, 28.70324175700005753 -25.01921620799993207, 28.70337451500006409 -25.01904551899991702, 28.70346554900004321 -25.01893551899991053, 28.7035755510000854 -25.01874965699994391, 28.70379555100004154 -25.01840069199994332, 28.70381451500009007 -25.01824138099993888, 28.70380692900005215 -25.01813138099993239, 28.70387141200006909 -25.01810862299993232, 28.70431520500005718 -25.01811241599995128, 28.70480451500003483 -25.0180744849999428, 28.70485003300007065 -25.01802896699990697, 28.70486899800005176 -25.01789620799991098, 28.70489555100004964 -25.01775207199995066, 28.70492968800004974 -25.01771034699993379, 28.70506244800003515 -25.01764207199994416, 28.70527995700007295 -25.01752928299993073, 28.70529779500003542 -25.01755338599991774, 28.70553065400008563 -25.0178444589999458, 28.70588962800007948 -25.01830931599994301, 28.70626627400008601 -25.01879706099992973, 28.70661556200008135 -25.01924689899993837, 28.70719770600004495 -25.01999839599994857, 28.70788040400003638 -25.02090865799993935, 28.70824027500003695 -25.02140083599994114, 28.70946807300003911 -25.02295675199991365, 28.70960037800006148 -25.0228985379999358, 28.70983852800003433 -25.02268155599995225, 28.71032430100007105 -25.02230495799994969)))</t>
+  </si>
+  <si>
+    <t>Seabe SP</t>
+  </si>
+  <si>
+    <t>Seabe</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.78537674100005006 -25.00490883299994493, 28.78736398400008056 -25.0056503409999209, 28.78752140700004247 -25.0057685639999363, 28.78722448100006659 -25.00693226699991101, 28.78712670200008006 -25.0075189419999333, 28.78691908000007516 -25.00947652499991136, 28.7868922710000561 -25.00968028099993035, 28.78662247600004775 -25.01173070999993797, 28.7862957970000366 -25.01338293099991006, 28.7859291800000392 -25.01353568799993354, 28.78531814900009067 -25.01387175499991145, 28.78434050300006675 -25.0139023069999098, 28.78259906900007081 -25.01393285899990815, 28.78140756100003728 -25.01381065199990417, 28.77994109100006881 -25.01368844599994645, 28.77929951000004394 -25.0137189979999448, 28.77847462000005407 -25.013993960999926, 28.77725256100006845 -25.01442168099993069, 28.77624436300004618 -25.01484940299991422, 28.77523616500008075 -25.01515491699990434, 28.77465568600007373 -25.01539932899993346, 28.77401410500004886 -25.01549098299994967, 28.77315866500003949 -25.01576594699992029, 28.7723337740000602 -25.01573539599991136, 28.77117281900007129 -25.01570484299992359, 28.77059234100005369 -25.01588815199994542, 28.77013406900005066 -25.01604090899991206, 28.76878980300006106 -25.01646862999990617, 28.76828416000006428 -25.01688425399993321, 28.76827287700007219 -25.01680244899995387, 28.76818833700008327 -25.01618953899992448, 28.76799669200005383 -25.014225167999939, 28.76775713500006759 -25.01147025899990695, 28.76770922400004338 -25.01072763299993085, 28.76770922400004338 -25.01000895999993645, 28.76770922400004338 -25.00921842199994671, 28.76756549000003815 -25.00840392699990389, 28.76746966600006772 -25.00766129899994894, 28.76737384300008671 -25.00689471599991975, 28.76723010900008148 -25.00612813399993684, 28.76715824200005045 -25.00557715099995448, 28.76691868500006422 -25.00440331999993759, 28.76679890600007639 -25.00356487099992364, 28.76687077300005058 -25.0026785079999172, 28.76694264000008161 -25.00215148199993109, 28.76741311200004247 -25.0021619509999482, 28.77094942100006847 -25.00273072799990359, 28.77421370500007924 -25.0032624109999233, 28.77604368300006854 -25.0035344349999491, 28.77940688600006069 -25.00404138799990506, 28.78201584100008859 -25.00446178799995778, 28.78437750200004075 -25.00480799999991177, 28.78537674100005006 -25.00490883299994493)))</t>
+  </si>
+  <si>
+    <t>Marapyane SP</t>
+  </si>
+  <si>
+    <t>Marapyane</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.86548924600003829 -25.05253057699991359, 28.86415399300005902 -25.05222689199990782, 28.86201178300007086 -25.05175262099993461, 28.86222361100004719 -25.05095560399990973, 28.86284793300006868 -25.04860655199991015, 28.8632114900000829 -25.04729396199991243, 28.86355144200007317 -25.0459860969999113, 28.86369791100008797 -25.0454295119999415, 28.86701806300004591 -25.0461327949999486, 28.86715322000003425 -25.04620037399990906, 28.86717011500007857 -25.04631863599990993, 28.8664943290000906 -25.0486838889999035, 28.86635917100005599 -25.0493089919999079, 28.86591991000005919 -25.05086330099993575, 28.86571717400005355 -25.05167424599994774, 28.86570203200005835 -25.05173985499993705, 28.86561580600005072 -25.05211350599995512, 28.86548924600003829 -25.05253057699991359)))</t>
+  </si>
+  <si>
+    <t>Koedoespoort SP</t>
+  </si>
+  <si>
+    <t>Koedoespoort</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.77373281300003782 -25.05518785499992873, 28.77262985100009018 -25.05512468899991063, 28.7722897310000576 -25.05574176399994712, 28.77190050500007601 -25.05652878399990868, 28.77155276200005574 -25.0572894709999332, 28.77040086400006658 -25.05697794999991856, 28.77034290600005306 -25.05750680999994984, 28.77024872700008018 -25.05748507599992081, 28.7701545460000716 -25.05745609899992132, 28.770125566000047 -25.0575357899999176, 28.77002414300005739 -25.05760823599990772, 28.76996618500004388 -25.05765894799992566, 28.76984302600004639 -25.05774588399992808, 28.76971986700004891 -25.0578038419999416, 28.76953150800005687 -25.05782557499992436, 28.76937212400008548 -25.05789077799994402, 28.76924172200006069 -25.05794873499991127, 28.76913305200008608 -25.0579849569999169, 28.76909682700005533 -25.05809362699994836, 28.76902438200005463 -25.05820229599993354, 28.76894469100005836 -25.05831096599990815, 28.76882153100007145 -25.05836167799992609, 28.76870561800006953 -25.05844136999991179, 28.76858245800008262 -25.05851381499991248, 28.7685027690000652 -25.05870217699992963, 28.76843756600004554 -25.05885431399991603, 28.76843756600004554 -25.05904267499994376, 28.76856796800007032 -25.05926001299991412, 28.76861143600007154 -25.0594483759999207, 28.76865490500006217 -25.05958602299995164, 28.7687563310000769 -25.05976713699993752, 28.76879255200003627 -25.05994101099992122, 28.76883602100008375 -25.06007141399993543, 28.76903887100007751 -25.06019457299993292, 28.76911131700006763 -25.06022355299995752, 28.76925621100008357 -25.06050609299995813, 28.76937212400008548 -25.06066547499995067, 28.76945181500008175 -25.06075965599995925, 28.76765514400005941 -25.06178839499995092, 28.76697414900007743 -25.06218685099992172, 28.76683649900007822 -25.06228102999995144, 28.76420120200003794 -25.06377499999990732, 28.76405162700007168 -25.0625862629999574, 28.76392928300003859 -25.06255567599993128, 28.76338637200007042 -25.06234157099993354, 28.76310344800003804 -25.06222687299992913, 28.76287405000005037 -25.06220393299992111, 28.76269053000004305 -25.06211217299994587, 28.76248407100007398 -25.06208923299993785, 28.7613523730000793 -25.06195159399993599, 28.76109238600008666 -25.06172219599994833, 28.7609929820000616 -25.06153102999991233, 28.76086299000007784 -25.06140103799992858, 28.76084005000006982 -25.06091165499992712, 28.76082475500004421 -25.06059814499991489, 28.76076358400007393 -25.0592217529999175, 28.76006774200004656 -25.05903823399995645, 28.75813314800006992 -25.05843415199990432, 28.75831666700008782 -25.05779948199995033, 28.75866841200007684 -25.05693541499994126, 28.75893604200007303 -25.05693541499994126, 28.75907368200006431 -25.0569583559999387, 28.75922661300006666 -25.05695070899992061, 28.7594483650000825 -25.05690482899990457, 28.75967011800008777 -25.0569583559999387, 28.75989951700006486 -25.05705011499992452, 28.76012891500005253 -25.057118935999938, 28.76019008800005849 -25.05717245999994702, 28.76025890700003629 -25.05682071699993685, 28.76053418500004 -25.05688953599991464, 28.76056477200006611 -25.05643838599991113, 28.76072535200006541 -25.05641544599990311, 28.76096239500003549 -25.05642309199993178, 28.7609776900000611 -25.05631603999995605, 28.76107709400008616 -25.05628545299992993, 28.76108474100004742 -25.05606370199990351, 28.76122238000004927 -25.05603311499993424, 28.76142119300004651 -25.05603311499993424, 28.76235408000007965 -25.05624721999993199, 28.76263700400005519 -25.05609428799994021, 28.76274405600008777 -25.05601017599991565, 28.76285875600007103 -25.05588782999990372, 28.76296580800004676 -25.05577312999992046, 28.76259877100005724 -25.05562784399995735, 28.76263700400005519 -25.05555902499992271, 28.76286640300008912 -25.05487847699993154, 28.76319520600003443 -25.05492435699994758, 28.76332519900006446 -25.05479436399991755, 28.76338637200007042 -25.05435850699990397, 28.76328696700005594 -25.05430497999992667, 28.76276699600003894 -25.05421322099994086, 28.76288934200005087 -25.05381559699992522, 28.76285111000004235 -25.05364737199994352, 28.7629046350000408 -25.05341797399995585, 28.76307286300004762 -25.05266860399990492, 28.76267523600006371 -25.05259978499992712, 28.76269053000004305 -25.05238567999992938, 28.762728763000041 -25.05207216999991715, 28.76269817600007173 -25.05188864999990983, 28.76297345500006486 -25.0518962959999385, 28.76326402600005849 -25.05190394399994602, 28.76330226000004586 -25.05159807699993735, 28.76398280600005819 -25.04962525299993104, 28.76373811600007002 -25.04957172599995374, 28.7638986950000799 -25.04890647099995249, 28.76402104100003498 -25.04879941799993048, 28.76411280000007764 -25.0487153049999165, 28.76402868700006366 -25.04844002799995906, 28.76397516100007579 -25.04823356899993314, 28.76388340200008997 -25.04805769699993334, 28.76376105600007804 -25.0476983039999368, 28.76458689100007859 -25.0473389149999548, 28.76450277800006461 -25.04720892199992477, 28.76428867300006686 -25.04705598999993299, 28.76415103400006501 -25.04691835099993114, 28.76399045400006571 -25.04674247899993134, 28.76386046300007138 -25.0466965989999153, 28.76378399700007549 -25.04666601299993545, 28.76360047900004702 -25.04649778899994317, 28.76342460400007894 -25.04636779499992372, 28.76283581500007358 -25.04653602099995169, 28.76161235700004681 -25.04668895299994347, 28.76104650800004947 -25.04683423799991715, 28.76085534300005975 -25.04692599699990296, 28.76043477900003609 -25.04708657699995911, 28.7600295080000592 -25.04729303599992818, 28.75967776500004902 -25.04750714099992592, 28.75954777200007584 -25.04759125399993991, 28.75941013300007398 -25.04767536599990763, 28.75923426000008476 -25.04777477199991154, 28.75900486200004025 -25.0479506449999576, 28.75889781000006451 -25.04805004999991525, 28.75878311000008125 -25.04810357699994938, 28.75868370400007734 -25.04804240399994342, 28.75836254800003644 -25.04775183299994978, 28.75846960000006902 -25.04763713299990968, 28.75882134400006862 -25.04732362199990803, 28.75898956900005032 -25.04719362899993484, 28.7591272090000416 -25.04710951699991028, 28.75947895100006235 -25.04681894499992723, 28.75984599000008757 -25.04668130599992537, 28.75975423100004491 -25.04636014899995189, 28.75941778000003524 -25.0453125619999355, 28.75992245700007288 -25.04522080299994968, 28.75984599000008757 -25.04505257699992171, 28.75968541300005654 -25.04489199799991184, 28.75950953900007789 -25.04454789999994091, 28.75979246300005343 -25.04440261499991038, 28.76004480200003854 -25.04436438399994813, 28.76017479400007915 -25.04453260699995099, 28.76043477900003609 -25.04513669099992512, 28.76192586900003789 -25.04488435199994001, 28.76229290600008426 -25.04485376599990332, 28.76233878500005403 -25.04493787799992788, 28.7625528910000412 -25.0449608179999359, 28.76286640300008912 -25.04499140499990517, 28.76404397900006416 -25.04486141399991084, 28.76418926800005238 -25.04530491599990683, 28.76490804800005208 -25.04528197599995565, 28.76477805500007889 -25.04483082499990587, 28.7647321770000417 -25.04467024699994226, 28.76552742600006241 -25.04461671999990813, 28.76569564900006526 -25.04454025399991224, 28.76565741700005674 -25.04436438399994813, 28.76649089700003969 -25.04399734499992292, 28.76710255400007554 -25.04384576699993659, 28.76746450900003538 -25.04369064299993397, 28.76820293900004799 -25.04278208699992092, 28.77373281300003782 -25.05518785499992873)))</t>
+  </si>
+  <si>
+    <t>Ramantsho SP</t>
+  </si>
+  <si>
+    <t>Ramantsho</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.93193390900006534 -24.90181914599992297, 28.93067053800007216 -24.90209379199990281, 28.93019448400008287 -24.90075717899992469, 28.93019552400005523 -24.90072556199993414, 28.93032139000007419 -24.90070149999991145, 28.93051203900006385 -24.90067373499994119, 28.93067307300003677 -24.90065707599995903, 28.93096552500009011 -24.90061080299994956, 28.93123021200005951 -24.90056082599994625, 28.93127215900005922 -24.90055067699995561, 28.93120152000005874 -24.89991492999990896, 28.93098180300006561 -24.89923747099993534, 28.93078039600004558 -24.89872479899992186, 28.93050575000006575 -24.8981022669999561, 28.9325198210000849 -24.89762621299990997, 28.93376488400008384 -24.8972417089999567, 28.93453389300003664 -24.89705861099992035, 28.93403953000006368 -24.89585016799992445, 28.93440572500009011 -24.89570368999994798, 28.93494947600004252 -24.89553613999993331, 28.93496502600004305 -24.89581414299993867, 28.93566561600005116 -24.89995806599995376, 28.93530290200004629 -24.9000614089999317, 28.93484515900007636 -24.90018957599994565, 28.93469959600008679 -24.90021489299994073, 28.93449978900008546 -24.90028062099992212, 28.93402245200007883 -24.90040214099991545, 28.93352685700006077 -24.90057408199993461, 28.93359503300007418 -24.90073478099992599, 28.9337584630000606 -24.90118763499992838, 28.93281277700003784 -24.90154449799990743, 28.93193390900006534 -24.90181914599992297)))</t>
+  </si>
+  <si>
+    <t>Malebitsa SP</t>
+  </si>
+  <si>
+    <t>Malebitsa</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.00121006200004103 -24.93710336699990648, 28.99993528100003459 -24.93785426599993116, 28.9999605650000376 -24.93789219199993568, 29.00012099900004614 -24.93817260299994132, 29.00037471700005653 -24.93856414299995095, 29.00055012800004306 -24.93884605299990653, 29.0006253040000388 -24.93899013999993031, 29.00074363600003835 -24.93921845299990991, 29.00088842000008071 -24.93944676499995694, 29.00133300700008476 -24.94010345499992809, 29.00008442100005368 -24.94082542599994667, 28.99974327600006063 -24.9402462279999213, 28.99925731000007545 -24.93939925799992352, 28.99871580400008497 -24.93860782599995218, 28.99820206800006872 -24.93767754799995373, 28.99767444600007593 -24.93678892199994834, 28.99721625000006497 -24.93602525999995123, 28.99680116900003668 -24.93529619799994634, 28.99638777300003767 -24.9346623229999409, 28.9984134170000516 -24.93342213299990817, 28.9990970680000828 -24.93483320799992953, 28.99969080200008875 -24.93455380399990418, 29.00014483400008203 -24.93537455399990677, 29.0006337920000874 -24.93631754199992656, 29.00121006200004103 -24.93710336699990648)))</t>
+  </si>
+  <si>
+    <t>Uitvlugt SP</t>
+  </si>
+  <si>
+    <t>Uitvlugt</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.05217366900006937 -24.92307301799991137, 29.05189981100005525 -24.92297052699990445, 29.05135814800007665 -24.92292128499991577, 29.05108731700005364 -24.92287204199993766, 29.0506277250000835 -24.92287204199993766, 29.05057027600008723 -24.92292128499991577, 29.05006964800008973 -24.92283921399990732, 29.04968392000006361 -24.92273252299992237, 29.04901915200008489 -24.92260121199990408, 29.04807534700006499 -24.92240424399994936, 29.04782913700006475 -24.92291307699991876, 29.04767320400003427 -24.92315928799990843, 29.04749265000003788 -24.92325777199994263, 29.04732851000005667 -24.92333163499995408, 29.04709050700006401 -24.92338908399995034, 29.04638470500003677 -24.92352039599995805, 29.04616311500006987 -24.92355322399993156, 29.04569531600003529 -24.92355322399993156, 29.04517827400007945 -24.92353680999991639, 29.04487461500008294 -24.92341370499991626, 29.04450530000008257 -24.92329880699992373, 29.04400467300007449 -24.92320032299994637, 29.04364356400003544 -24.92303618299990831, 29.04330707800005484 -24.92301156099995296, 29.04311011000004328 -24.92300335399994538, 29.0429213490000393 -24.92305259599993406, 29.04175595500004192 -24.92387329699994325, 29.04161643600008347 -24.92377481299990905, 29.04150153600005524 -24.92358605199990507, 29.0414030530000673 -24.92343011999992086, 29.04120608500005574 -24.92312645999993492, 29.04120608500005574 -24.92301156099995296, 29.04118967000005114 -24.92274072999992995, 29.04105835900008969 -24.9225355549999108, 29.04086139200006755 -24.92260941899991167, 29.040467455000055 -24.92268328199992311, 29.03990117200004306 -24.92281459399993082, 29.03975344500008759 -24.92283921399990732, 29.03895736500004432 -24.92261762599991926, 29.03865370700003723 -24.92335625599991999, 29.03862908600007131 -24.92338908399995034, 29.03754576000005727 -24.92203492799990272, 29.03716003200008799 -24.92148505899990596, 29.0362408470000446 -24.92022938699994938, 29.03552199300008851 -24.91930375399994091, 29.0348884190000831 -24.91803660599993009, 29.03420415900006901 -24.91714960099994869, 29.03291166700006443 -24.91608519699991575, 29.03093756200007647 -24.91427673999993431, 29.03218298300004108 -24.91451624299992318, 29.03776685100007171 -24.91570007699993994, 29.04010714800006099 -24.91618592799994758, 29.0409419910000679 -24.9163501599999222, 29.04170156100008171 -24.91648017699992579, 29.04322754500003612 -24.91661703599993416, 29.0460742220000725 -24.91690444099992874, 29.04948886600004698 -24.91723290399994539, 29.04981048600006943 -24.91725343299992801, 29.05157597400005898 -24.91739713499993059, 29.0529582540000888 -24.91756820999995625, 29.05321828900008541 -24.91762979599991468, 29.05417938500005448 -24.91763966599995683, 29.05513293900008875 -24.9177985929999295, 29.05509320900006287 -24.91863295399991785, 29.05382180100008327 -24.92235447099994872, 29.05196766400007391 -24.92214257099993802, 29.05199850500008552 -24.92239381099994944, 29.05208199600008356 -24.92274741599993604, 29.05217366900006937 -24.92307301799991137)))</t>
+  </si>
+  <si>
+    <t>Rathoke SP</t>
+  </si>
+  <si>
+    <t>Rathoke</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.9671790450000799 -24.97541156099993032, 28.9672530730000517 -24.97526672599991571, 28.96761056400004009 -24.97462534299995696, 28.96756771400004027 -24.97461709399993879, 28.96615393800004767 -24.97419370599993727, 28.96590435300004174 -24.97475758199993834, 28.96514635300007967 -24.97450799799992183, 28.96563211100004764 -24.97323924099993064, 28.96694142800004101 -24.97110966899992945, 28.96694891400005645 -24.97108775799995328, 28.96796574100005728 -24.97145751199991537, 28.96872374100007619 -24.96984907499995643, 28.96896456400008901 -24.96937451199994484, 28.96935232500004531 -24.968610392999949, 28.96986074000005829 -24.96744566199993187, 28.97026747200004593 -24.96663219999993544, 28.97096076300005052 -24.96514393199993265, 28.97145069000004014 -24.96534729899991589, 28.97202381200008858 -24.96568932299993548, 28.9721809570000346 -24.96541200399991567, 28.97236583500006191 -24.96526410299992449, 28.97260617700004559 -24.96494056599993883, 28.97288349200005086 -24.96529183499990268, 28.97380788300006316 -24.96678934599992772, 28.97479285900004697 -24.96835969199992178, 28.97522969400006332 -24.96915145399992753, 28.97585764200005087 -24.97064396999991231, 28.97588661400004639 -24.97070958899990956, 28.9769224260000442 -24.97305565799990745, 28.97751397100006443 -24.97442986499993367, 28.9780782170000748 -24.97534903699994402, 28.9774490410000567 -24.9754763389999539, 28.97720737800005963 -24.97590596299994559, 28.97699256700008164 -24.97628188399994542, 28.97680460700007643 -24.97671150499991199, 28.97637498400007416 -24.97663095099994734, 28.97581110400005855 -24.97676520799990385, 28.97546203500007778 -24.97703372199993055, 28.97487130200005367 -24.97676520799990385, 28.97446853100007047 -24.97681891099995255, 28.97430742300008433 -24.97676520799990385, 28.97368984100006628 -24.9770068729999366, 28.97342132700003958 -24.9771679789999439, 28.97334077100003924 -24.97671150499991199, 28.97326021700007459 -24.97614762499995322, 28.97315281300006973 -24.97579855699990503, 28.97312595900007182 -24.97518097299990814, 28.97213245800008963 -24.97523467699994626, 28.97113895400008232 -24.97526152799991905, 28.97036026200004244 -24.97531522899993206, 28.96931305700007897 -24.97542263499991577, 28.96858806800008779 -24.97553004299993518, 28.9678899300000694 -24.97553004299993518, 28.9671790450000799 -24.97541156099993032)))</t>
+  </si>
+  <si>
+    <t>Doornlaagte SP</t>
+  </si>
+  <si>
+    <t>Doornlaagte</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.92104829300006941 -24.95122997599992232, 28.92105995200006419 -24.95128943699995716, 28.92122364100004006 -24.95212427699993896, 28.921264567000037 -24.9525065449999488, 28.9205595750000839 -24.95260144899992838, 28.92016640700006747 -24.95264212199992926, 28.91980035400007409 -24.95268279399994071, 28.91916314900004181 -24.95281836899994232, 28.91900045900007399 -24.95212693499991019, 28.91879709600004844 -24.95115079299995386, 28.91841748500007725 -24.95121858199991038, 28.91784807000004776 -24.95131348399991111, 28.91756336200006672 -24.95136771399995723, 28.9169261580000807 -24.95146261699994739, 28.91595001600006754 -24.95159819099990273, 28.91515012100006743 -24.9517337669999506, 28.91463493500003779 -24.95177443799991579, 28.91426754900004426 -24.95186597199995049, 28.91376760700006798 -24.94913933599991651, 28.91373883100004605 -24.94890712599993776, 28.9146891650000839 -24.94869687999994312, 28.91565175000005183 -24.94850707499995224, 28.91665500700008806 -24.94845284499990612, 28.91687192700004516 -24.948493517999907, 28.91702106000008143 -24.94850707499995224, 28.91772605100004512 -24.94838505699993902, 28.9188106540000831 -24.94823592499994902, 28.91927161000006663 -24.94820880899993654, 28.9204163960000642 -24.9480072049999535, 28.92104829300006941 -24.95122997599992232)))</t>
+  </si>
+  <si>
+    <t>Spitspunt SP</t>
+  </si>
+  <si>
+    <t>Spitspunt</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.06709276700007649 -24.97860764999995808, 29.06747347000003856 -24.97888587599993571, 29.06903475200005005 -24.98066822499993123, 29.07113373900006081 -24.98283853499992802, 29.07132582500008766 -24.98424455399992894, 29.06813942400003725 -24.98816491099995574, 29.06765371300008383 -24.98816390999991199, 29.06671772100008866 -24.98821761399995012, 29.06612299400006805 -24.98825173799991717, 29.066107655000053 -24.98825261799993314, 29.06628507200008471 -24.98611094699992918, 29.06544868000008819 -24.98619965499995033, 29.0648150490000603 -24.98627569099994616, 29.06457426900004748 -24.98627569099994616, 29.06371253100007834 -24.98638974499993992, 29.06361795800006576 -24.98642126999993707, 29.06356046100006552 -24.9864404349999063, 29.06344886200008659 -24.98638342199990348, 29.06239458000004561 -24.98584482199993317, 29.06154236700007232 -24.98542350099995701, 29.0587072070000545 -24.98402184199994736, 29.05815953500007254 -24.98374939499990433, 29.0571173300000396 -24.98323542999992242, 29.05566110000006574 -24.98250731599995333, 29.05501310100004275 -24.98219494599993595, 29.0563419960000715 -24.98030462999992096, 29.05663123800007952 -24.98046188799992251, 29.05739494500005549 -24.98087710699991248, 29.05822299100003647 -24.97979349099995261, 29.05875457600006939 -24.98004905999994207, 29.05960148800005527 -24.97866686499992284, 29.06205709100004242 -24.97868114299990339, 29.06228552000004584 -24.97868828099990424, 29.06295652700003984 -24.97865972699992199, 29.06337769300006357 -24.97872397199995476, 29.06403442300006645 -24.97880963299991208, 29.06493200000005572 -24.97876601899992011, 29.0670342410000444 -24.97856487699993977, 29.06709276700007649 -24.97860764999995808)))</t>
+  </si>
+  <si>
+    <t>Matlerekeng SP</t>
+  </si>
+  <si>
+    <t>Matlerekeng</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.94841527200009068 -24.97867287799994074, 28.95002420700006951 -24.97877511799993044, 28.95005111200003967 -24.97854373399991346, 28.95082060200007845 -24.97852758999994194, 28.95087441300006503 -24.97901188499992031, 28.95198290900003713 -24.97894193099995164, 28.95259096900008444 -24.97899574199993822, 28.95312369300006594 -24.97901188499992031, 28.95285464000005504 -24.97981904199991732, 28.95280083000005789 -24.97994818799992345, 28.95269859000006818 -24.98049167399994985, 28.95294611800005669 -24.98057777099995747, 28.9527282870000704 -24.98117751299992051, 28.95505011000005879 -24.98186922399992227, 28.95477567600005386 -24.98288624099990329, 28.95607789100006357 -24.98311224699995137, 28.95588119400008509 -24.98390927399992734, 28.95543813700004421 -24.98539955399991186, 28.95414924700008896 -24.98511760899992851, 28.95384819100007689 -24.98616737399993326, 28.95373492600003829 -24.9864424479999343, 28.95371272200003432 -24.98649636799990503, 28.95231251700005259 -24.98642146699995692, 28.95144092800006774 -24.98635265699994079, 28.94994683200008012 -24.986157976999948, 28.94817658700003449 -24.98598526999995784, 28.94714034700007232 -24.98581256299991082, 28.94619046100007154 -24.98572620799990318, 28.94511104200006457 -24.98568303299992976, 28.94415714500007653 -24.98572209399992516, 28.94313494900006845 -24.98573912999995628, 28.94210446300007789 -24.98577514799995924, 28.94105243500007418 -24.98589891599993962, 28.93967078200006426 -24.98602844599992068, 28.93824595100005581 -24.98602844599992068, 28.93556436800008669 -24.98646139799990351, 28.93444866200007937 -24.98646139799990351, 28.93460389000006217 -24.98587928999995711, 28.93437104700007012 -24.98585018599993646, 28.93381804400007695 -24.98563674599995466, 28.93344937700004493 -24.98559793799995532, 28.93319713100004265 -24.98553972799993517, 28.93287697100004152 -24.98545241199991551, 28.93262472500003923 -24.98544270999991568, 28.93218814500005465 -24.98545241199991551, 28.93182917800004361 -24.98553972799993517, 28.93165454500007172 -24.98571435999991763, 28.93150901900008876 -24.98585988599995744, 28.93044122900005277 -24.9858653299999105, 28.93052315100004535 -24.98536209099995631, 28.93052191800006767 -24.98535737699995707, 28.93040786300008449 -24.9853301029999102, 28.93046463300004234 -24.98484991599991645, 28.93082859700007248 -24.98446191699991914, 28.9310140420000721 -24.98409377099994799, 28.93108290000003535 -24.98395707199995286, 28.93140132700006006 -24.98396320899990997, 28.93103093000007675 -24.98178771899995354, 28.93088000600005216 -24.98131876299993337, 28.93149447800004737 -24.98094751999991558, 28.93312867200006622 -24.97948880899991764, 28.93441992200007462 -24.9802436989999137, 28.93689920200006327 -24.98147217199993975, 28.9369492440000613 -24.98134491799993384, 28.93726573100008181 -24.98054010299995298, 28.93832041700005675 -24.98101901899991617, 28.93864758500006928 -24.98058902599990461, 28.93948075400004427 -24.97955622699993228, 28.94020779500004892 -24.98021175699994956, 28.9404461690000403 -24.98043821199991044, 28.94092149800007974 -24.98087040499990508, 28.94103090600003725 -24.98058906899990461, 28.94155710900008671 -24.98054217999992943, 28.94157284500005289 -24.98050028899990593, 28.94168571700004122 -24.98019983799991905, 28.94183962500005691 -24.9795822769999063, 28.94198491500003456 -24.97906569599990689, 28.9427813100000435 -24.97910336299992196, 28.94405123800004276 -24.97805943799994566, 28.94622518400007039 -24.97653660199995329, 28.94774264000005815 -24.97817782199990688, 28.94841527200009068 -24.97867287799994074)))</t>
+  </si>
+  <si>
+    <t>Tshikanosi SP</t>
+  </si>
+  <si>
+    <t>Tshikanosi</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.94106264200007672 -25.29005731299992021, 28.94108456400005025 -25.29029056899992156, 28.94110253400003785 -25.29040070899992543, 28.94071808500007137 -25.29050245099995209, 28.94039016700008915 -25.2905844299999103, 28.9409921640000789 -25.29231491599995252, 28.94023397500006922 -25.29252154099992822, 28.94023964400008708 -25.29241385099993522, 28.94017123500003663 -25.29228615599993191, 28.93985655900007714 -25.29119619099992633, 28.93967869800007975 -25.29079030399992689, 28.93857864700004257 -25.29102245199993604, 28.93738038700007564 -25.29119032299990977, 28.93735150800006295 -25.29060431199991399, 28.93733752300005335 -25.29045247099992366, 28.93718383100008396 -25.29038670699992508, 28.93700632800005224 -25.2903151099999377, 28.936879541000053 -25.29027781999991475, 28.93677512800007889 -25.29018981399991617, 28.93649210400008087 -25.29023855299993784, 28.93644055700008266 -25.28988011399991365, 28.93628157300008752 -25.28863853499990455, 28.93626695800008974 -25.28854754599990429, 28.93704909100006262 -25.28844553699991593, 28.93749284400007582 -25.28839810099992746, 28.93804524000006495 -25.28832312299994101, 28.93916449500005683 -25.28816431399991416, 28.93955138700005136 -25.28810628099995483, 28.93991847000006601 -25.28807337299991786, 28.94010680100006994 -25.28804467899993824, 28.94074632900003508 -25.2879848139999126, 28.94078257300003543 -25.2883373709999546, 28.94079245800008948 -25.28879536299990605, 28.94080234300008669 -25.28893374899990931, 28.94083529200008797 -25.28905895599990572, 28.94083858600004078 -25.28936867699991353, 28.94088801100008368 -25.28958943599991471, 28.94100992200003475 -25.28994528599992009, 28.94106264200007672 -25.29005731299992021)))</t>
+  </si>
+  <si>
+    <t>Kwaggafontein A</t>
+  </si>
+  <si>
+    <t>Kwaggafontein</t>
+  </si>
+  <si>
+    <t>MP315</t>
+  </si>
+  <si>
+    <t>Thembisile</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.01062861500008694 -25.1597306699999308, 29.01040928100007932 -25.16079363999995167, 29.01101584100007358 -25.1612640339999416, 29.01157288600006723 -25.16168491199994151, 29.01333067300004132 -25.16304657799992128, 29.01395982100007132 -25.16352866599993376, 29.0135905510000498 -25.16424191499993412, 29.01341506800008574 -25.16458086099993352, 29.01322411600006035 -25.1649648629999092, 29.01211728000004086 -25.16719069899994565, 29.01139010100007454 -25.1686257519999117, 29.01101603800003659 -25.16936394799995469, 29.01017195900004708 -25.16869842399995605, 29.00933368300007942 -25.1680134919999432, 29.0080967150000788 -25.16705254199990804, 29.00676774000004343 -25.16596891699992966, 29.00611347700004217 -25.16547821899990822, 29.00557368700003735 -25.165190255999903, 29.0058940000000689 -25.16480587999990348, 29.00586502800007338 -25.16461273699991352, 29.00584467200008021 -25.1644770289999542, 29.00579534400003467 -25.16419750499994734, 29.00591044200007218 -25.1638850959999445, 29.00595397100005357 -25.16380473499992831, 29.00633794900005569 -25.16309585299995888, 29.00653338900008293 -25.16274504399990519, 29.00710227100006477 -25.16193789999994124, 29.00680187700004353 -25.16183341599992218, 29.00836914200004912 -25.15865970699991294, 29.01027597900008459 -25.15945639899990738, 29.01062861500008694 -25.1597306699999308)))</t>
+  </si>
+  <si>
+    <t>Waterval A</t>
+  </si>
+  <si>
+    <t>Waterval</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.84665479200003801 -25.98021166699993501, 30.84673372800006064 -25.98039118899993127, 30.84669938100006448 -25.98128421099994512, 30.84642460400004893 -25.98176506999993762, 30.84614982900006908 -25.98207419199991364, 30.84618417600006524 -25.98234896899992918, 30.84645895100004509 -25.98276113199995052, 30.8462185230000614 -25.98282982499995342, 30.8450507260000677 -25.98262374399990904, 30.84453552100006846 -25.98258939699991288, 30.84347076400007381 -25.98231462199993302, 30.84213123200004247 -25.98186810999993668, 30.84137559800007011 -25.98179941699993378, 30.84055127000004859 -25.98176506999993762, 30.83938347300005489 -25.98131855799994128, 30.83842175700004873 -25.98104378199991515, 30.83649832600008267 -25.98018510699995431, 30.83526183300006096 -25.97966990399993392, 30.8338879540000903 -25.97867383999994217, 30.83210960600007411 -25.97743333599993321, 30.83090898900007915 -25.97640841899993802, 30.83044045500008679 -25.9757934689999388, 30.83026821500004644 -25.97563558199993849, 30.83025500400003693 -25.97554310799995392, 30.83026064000006272 -25.97513172399993664, 30.83018737900005135 -25.97488376499995866, 30.83015920200006121 -25.97478796299992609, 30.8301704720000771 -25.97465271399994435, 30.83015920200006121 -25.97452873499992165, 30.8302268270000468 -25.97429768299991792, 30.83029445200008922 -25.97396519399995896, 30.83031135700008463 -25.97380740199992033, 30.83033523700004253 -25.9736665169999128, 30.83085799300005192 -25.9736665169999128, 30.83177656500004105 -25.97368905799993399, 30.83216540800003713 -25.97369469399990294, 30.83263314700008095 -25.97370032999992873, 30.83297850300004939 -25.97370548299994653, 30.83301072000006116 -25.97370596599995451, 30.8333375740000406 -25.97369469399990294, 30.83359116700006552 -25.97370596599995451, 30.83392365600008134 -25.97367215199994916, 30.83425051000006079 -25.97361579799991205, 30.8344590200000539 -25.97350872599992044, 30.83471825000003719 -25.97337347499990301, 30.8347464260000379 -25.97313678799991976, 30.83464498900008266 -25.9730015379999486, 30.83450973900005465 -25.97291700699992134, 30.83434631200003651 -25.97280993399994031, 30.8342392400000449 -25.9726915909999434, 30.83426741600004561 -25.97249998699993512, 30.83431250000006685 -25.97238727899991773, 30.83436885400004712 -25.97230838299992683, 30.83443647900008955 -25.97213932099992917, 30.83448719700004403 -25.97186882099992999, 30.83471261400006824 -25.97194771699992089, 30.834763333000069 -25.9716659459999164, 30.83459990600005085 -25.97151942499993993, 30.83441393700007893 -25.97142925899993315, 30.83428995800005623 -25.97135036299994226, 30.83420542700008582 -25.97127146699995137, 30.83403636500008815 -25.97120947799993473, 30.83395746900004042 -25.97115312399995446, 30.83393492700008665 -25.97103477999991128, 30.83385603100003891 -25.97092770799991968, 30.83372078200005717 -25.9708375419999129, 30.83361370800008672 -25.97069102099993643, 30.83354608400009056 -25.9705670409999243, 30.83351227100007463 -25.97040361499995242, 30.83351227100007463 -25.97033035399994105, 30.8333601150000618 -25.97016129199994339, 30.83305094000007784 -25.97003360099995461, 30.83292785500003674 -25.96982259799995063, 30.8330685230000654 -25.96945334399993044, 30.8335256960000379 -25.96945334399993044, 30.83414112100007287 -25.9697346799999309, 30.83435212400007686 -25.9697346799999309, 30.83480929600005993 -25.96978742999993983, 30.83514338400004817 -25.96982259799995063, 30.83542472000004864 -25.96985776499991516, 30.83554780600007916 -25.96955884399994829, 30.83560055700007752 -25.96899616899992225, 30.83553022200004534 -25.9687324169999556, 30.83545988800005944 -25.96836316199994599, 30.83524888500005545 -25.96797632399994882, 30.83498513200004254 -25.96758948499990538, 30.83421015300007184 -25.96688189499991495, 30.83442299000006415 -25.96680348099994262, 30.8350965080000492 -25.96580784699995093, 30.83755630900003553 -25.96478292999995574, 30.83940115800004378 -25.96440224699995269, 30.8399575430000823 -25.96481221299995923, 30.84189024400006929 -25.96469508099994528, 30.84314942700007123 -25.96443152999995618, 30.84420362900004875 -25.96431439599990654, 30.84552137900004709 -25.96405084599990687, 30.84683913000003486 -25.96387514599990709, 30.84798338300004161 -25.96382416699992746, 30.84836258700005374 -25.96398107899995011, 30.84863718100007191 -25.96392877399995314, 30.84899023400004126 -25.96399415499990937, 30.84936943800005338 -25.96430797899995468, 30.84991863000004741 -25.96430797899995468, 30.8505462780000812 -25.96496177899990698, 30.85180157300004566 -25.96510561499991354, 30.85262536100003672 -25.96510561499991354, 30.85374989700005699 -25.96484409499993262, 30.8539591130000872 -25.96453027099994415, 30.85440369800005556 -25.96459565099991096, 30.85493981200005464 -25.96481794299995727, 30.85550208000006478 -25.96511869099992964, 30.8558812840000769 -25.96530175499992765, 30.85636509600004729 -25.96541943799991259, 30.85683583300004784 -25.96543251499991811, 30.85721503500008112 -25.96531483199993318, 30.85776422700007515 -25.96521022299992865, 30.85814343100008728 -25.9652756029999523, 30.85835264600007122 -25.9656286539999428, 30.85861416700004156 -25.96594247799993127, 30.85887568700007932 -25.96604708599994638, 30.8591633590000356 -25.96612554199992928, 30.85946410600007539 -25.96615169399990464, 30.86002637500007495 -25.96615169399990464, 30.8603532740000901 -25.96611246599991318, 30.86047095800006446 -25.96649166999992531, 30.86009175500004176 -25.96687087399993743, 30.8612293660000887 -25.96738083699995059, 30.86159549400008473 -25.96745929399992292, 30.86204007800006366 -25.9679823339999416, 30.86243235800003504 -25.96816539799993961, 30.86354381700004978 -25.96887150099991004, 30.86409300900004382 -25.96876689299995178, 30.86478603800009068 -25.96843999399993663, 30.86523062100008019 -25.96841384199990443, 30.86583211700008178 -25.96925070599991159, 30.86615901700008635 -25.96976066899992475, 30.86638130900007582 -25.97020525299990368, 30.86689127200008897 -25.970610608999948, 30.86737508400005936 -25.97096366099992792, 30.86771506000008003 -25.97098981299990328, 30.86842116500008615 -25.97109442099991838, 30.86885267200005956 -25.97130363599995917, 30.86974184000007426 -25.97152592799994864, 30.87042179100006933 -25.97170899199994665, 30.87120635100006893 -25.97153900399990789, 30.87163785900008861 -25.97121210399990332, 30.87209551800003737 -25.97083289999994804, 30.87244857100006357 -25.97051907699994899, 30.87261855800005605 -25.97024448099995197, 30.87286700200007772 -25.97007449299991322, 30.87322005400005764 -25.96972143999994387, 30.87329851000004055 -25.96942069299990408, 30.87349465000005466 -25.96896303299990905, 30.87369079000006877 -25.96876689299995178, 30.87362541000004512 -25.96847922199992809, 30.87376924600005168 -25.96830923299995675, 30.87386077800005069 -25.96813924599990742, 30.87403076700007887 -25.9679954099999577, 30.8740569180000648 -25.96769466199992848, 30.87430536300007589 -25.96748544599995512, 30.87497223800005486 -25.96732853399993246, 30.87535144000008813 -25.9670800899999108, 30.87570449300005748 -25.9667270389999203, 30.87684210400004758 -25.96658320199992431, 30.8775482090000537 -25.96645244099994443, 30.87809740000005831 -25.96645244099994443, 30.87839814800008753 -25.96604708599994638, 30.87896360700005971 -25.96561870799990857, 30.87906122900005812 -25.96265690999990738, 30.87911817000008341 -25.96097718999993731, 30.87895542600006138 -25.96078956099995594, 30.87899591600006488 -25.96029357399993387, 30.87914545800003907 -25.96017220199991016, 30.87919918300008248 -25.9585873319999223, 30.87922575600003938 -25.95780342199992674, 30.87924390700004551 -25.95737839199995278, 30.8794822750000435 -25.95730183599994234, 30.87953535200006172 -25.95720326699995439, 30.87956947100008165 -25.95700233399992385, 30.87966804200004844 -25.95672936999994818, 30.87979315100005806 -25.95642228599990631, 30.8799637520000374 -25.95616069499993728, 30.88009644400005982 -25.95596734599990896, 30.88009644400005982 -25.95581569899991337, 30.88117757800006302 -25.95418373699993708, 30.88220979000004718 -25.95376925699991943, 30.88313211800004865 -25.9544870069999547, 30.88450971600008188 -25.95986128199990617, 30.88479442300007349 -25.96167441699992651, 30.8849192940000421 -25.96244362499993485, 30.88489045000005717 -25.96289560299993582, 30.88482179100003577 -25.96296189499992124, 30.88471998700003951 -25.96299977499995748, 30.88460871200004476 -25.96306133199993837, 30.88452111200007266 -25.96318917999991527, 30.8845353190000651 -25.9632886169999324, 30.8845353190000651 -25.9633549079999284, 30.88446429100008572 -25.96337621599991508, 30.88437432400007765 -25.96338095099991961, 30.88434354600008191 -25.96340936199993621, 30.88433407600007286 -25.96346855099994855, 30.88429382700007864 -25.96349459399993975, 30.88422990400005119 -25.96349695999992946, 30.88416361200006577 -25.96350406399994881, 30.88411389300006249 -25.96354194499991763, 30.88404286700006196 -25.96356325299990431, 30.88397894300004509 -25.96358692699993753, 30.88391502000007449 -25.96361533899994356, 30.88387713700006998 -25.96368163099992898, 30.88381558200006793 -25.96369110099993804, 30.88371140900005685 -25.96368399799990812, 30.88361197100005029 -25.96375029099993981, 30.88349122700003591 -25.96377396499991619, 30.88331366000005573 -25.96385209399994665, 30.88309111000006624 -25.96395863399993686, 30.88293485200006216 -25.96402492599992229, 30.88286856100006617 -25.96409831999994822, 30.88282594500003597 -25.96412672999991855, 30.88276912400004903 -25.96415750899990371, 30.88272887500005481 -25.9641456709999261, 30.88268389200004549 -25.96411489299993036, 30.88265784800006486 -25.96411725999990949, 30.88264601100007667 -25.96412909799994395, 30.8826223350000646 -25.96417644899992183, 30.88256551400007766 -25.96418118399992636, 30.8824873850000472 -25.96418118399992636, 30.88238558000006151 -25.96418591899993089, 30.88237137500004792 -25.96421432999994749, 30.88236190400004944 -25.96427115099993443, 30.8823263920000386 -25.964287724999906, 30.88229798000008941 -25.96435638299993798, 30.88227193700004136 -25.96441793899992945, 30.88220564600004536 -25.96443451199991159, 30.88211331100006873 -25.96443451199991159, 30.88201860800006671 -25.96444161499994152, 30.88186235100005206 -25.9644676569999433, 30.88181500000007418 -25.96451974399991514, 30.88174397300008422 -25.96454341999992721, 30.88170845900003769 -25.96460260899993955, 30.88170845900003769 -25.96466179699990562, 30.88170609300004799 -25.96475176399991369, 30.88164690300004622 -25.96487724499991145, 30.88157114300008743 -25.96489381699990417, 30.8815143200000648 -25.96488197999991598, 30.88146223400008239 -25.96487724499991145, 30.88142672100008213 -25.96488197999991598, 30.88140304400008063 -25.96493880099990292, 30.88141725100007307 -25.96498615199993765, 30.88143145600008665 -25.965028767999911, 30.88141014800004314 -25.96506191399993213, 30.88135806200006073 -25.96505244299993365, 30.88126336100003755 -25.96515661599994473, 30.88118049600006998 -25.9653720629999043, 30.88114261500004432 -25.96553779199990686, 30.88109999900007097 -25.96558750999992071, 30.88102660500004504 -25.96560408299990286, 30.88109526400006644 -25.96568457999995871, 30.88103134000004957 -25.96587161699994795, 30.88098398900007169 -25.96593554099990797, 30.88075330200007329 -25.96599374399994531, 30.88064014300005056 -25.96606696499992495, 30.88054029500005981 -25.96616681199992627, 30.88035391500005744 -25.96624668899994504, 30.88014090900009023 -25.96624668899994504, 30.88002109300003895 -25.96626000199995588, 30.87996784100005243 -25.96628662799992071, 30.87991459000005534 -25.96638647499992203, 30.87986133800006883 -25.96653291699993815, 30.87982140000008258 -25.96673260999995136, 30.87969492700005958 -25.9670920579999347, 30.87954182900006117 -25.96747147599995742, 30.87980142900005376 -25.96755800899995847, 30.88004106200008891 -25.96756466599993018, 30.88034726000006458 -25.96769113799990691, 30.88056026500004236 -25.96779764199993679, 30.88081321000004209 -25.9680173029999537, 30.88079989700008809 -25.96825693599993201, 30.88075330200007329 -25.96850322499994945, 30.88045376200005876 -25.96867629299993041, 30.88012094000004026 -25.96863635399995474, 30.8798813090000408 -25.96864966699990873, 30.87912912800004506 -25.96860972799993306, 30.87900265600006833 -25.96921546499993383, 30.87891612300006727 -25.96976794999994809, 30.87885621500004163 -25.97005417699995178, 30.87892943600007811 -25.9703204349999055, 30.87902262600005088 -25.97056672399992294, 30.87903593900006172 -25.97071316699992849, 30.87894940600006066 -25.97089288899991288, 30.8788096190000374 -25.97093948499991711, 30.87873639900004719 -25.97109258299991552, 30.87868980300004296 -25.97119242999991684, 30.87847679700007575 -25.97119908599995597, 30.87835032500004218 -25.97111255199990865, 30.8783103860000665 -25.97083963699992637, 30.87795093800008317 -25.97067322799995281, 30.87757152000006045 -25.97064660199993114, 30.87739246800003912 -25.97083302399994409, 30.8771750490000727 -25.97086596599990571, 30.87708281000004717 -25.97093843899995136, 30.87695104100004073 -25.97114926899990905, 30.87677974200005337 -25.97150504599994747, 30.87664797200005751 -25.97176858399990351, 30.87643714200004297 -25.97205188699990686, 30.87616042700005892 -25.97215071399995168, 30.8759232430000452 -25.97219683299994131, 30.87579147500008503 -25.97224954099993965, 30.87558064500007049 -25.97247354899991478, 30.87518533700006174 -25.9730533329999389, 30.87484273700005133 -25.97340910799994163, 30.87461873000006563 -25.97360676099992816, 30.87442766500004154 -25.97392300699993939, 30.87433542600007286 -25.97419313399990415, 30.87492179800005943 -25.97432490399995686, 30.8753698130000771 -25.97436443399993777, 30.87585735800007569 -25.97449620199995479, 30.8760484240000892 -25.97470044399995004, 30.87594300800003566 -25.97494421799990505, 30.87552793600008272 -25.97496398199990608, 30.87509968800003435 -25.97482562499993719, 30.87504697900004658 -25.97498374799994281, 30.87508651000007376 -25.97516822399995817, 30.87496132900008661 -25.97542517499994119, 30.87469779100007372 -25.97584683499991343, 30.87456602200006728 -25.97609719599995515, 30.8744671950000793 -25.97634755699994002, 30.87427613000005522 -25.97663744899995208, 30.87395329600008154 -25.97701299099992411, 30.87372270000008712 -25.97736876699991626, 30.87355799000005163 -25.97757300899991151, 30.87322856700006923 -25.97810008499993728, 30.87303750100005573 -25.97827797199994393, 30.87319562400006134 -25.97873257599991348, 30.87450013800008719 -25.97954954299990504, 30.87480470100007324 -25.97977381299995159, 30.8754966110000737 -25.97979178499991804, 30.87601283700007571 -25.97980276899994578, 30.87647414400004209 -25.97976981799990881, 30.87683660000004693 -25.97978080199993656, 30.87717708900004254 -25.97978080199993656, 30.87760544600007506 -25.97971490099990888, 30.87778118300008146 -25.97971490099990888, 30.87815462200006777 -25.97959408199994868, 30.8783852760000741 -25.97955014799993023, 30.87871478100004197 -25.97945129599992242, 30.87901133500008655 -25.97937441199991326, 30.87945067700007939 -25.97920965899993462, 30.87962641400008579 -25.97915474099994526, 30.87992296800007352 -25.97909982399994533, 30.88023050700007843 -25.97907785599994668, 30.88072476400003552 -25.97894605499993759, 30.88107623700005888 -25.97890211999992971, 30.88146066000007295 -25.97870441699990351, 30.88209694500005753 -25.979051492999929, 30.88196002700004783 -25.97928425399993557, 30.88182310800004871 -25.97973608499995635, 30.88180941700005633 -25.98006468999994922, 30.88183680100007678 -25.98051652099991315, 30.88189156700008198 -25.98095465899990586, 30.88168618900004958 -25.98129695699992681, 30.88157665500006033 -25.98152971799993338, 30.88104267200003505 -25.98176247999992938, 30.88045392300006142 -25.98196785599992609, 30.87991994100008242 -25.98213215899994566, 30.87934488300004432 -25.98213215899994566, 30.87838645300007556 -25.98203631699993821, 30.87775662800004284 -25.98210477499992521, 30.87727741300005846 -25.98199523999994653, 30.87697619100003976 -25.98194047399994133, 30.87608622200008313 -25.98161186899994846, 30.87564808300004415 -25.98132433999995783, 30.87518533700006174 -25.98103853399993568, 30.87380176100003837 -25.98083429199994043, 30.87349210400003585 -25.9808672339999589, 30.87343939700008377 -25.98085405799992031, 30.87336692400003813 -25.98057075399992755, 30.87292549800008601 -25.98063004999994519, 30.87275419800005238 -25.98056416599990825, 30.87261584100008349 -25.98046533899992028, 30.87231277200004342 -25.9803401569999437, 30.87214147200006664 -25.98016885899994577, 30.87191087600007222 -25.97997779399992169, 30.87178569600007449 -25.97978672899995445, 30.87170004600005768 -25.97964178299992, 30.87123848800007408 -25.9782263639999087, 30.87208181000005425 -25.97741817999991554, 30.87149616900006777 -25.97676226299995506, 30.87100423200007526 -25.97653971999994837, 30.87079340200006072 -25.97630546399994955, 30.87048886800005221 -25.97618833599995014, 30.87028975100008665 -25.97611805899992987, 30.87005549600007726 -25.9760126439999226, 30.86973925000006602 -25.97591894199990747, 30.86946985500003393 -25.97587209099992833, 30.86934101400004238 -25.97587209099992833, 30.86918874800005597 -25.97596579299994346, 30.86896620500004929 -25.97591894199990747, 30.86880222700006016 -25.97594236699995918, 30.86859139500006677 -25.9759775059999356, 30.86846255400007522 -25.97598921899992774, 30.8683454260000758 -25.97598921899992774, 30.86818144700004041 -25.97602435699991474, 30.86801746800006185 -25.97608292099994287, 30.86784177600003432 -25.97609463399993501, 30.86760752000003549 -25.97610634599993773, 30.86726784900008624 -25.97630546399994955, 30.86703359300008742 -25.97635231399993927, 30.86689304000003631 -25.97648115599992025, 30.86674077100008162 -25.97648115599992025, 30.86645966600008251 -25.97634060299992598, 30.86635425000008581 -25.97614148599990358, 30.86640110100006495 -25.97576667499993164, 30.86640110100006495 -25.97546214199991255, 30.86652994100006708 -25.97504048199994031, 30.86647137800008522 -25.97451340599991454, 30.86628397300006554 -25.97405660599991961, 30.86596772800004373 -25.97371693499991352, 30.86565148200008935 -25.97340068799991286, 30.86514783100005843 -25.97283847499994636, 30.86487843800006203 -25.97249880399994026, 30.86452705300007437 -25.97233482399991544, 30.86417566900007614 -25.97224112199995716, 30.86370656700006521 -25.9721131469999591, 30.86322476400005144 -25.97196489999993219, 30.86282943800006251 -25.9718042989999276, 30.86255765300006715 -25.97160663599993313, 30.86234763700008443 -25.97137191199993822, 30.86222409800006972 -25.9709642329999042, 30.86216232800006765 -25.97055655399992702, 30.86195231100003866 -25.97022299799994016, 30.86176700300006814 -25.96985238199994228, 30.86148286300004884 -25.9696423649999133, 30.86076633500005073 -25.96929645499994876, 30.86007451700004367 -25.96886406899994881, 30.8595433000000412 -25.96853051099992626, 30.85917268100007504 -25.9682957889999102, 30.85890089500009026 -25.96822166399994103, 30.85838203100007604 -25.96811047899990399, 30.85760373400006529 -25.9679622309999445, 30.85689956100003428 -25.96781398599995327, 30.85605949500006773 -25.96762867699993649, 30.85529355300008092 -25.9675421979999328, 30.85462644000006094 -25.96751749099991002, 30.85419405400006099 -25.96751749099991002, 30.85225449000006392 -25.96761632299995881, 30.85109322100004192 -25.96765338399995926, 30.8496972300000607 -25.96769044599994913, 30.84963546100004805 -25.9683699109999111, 30.84862244000004239 -25.96864169699995273, 30.84828888400005553 -25.96776456999992888, 30.84762177200008182 -25.96780163099992933, 30.84725115600008394 -25.96785104699995372, 30.84685583100008444 -25.96811047899990399, 30.84638638200004834 -25.96834520399994517, 30.84581810200006657 -25.9683946189999233, 30.84555866900007004 -25.96848109699993756, 30.84523746800005028 -25.96851815799993801, 30.8449656820000655 -25.96851815799993801, 30.84455800300008832 -25.96850580399990349, 30.84415682400003789 -25.96849668699991298, 30.84407149000008985 -25.96874913499993909, 30.84400644000004377 -25.96890091599993866, 30.84389079600003924 -25.96898764899992784, 30.84374624100007622 -25.96900933299991721, 30.84358723100007182 -25.96897319499993273, 30.8435149540000566 -25.96897319499993273, 30.84340653800006748 -25.96893705399992314, 30.84329089400006296 -25.96890091599993866, 30.84317421000008608 -25.96890722399990636, 30.84316201100006083 -25.96893819099994971, 30.8428037480000512 -25.9694941169999538, 30.84274158600004512 -25.96956586799990419, 30.84253198200008228 -25.96934903599992595, 30.84230792200008864 -25.96905992699993249, 30.84204772300006425 -25.96875636199990822, 30.8419648840000491 -25.96867670899990799, 30.84090124500005459 -25.96882700599991267, 30.84013530200007835 -25.96898760699991726, 30.83799807500008683 -25.96970413499991537, 30.83741744100007054 -25.97006239699993557, 30.83707153200003859 -25.97049478399992495, 30.83644354100005103 -25.97143024999991212, 30.83544790800004876 -25.97263086699990708, 30.83518435700005966 -25.97304083399990304, 30.83563684000006333 -25.97316565699992452, 30.83594853100004229 -25.97318072299992764, 30.83622681900004636 -25.9732045759999437, 30.83646535200006156 -25.97328408699991087, 30.83657666600004177 -25.97323638099993559, 30.83669593100006523 -25.97321252699993011, 30.83690265900008853 -25.97318867399991404, 30.8371173380000414 -25.973244331999922, 30.83737972300008323 -25.97336359699994546, 30.83757850000006329 -25.9734510599999453, 30.83791244500008588 -25.97353056999992305, 30.83819868300008693 -25.973586227999931, 30.83842926400006945 -25.97371344499993029, 30.83878706200005126 -25.97380885699993769, 30.83912100700007386 -25.97391221999993149, 30.83903354500006344 -25.9743018229999052, 30.83865189500005499 -25.97418255699994916, 30.83859623700004704 -25.97434952999992674, 30.8385803340000848 -25.97448469799991244, 30.83856443200005515 -25.97470732799990856, 30.83844516600004226 -25.97486634899991031, 30.83842926400006945 -25.97500946799993926, 30.83904149700003927 -25.97518439199990326, 30.83908125100003872 -25.97531956099993522, 30.83920051800004103 -25.97560579799994684, 30.83928797900006202 -25.97593974199992317, 30.83951856000004454 -25.97609876299992493, 30.83975709200007032 -25.976289589999908, 30.84011489000005213 -25.97640885599992089, 30.84031366700008903 -25.97655197499994983, 30.8401069380000763 -25.97684616499992671, 30.84000357500008249 -25.97723576699991099, 30.84004333000007136 -25.97741864099992881, 30.84013079200008178 -25.97772078199994894, 30.84013960700008283 -25.9778054029999339, 30.84017054700007066 -25.97810243299994681, 30.84036932400005071 -25.9781580899999085, 30.84067941700004667 -25.97821374799991645, 30.84088767000008602 -25.97825539899992009, 30.84099745800006076 -25.97827735599992138, 30.841267794000089 -25.97839662199993427, 30.8414506690000394 -25.97843637799991257, 30.8417925650000484 -25.97849998699990692, 30.84208675400003585 -25.97853974099990637, 30.84226167800005669 -25.97857949699994151, 30.84252406300004168 -25.9786351539999032, 30.84265128100008724 -25.9786987629999544, 30.84288186200006976 -25.97879417499990495, 30.84305678300006548 -25.97887368699991839, 30.8431919520000406 -25.97891344099991784, 30.84329531600008067 -25.97893729499992332, 30.84345433700008243 -25.97895319699995298, 30.84360540800008721 -25.97901680499995791, 30.84376442900008897 -25.97908041399995227, 30.84395525500008262 -25.97913607099991395, 30.84409042400005774 -25.9791837779999355, 30.84427329700008613 -25.97922353299992437, 30.84442436600005522 -25.97924738599994043, 30.84453568200007112 -25.97927123899995649, 30.8446867530000759 -25.97929509299990514, 30.84484577400007765 -25.97930304399994839, 30.84496504000009054 -25.97935074999992366, 30.84510020800007624 -25.97940640699994219, 30.84524332600005891 -25.97949386799990634, 30.84546595700004445 -25.97957337999991978, 30.84557727200007093 -25.9796210859999519, 30.84566473400008135 -25.97968469499994626, 30.84581580400003986 -25.97972444899994571, 30.84595892300006881 -25.97972444899994571, 30.84605433600006563 -25.97987551999995048, 30.84617360200007852 -25.98001068799993618, 30.84637237900005857 -25.98008224899990637, 30.84661886200007075 -25.98012995399994907, 30.84665479200003801 -25.98021166699993501)))</t>
+  </si>
+  <si>
+    <t>Mbejeka SP B</t>
+  </si>
+  <si>
+    <t>Mbejeka</t>
+  </si>
+  <si>
+    <t>MP301</t>
+  </si>
+  <si>
+    <t>Albert Luthuli</t>
+  </si>
+  <si>
+    <t>DC30</t>
+  </si>
+  <si>
+    <t>Gert Sibande</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.80497386800004733 -25.98257217499991611, 30.80330034500008196 -25.98302154699990751, 30.80347358200003782 -25.98313312299995914, 30.80360646000008273 -25.98332136799990622, 30.80340714100003652 -25.98370893099991008, 30.80336284800006297 -25.98386395599993648, 30.80341821500007882 -25.98412971399994831, 30.8034846550000907 -25.98425151899994034, 30.80409368200008657 -25.98460586299995612, 30.80478022300007979 -25.98522596399993745, 30.80458090500007984 -25.98542528299992682, 30.80510134600007177 -25.98590143199993463, 30.80479481400004715 -25.98629780899995012, 30.80445909900004153 -25.98673192499995821, 30.80361753300007877 -25.98785032099993941, 30.80320676100006949 -25.98842056999990291, 30.8031980300000896 -25.98843268999991096, 30.8026763090000486 -25.98915696299991396, 30.80233303700003944 -25.98933413499992184, 30.80197869400006994 -25.98945594099990331, 30.80108176100003448 -25.98962203899992573, 30.79911072500004821 -25.98978813799993759, 30.79805274200003851 -25.9898563759999206, 30.79714505400005464 -25.98996983599994337, 30.79669120800008386 -25.99015137499992534, 30.79725851400007741 -25.99055983399995284, 30.79789389600006189 -25.99085483299995758, 30.79848389400007136 -25.99114983199990547, 30.79880158400004575 -25.99121790899994267, 30.79905120000006491 -25.99126329299991767, 30.79923273700006803 -25.99128598499993359, 30.79964119800007438 -25.99158098399993833, 30.80009504200006631 -25.99173982899992552, 30.80043542500004605 -25.99192136699991806, 30.80098003800003426 -25.99210290499991061, 30.80138849900004061 -25.99230713499991907, 30.80202387900004624 -25.99267020999991473, 30.80124685800007001 -25.99372702299990578, 30.79976084000008996 -25.99397447799992733, 30.79832229900006269 -25.9932192429999418, 30.7963443040000584 -25.99246400899994569, 30.79570134900006906 -25.99188226299992266, 30.79500552700005755 -25.99112965199992686, 30.79483746200008909 -25.99109145499994611, 30.79460050900007673 -25.9912602119999292, 30.79440812700005381 -25.99139722699993627, 30.79391748000006146 -25.99176521099991533, 30.79205216100007192 -25.9931216769999196, 30.79134494000004452 -25.99360465699993483, 30.79023640300005127 -25.99441294799993329, 30.78999383500007525 -25.99456819199991742, 30.78940682000006746 -25.99499511199991275, 30.78878099400003521 -25.99549480299992865, 30.78848506100007398 -25.99576162799991152, 30.78804843800008939 -25.99620310199992446, 30.78728677400005154 -25.99548995099991089, 30.7873226270000373 -25.99525726299992812, 30.78739942000004248 -25.99454692299991621, 30.78730342800008657 -25.99324143199993387, 30.78730342800008657 -25.9924350999999092, 30.78701365400007717 -25.99194614099991441, 30.78674367600007145 -25.99156817299990507, 30.78633331100007808 -25.99115780599993286, 30.78602013500005796 -25.99066104899992524, 30.78572856000005231 -25.99011029499990855, 30.78518860600007656 -25.98952714399990782, 30.78430308000008608 -25.98884680099990874, 30.78351474600003712 -25.98791807899993955, 30.78402230300008569 -25.98752931199993554, 30.78465944900005979 -25.98678417499991156, 30.78618212200007065 -25.98530469799993625, 30.78676527300007137 -25.9844947669999442, 30.7870784470000558 -25.98409519999995609, 30.78745641500006514 -25.98342565699994111, 30.78767239700005121 -25.98309088499991049, 30.78790997700008347 -25.98263732299994899, 30.78834194100005561 -25.98250773399990976, 30.78861191800007191 -25.98269131799992238, 30.78892509200005634 -25.98286410399992974, 30.78911947600005306 -25.98301529099995832, 30.78927066300008164 -25.98314487999994071, 30.78954064000004109 -25.98333926399993743, 30.78968102900006443 -25.98359844199995905, 30.78983221600003617 -25.9838252229999398, 30.79067454500005852 -25.98381442399994512, 30.79164646400005267 -25.98363083899994308, 30.79201363300006733 -25.98351204999994479, 30.79268317600008231 -25.98337166099992146, 30.79351470700004256 -25.98335006299993211, 30.79454062000007752 -25.98325287099993375, 30.79572852100005775 -25.98311248299995668, 30.79674363500004119 -25.9830044919999068, 30.79738054000006287 -25.98296508499993251, 30.79761707200003684 -25.98288281499992536, 30.79785360100004254 -25.98273883899992143, 30.79817240400006995 -25.98268741899994438, 30.79847063700003673 -25.98264628399994081, 30.79869688400003724 -25.9826051479999478, 30.79897455000008222 -25.9825434449999193, 30.79920802600008756 -25.98240850699994553, 30.80037491000007321 -25.98211678599994912, 30.80164787400008208 -25.98222286599991548, 30.80297387800004572 -25.98219634599990968, 30.80361036000005015 -25.98232894699992812, 30.80411424200008241 -25.98214330599995492, 30.80497386800004733 -25.98257217499991611)))</t>
+  </si>
+  <si>
+    <t>Los-my-cherry</t>
+  </si>
+  <si>
+    <t>Tjakastad</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.77993673800006036 -26.01056232799993495, 30.7794849290000343 -26.010854674999905, 30.77881606300007888 -26.01120670899990728, 30.77765434800005551 -26.01173476099995696, 30.77691507400004411 -26.01219240699992952, 30.77603498900003842 -26.01272045899992236, 30.77511969800008274 -26.01328371499994319, 30.77438042600005019 -26.01398778399993716, 30.77427476000008255 -26.01428715799994507, 30.77426259900005334 -26.0143216109999571, 30.77401105200004849 -26.01457315799990511, 30.77380524000005835 -26.01493904499994869, 30.77369090100006588 -26.01523632799995767, 30.77348509000006516 -26.0153735359999132, 30.77348509000006516 -26.01557934699991392, 30.77295912700003555 -26.01585376199994926, 30.7724560330000827 -26.01592236599992702, 30.77188433500003839 -26.01592236599992702, 30.77119829700006903 -26.01589949799995338, 30.7709696170000484 -26.01603670699995519, 30.77032931500008317 -26.0158766299999229, 30.76996342800003958 -26.01603670699995519, 30.76932312600007435 -26.01612817699992775, 30.76900297500003489 -26.01585376199994926, 30.76875142800008689 -26.0150762519999148, 30.76843127700004743 -26.01461889399990923, 30.7683855410000433 -26.01381851599995798, 30.76843127700004743 -26.01301813799994989, 30.7685456160000399 -26.01176040299992565, 30.7685456160000399 -26.01139451699992833, 30.76856848500005981 -26.01093715699994391, 30.7685456160000399 -26.01054840199992668, 30.76840840900007379 -26.01009104399992111, 30.76822546600004671 -26.00954221299991787, 30.76804252200008705 -26.00903911899990817, 30.76756229600005099 -26.00892477899992627, 30.7669143120000399 -26.00857338499992011, 30.76633787800005848 -26.00880528299995831, 30.76643726400004653 -26.00901730499992937, 30.76627824800004873 -26.00926907999991045, 30.76571506600004113 -26.01015691799995011, 30.76537053200007676 -26.01026955399993312, 30.76501274700007116 -26.01044844699993064, 30.76495974100004105 -26.01038219099990556, 30.7637207420000891 -26.00945459799993387, 30.76378700000003619 -26.00934858799990934, 30.76385141400004386 -26.00927465099994151, 30.76439434800005301 -26.00857202899993581, 30.76469775100008519 -26.00818878199993378, 30.76492131300005894 -26.00759794099991495, 30.76474565800003802 -26.00737437999993062, 30.76445822300007649 -26.00686338299993849, 30.76401110000006156 -26.00638432299990654, 30.76372366500004318 -26.00609688699995559, 30.76340429100008578 -26.00555395099991074, 30.76302104200004806 -26.00529845299990939, 30.76241423300007227 -26.00462776899991013, 30.76211082900005067 -26.0041966159999447, 30.76182339400008914 -26.00365367999995669, 30.76072364500004142 -26.00334207399993147, 30.76076406500004623 -26.00308944499994368, 30.76076911700005212 -26.0030187079999564, 30.76077922200005332 -26.00263471199991727, 30.76070343400004958 -26.00237702999993417, 30.76054680400005736 -26.00221029499994074, 30.76032449100006261 -26.00210924299994986, 30.75998596700003418 -26.00200313799990681, 30.75978891700003715 -26.00190713999995751, 30.75958176100004948 -26.0018212459999063, 30.75944534100005967 -26.00180608799990978, 30.7593594470000653 -26.00175050899991902, 30.75925839500007442 -26.00162924699992573, 30.75909166000008099 -26.00147766999992882, 30.7589148190000401 -26.00135135499994021, 30.75875313700004199 -26.00124019799994812, 30.7586419800000499 -26.00115935699994907, 30.75852577000006249 -26.00110377899994774, 30.7584398750000787 -26.00102293699995926, 30.7584146130000704 -26.00091683299990564, 30.7587753750000843 -26.00081563199995571, 30.76000302900007455 -26.00031487799992647, 30.76071377600004553 -26.00010488499992789, 30.76131145000005063 -25.99987873799994986, 30.76231295700006285 -25.99965259199990442, 30.76286217000006218 -25.99958797899995488, 30.76357291700009 -25.99950721099992279, 30.76434827800005678 -25.99942644499992639, 30.76522055800006683 -25.99929721799992421, 30.76588284400008888 -25.99929721799992421, 30.76641590500008761 -25.99942644499992639, 30.76709434400004284 -25.99957182499991859, 30.76835430500005941 -25.99994335199994566, 30.76933965900008161 -26.00028257199994641, 30.77034727900007738 -26.00058139199995821, 30.77059711400005426 -26.00065548199995646, 30.7721408260000544 -25.99866817299994182, 30.7722792410000352 -25.99843033299993067, 30.77289652600006775 -25.99853793299990912, 30.77338174100003698 -25.99839340099993024, 30.77382566000005681 -25.99843469599994705, 30.77423861000005445 -25.99840372599993543, 30.77452767500005848 -25.99844501999990598, 30.77489932700007103 -25.99862052199995333, 30.77435217000004286 -25.99929156499990768, 30.77394954600003985 -25.99965289599992957, 30.77359853900009057 -26.00002454999992096, 30.77407343000004403 -26.00032393699990507, 30.77472382400003426 -26.00054073599994808, 30.77521936400006553 -26.00072656199995436, 30.77560134200007269 -26.00074720899993963, 30.77607623300008299 -26.00078850499994587, 30.7762104410000461 -26.00084012499991104, 30.77633432600003971 -26.00098465599995734, 30.77648918200003436 -26.0010775699999499, 30.77674727500004792 -26.0010878929999194, 30.77690213100004257 -26.00104659799990259, 30.77719119500005718 -26.00111886399992045, 30.77746993700003486 -26.00121177899995928, 30.77777964800003474 -26.00110854099995095, 30.77799644700007775 -26.00099497999991627, 30.77814097800006721 -26.00094336099994052, 30.77846101400007228 -26.00117048299995304, 30.77888428600005 -26.00125307299992983, 30.77936950100007607 -26.00141825199995083, 30.7796688890000496 -26.0014595469999108, 30.7799682780000694 -26.00137695699993401, 30.78030896000007033 -26.0010775699999499, 30.78068061500005115 -26.00080915299992057, 30.78067029100003538 -26.00064397299991015, 30.78061867200005963 -26.00050976399995761, 30.78070126200003642 -26.00034458499993661, 30.78083547000005638 -26.00017940599991562, 30.78092838400004894 -26.00000390299993569, 30.78096967900006575 -25.99985936999991054, 30.78096967900006575 -25.99967354199992542, 30.78093870800006471 -25.99948771599991915, 30.78084579300008272 -25.99936383099992554, 30.78077352800005428 -25.99921929899994666, 30.78077352800005428 -25.99904379599990989, 30.78074255700005324 -25.99893023599992148, 30.78076320400003851 -25.99884764499995526, 30.78072190900007854 -25.99868246499994484, 30.78079417600008583 -25.99836242999992919, 30.78115550700005087 -25.99806304199995566, 30.78152715900006342 -25.99820757399993454, 30.7817852530000664 -25.99819724999991877, 30.78218787800005884 -25.99813530799991668, 30.78236338300007446 -25.99835210599991342, 30.78238403000005974 -25.99862052199995333, 30.78239435300008608 -25.99901282299992999, 30.78242532300004086 -25.99948771599991915, 30.78233241100008399 -25.9999109879999537, 30.78256985600006601 -25.99997293099994522, 30.78270406500007539 -26.00021037599992724, 30.78282794900007957 -26.00089174199990794, 30.78255953200005024 -26.00200670499992839, 30.78223949700003459 -26.00200670499992839, 30.78171298700004854 -26.00191379199992525, 30.78107291600008466 -26.00205832299991471, 30.78076320400003851 -26.00219253199992409, 30.78056705400007331 -26.00228544599991665, 30.7808148230000711 -26.00278098399991222, 30.78087676500007319 -26.00298745799995004, 30.78100064900007737 -26.00323522799993725, 30.7811245350000604 -26.00337975999991613, 30.78133101000008764 -26.00364817699994546, 30.78156845500006966 -26.0038856229999169, 30.78172331100006431 -26.00423662799994418, 30.78190913800006001 -26.00436051399992721, 30.78211561200004098 -26.00461860699994077, 30.78236338300007446 -26.00483540499993751, 30.78242532300004086 -26.00515544099994258, 30.78227046800003563 -26.00536191499992356, 30.78209496500005571 -26.00552709499993398, 30.78204334600007996 -26.00567162699991286, 30.78237370500005454 -26.00609489999993684, 30.78244597200006183 -26.00639428799991038, 30.78224982100005036 -26.00680723799990801, 30.78174395800004959 -26.00710662499994896, 30.78104194500008362 -26.0070240339999259, 30.78080450000004475 -26.00743698399992354, 30.78063932000003433 -26.0075092499999414, 30.78056705400007331 -26.00776734299995496, 30.78041219800007866 -26.00802543699995795, 30.7803399320000608 -26.00822158699992315, 30.78029863600005456 -26.00839709099994934, 30.78027799000005871 -26.00860356399994089, 30.78022637100008296 -26.00886165799994387, 30.78005086700005677 -26.00901651399993852, 30.77992698200006316 -26.00932622599992783, 30.77971018400006642 -26.00960496599992666, 30.77946241500006863 -26.00981143999990763, 30.77961727100006328 -26.01020374299992, 30.77993673800006036 -26.01056232799993495)))</t>
+  </si>
+  <si>
+    <t>Malahleka SP</t>
+  </si>
+  <si>
+    <t>Malahleka</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((31.00833302600005936 -26.07266262899992171, 31.00751054300008036 -26.0731025629999067, 31.00718928800006324 -26.07334350299993275, 31.00705293900006154 -26.07402524699995183, 31.00698850300005915 -26.07434742299994923, 31.00670740700007855 -26.07539149999990968, 31.00598458500007837 -26.07619463499992207, 31.00544921100004103 -26.07667902099990442, 31.00542760500007944 -26.07677470699991318, 31.00541039700004831 -26.07682878799994342, 31.00530030600003784 -26.0768278139999552, 31.0051709480000568 -26.07683629799993241, 31.00503310700008797 -26.07682145099994386, 31.00488042200004202 -26.07678964399991628, 31.00449022600008675 -26.07671117999990429, 31.00365894000003664 -26.07652032299995426, 31.00354654500006291 -26.0764863929999251, 31.00349989300008247 -26.07644822099990733, 31.00344263500005582 -26.07638248199992859, 31.00315210900004104 -26.07570388099992442, 31.00265588300004538 -26.07465204999994057, 31.00264290600006234 -26.07462617799990312, 31.00203208300007418 -26.07486154099990472, 31.00167532200003961 -26.07501721899990343, 31.00042989700006046 -26.07548425299995642, 30.99979421400007595 -26.07572425699993346, 30.99957366900008537 -26.07582155499994769, 30.999430966000034 -26.07589290599992182, 30.997955690000083 -26.07641088499991611, 30.99819008300005407 -26.07595381999993833, 30.99848298700004534 -26.07534360199991852, 30.99869046100008063 -26.07483102099990901, 30.99884141400008275 -26.07444062699994447, 30.99904438700008313 -26.07391569499992556, 30.99931288200008339 -26.07325665999991315, 30.99955789900008085 -26.07275641799992627, 30.99960578600007466 -26.07265864699991198, 30.99984987300007333 -26.07204843099992786, 31.000093960000072 -26.07159686999995074, 31.00031363800007966 -26.07104767499993159, 31.00053331500004106 -26.07060831899991626, 31.00075299400003814 -26.07027880199990477, 31.0009726720000458 -26.06990046799995753, 31.00122896200008427 -26.06961976699994921, 31.00150966300003574 -26.06924143299994512, 31.00185138400007645 -26.06888750699994262, 31.00226633200009019 -26.0685579889999417, 31.00255923600008146 -26.06869223799992596, 31.0027667100000599 -26.06888750699994262, 31.00303520500006016 -26.0691560029999323, 31.00315724900008263 -26.06935127199994895, 31.00341354000005367 -26.06959535899994762, 31.00375526100003754 -26.06988826299993889, 31.00409698200007824 -26.07009573699991734, 31.00420682300006092 -26.07026659699994298, 31.00436547900005735 -26.07048627399990437, 31.00463397500004703 -26.07075477099994032, 31.00491467300008708 -26.07091342699993675, 31.00515876000008575 -26.0710720839999226, 31.00530521200005296 -26.07121853599994665, 31.00548827800008667 -26.07130396599990263, 31.00570795500004806 -26.0714260099999251, 31.00595204200004673 -26.0711453099999062, 31.00629376300008744 -26.07115751299994599, 31.00678193700008478 -26.07115751299994599, 31.00711145400003943 -26.07115751299994599, 31.00739215500004775 -26.07109649199992418, 31.0079901670000595 -26.07096224499991877, 31.0082220500000858 -26.07116971799990779, 31.00838070600008223 -26.07126735399992867, 31.00860038500007931 -26.07153584999991836, 31.00877124400005869 -26.07182875199993077, 31.00863699700005327 -26.07209724899990988, 31.00830748000004178 -26.072573216999956, 31.00833302600005936 -26.07266262899992171)))</t>
+  </si>
+  <si>
+    <t>Nhlaba SP</t>
+  </si>
+  <si>
+    <t>Nhlaba</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.90629029100006164 -26.08175850099991067, 30.90638714700008904 -26.08209750199995369, 30.90675843500008568 -26.08214593099995682, 30.90719429300008869 -26.08246878899990406, 30.90704900800005817 -26.08293693399991753, 30.90650014800007739 -26.08306607699995538, 30.9053862850000769 -26.08324364899993952, 30.90524100000004637 -26.08343736499995202, 30.90514414300008639 -26.08367950799993196, 30.90485924800003659 -26.08378924599992388, 30.90488931800007322 -26.08415008099990473, 30.9049344230000429 -26.08445077399994716, 30.90506973400005108 -26.08479657299994869, 30.90519001200004823 -26.08506719799993334, 30.90523511600008533 -26.08542803199992477, 30.90522008200008486 -26.08578886499992677, 30.90524181300008877 -26.085998932999928, 30.90541337000007616 -26.08605611799993085, 30.90571174100006147 -26.08626124899990373, 30.90586092700004883 -26.08639178599992192, 30.90615929800003414 -26.08639178599992192, 30.90653226200004156 -26.08642908299992769, 30.90668144800008577 -26.08655961999994588, 30.90681198500004712 -26.08689528799993695, 30.90701711500008741 -26.08739878899990572, 30.90705441200003634 -26.08792093899995734, 30.90703576400005659 -26.08814471799990997, 30.9072222460000603 -26.088349846999904, 30.9072222460000603 -26.08855497799993373, 30.9072222460000603 -26.08872281199995768, 30.90737143200004766 -26.08887199799994505, 30.90755791400005137 -26.08903983199991217, 30.90765115500005322 -26.08922631299992645, 30.90783763700005693 -26.08945009199993592, 30.90791223000007903 -26.08959927899991271, 30.9081919530000846 -26.08967387099994539, 30.90839708300006805 -26.08967387099994539, 30.90882599200006098 -26.08982305499995391, 30.90914301100008288 -26.09014007599995466, 30.90946003100003736 -26.09043844699993997, 30.91000082900006873 -26.09043844699993997, 30.91041109000008191 -26.09041979899990338, 30.91072810900004697 -26.09041979899990338, 30.91093323900008727 -26.09043844699993997, 30.91186564900004896 -26.09066222699993887, 30.91235050300008425 -26.0908673559999329, 30.91270481900005507 -26.09092330099991841, 30.91315237500003832 -26.09116572799990763, 30.91369317400005912 -26.09140815399990743, 30.91447639900007971 -26.09114707899993846, 30.91477477100005444 -26.09148274699992953, 30.91507314100005033 -26.09198624799995514, 30.91494260400008898 -26.09235921299995198, 30.91486801100006687 -26.09263893599995754, 30.91468153000005259 -26.0929559549999226, 30.91464423300004682 -26.09347810499991738, 30.91477477100005444 -26.09377647599990269, 30.91492395600005239 -26.09398160599994299, 30.91520367900005795 -26.09433592299990323, 30.9156139390000817 -26.09482077599994909, 30.91643446000006179 -26.09538022199990337, 30.91714309200006028 -26.0956972419999147, 30.91768389000003481 -26.0958837239999184, 30.91807550300006824 -26.09599561299995685, 30.9184671150000554 -26.0961261499999182, 30.91902656100006652 -26.09638722499994401, 30.91938087600004792 -26.09670424599994476, 30.91934358200006727 -26.0970958569999425, 30.91910115400008863 -26.09769259999990254, 30.91878413500006673 -26.09825204599991366, 30.91867224500003886 -26.09858771399990474, 30.91850441000008232 -26.0989420299999324, 30.91820604000008643 -26.09933364299990899, 30.91794496500006062 -26.09972525399990673, 30.91757200100005321 -26.10011686599995073, 30.9173855190000495 -26.10034064499990336, 30.91708714800006419 -26.10067631299995128, 30.9167141850000462 -26.10104927699995869, 30.91667688700005101 -26.10151548199991112, 30.91652770100006364 -26.10190709499994455, 30.91635986800008595 -26.10237329999995382, 30.9160614970000438 -26.10278355999992073, 30.91578177200005939 -26.10315652499991756, 30.91565123700007689 -26.10352948899992498, 30.91552069800007985 -26.10388380499995264, 30.91531556800003955 -26.10423812099992347, 30.91511043800005609 -26.10448054699992326, 30.91484936300008712 -26.10459243699995113, 30.91443910200007394 -26.10455513999994537, 30.91376776700008122 -26.10442460299992717, 30.91335750600006804 -26.10442460299992717, 30.91290994900003852 -26.10433136199992532, 30.91261157800005321 -26.10448054699992326, 30.91242509600004951 -26.10500269699991804, 30.91201483500003633 -26.10558079199995518, 30.91151133400006756 -26.10539430899990521, 30.91151133400006756 -26.10479756699993459, 30.91126890700007834 -26.10477891799990857, 30.91095188800005644 -26.10470432599993273, 30.91028055200007429 -26.10399569499992367, 30.90998218100008899 -26.10386515599992663, 30.90957192000007581 -26.10367867399992292, 30.90904977100007045 -26.10351084099994523, 30.90847167600009016 -26.10326841399995601, 30.90809871200008274 -26.10306328399991571, 30.90781898900007718 -26.10306328399991571, 30.90705244100007576 -26.10209393799993904, 30.9057672270000694 -26.10103223799995931, 30.90520843800004513 -26.0999984769999287, 30.90442613200008282 -26.0990764749999471, 30.90294533900004126 -26.09742804399991201, 30.90224685200007571 -26.0965060419999304, 30.90149248700004136 -26.09443852099991545, 30.901162753000051 -26.09323499399994262, 30.90109257900007833 -26.09324749999990445, 30.90088115400004654 -26.09324749999990445, 30.90076275500007341 -26.09329824199994619, 30.90066127000005736 -26.0933828119999589, 30.90055132900005219 -26.09356886699993083, 30.9002553330000751 -26.09328978499991081, 30.89991705100004538 -26.09285001999995757, 30.89964642600006073 -26.09253710899992029, 30.89955339800008005 -26.09258785199995145, 30.89932505900003434 -26.09262167799994359, 30.89907134800006361 -26.09270624899994573, 30.89880072300007896 -26.09243562399990424, 30.89872460900005535 -26.09228339799994956, 30.89870769500004144 -26.09204660199992531, 30.89882609400007141 -26.09188591699995641, 30.89896140600006902 -26.09168294799991372, 30.89897832000008293 -26.09150535199995602, 30.89891066400008413 -26.09141232299992907, 30.89861466800005019 -26.09091335799990929, 30.89834404300006554 -26.09046513499993125, 30.89835250000004407 -26.09036365099990462, 30.89850472700004502 -26.09021142499994994, 30.8987499800000478 -26.08994925699994383, 30.8988768360000563 -26.0897547439999471, 30.89908826200007752 -26.08949257599994098, 30.89939271500008999 -26.08918812299992851, 30.89944345700007489 -26.08904435399995236, 30.89947728500004587 -26.08879064299992478, 30.89943500000003951 -26.08849464599995827, 30.89928277300003856 -26.08804642499995907, 30.89885992200004239 -26.08752208699991115, 30.89835250000004407 -26.08685398199992278, 30.89768171400004348 -26.08591354399993634, 30.89737249600005953 -26.08550125199991498, 30.89683136500008231 -26.08529510699992215, 30.89629023400004826 -26.08529510699992215, 30.89551719000007779 -26.08526933999991115, 30.89529234700006555 -26.08500361599993767, 30.89523374000003741 -26.08493435399992677, 30.89446069600006695 -26.08467667399992251, 30.89358457900004851 -26.08465090499993266, 30.89219309900005328 -26.0839551639999172, 30.89059547400006522 -26.08302751099995476, 30.88964205200005608 -26.08449629599994068, 30.88822701300006202 -26.0836843869999484, 30.88800340900007768 -26.08406558599995151, 30.88782468900006961 -26.08452231399991206, 30.88754668100006029 -26.08495918499994559, 30.88716938400006029 -26.0854556269999307, 30.88679208600007087 -26.08585278299995025, 30.88631550000008019 -26.08624993799992353, 30.88554104900003949 -26.08664709399994308, 30.8851041780000628 -26.08690524299993285, 30.88478645400005007 -26.08704424699993751, 30.88438929900007679 -26.0870839619999515, 30.88391271200003985 -26.0870839619999515, 30.88331698100006406 -26.08700453199992353, 30.88260210200007805 -26.08682581199991546, 30.88222480500007805 -26.08674638099995491, 30.88180779300006407 -26.08684566999994559, 30.88180779300006407 -26.08559463299991421, 30.88196665500004201 -26.08489961099991206, 30.88284039600006281 -26.08511804599993411, 30.88345598500006872 -26.08531662399991546, 30.88452830400007088 -26.08515776199993752, 30.88542190200007553 -26.08501875699994343, 30.88583891500007894 -26.08478046499993752, 30.88603749100008145 -26.08442302499992138, 30.88620013400003472 -26.08423793499991916, 30.88635752600004025 -26.08409711099994865, 30.88654805300006956 -26.08397285399991006, 30.88673858000004202 -26.08387344799990615, 30.88687112100006971 -26.08369120499992277, 30.88697052600008419 -26.08362493499993207, 30.88704508100005341 -26.08345925899993745, 30.8871444860000679 -26.08335985399992296, 30.88743441800005485 -26.08328529999994316, 30.88760009400004947 -26.08318589499992868, 30.88775748700004442 -26.08312790799993763, 30.88803913500004228 -26.08301193499994497, 30.88813025600006767 -26.0829705159999321, 30.88850686200004247 -26.08294864699990967, 30.88971935700004678 -26.08251214799992113, 30.89023472000008042 -26.0811206679999259, 30.89080161900005805 -26.08063107399993896, 30.89152312700008451 -26.08039915999995628, 30.89209002600006215 -26.07960034799992854, 30.89270846200008691 -26.0798322609999218, 30.89312075200007257 -26.08032185499990874, 30.8933268970000654 -26.08078568199994152, 30.89355881100004808 -26.08114643699991575, 30.89379072400004134 -26.08153295899995783, 30.89430608600008554 -26.08184217699994178, 30.89479568200005133 -26.08189371299994264, 30.89549142200007736 -26.0815071909999574, 30.89657368400008863 -26.08070837799994024, 30.89626446700003726 -26.08034762499994486, 30.89623869800004741 -26.07985802899992223, 30.89624007000008987 -26.07985713699991948, 30.89617924400005222 -26.07971759299994119, 30.8959646310000835 -26.07905944799995268, 30.89577863400006663 -26.07868745199994009, 30.89570709600008058 -26.07853007099993192, 30.89575002000003678 -26.07808653799992271, 30.89583586400004833 -26.07768592899992655, 30.89585017100006326 -26.0774570089999429, 30.89595032300007915 -26.07714224399995828, 30.89557832900004541 -26.07662717399995245, 30.89527787100007572 -26.07622656399991001, 30.89500602900005788 -26.07574010899992345, 30.89477710900007423 -26.07528226899995616, 30.89467695600006891 -26.07482442899993202, 30.89473418600005061 -26.07452397099990549, 30.8950775660000545 -26.07423782199992957, 30.89530648600003815 -26.074023208999904, 30.89552109900006371 -26.07379428999990978, 30.89553791700006968 -26.07377054399995586, 30.89553795000006176 -26.07377049999990959, 30.89564968100006581 -26.0736127589999569, 30.89576432600006228 -26.07345090899991646, 30.89613632100008545 -26.07315045199993619, 30.89647970100008934 -26.07289291699993328, 30.89678015900005903 -26.07270691899992698, 30.89723799900008316 -26.07249230699994769, 30.89739538100008076 -26.0722633869999072, 30.89773876100008465 -26.07192000699990331, 30.89798198900007264 -26.07159093399991434, 30.89819660200004137 -26.07137632199993504, 30.89836829100005389 -26.07111878699993213, 30.89845413600005486 -26.07086125199992921, 30.89852567300005148 -26.07054648699994459, 30.8986258260000568 -26.07030325999994602, 30.89869770100006008 -26.07000218299992866, 30.89876898600005006 -26.06990238399993132, 30.89882601300007536 -26.06975981399995135, 30.89891155500004061 -26.0695459609999034, 30.89901135300004853 -26.06944616199990605, 30.89919669300007854 -26.06934636399995497, 30.89926797900005795 -26.06901845499993442, 30.89928223500004378 -26.06867628799994918, 30.89882601300007536 -26.06816303799990919, 30.89875472800008538 -26.06787789899993868, 30.89875472800008538 -26.06756424699995023, 30.89875472800008538 -26.06739316299990605, 30.89862641600007009 -26.06713653899993233, 30.89834127700004274 -26.06693694099993763, 30.89794208300008904 -26.06659477499994182, 30.8977424870000732 -26.06618132399995602, 30.89758566000006113 -26.06579638699992074, 30.89741457600007379 -26.06546847699991076, 30.89750011800003904 -26.06526887899991607, 30.89758566000006113 -26.06514056799994705, 30.89768545800006905 -26.06494096999995236, 30.89777100000003429 -26.06476988599990818, 30.89802762500005429 -26.06455603299991708, 30.89809890900005485 -26.06447049199994126, 30.89824147900003481 -26.06424238199991805, 30.89839830400006804 -26.06411406899991334, 30.89856938800005537 -26.06391447099991865, 30.89884027000005062 -26.06375764499995284, 30.89895432500009065 -26.06367210299993076, 30.89903986700005589 -26.06350102099992228, 30.89912540900007798 -26.06332993699993494, 30.89931075000004057 -26.06321588099990549, 30.89946757400008437 -26.06311608299995441, 30.89965291500004696 -26.06291648599994915, 30.89980974200005903 -26.06268837499993651, 30.89995231100004958 -26.06260283299991443, 30.90008062300006486 -26.06253154799992444, 30.90013765100007959 -26.0623889789999339, 30.9002659640000843 -26.06214661099994601, 30.90040853300007484 -26.06190424299995811, 30.90044909100004134 -26.06186996899992891, 30.90075476700008039 -26.06247000199994091, 30.90104042700005493 -26.06284587199991165, 30.90113063600006171 -26.06298118399990926, 30.90128098300004922 -26.06323677399990402, 30.90140126100004636 -26.06347732999995515, 30.90164181600005122 -26.06376298999992969, 30.90180719800008546 -26.0640636839999047, 30.90195754600006239 -26.06430423999995583, 30.90212292800003979 -26.06463500399991062, 30.90239355300008128 -26.06517625399993676, 30.90255893600004811 -26.06547694799991177, 30.90275438600008329 -26.0656723999999258, 30.90291976800006069 -26.06592798999992056, 30.90305508100004772 -26.06627378899992209, 30.90326556600007279 -26.06649930999992648, 30.90356626100003723 -26.06670979599994098, 30.903716609000071 -26.06693531699994537, 30.90407744100008358 -26.06716083699990349, 30.9044683450000548 -26.06725104599991027, 30.90463372700008904 -26.06755174099993155, 30.90479910900006644 -26.06797271199991428, 30.90463372700008904 -26.06846885899994959, 30.90448338000004469 -26.06881465799995112, 30.90475400500008618 -26.06934087299993053, 30.90461869100005288 -26.06973177599991232, 30.90449841600008085 -26.0702279219999582, 30.90460365800004183 -26.07069399899995688, 30.90454351900007168 -26.07119014499994591, 30.90424282300006098 -26.0715960829999176, 30.90422778900006051 -26.07192684699992924, 30.90422778900006051 -26.07239292399992792, 30.90400226900004554 -26.07281389499991064, 30.9035061230000565 -26.07321983299993917, 30.90319039300004533 -26.07361073599992096, 30.90323549700008243 -26.0741519859999471, 30.90307819800005973 -26.07462388499993722, 30.90335227900004611 -26.07505918899994413, 30.90362670800004707 -26.0754143329999124, 30.90404642500004684 -26.07567262099991012, 30.90411099600004263 -26.07601162199995315, 30.90401413800003638 -26.07636676599992143, 30.90419171000007736 -26.07667348099994342, 30.90464371200005189 -26.07686719699995592, 30.90504728500008014 -26.07704476899994006, 30.90525714400007473 -26.07733534099992312, 30.9052732860000674 -26.07765819899992721, 30.90606429000007438 -26.07775505699993346, 30.90638714700008904 -26.07781962899991868, 30.90625800400005119 -26.07820705899990799, 30.90601586100007125 -26.07841691699991316, 30.90556385900003988 -26.0795146349999527, 30.90599971700004289 -26.07991820799992411, 30.90606959400008691 -26.08058203999991065, 30.90609657500004914 -26.08083835399992267, 30.90625800400005119 -26.08120964199991931, 30.90630643300005431 -26.08151635699994131, 30.90629029100006164 -26.08175850099991067)))</t>
+  </si>
+  <si>
+    <t>Enkhaba SP</t>
+  </si>
+  <si>
+    <t>Enkhaba</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.99379133300004696 -26.12878301899991129, 30.99380235400008132 -26.12878301899991129, 30.9940008750000402 -26.12878301899991129, 30.99423545800004831 -26.12882739899993112, 30.99445102100008853 -26.12894152099994471, 30.99471730300007266 -26.12916976399992564, 30.99492018700004792 -26.12925852499995472, 30.99510404900007643 -26.1293029049999177, 30.99536399300006906 -26.12942970699992884, 30.9954907930000445 -26.12946140699995112, 30.99566831700008152 -26.12945506699992393, 30.99592826000008472 -26.12941702799992072, 30.99602336100008415 -26.12961990799993828, 30.99643546600003674 -26.12977207199992336, 30.99649252700004354 -26.1301080939999224, 30.9964176870000756 -26.13012221599990426, 30.99615650300006564 -26.13017149699993524, 30.99616284300003599 -26.13028561799990257, 30.99585217900005318 -26.13038071899995884, 30.99594728000005261 -26.13086256499991578, 30.99604109700004528 -26.13134337799994, 30.99623617700007117 -26.1319645919999175, 30.99592563500004871 -26.13206662699991512, 30.99588127200007648 -26.13196015499994473, 30.99577480100003868 -26.13158306899993022, 30.99513153600008764 -26.13168066799994449, 30.99487866700007999 -26.13171172199992043, 30.99463023400005568 -26.13176495799990562, 30.99430638300003693 -26.13183593899992729, 30.99395591600006128 -26.13191135599993231, 30.99364981000007901 -26.1319645919999175, 30.99341024900007824 -26.1319912099999101, 30.99313519800006134 -26.13203557299993918, 30.99289120100007722 -26.13207549899993865, 30.99262945900005661 -26.13212429899994049, 30.99229539400005251 -26.13218130199993539, 30.99172478600007707 -26.1322066629999199, 30.99160432500008255 -26.1321559419999403, 30.99143314300005159 -26.13205449999992425, 30.99121124000004102 -26.13208620099993595, 30.99106541700007256 -26.13208620099993595, 30.99088155600009031 -26.13209254199995257, 30.99067867300004764 -26.13207352099993841, 30.99046944900004519 -26.13207352099993841, 30.99032362800005558 -26.13210522099990385, 30.99019682700009071 -26.13216228099992122, 30.99001296400007277 -26.13217496199990819, 30.98984812300005842 -26.13219398199993293, 30.98965792000007013 -26.13227006299990762, 30.98942967700008921 -26.13232078399994407, 30.98933457600008978 -26.13206083999995144, 30.98930287500007807 -26.13185161699993841, 30.98929019500008053 -26.13166141499993955, 30.98926483500008544 -26.13145853299994315, 30.98929653400006146 -26.1313380709999592, 30.98929653400006146 -26.13119224899992332, 30.98927117600004522 -26.13100838699995165, 30.9892458150000607 -26.13060262199991257, 30.9891950940000811 -26.13007005499991919, 30.98917607400005636 -26.12961356899995735, 30.98911901200006014 -26.12887811999991072, 30.98911270000007789 -26.12851825899991809, 30.98951843800006145 -26.12855477499994095, 30.9898417820000418 -26.12858647599995265, 30.99019048700006351 -26.12861817599991809, 30.99038702900008957 -26.12861817599991809, 30.9906469730000822 -26.12863085699990506, 30.99095129600004839 -26.12860549599992055, 30.99128732100007255 -26.128592815999923, 30.99175648700008878 -26.12864353799994888, 30.99216225200007102 -26.12866889599990827, 30.99266945800007989 -26.12869425699994963, 30.99301816300004475 -26.12869425699994963, 30.99334150800007137 -26.12871961799993414, 30.9937219120000691 -26.12878301899991129, 30.99379133300004696 -26.12878301899991129)))</t>
+  </si>
+  <si>
+    <t>Kalwerskraal SP</t>
+  </si>
+  <si>
+    <t>Kalwerskraal</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.90188827300005414 -26.16524254199993038, 30.90224995200009062 -26.16588243899991539, 30.90250747600003933 -26.16639748199992255, 30.90276499800006604 -26.16654055099991183, 30.90322281300007035 -26.16634025499990912, 30.90356617600008349 -26.16611134599992283, 30.9043037740000841 -26.16597149699992997, 30.90631011700008912 -26.16612011399990934, 30.90730991100008396 -26.16653894699993543, 30.90779039600005262 -26.16687305499993954, 30.90780582600007165 -26.16705821199991533, 30.90794469400003663 -26.16724336999993739, 30.90796012500004508 -26.16742852699991317, 30.90800641400005588 -26.16759825399992678, 30.90805270100008784 -26.16778341199994884, 30.90808356200005846 -26.16799942899990583, 30.90811442300008594 -26.16809200799991686, 30.90820700000006127 -26.16812286699990864, 30.9082532900000615 -26.1683543139999415, 30.90831500900003448 -26.16850861199992551, 30.90842301800006453 -26.16855490199992573, 30.90866989400007014 -26.16852404199994453, 30.90883962200007318 -26.16864747999994734, 30.90904020900006799 -26.16872462899993934, 30.90931794600004423 -26.16878634799991232, 30.90951853100006019 -26.16878634799991232, 30.90978083900006368 -26.16877091899993957, 30.91007400500006952 -26.16881720799995037, 30.9102283020000641 -26.16889435699994237, 30.91045974900004012 -26.16886349699990433, 30.91058318800008919 -26.16892521599993415, 30.91096893200005979 -26.16904865499992638, 30.91113866000006283 -26.16903322499990736, 30.91132381700003862 -26.16914123299994799, 30.91152440600006912 -26.1692492419999212, 30.91163241300006348 -26.16931096099995102, 30.91180214100006651 -26.16940353999990521, 30.91207987700005333 -26.16931096099995102, 30.91215702600004533 -26.16921838299992942, 30.91231132400008619 -26.1692492419999212, 30.91255819900004553 -26.16926467199994022, 30.91263534900008381 -26.16923381199995902, 30.91274335800005701 -26.169295530999932, 30.91285468300003458 -26.16955529099993782, 30.91211576700004571 -26.17096595299994988, 30.91226410600006602 -26.17382150799994633, 30.91222702100003517 -26.17452612499994302, 30.91193034100007253 -26.1759353589999364, 30.91222702100003517 -26.1765287209999542, 30.91311706400006187 -26.17830880699995078, 30.91287934000007454 -26.17822018899994418, 30.91250608300003933 -26.17809772699990845, 30.91236600700005965 -26.17805411099993762, 30.91206153100006304 -26.17795429599993895, 30.91186777300003996 -26.17788887199992587, 30.91169666300004337 -26.17784273899991376, 30.91146432300007518 -26.17776892699993141, 30.91112629400004153 -26.1776573689999168, 30.91098454100006165 -26.17761039799995615, 30.91073542400005181 -26.1775315529999375, 30.91035713600007284 -26.17740573599991194, 30.91021118900005149 -26.17735624799991001, 30.9099763310000526 -26.17728159699993284, 30.90965591800005541 -26.17717674999994415, 30.90946970900006363 -26.17711635699993167, 30.90920968900007892 -26.17703164199991761, 30.90892801900008635 -26.17694578499992986, 30.9088854990000641 -26.17716518699995731, 30.90870609000006652 -26.17767317699991736, 30.90863553600007663 -26.17787072799990256, 30.9085932030000663 -26.17792918699990423, 30.9084722530000704 -26.17809851699990986, 30.90835735100006332 -26.1782275309999477, 30.90827873300008832 -26.17832025899991777, 30.90820616300004531 -26.17846136699995441, 30.90813762500005168 -26.17856618999991269, 30.9080993240000339 -26.17860045899993793, 30.90805296000007729 -26.17870931399994561, 30.90804288100008534 -26.17878994799991688, 30.90811141800008954 -26.17888469199994006, 30.90817189500006634 -26.17907821199992213, 30.90813762500005168 -26.17932212799991021, 30.90812222000005249 -26.17958820599994851, 30.90799956500006829 -26.17999000699995804, 30.90794458300007364 -26.18076823199993441, 30.90788114000008591 -26.18097124899992423, 30.90768235400008734 -26.18133498499992129, 30.90736091300004773 -26.18157606599993414, 30.90719173300004741 -26.1816521969999485, 30.90681953900008239 -26.18171563799995738, 30.90634160500007965 -26.18173255699991842, 30.90589750900005583 -26.18166065599990588, 30.90563951000007137 -26.18163950799993245, 30.90529692100005832 -26.18158875399990393, 30.90501777500008984 -26.18150839399993401, 30.9046328910000625 -26.18158029499994655, 30.90390964800008078 -26.18180445799993095, 30.90364319000008209 -26.18170294999993075, 30.90300030600008085 -26.18153799999993225, 30.90295221700006323 -26.18175700799992001, 30.90291865700004337 -26.18196955399992021, 30.90287391100008563 -26.18243659499995601, 30.90284035200005519 -26.18250371499993889, 30.90270890700008977 -26.18255125899992208, 30.90253831200004697 -26.18272744799992324, 30.90210762800006705 -26.18311058999995566, 30.90184474200003706 -26.1834322049999173, 30.90163219700008312 -26.18372585299994171, 30.90151473800005988 -26.18377339599993547, 30.90146999100005587 -26.18386288899995407, 30.90143922700008261 -26.1840139069999509, 30.90136371800008419 -26.18413695999993251, 30.90127981800003454 -26.18427679299992406, 30.90118193500006782 -26.18437187999995786, 30.9010225260000766 -26.18448374599995532, 30.90089108300009002 -26.18457883199994285, 30.90080159100006085 -26.18463196799990556, 30.90067574100004322 -26.18469908799994528, 30.90055475800005524 -26.18474591199992574, 30.90046603500007905 -26.18481534699992608, 30.90038502700008394 -26.18501593699994601, 30.90017672100003665 -26.18524738899992599, 30.9000841410000362 -26.18523581699992064, 30.899937555000065 -26.18515095099991186, 30.89969067400005542 -26.18504679799991663, 30.89950551300006509 -26.18510851899992531, 30.89938593000005085 -26.18509308999995255, 30.89932806800004528 -26.18502365399990595, 30.89921234300004471 -26.18498507799995423, 30.8990966160000653 -26.18506608599994934, 30.89898474900007841 -26.18515095099991186, 30.89889602500005594 -26.18512780599991174, 30.89877258500007429 -26.18514323599993077, 30.89868386200004124 -26.18518952799990984, 30.89864528700007895 -26.18527439199993978, 30.89860671100007039 -26.18538625999991609, 30.89856042100007016 -26.18543254999991632, 30.89851027300005626 -26.18542869299994891, 30.89839840600006937 -26.18544026499995425, 30.89832125500004167 -26.18550584399991976, 30.89835597300003656 -26.18555213299993056, 30.89839454800005569 -26.1856987189999586, 30.89834825800005547 -26.18582601699995394, 30.89828653800003622 -26.18590702499994904, 30.89816695600006824 -26.18596102999993036, 30.89803580000005923 -26.18599960399990323, 30.89791235800004188 -26.18609604199991736, 30.89791235800004188 -26.18618090899991557, 30.89786606800004165 -26.18636221199994907, 30.89770791000006511 -26.18650108599990745, 30.89690336300003537 -26.18650108599990745, 30.89632068700007039 -26.18681184599995504, 30.89577685700004395 -26.18754990199994381, 30.89534956100004592 -26.18867640699994581, 30.89348499900006573 -26.18747221199993191, 30.89290232400009018 -26.18665646599993124, 30.89197004300007166 -26.18552995999993982, 30.89191465900006506 -26.18553158899993605, 30.89064931200005049 -26.18556880499994577, 30.88948396000006369 -26.18545227099991735, 30.88897897500004319 -26.18498612899992395, 30.88827976400006037 -26.18479190399995105, 30.8873086380000359 -26.1845199889999094, 30.88765824300008944 -26.18401500199991006, 30.88793015900006367 -26.18347117299992988, 30.88835745400007227 -26.18288849699990806, 30.88866821400006302 -26.18226697799991598, 30.88894012900004782 -26.18152892099993778, 30.88870705900006897 -26.18129585099995893, 30.88882359500007624 -26.18098508999992191, 30.88874590500006434 -26.18063548499992521, 30.88851283400003922 -26.18024703499992256, 30.88870705900006897 -26.17970320399990669, 30.88913435500006699 -26.17904283799992982, 30.88925089000008484 -26.17826593699993509, 30.88919685300004403 -26.17783947499992792, 30.88919685300004403 -26.17747891399994842, 30.88934531900008551 -26.17688504899990676, 30.88930290000007517 -26.17673658299992212, 30.88913322500008007 -26.1765669069999376, 30.88906959600006985 -26.1762487649999116, 30.88900596800004905 -26.17588820599991095, 30.88904838700005939 -26.17561248199990587, 30.88913322500008007 -26.17537917699991112, 30.88930290000007517 -26.17493377899995721, 30.88938773800003901 -26.17440354199993635, 30.88936653000007482 -26.17425507599995171, 30.88932411000007505 -26.17385209599990503, 30.88949378500007015 -26.17355516399993576, 30.88966346100005467 -26.17338548799995124, 30.8898119270000393 -26.17304613599992535, 30.89000281300008055 -26.17306734599992524, 30.89017248800007565 -26.17289766999994072, 30.89032095500004971 -26.17257952799991472, 30.89032095500004971 -26.1722401769999351, 30.89053304900005514 -26.17177356899992446, 30.89103345500006981 -26.17154791499990552, 30.89123374900003682 -26.17143346099993551, 30.8917201790000604 -26.17137623399992208, 30.89192047200003799 -26.17137623399992208, 30.89226383500005113 -26.17137623399992208, 30.89252135700007784 -26.17123316699991165, 30.89286471900004472 -26.17097564499994178, 30.89320808200005786 -26.17080396399995834, 30.89340837600008172 -26.17080396399995834, 30.89375173800004859 -26.17097564499994178, 30.89409510100006173 -26.17080396399995834, 30.89446707600006903 -26.17066089599995848, 30.89495350600003576 -26.17046060199993462, 30.89529686800005948 -26.17023169299994834, 30.89569745800008604 -26.16988833099992462, 30.89581191200005605 -26.16957358299993075, 30.89604082000005292 -26.16911576699993702, 30.89647002300006307 -26.16877240399992388, 30.89675615800007336 -26.16840042799992716, 30.89707090700005665 -26.16831458699994073, 30.89738565600003994 -26.16794261199993343, 30.89761456300004738 -26.16762786299995014, 30.89815822000008438 -26.16702697899995655, 30.89875910400007797 -26.16679807099990285, 30.89913108000007469 -26.16668361699993284, 30.89958889600006842 -26.16654055099991183, 30.89987503100007871 -26.16622580099993911, 30.90024700700007543 -26.1659682789999124, 30.90044730200008871 -26.16582521199995881, 30.90070482300006915 -26.16539600999993809, 30.90107679900006588 -26.16551046299991867, 30.90159184300006245 -26.16522432699991896, 30.90187163800004555 -26.16522432699991896, 30.90187797900006217 -26.16522432699991896, 30.90188827300005414 -26.16524254199993038)))</t>
+  </si>
+  <si>
+    <t>Etjelembube SP</t>
+  </si>
+  <si>
+    <t>Etjelembube</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.84473656700004085 -26.21491252299995267, 30.84462361300006705 -26.21523020599994425, 30.84559784300006413 -26.21635268899990479, 30.84621909100007997 -26.21710806999993792, 30.84584493000005523 -26.21734809799994537, 30.84489187900004481 -26.21783521199995448, 30.84568255900006761 -26.21888003999993089, 30.84528015900008313 -26.2191130079999084, 30.84528015900008313 -26.21926125999993928, 30.84498365500007822 -26.21936715499992943, 30.84452477800004999 -26.21939539299995658, 30.84420003500008534 -26.21953658599994696, 30.84453183800007992 -26.2201225349999163, 30.84410120000006827 -26.22030608599993684, 30.84413649800006851 -26.22041904099995691, 30.84426357100005589 -26.22080026199995473, 30.84432710800007271 -26.22115324299994654, 30.84446721600005503 -26.22144046599993317, 30.84434759600003417 -26.22144412699992699, 30.84430580300005431 -26.22145031899992773, 30.84428258500008724 -26.22146270099995036, 30.84427175000007537 -26.2215261659999328, 30.84425472300006277 -26.22155712399995764, 30.84422531300003811 -26.22156950699991285, 30.84419280600008051 -26.221606655999949, 30.84416339700004528 -26.22159427199994752, 30.84414791700004344 -26.22157105499991303, 30.84413398700007747 -26.22157260299991322, 30.84412160400006542 -26.22155093099991063, 30.84410302900005263 -26.22151378299992075, 30.84405659300006164 -26.22152152199993225, 30.84401634600004627 -26.22152771399993298, 30.84399932000007993 -26.22152771399993298, 30.84398229400005675 -26.22148591999990686, 30.84395288500007837 -26.22147508499995183, 30.84391573400006337 -26.2214781809999522, 30.8438847770000848 -26.22149985099991909, 30.84388322800003834 -26.22154009599995561, 30.84385846200007109 -26.22153080899994393, 30.8438151210000342 -26.22151687699994227, 30.84377797200005489 -26.22152461799993262, 30.84373308300007466 -26.22156950699991285, 30.84372069900007318 -26.22159117699993658, 30.84373463100007484 -26.22160975199994937, 30.84376404100004265 -26.22161749099990402, 30.84377797200005489 -26.2216391629999066, 30.84377023200005397 -26.22166392799994128, 30.8437671360000536 -26.22170726899992133, 30.8437284390000741 -26.22173048799993467, 30.84372689100007392 -26.22178311599992639, 30.84370522100005019 -26.22183419599991794, 30.84367581100008238 -26.22185896199994204, 30.8436309220000453 -26.22186979899993275, 30.8436185390000901 -26.22189920799991114, 30.8435829370000647 -26.22193480999993653, 30.84353185700007316 -26.22195183599990287, 30.84349470700004758 -26.22196731399992586, 30.84346684400009053 -26.221956478999914, 30.84344207900005586 -26.22191933099992411, 30.84341112100008786 -26.22188837299995612, 30.84337087600005134 -26.22185896199994204, 30.84337087600005134 -26.22181252599995105, 30.84331979500007037 -26.2218078819999505, 30.84327181200006862 -26.22182490799991683, 30.84324704300007625 -26.22181562299994084, 30.84324085300005436 -26.22184193599991886, 30.84319751200007431 -26.2218899209999563, 30.84314797900003668 -26.22188527699995575, 30.84310154200005627 -26.22191778299992393, 30.8430504610000753 -26.22191623499992374, 30.84299938100008376 -26.22192087799993487, 30.84295139600004632 -26.22191778299992393, 30.84289567300004364 -26.22194719399993801, 30.84285387900007436 -26.22197041099991566, 30.84282601700004989 -26.22194719399993801, 30.84277184100005798 -26.22191313799993395, 30.84275326700003461 -26.22190539999991188, 30.84269289900004196 -26.22190075599991133, 30.84266348900007415 -26.22187444199994388, 30.84263098300004913 -26.22183883999991849, 30.84258454600006871 -26.22183419599991794, 30.84252727400007643 -26.22185122299993054, 30.8424746460000847 -26.22186360599994259, 30.84244214000005968 -26.22185896199994204, 30.84242046900004652 -26.22184348399991904, 30.84241892100004634 -26.22182800499990663, 30.84237867600006666 -26.22183883999991849, 30.84236319700005424 -26.22186670199994296, 30.84232759600007512 -26.22188218099995538, 30.84227651500003731 -26.22188682499995593, 30.84218364300005533 -26.22189765999991096, 30.84215578000004143 -26.22192552199993543, 30.84208612400004768 -26.22193016599993598, 30.84206755000008116 -26.22191468699992356, 30.84204897500006837 -26.22188837299995612, 30.84201337300004298 -26.22188218099995538, 30.8419824160000644 -26.22189920799991114, 30.84194526600003883 -26.22191468699992356, 30.84191121200007046 -26.22191313799993395, 30.8418694190000906 -26.22194409699994821, 30.84182143600008885 -26.22195338399990305, 30.8417440410000836 -26.22195493199990324, 30.84168831500005581 -26.22195802899994987, 30.84165581100006648 -26.22197041099991566, 30.84161711300004072 -26.22198743799992826, 30.84162330400005203 -26.22206947599994464, 30.84158151100007217 -26.22209733799991227, 30.84154900500004715 -26.22210817399991356, 30.84150102100005597 -26.22213139199993748, 30.84147315900008834 -26.22217163699991715, 30.84143668500007607 -26.22221150399991529, 30.84136579300007952 -26.22224123199993073, 30.84133606400007466 -26.22227782199990997, 30.84133606400007466 -26.2223349909999115, 30.84130405000007613 -26.22235785999993141, 30.8412697470000694 -26.22237844099993254, 30.84121029100003852 -26.22237844099993254, 30.8411805620000905 -26.22235557299995889, 30.84115083300008564 -26.22231669699993972, 30.84109594800008836 -26.22228925699994306, 30.84102505900006008 -26.22229382899990924, 30.84101362400008384 -26.22232584499994346, 30.84097932300005596 -26.22236929399991823, 30.8409107170000425 -26.22241731699995171, 30.84086955400005081 -26.22240130999995245, 30.84082610500007604 -26.22240130999995245, 30.84075064000006705 -26.22236471999991636, 30.84074855800008663 -26.22236457199994675, 30.84068661000003431 -26.22236014599991449, 30.84062029200003963 -26.22236700699994572, 30.84054711400005999 -26.22238758899993627, 30.84049420900004179 -26.22240806799993607, 30.84048300400007747 -26.22237628899995343, 30.84044604200005324 -26.22236298199993598, 30.84038838100008206 -26.22234228399992162, 30.84032037100007528 -26.22227575199991634, 30.84021687700004577 -26.2222254829999315, 30.84015921600007459 -26.22218408599991335, 30.84012668900004428 -26.22214712399994596, 30.84011265900005583 -26.22212496899993539, 30.84010699800006705 -26.22200302699991425, 30.84015596800009007 -26.2218634629999201, 30.84022452600004272 -26.22168716999993876, 30.8402637020000725 -26.22155005399991978, 30.84026125400004048 -26.22148149699995656, 30.84023432000003595 -26.22144721699993397, 30.84019269700007726 -26.22141048999992563, 30.84009965300003842 -26.2213835559999211, 30.83954384200006871 -26.22121950599995444, 30.83924512500004766 -26.22115584499994156, 30.83901006800005007 -26.22120726399992918, 30.83885211300008677 -26.22127850499992974, 30.83875217400003521 -26.22132312099995488, 30.83863174300006449 -26.22136464799990563, 30.83852377100004105 -26.22140825299993594, 30.83832859300008522 -26.22147262099991849, 30.83810018900004479 -26.22152868299991724, 30.83612502300007918 -26.22223075899995592, 30.83605070400005843 -26.22226059699994494, 30.83540817100004006 -26.22252040399990847, 30.83532994900008362 -26.22254554599993526, 30.83528804400003764 -26.22254833999994617, 30.83522937900005445 -26.2225176099999544, 30.83500031500005889 -26.22203148299990971, 30.8349969980000651 -26.22202592999991566, 30.83469776900005854 -26.22129758699992408, 30.83452184800006535 -26.22088491499994234, 30.83429331500008175 -26.22033413499991639, 30.83416284700007282 -26.22003909699992619, 30.83441929300005313 -26.21995293599991328, 30.83445555200006538 -26.21993206099995177, 30.83448302000005015 -26.21991008499992404, 30.83450609300007272 -26.21988811199992142, 30.83452916700008473 -26.21985734699995874, 30.83455993000006856 -26.21982658199993921, 30.83458410300005426 -26.21981010099995046, 30.83463354600007733 -26.21976944799990861, 30.8346807920000856 -26.21974966999994194, 30.83472584000008965 -26.21973428999990574, 30.83476099900008194 -26.21971341299990854, 30.83479506000008996 -26.21967935199995736, 30.83482252800007473 -26.21965298199995686, 30.8348337590000483 -26.21961437299995623, 30.83483455800006823 -26.219598666999957, 30.83484333300003755 -26.21956883099994684, 30.83485649700008935 -26.21953987299991695, 30.83488984300004176 -26.21948809799994251, 30.83492143300009047 -26.2194328139999584, 30.8349477590000447 -26.21939420299992207, 30.83496969800006582 -26.21936348899993163, 30.83499163600004067 -26.2193222449999439, 30.83501357400007237 -26.21927398099995798, 30.83502410500005908 -26.21922834999992347, 30.83502761500005818 -26.21918183999991925, 30.83502147200005084 -26.21912304399995719, 30.83501620700008061 -26.21905020999992075, 30.83501971700007971 -26.21899843599993574, 30.83502586100007647 -26.21896157999992738, 30.8350074300000756 -26.21891945799990253, 30.83499602400007689 -26.21888611199995012, 30.83498812600004158 -26.21884750099991379, 30.8349837380000622 -26.21880625699992606, 30.83513830700007929 -26.21877450099992757, 30.83516122400004633 -26.21872866699993665, 30.83522997600005056 -26.21870116599990297, 30.83532164600006809 -26.21871033299993314, 30.83532622900008846 -26.21865533099992263, 30.83532622900008846 -26.2185911629999282, 30.83535831300008567 -26.21853616099991768, 30.83541789800005972 -26.21848574299991697, 30.83550498400006745 -26.21842157499992254, 30.83551873400006116 -26.21838490699991553, 30.83556915200006188 -26.21836198899995907, 30.8356470720000857 -26.21831157099995835, 30.83577082500005417 -26.21829323699995484, 30.83580290900005139 -26.21825656999993726, 30.83587624500006541 -26.21827490399994076, 30.83600458300008995 -26.21833448899991481, 30.83604583300007107 -26.21836198899995907, 30.83611000100006549 -26.21834365599994499, 30.83620625400004656 -26.2183161549999113, 30.83626125600005707 -26.21835282299991832, 30.83624484600005644 -26.21836940999992294, 30.83624484600005644 -26.2183992309999212, 30.83627918500008036 -26.21842724199990471, 30.83632255900005248 -26.21843808699992451, 30.83637225700005047 -26.21844169999991436, 30.83638852300003919 -26.21842453199991496, 30.83638129400003436 -26.21841188199994122, 30.83641292100008968 -26.21839832599994224, 30.83644454800008816 -26.2183992309999212, 30.8364715870000623 -26.21841613199995891, 30.83649515100006511 -26.21843085799991968, 30.83652677900005301 -26.21843718299993498, 30.83665780300003689 -26.2184335689999557, 30.83671382800008587 -26.2184543519999238, 30.83676804600008836 -26.21847242599994843, 30.83680870800003504 -26.21846248499991816, 30.83683491500005402 -26.21845796799993877, 30.83685027600006379 -26.21842995399993015, 30.83686563700007355 -26.21842633999995087, 30.83688913100007767 -26.21838838699994767, 30.83693250600003921 -26.21841820699995651, 30.83695600000004333 -26.21841820699995651, 30.83695690300004344 -26.21839380899990601, 30.83699666300003628 -26.21838657999995803, 30.83701563800008216 -26.21838206199993238, 30.83704365100004452 -26.21833959199994979, 30.8371032910000622 -26.21835675999994919, 30.83713491800006068 -26.21838025499994274, 30.83716654500005916 -26.21839019499992673, 30.83721805100003621 -26.21837392899993802, 30.83725419600006035 -26.21839109699993742, 30.83728130500009001 -26.21838838699994767, 30.83734004200005074 -26.21836850799991225, 30.83735992100008616 -26.21840284499995732, 30.83737076400007027 -26.21844169999991436, 30.8373987760000432 -26.21845977399993899, 30.83745299400004569 -26.21845344799993427, 30.83751263300007395 -26.21842633999995087, 30.83755781500008197 -26.2184091709999052, 30.83752347700004748 -26.21838477299991155, 30.83755871800008208 -26.21836308599995391, 30.83761112900003809 -26.21838477299991155, 30.83763552600004232 -26.21839380899990601, 30.83767257400006656 -26.21838386799993259, 30.83769335800008093 -26.21840284499995732, 30.8377403470000786 -26.21841820699995651, 30.8377990830000499 -26.21842182299991464, 30.83784155300008933 -26.2183956159999525, 30.83788312000007181 -26.21839832599994224, 30.8379228780000858 -26.21837212199994838, 30.83797619300008819 -26.21837392899993802, 30.83804215800006432 -26.21842091799993568, 30.83809908600005656 -26.21842091799993568, 30.8381225810000501 -26.21842362899991485, 30.83814697900004376 -26.21844169999991436, 30.83816234000005352 -26.21843266499990932, 30.83821475100006637 -26.21843628099992429, 30.83829969100008839 -26.21840826699991567, 30.83832837800008519 -26.21837674899995818, 30.83835817900006759 -26.21840790399994603, 30.83841236200004232 -26.21840790399994603, 30.83846654500007389 -26.21844041399992875, 30.83849499100006142 -26.21845260499992492, 30.83853156500003934 -26.21841332199994667, 30.83857355700007474 -26.21843364099993323, 30.83862909500004434 -26.21840248699993481, 30.83865889600008359 -26.218416030999947, 30.83869953200007785 -26.21839300299990327, 30.83874829800004136 -26.21841467699994155, 30.83879706300007228 -26.21840790399994603, 30.83883363600006078 -26.21841332199994667, 30.83890407300003744 -26.21838487499991288, 30.83892710200007059 -26.2183591389999151, 30.83894064800006163 -26.21833475699992277, 30.83896909400004915 -26.2183076649999407, 30.83899347700008775 -26.21826973799994676, 30.83901515000007976 -26.21822774499992192, 30.83901921400007495 -26.21818710699994881, 30.83901921400007495 -26.21814917799991917, 30.83903682300007176 -26.21811260599992011, 30.83907068800004936 -26.21808822299993835, 30.83913977100007742 -26.21808551399993803, 30.83918582600006175 -26.21809228799992297, 30.83923594600008755 -26.21804487699995434, 30.83928471100006163 -26.21809093099994925, 30.8393185750000498 -26.21808822299993835, 30.83935921300007976 -26.21806248699994057, 30.83939443200006281 -26.21802455799991094, 30.83946893400008094 -26.21800830299991958, 30.83959115800007567 -26.21796594999995023, 30.83966845700007298 -26.21791864299990493, 30.8396873670000673 -26.21784300399991707, 30.83974724700004799 -26.21780518599990728, 30.83980397600004153 -26.21776736499992921, 30.83988276700006281 -26.21778312299994695, 30.83994264600005408 -26.21783354899991991, 30.84004189000006591 -26.21785193399995251, 30.84006172400006562 -26.21782328399990547, 30.84010800300006849 -26.21776818999995839, 30.84011241000007431 -26.21772411499995314, 30.84013224400007402 -26.21766902199993865, 30.84017191000003777 -26.21763816899994026, 30.84019835600008719 -26.21759409399993501, 30.84022920900008558 -26.21755442599993557, 30.84027769200008606 -26.21756103799992843, 30.84029311800009054 -26.21752798099993242, 30.84035261800005401 -26.21747509199991555, 30.84037686000004896 -26.21744203499991954, 30.84039008300004525 -26.21741118299991058, 30.84044958400005498 -26.21739355299990848, 30.84043195400005288 -26.21734727399990561, 30.8404870480000568 -26.21726573499995538, 30.84049145600005204 -26.21722827099995357, 30.84049806600006605 -26.2171996219999528, 30.84054875200007473 -26.2171819919999507, 30.84054214200006072 -26.21715554699994755, 30.84056858600007445 -26.21713571399993725, 30.8405575680000652 -26.21710706499993648, 30.84058842000007417 -26.2170762119999381, 30.84059723600006464 -26.21705637799993838, 30.84063249600006884 -26.21703874799993628, 30.84068979200003469 -26.21700128499992388, 30.84076472000003832 -26.21696161699992444, 30.84084709400008251 -26.21693513299993583, 30.8409354060000851 -26.21686285199990607, 30.84096692300005316 -26.21676830399991331, 30.84094486000003599 -26.21669581499992319, 30.84089128300007587 -26.21663908699991907, 30.84087867700003471 -26.21657920699993838, 30.84096692300005316 -26.21655399399992348, 30.84100474100006295 -26.21650356799995052, 30.84098583100006863 -26.2164342319999264, 30.84103625700004159 -26.21640271599994776, 30.84109613800006855 -26.21634598799994365, 30.84107092500005365 -26.21631131999993158, 30.84105795700008912 -26.21628392699994947, 30.8410760950000622 -26.21625445299991952, 30.84107496100006074 -26.2161943729999507, 30.84112030400007143 -26.21618643799990878, 30.84113163900008203 -26.21617283399990583, 30.84116904900008649 -26.21619550699995216, 30.84121552600004179 -26.21614789699992798, 30.84125520100008089 -26.2161082209999563, 30.84132888400006323 -26.21604360699990366, 30.84135949100004837 -26.21599712999994836, 30.84136969400003636 -26.21597332499993627, 30.84143544100004419 -26.2159563209999078, 30.84148191800005634 -26.21592457999992121, 30.84152272700004005 -26.21590077499990912, 30.84157940600005077 -26.21583502699991186, 30.84164175300008992 -26.21576247799993098, 30.84169163100006017 -26.21574207299994441, 30.84176078000007237 -26.21575907699991603, 30.84179025300005605 -26.21576134399992952, 30.84179025300005605 -26.21570806599993375, 30.84179252000006954 -26.21568086099995298, 30.8418582680000668 -26.21563324999993938, 30.84189114300005485 -26.21562758099992152, 30.84190247800006546 -26.21561737899992295, 30.84190361100007749 -26.2155992419999393, 30.84193081700004768 -26.21561964599993644, 30.84194328700004917 -26.21559697399993638, 30.8419704930000762 -26.21557203599991226, 30.84201470300007486 -26.21552669199991215, 30.84206798100007063 -26.21546434399994041, 30.84209518700004082 -26.21538159299990411, 30.84209632100004228 -26.21536458999992192, 30.84213826300003802 -26.21535552099993538, 30.84214960000008432 -26.21530790999992178, 30.84216887000008001 -26.21529430699990826, 30.84221194600007721 -26.21528523899991114, 30.84223688500003391 -26.21524556299993947, 30.84225502300006383 -26.21523195999992595, 30.84231850300005817 -26.21525122999992163, 30.84234457600007318 -26.21524782999995296, 30.84240125500008389 -26.21523876199995584, 30.84251066700005595 -26.21520914199993513, 30.84255634600003759 -26.21521182899994074, 30.84258590300004244 -26.21519301999995832, 30.84263964400008717 -26.21514733999993041, 30.84267457500004639 -26.21510703499990314, 30.84271219400005748 -26.21508553999990454, 30.84275249800003849 -26.21507479099994953, 30.84276055900005531 -26.21504792099995029, 30.84275518600009036 -26.21501836399994545, 30.84288147500006971 -26.21503717299992786, 30.84291640600008577 -26.21498074499993436, 30.84292715500004078 -26.21490282199994226, 30.84306150500003696 -26.21490550899994787, 30.84318510700006755 -26.21495387499993512, 30.84327915300008272 -26.21499686599992174, 30.84331677100004754 -26.21501836399994545, 30.84337051100004601 -26.21491894399991907, 30.84342693800005009 -26.21484908199994379, 30.84349411400006602 -26.21483295999991014, 30.84353173300007711 -26.21483295999991014, 30.84355322900006513 -26.21488132599995424, 30.8435908470000868 -26.21491357099995412, 30.84364189900009023 -26.21491625699991346, 30.84369295300007252 -26.21491357099995412, 30.84373325900008922 -26.21491625699991346, 30.84376012900008845 -26.21485982999990938, 30.8438058080000701 -26.21478996699994468, 30.84383536500007494 -26.21476309699994545, 30.84387298300003977 -26.21476309699994545, 30.8439240370000789 -26.21472547899992378, 30.84399389900005417 -26.21472816699991881, 30.84406376100008629 -26.21476309699994545, 30.84407719700004691 -26.21481952399994952, 30.8440745100000413 -26.21485445599995501, 30.84411481400007915 -26.21488669999990861, 30.84414974600008463 -26.21488401199991358, 30.84417392900007826 -26.21488132599995424, 30.8442169210000543 -26.21488669999990861, 30.84427603600005341 -26.21487595199994303, 30.84439426400007278 -26.21489744799993105, 30.84442919600007826 -26.21489744799993105, 30.84446681400004309 -26.21494312699991269, 30.84452592800005277 -26.21494850099992391, 30.84457160600004499 -26.2149458139999183, 30.84461191300005112 -26.2149296919999415, 30.84464415600007214 -26.21490550899994787, 30.84470058300007622 -26.21489207399991983, 30.84473656700004085 -26.21491252299995267)))</t>
+  </si>
+  <si>
+    <t>Dundonald SP</t>
+  </si>
+  <si>
+    <t>Dundonald</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.87756874300004029 -26.23403556199991726, 30.87756322100005946 -26.23410949799995251, 30.87754129300003569 -26.23416431999993392, 30.87750017700005856 -26.23419995499995139, 30.87745906000003515 -26.23421640099991237, 30.8773960140000554 -26.23425751799993577, 30.87730281600005355 -26.23430685799991124, 30.87722332400005598 -26.2343973139999207, 30.87713835000005247 -26.234487771999909, 30.87708900900008757 -26.23456726399990657, 30.87702322300003743 -26.23457822899990788, 30.8770149990000391 -26.23462208599994483, 30.87693276600003855 -26.23470980199994074, 30.8768889070000796 -26.2347509189999073, 30.87686423800005286 -26.2348084809999591, 30.87679571000006717 -26.23484685799991212, 30.87700951700009 -26.23504695899993067, 30.87747002400004703 -26.23556777099992132, 30.87772220700009029 -26.23577335399994581, 30.87803469400006406 -26.23608035999990307, 30.87835594600005606 -26.23641268999995191, 30.87831968800009008 -26.23645584699994515, 30.87876594100004013 -26.23672426899992161, 30.8790075210000623 -26.23689874399991595, 30.87899242200006711 -26.23697256099995911, 30.87894880400006059 -26.23702624499992453, 30.8789337050000654 -26.23705811999991511, 30.87912663500003418 -26.23720071999991887, 30.87973058500006118 -26.23773420999992823, 30.880202003000079 -26.23822743699992088, 30.8802590000000805 -26.23827730999994401, 30.88023989500004518 -26.23829314199991813, 30.87966299900006106 -26.23876992999993263, 30.87964075300004652 -26.23879525799992507, 30.87976722800004836 -26.23886692699994683, 30.87983046500005457 -26.23890346399991813, 30.87989651200007302 -26.23899902299990572, 30.879963966000048 -26.23914517099990462, 30.88000331400007781 -26.23927867199995489, 30.88003001300006645 -26.23938406899992515, 30.88011573600005022 -26.23959907499994415, 30.88015789400003541 -26.23973398099991527, 30.88021270000007235 -26.23984640299994453, 30.88025204700005588 -26.24002908899990416, 30.88030966400003763 -26.24028203899990785, 30.88034058000005189 -26.24037759599991659, 30.88038695400007327 -26.24043802399995684, 30.88044035400008624 -26.24056309299993472, 30.88045721800006049 -26.24059962999990603, 30.88047127000004366 -26.24066567699992447, 30.88049234900006468 -26.24073313199994573, 30.88052607500003433 -26.2408343119999472, 30.88052024800003892 -26.24094352299994171, 30.88048713300008785 -26.24095456199995624, 30.88039330600008725 -26.24098767699990731, 30.88024980600005165 -26.24104838899995684, 30.88024980600005165 -26.24113669699994489, 30.88022220900006687 -26.24124156199991376, 30.88017253500004244 -26.24131331199993156, 30.88006215200005045 -26.24137402299993482, 30.87999592000005578 -26.24139609999991762, 30.87989105600007633 -26.24146233199991229, 30.87979722900007573 -26.24155063799992149, 30.8796923630000606 -26.24161134999991418, 30.87968684400004804 -26.24172725299990816, 30.87965924800005268 -26.24183211999991272, 30.87965924800005268 -26.24190386999993052, 30.87961509400008708 -26.24196458099993379, 30.87955990200003953 -26.24201977399991392, 30.87946055500003695 -26.24206392699994694, 30.87936672900008261 -26.24206944699994892, 30.87930601700008992 -26.2421135999999251, 30.87920115200006421 -26.24212463899993963, 30.8791238830000907 -26.24214671599992244, 30.8790521330000729 -26.24219086999994488, 30.87896382400003858 -26.24219638899995743, 30.87891967000007298 -26.24216879299990524, 30.87877617100008365 -26.24221846599994024, 30.87861059400006525 -26.24229021599995804, 30.87841742100005149 -26.24236196699990842, 30.87826288300004762 -26.24245027299991762, 30.87814594200006013 -26.24251187699991306, 30.8779817070000604 -26.24218540599991911, 30.87753564100006543 -26.24190289799992115, 30.8769706250000695 -26.24147170199995571, 30.87582572400003755 -26.24074312699991651, 30.87496698100005688 -26.24006846999992604, 30.87460370800005194 -26.23967652999994016, 30.87412910200004035 -26.23939607999994905, 30.8733740440000588 -26.23887832599990588, 30.87246797500006323 -26.2384468649999576, 30.87179921000006289 -26.23829585399994357, 30.87146954300004609 -26.23823245699992412, 30.87152796800006627 -26.23808155399990483, 30.87157913600003667 -26.23782270399993877, 30.87160923500005083 -26.23774444699995456, 30.87166341300007844 -26.23767822999991495, 30.87168749100004561 -26.23762405199994419, 30.87170555100004776 -26.23753676599994833, 30.87176875900007644 -26.23738326199992343, 30.87175972900007537 -26.2373200539999516, 30.87176875900007644 -26.23725383699991198, 30.87178681800008917 -26.23716053099991541, 30.87180487700004505 -26.23709732299994357, 30.87186206500007302 -26.23698896899992405, 30.87188915400008682 -26.23693779999990738, 30.87191323200005399 -26.23682041499995421, 30.87191022300004306 -26.23675720699992553, 30.87196139200005973 -26.23671506999994563, 30.87199149000008447 -26.23668496899995262, 30.87200653900003999 -26.23664885299990601, 30.87203964800005451 -26.23661273299995855, 30.87206372700006796 -26.23654049599991822, 30.87210887500003764 -26.23645922899993366, 30.87211489500003836 -26.23640806199995268, 30.87212392500003943 -26.236344853999924, 30.87217509200007726 -26.23621542799992312, 30.87220519000004515 -26.23614620199992942, 30.87221422100003565 -26.23607697499994629, 30.87223529100003816 -26.2359625989999472, 30.87225635900006182 -26.23584822399993755, 30.87231354700008978 -26.23573685799993882, 30.87237073400007148 -26.23566161099995497, 30.87239481300008492 -26.23559840499990514, 30.87239481300008492 -26.2355081079999195, 30.87240986300008672 -26.23546596899990391, 30.87244297100005497 -26.23541179099993315, 30.87246705000006841 -26.23536062399995217, 30.87250015900008293 -26.23526731699990933, 30.8725392870000519 -26.23521313999992799, 30.87267172200006371 -26.23511381299994127, 30.87269580100007715 -26.2350807059999056, 30.87271687000009024 -26.23505361599995922, 30.87274997900004792 -26.23503254799993556, 30.87278007800006208 -26.23500846799993269, 30.87281318600008717 -26.23497535899991817, 30.87286435400005757 -26.23493622999990293, 30.87293358200008697 -26.23483389499995155, 30.87358371500005205 -26.23427706699993678, 30.87423986900006412 -26.23372023999991143, 30.87598860800005696 -26.23389481299994941, 30.87679224600003636 -26.23394598099991981, 30.87702099600005567 -26.23395500999993146, 30.87711430300004167 -26.23393093099991802, 30.87716547100006892 -26.23391889199990601, 30.87729188600008001 -26.23391889199990601, 30.87732198400004791 -26.2339519999999311, 30.8773821810000868 -26.23397607899994455, 30.87748752800007424 -26.23397908899994491, 30.87753869600004464 -26.23401520799990294, 30.87756874300004029 -26.23403556199991726)))</t>
+  </si>
+  <si>
+    <t>Holeka SP</t>
+  </si>
+  <si>
+    <t>Holeka</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.93164914200008297 -26.24740325199991275, 30.93142817400007516 -26.24788938399990457, 30.93160494900007507 -26.24853018999993992, 30.93192975500005559 -26.24909318799990388, 30.93184570300007863 -26.2493033199999104, 30.93172166400006518 -26.24945654399994055, 30.93160492300006581 -26.24954409999992322, 30.93134955000004993 -26.24953680399994482, 30.9312765860000809 -26.24963165599990589, 30.93129847500006235 -26.24977758399995764, 30.93140062400004808 -26.24987973299994337, 30.93121821500005808 -26.25014969799991604, 30.93110147300006929 -26.25037588599991523, 30.93099932400008356 -26.25041966599991383, 30.9305980240000622 -26.25033210799995231, 30.93021131600005447 -26.25031021899991401, 30.92990486900004043 -26.25041966599991383, 30.9296494960000814 -26.25041966599991383, 30.92924089800004595 -26.25031751599993868, 30.92913875000004964 -26.2504488499999411, 30.92900011800008997 -26.25036129399995843, 30.92887608200004479 -26.25033210799995231, 30.928708264000079 -26.25025184799994804, 30.92858422600005497 -26.25021536599990668, 30.92845289100006312 -26.25017158799994377, 30.92828507400008675 -26.25017888499991159, 30.92810266600008617 -26.25011321699992095, 30.92804429400007393 -26.25025184799994804, 30.92795673800003442 -26.25038318399992932, 30.92781810700006417 -26.25049262799990402, 30.9277378470000599 -26.25055099899992683, 30.92757732700005135 -26.25060207399991441, 30.92751895600008538 -26.25057288799990829, 30.92746788100004096 -26.25065314799991256, 30.92740221400003975 -26.25072611199993844, 30.92738032500005829 -26.25085744799991971, 30.92730736100008926 -26.25091581799995311, 30.92721250900007135 -26.25103985599992029, 30.92716873000006217 -26.25109093099990787, 30.9270592850000412 -26.25112011599992456, 30.92700821000005362 -26.25116389399994432, 30.92697172900005853 -26.25118578199993635, 30.92690606100006789 -26.25128063599993311, 30.92682580100006362 -26.2513900819999435, 30.92670905900007483 -26.25152141599994593, 30.92663609500004895 -26.25160897299991802, 30.92661420700005692 -26.25171112199990375, 30.92657042800004774 -26.25176219699994817, 30.92645368700004838 -26.25184245699995245, 30.92633694500005959 -26.25194460599993818, 30.92630775900005347 -26.25201756999990721, 30.92627857300004734 -26.25210512599994672, 30.92613994100008767 -26.25222916399991391, 30.92608157100005428 -26.25246264799994833, 30.92603779300003453 -26.25257938999993712, 30.92599401500007161 -26.25272531699994261, 30.92599401500007161 -26.252834762999953, 30.92600131100005001 -26.2529952829999047, 30.92597942300005798 -26.25316309899994849, 30.92592105100004574 -26.2534914359999334, 30.9262202010000351 -26.25371762299994316, 30.92645368700004838 -26.25414081299993541, 30.92668717000003653 -26.25433781499992847, 30.92693524700007401 -26.25453481699992153, 30.92701550700007829 -26.25491422899995086, 30.92732925000007072 -26.25506745199993475, 30.92743869600008111 -26.25519878499994775, 30.92749706700004708 -26.25532282499995063, 30.9275554380000699 -26.25552712299992209, 30.92780351400006111 -26.25590653399990515, 30.92759921600008965 -26.25599409099993409, 30.92742410300007805 -26.25608164699991676, 30.92710306300006096 -26.25612542499993651, 30.92674554100005935 -26.25614001799993957, 30.92666528100005507 -26.25622027799994385, 30.92648287200006507 -26.2563516129999357, 30.92619831300004307 -26.25649024399990594, 30.92589186600008588 -26.25655591099990716, 30.92561460400008855 -26.2565340219999257, 30.92545408400008 -26.25643916899991837, 30.92541030500007082 -26.25616190699992103, 30.92492874500004518 -26.2560597579999353, 30.92467685500008656 -26.25603877299994338, 30.92453927100007149 -26.25599454999991167, 30.92441642800008594 -26.2559306709999305, 30.92421496600007913 -26.25579799999991337, 30.92402333300003647 -26.25581274299992174, 30.92380712900006756 -26.2558323969999492, 30.923630236000065 -26.2558323969999492, 30.92344351400004143 -26.25578325999993012, 30.92332558600008952 -26.25577834699993218, 30.92306024500004469 -26.25566533099993194, 30.92291774800008852 -26.25577343299994482, 30.92278507800006082 -26.25591592999995783, 30.92269171800006688 -26.25609773799993718, 30.92262292600008777 -26.2562500619999355, 30.92259344400008558 -26.25642204199994012, 30.92259344400008558 -26.25663333299991109, 30.92245586100005994 -26.25675617399991779, 30.92233793100007233 -26.256849534999958, 30.92215121000003819 -26.25691832599994768, 30.92201362500009054 -26.25692815399992242, 30.92185638700004802 -26.25698220499992885, 30.92174828600008141 -26.25710996099991235, 30.92162544300003901 -26.25720332199995255, 30.92152716900005771 -26.25735073199990666, 30.92146329100006596 -26.25745391999993217, 30.92139450000007628 -26.2575964179999346, 30.92131588000006559 -26.25771434699993279, 30.92122252000007165 -26.25781262099991409, 30.92108984900005453 -26.25791089499995223, 30.92103088500005015 -26.25802390999990621, 30.92094735200004152 -26.25805830599995261, 30.92082450900005597 -26.25811235699995905, 30.92076807900008362 -26.25816173299995171, 30.92072937400007504 -26.2580706049999435, 30.92070268600008376 -26.25798787399992307, 30.92069201000003886 -26.25792115499990587, 30.92070001700005832 -26.25787845499991136, 30.92071336100008239 -26.25780106199994179, 30.92072403600008101 -26.25775035499992782, 30.92072136700005558 -26.25770765499993331, 30.92069468000005372 -26.25764894299993557, 30.92068400500005509 -26.25759023099993783, 30.9206893420000597 -26.25749415599995018, 30.9206759990000819 -26.2574060859999463, 30.92067866700006107 -26.25732602499994073, 30.92065998700007867 -26.2572352879999471, 30.92066265500005784 -26.25719792499995719, 30.92065464800003838 -26.25708850699993491, 30.92065464800003838 -26.25701111299991908, 30.92065198000005921 -26.25693105099992408, 30.92065731800005324 -26.25684298199990963, 30.92068400500005509 -26.25677626299994927, 30.9206893420000597 -26.25661880899991729, 30.92069201000003886 -26.25654141399991204, 30.92069468000005372 -26.25642132099994797, 30.92071336100008239 -26.25637328199991316, 30.92074538600007827 -26.25631723999993028, 30.92076406700005009 -26.25626386499993714, 30.92077741100007415 -26.25615711499995086, 30.92079876100007141 -26.25613042699990274, 30.92080142900005058 -26.2560930649999591, 30.92078808600007278 -26.25600499599994464, 30.92077741100007415 -26.25587689699995053, 30.92080142900005058 -26.25578082199990604, 30.9207960930000354 -26.25571143599995594, 30.92079342300007738 -26.25550060399990571, 30.92078808600007278 -26.25538584799994624, 30.92079342300007738 -26.25529244099993775, 30.9208121040000492 -26.25522038599990537, 30.9207960930000354 -26.25516700999992281, 30.9207560610000769 -26.25508961699995325, 30.92074538600007827 -26.25502823599993008, 30.92074538600007827 -26.25495617999990827, 30.92077207400006955 -26.25488945999995849, 30.9208121040000492 -26.2548307499999396, 30.92084146100006592 -26.25476402999993297, 30.92084946700003911 -26.25468129899991254, 30.920881492000035 -26.25461991799994621, 30.92088416100006043 -26.2544758059999026, 30.92087615500008724 -26.25437706199994636, 30.92087615500008724 -26.25433169399991584, 30.92083345500003588 -26.25421426899993094, 30.92082811600005243 -26.25415555499995435, 30.92083345500003588 -26.25407015699994417, 30.92083612300007189 -26.2540141129999256, 30.92082544800007327 -26.25396073899992189, 30.92080943600007004 -26.25388334499990606, 30.92078363800004581 -26.25377792799991994, 30.92076584600005162 -26.25363559599992413, 30.92068756300005816 -26.25349326299993891, 30.92068756300005816 -26.25343277099995021, 30.92070535500005235 -26.25325841299991225, 30.92071247200004791 -26.25309472999992977, 30.92074805500004686 -26.25303779699993356, 30.92076940600009038 -26.25293460599993978, 30.92078008100008901 -26.25287411399995108, 30.92079787100004751 -26.25277803999995285, 30.92074805500004686 -26.25270687299990868, 30.92074449700004379 -26.25263570599992136, 30.920755171000053 -26.25257521499992208, 30.92075161300004993 -26.25250404799993476, 30.92076228800004856 -26.25243288199993685, 30.92077652100005025 -26.2523510399999509, 30.92080854600004614 -26.25216600699991432, 30.92077296300004718 -26.25211619099991367, 30.92066766600004257 -26.25201756999990721, 30.92092304000004788 -26.2519737919999443, 30.92120759600004476 -26.25185704999995551, 30.92124408000006497 -26.25156519499995511, 30.92117841200007433 -26.25145574999993414, 30.9212367830000403 -26.25126604199994063, 30.92131704300004458 -26.25106174599994802, 30.92117111500004967 -26.2509304099999099, 30.92139730300004885 -26.25080637199994271, 30.92157241500007103 -26.25072611199993844, 30.92165997200004313 -26.2505582959999515, 30.92200290000005225 -26.25034669999990911, 30.92212694000005513 -26.25034669999990911, 30.92228016400008528 -26.25022995799992032, 30.92254283300007955 -26.24998188399990795, 30.92284928000003674 -26.24980676999990692, 30.92327246900003956 -26.2495076179999387, 30.92349136000007093 -26.24940546899995297, 30.92347676800005729 -26.24927413499995055, 30.92335272900004384 -26.24924494899994443, 30.92311194900008786 -26.24920117099992467, 30.92306817100006811 -26.24904794699995136, 30.92300250400006689 -26.24892390899992733, 30.92292954000004102 -26.24882905599992, 30.92282009500007689 -26.24869042499994976, 30.92273253800004795 -26.24860286899991024, 30.9226814640000498 -26.24842775599995548, 30.92264498200006528 -26.24827453199992533, 30.92242609100003392 -26.24820156899994572, 30.9223896090000494 -26.24816508699990436, 30.92238231200008158 -26.24787323199990396, 30.92250635100003819 -26.24762515499992332, 30.92298061500008544 -26.24784404499990842, 30.92323598800004447 -26.24753759899994066, 30.92368106600008559 -26.24761785899994493, 30.92387806800007866 -26.24756678299991108, 30.92406047700006866 -26.2473114119999309, 30.92417721900005745 -26.24729681899992784, 30.92421370100004197 -26.24693199999995841, 30.92437928300006433 -26.24667405599990389, 30.9247770280000509 -26.24654147599994758, 30.92552832000006902 -26.24627631299995301, 30.92557251300007692 -26.24598905499993862, 30.9259481600000754 -26.24598905499993862, 30.92641219400007913 -26.24601115199993728, 30.92665525800003934 -26.24594486099994128, 30.92687622600004715 -26.2457680869999308, 30.92705300000005764 -26.24543663499991908, 30.92716348500005097 -26.2451272789999166, 30.92811364900006765 -26.24472953599990888, 30.92877655400008052 -26.24649728099990398, 30.9298813960000416 -26.2462984109999411, 30.93045591300005981 -26.24671825099994749, 30.93094204300007277 -26.2470718009999473, 30.93164914200008297 -26.24740325199991275)))</t>
+  </si>
+  <si>
+    <t>Betty's Goed SP</t>
+  </si>
+  <si>
+    <t>Betty's Goed</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.83845803700006627 -26.31510377799992284, 30.83798540600008664 -26.31484120599992593, 30.83756697800004076 -26.31460874499992997, 30.83737216400004399 -26.3145005149999065, 30.83459715700007564 -26.31478203899990831, 30.83310911000006627 -26.31510377799992284, 30.83154062700003806 -26.31590812699994331, 30.83073627800007444 -26.31639073899992809, 30.83034480100008068 -26.31640077599990946, 30.82916779500004623 -26.31643095499993024, 30.82788083600007667 -26.31582769299990332, 30.8269558340000458 -26.31522442999994382, 30.82659387600006085 -26.31506355999994184, 30.82582974400008879 -26.31433964499990452, 30.82530691700003445 -26.31425920999993195, 30.8250253940000789 -26.31377660199990487, 30.82438191400007099 -26.31321355599993694, 30.82369821700007151 -26.31289181599993299, 30.82333625900008656 -26.31224833599992508, 30.82265256200008707 -26.31192659499993169, 30.82176777700004777 -26.31132333399995105, 30.82104386200006729 -26.31096137599990925, 30.81987755500006188 -26.31035811399993918, 30.81935472800006437 -26.30999615599995423, 30.81911768800006257 -26.30980901899994251, 30.81904021100007185 -26.3093575329999112, 30.81892108800008145 -26.30876687699992544, 30.81910473800007821 -26.30778410599992867, 30.8192040060000636 -26.30741680899990342, 30.81927845900008833 -26.30685097199994971, 30.81945714400006864 -26.30662265099994102, 30.81954152300005489 -26.30623053599993, 30.81985422200006042 -26.30517331299995476, 30.82050940300007369 -26.30459258499990938, 30.82134326900006727 -26.30395725999994738, 30.82189421600008927 -26.30334674999994604, 30.82259903100003839 -26.30252281099990341, 30.82463254000003872 -26.30014980299995386, 30.82494877300007374 -26.2996024769999508, 30.82497309900008986 -26.29865377699991313, 30.82407764200007705 -26.29812013199995135, 30.82323837200004846 -26.29735715899994375, 30.82285052900004985 -26.29693752399992945, 30.82260256100005336 -26.29668955799991181, 30.82236731200003987 -26.29631442999993851, 30.82220200100005059 -26.2961046129999545, 30.82219564300004322 -26.29592658599995048, 30.82204940600007603 -26.29576127399991492, 30.82183958900003518 -26.29564047099995605, 30.82182687300007728 -26.29508731599992188, 30.82180144000005839 -26.29464860599995291, 30.82189681200003406 -26.29450872799992567, 30.82178236600003629 -26.29409544999992931, 30.82183999600005109 -26.29396578199992973, 30.82185866300005728 -26.29392378199992208, 30.82202397500003599 -26.29384112699995057, 30.82208755500005282 -26.29379026199995906, 30.82246268300008296 -26.29382841099993584, 30.82260256100005336 -26.29379026199995906, 30.82266649300004246 -26.29375558199990337, 30.82276440700007925 -26.29359079999994719, 30.82283127400006606 -26.2933949729999199, 30.82291963600005147 -26.29331377699992345, 30.82315606100007699 -26.29272868299995025, 30.82323487100006787 -26.29264270999993869, 30.82331845500004874 -26.29260211199994046, 30.82338054600006672 -26.29253285599992296, 30.82351667000006046 -26.2925161389999289, 30.82366473400008999 -26.2924349409999536, 30.82388921900007972 -26.29237285199991447, 30.82416863200006674 -26.29235135699991588, 30.82440744500007668 -26.29231553599993276, 30.82457939100004296 -26.29229881999992813, 30.82472984300005692 -26.29225583299995606, 30.82489005200005749 -26.29223402299993495, 30.8250141360000498 -26.29227068499994857, 30.82503951700005018 -26.29234400799992954, 30.82510437900003808 -26.29238348899991706, 30.82531024700006128 -26.29241450999995777, 30.82545689200009065 -26.29241450999995777, 30.82566840000004049 -26.29244271099992147, 30.82599271100008309 -26.29252731399992626, 30.82613371600007213 -26.29256961499993395, 30.82643546800005652 -26.29257525599990686, 30.82674567700007628 -26.2926034569999274, 30.82692616500008853 -26.29243707199992741, 30.82711511200005816 -26.29224530399994819, 30.82738866100004316 -26.29195765399992979, 30.82757196800008614 -26.29176870699990332, 30.82765375100007077 -26.2915910399999575, 30.82770451300007153 -26.29130902999992259, 30.82774117400003888 -26.29111726299993279, 30.82777501500004291 -26.29095087599995395, 30.82783987800007708 -26.29085217399995145, 30.82789628100005075 -26.29061246499992421, 30.82792730100004519 -26.29047145999993518, 30.82800062300003674 -26.29022893199993405, 30.82801190400004998 -26.29014714799990315, 30.82797524300008263 -26.29002588399993101, 30.82795268200004557 -26.28985667799992143, 30.82792448100008187 -26.28962542999994412, 30.8279131990000792 -26.28946468399993819, 30.82791038000004846 -26.2893321389999528, 30.82795268200004557 -26.28916011399991248, 30.8279865230000496 -26.28898244799995609, 30.82801754400009031 -26.28874273799993944, 30.82804960000004257 -26.28853425699992385, 30.82802422600008185 -26.28841302499995436, 30.82802986500007592 -26.28832280599993965, 30.82802140600006169 -26.28827769699995542, 30.82796502000007877 -26.28820721199991794, 30.82789171600006739 -26.28806624399993552, 30.82780149700005268 -26.2878858059999061, 30.82769718100007594 -26.2877758509999353, 30.82755057500008888 -26.28768563199992059, 30.82742934200007312 -26.28756721899992499, 30.82738141400005816 -26.28748545799993508, 30.82736167800004523 -26.28733321299995396, 30.82737859400003799 -26.2871443159999103, 30.8273842330000889 -26.28690467199993464, 30.82737231600003724 -26.28677473799990594, 30.82839343400007692 -26.28615318699991121, 30.82904526000004353 -26.28590248499995141, 30.83049933200004489 -26.28545122099990294, 30.83260522900008027 -26.28444841199990378, 30.83486154900003839 -26.28344560399995089, 30.83646604200004049 -26.28259321699994189, 30.8371425320000867 -26.2822972529999106, 30.8381226110000739 -26.28377596799992943, 30.8382920960000888 -26.28370064099993897, 30.83839567000006809 -26.283681809999905, 30.83862165000005007 -26.283681809999905, 30.83893237200004478 -26.28381363199991938, 30.83917718400005015 -26.28395486899995603, 30.83935608500007675 -26.28403019499995708, 30.83981746000006297 -26.28432208599991782, 30.83966948100004402 -26.28636061299994253, 30.83981851300006838 -26.28646316799995475, 30.83989421600006153 -26.28654968499995448, 30.84025109900005646 -26.28671190599993679, 30.84041331900004934 -26.28678760699995109, 30.84092160600005172 -26.28707960299993829, 30.84126767600008634 -26.28716612099992744, 30.84150559800008295 -26.2875770759999341, 30.84159211500008269 -26.28775011099992298, 30.84158866600006377 -26.28780299599992532, 30.84161020100003725 -26.28784128099994177, 30.84161020100003725 -26.28789392299995598, 30.84164609500004417 -26.28800878099991678, 30.84163891600007901 -26.28804706499994381, 30.84162695200006965 -26.28808295899995073, 30.84164130900006739 -26.28810449499991364, 30.84169873700005837 -26.28812124499995662, 30.84176573700005974 -26.28816670899993824, 30.84182077300005176 -26.28820738599995366, 30.84189016600004152 -26.28824088699991535, 30.84186863000007861 -26.28832224499990389, 30.84184709500004828 -26.28839163699990422, 30.84180402300006563 -26.28841077999993558, 30.84178009500004691 -26.28844427999990785, 30.84182316700008641 -26.28856870799995704, 30.84181120200008763 -26.28871706499995753, 30.84170352300003515 -26.28888456499993254, 30.84164609500004417 -26.28904010299993388, 30.8416054160000499 -26.28914777999995067, 30.84160063000007312 -26.28924588699993592, 30.84158866600006377 -26.2893033149999269, 30.84158866600006377 -26.28936792399991873, 30.84161020100003725 -26.28942535199990971, 30.84161977300004764 -26.28945645899995043, 30.84165088000008836 -26.28945885299992824, 30.84165805900005353 -26.28948995799993327, 30.84162695200006965 -26.2895234589999518, 30.84161738000005926 -26.28955217299994729, 30.84164609500004417 -26.28959524499992995, 30.84163891600007901 -26.28965745799990827, 30.84163413000004539 -26.28970770899991294, 30.84164609500004417 -26.28974599499991882, 30.84167481000008593 -26.28976992299993753, 30.8417154870000445 -26.28978906599991205, 30.8417322380000769 -26.28982735199991794, 30.84171309400005612 -26.28991110199990544, 30.84170591600008038 -26.29005467299992915, 30.8416484880000894 -26.29015517299990279, 30.8416484880000894 -26.29032745799992199, 30.84166284500008715 -26.29071031599994512, 30.84171788000008974 -26.29099506599993674, 30.84169873700005837 -26.29105728099995076, 30.84165327300007675 -26.29108838699994521, 30.8416939510000816 -26.29118649499991989, 30.84170591600008038 -26.29122238799993738, 30.84165805900005353 -26.29124392299991086, 30.84166045200004191 -26.29129178099992714, 30.84163652300009062 -26.2913133149999112, 30.84165566700005456 -26.29138510299992504, 30.84169155900008263 -26.29144731599990337, 30.84168438000006063 -26.29149995799991757, 30.84166762900008507 -26.29153585199992449, 30.84165327300007675 -26.29155499499995585, 30.84167959500007328 -26.29159328099990489, 30.8416891660000374 -26.29167463699991458, 30.84164609500004417 -26.29170335199995634, 30.84161020100003725 -26.29173924599990642, 30.84166762900008507 -26.29181581499994991, 30.84174180900004103 -26.29187324499991973, 30.84180402300006563 -26.29194024499992111, 30.84188538000006474 -26.29198570899990273, 30.84189973800005191 -26.29203117299994119, 30.84191648700004862 -26.2920527089999041, 30.84194759500007876 -26.2920527089999041, 30.84196434400007547 -26.29207185199993546, 30.84194998700007773 -26.29211492299992869, 30.84190691700007392 -26.29216517299994393, 30.84195716600004289 -26.2921795309999311, 30.84194520100004411 -26.29223935199991047, 30.84191170200006127 -26.2922824229999037, 30.84189734500006352 -26.29234224499992933, 30.84188059400008797 -26.29236378099994909, 30.84183752300003789 -26.29238053099993522, 30.84183991600008312 -26.29247863799992047, 30.84182555900008538 -26.29253606599991144, 30.8418542720000346 -26.29268681599995716, 30.84188538000006474 -26.29280645899990532, 30.84190930900007288 -26.29289978099990321, 30.84190213000005087 -26.2929548159999058, 30.8419547730000545 -26.29302660199994079, 30.8419547730000545 -26.29308642499995585, 30.84194280900004514 -26.29314624499994579, 30.84194280900004514 -26.29317256599995289, 30.84196673700006386 -26.29318931599993903, 30.84193802200007894 -26.29328503099992531, 30.84191409500004966 -26.29338792399994418, 30.84192606000004844 -26.29344774499992354, 30.84196434400007547 -26.2935434589999204, 30.84200262900003509 -26.29361045899992178, 30.84207202300007111 -26.2936989949999429, 30.84211509500005377 -26.29375163799994652, 30.84212705900006313 -26.29379470899993976, 30.84210552200005395 -26.29382581499993421, 30.84208398800006989 -26.29386170899994113, 30.84208877300005724 -26.29391435199994476, 30.84210073900004545 -26.29396938799993677, 30.84208637900007943 -26.29401724499990678, 30.84205527300008498 -26.29404595899995911, 30.84197630900007425 -26.29412970899994662, 30.84193563000007998 -26.29418235199995024, 30.84190691700007392 -26.29423738799994226, 30.84190930900007288 -26.29431874499994137, 30.84192127300008224 -26.29439531699995314, 30.84190213000005087 -26.29443120799993494, 30.84190213000005087 -26.29453649499993162, 30.84191648700004862 -26.29463460199991687, 30.84191648700004862 -26.29467767499994579, 30.84191648700004862 -26.29470878099994025, 30.84187341600005539 -26.29472313799993799, 30.84185188000003564 -26.2947614249999333, 30.84183991600008312 -26.29482124499992324, 30.84186384500003442 -26.29487149499993848, 30.84184231000006093 -26.29489542399994662, 30.8418447020000599 -26.29499353099993186, 30.84190452300003926 -26.29504617399993549, 30.84190691700007392 -26.29509881699993912, 30.84188777300005313 -26.29524238799990599, 30.84187580900004377 -26.29531656699992936, 30.84187341600005539 -26.29535963699993317, 30.84183034500006215 -26.29543860199993333, 30.84183512900006008 -26.29548885299993799, 30.84183034500006215 -26.29553192399993122, 30.84181359500007602 -26.29560131699992098, 30.84183752300003789 -26.29562285199995131, 30.84183752300003789 -26.29566113799995719, 30.84180402300006563 -26.29569463699994003, 30.84174420200008626 -26.29572335199992494, 30.84167959500007328 -26.29576642499995387, 30.84158148700004176 -26.29584060199994155, 30.8415479870000695 -26.29589324499994518, 30.84151209500004143 -26.29595306599992455, 30.84147859500006916 -26.29601288799995018, 30.84145705900004941 -26.29604638799992244, 30.84145466600006102 -26.29608228099993994, 30.84147380900003554 -26.29611099499993543, 30.84151448700004039 -26.29614449499990769, 30.8415288450000844 -26.29617560199994841, 30.84155038000005788 -26.29619235199993454, 30.84159823700008474 -26.29621628099994268, 30.84160780900003829 -26.2962713169999347, 30.84158627300007538 -26.29630720899990592, 30.84155277300004627 -26.29635028099994543, 30.84153841600004853 -26.29638856699995131, 30.84153602300006014 -26.29648428099994817, 30.84151209500004143 -26.29653453099990656, 30.84150970200005304 -26.29657042399992406, 30.84148816700007956 -26.29665895999994518, 30.84149295200006691 -26.29672595899995713, 30.84152405900005078 -26.29680492399995728, 30.84154320200008215 -26.29686953099991342, 30.8415479870000695 -26.29691978099992866, 30.84153363000007175 -26.2969437099999368, 30.84150932000005696 -26.29706633199992893, 30.84154830900007482 -26.29712664199990968, 30.84157125900003393 -26.29719038799993314, 30.84157890700004145 -26.29725923299992019, 30.84155851000008397 -26.29731533099993612, 30.8415202610000847 -26.29732043099994598, 30.84146167000005789 -26.2973066819999417, 30.84146105300004592 -26.29730979099991828, 30.8414228210000374 -26.29730463299995336, 30.84141316700004154 -26.29729238299995586, 30.84138001800005213 -26.29730003199995281, 30.84134687000005215 -26.29732043099994598, 30.84130607300005522 -26.2973663289999422, 30.84128567400006204 -26.29741732499991258, 30.84123212600007946 -26.29743517499991867, 30.84122702800004845 -26.2974759719999156, 30.84121172900006513 -26.29751166999994894, 30.84121172900006513 -26.29754481899993834, 30.84122447800007194 -26.29759836499994208, 30.84124232500005292 -26.29765956199992161, 30.84127292400006581 -26.29772840799995492, 30.84128567400006204 -26.29777685499993822, 30.84127802400007567 -26.29779725499992082, 30.84121427900004164 -26.29784570199990412, 30.84118367900003932 -26.29789414899994426, 30.84118113000005224 -26.29793494799992004, 30.8411556310000492 -26.29797319499994046, 30.84116328100003557 -26.29801399199993739, 30.84114798100006283 -26.29810578699994039, 30.84110208400005604 -26.29814913499990325, 30.84106638500009012 -26.29821033199993963, 30.84107403400008707 -26.29825877899992292, 30.84107148600008941 -26.29829447799994568, 30.84110208400005604 -26.29833782299994027, 30.84106893600005606 -26.29838882199993577, 30.84106128500008026 -26.29843726899991907, 30.8410587370000826 -26.29848061599994935, 30.8410587370000826 -26.29851886399995919, 30.84103833700004316 -26.29855456199993569, 30.84104088700007651 -26.29857751099990537, 30.84100518900004317 -26.29860810899992885, 30.84102303800005984 -26.2986489069999152, 30.84101028900005304 -26.29867950399994925, 30.84102558800003635 -26.29872030299992502, 30.84098989000005986 -26.29880189899995457, 30.84095674200005988 -26.29885289599991438, 30.84092104400008338 -26.29889624299994466, 30.84086749800007965 -26.29896253999993405, 30.8408445480000637 -26.29901098799990677, 30.84079355100004705 -26.2990415839999514, 30.84080375100006677 -26.29908493299990369, 30.84082924900008038 -26.29912573099994688, 30.84084709800004021 -26.29917417799993018, 30.84090574500004323 -26.29917672899995296, 30.84094654300008642 -26.29919712599991044, 30.84096694100009017 -26.29923537499990971, 30.8409363430000667 -26.2992914709999468, 30.84090064500009021 -26.29933736899994301, 30.84087514600008717 -26.29940366499994298, 30.84083944900004326 -26.2994750609999528, 30.8407961010000804 -26.29950565999990886, 30.84075020400007361 -26.29950310999993235, 30.84072470500007057 -26.29953370799995582, 30.84067370800005392 -26.29955155599992622, 30.84066860800004406 -26.29958980499992549, 30.84063546000004408 -26.29958470499991563, 30.8406150610000509 -26.29960000399995579, 30.84058446300008427 -26.29960765399994216, 30.84052836500006833 -26.29962550299995883, 30.84047991900007446 -26.29962040299994896, 30.84044677000008505 -26.29962040299994896, 30.84045697000004793 -26.29967139999990877, 30.84044932000006156 -26.29969689899991181, 30.84045442000007142 -26.29973514599993223, 30.84038812400007146 -26.2998218419999148, 30.84031672900005105 -26.30001053099994124, 30.84029122900005859 -26.30011252599990712, 30.84025808100005861 -26.30013547499993365, 30.84024278200007529 -26.30020432099991012, 30.84021983300004877 -26.30029101599990327, 30.84017903400007299 -26.30038281099990627, 30.84017903400007299 -26.3004542069999161, 30.84015608600003588 -26.30050265399995624, 30.84016118700003517 -26.30054345199994259, 30.84017903400007299 -26.30057659999994257, 30.84013058800007911 -26.30059699999992517, 30.84009744000007913 -26.30062249799993879, 30.84009234000006927 -26.30067349499995544, 30.84009489000004578 -26.30071429199995237, 30.84005154200008292 -26.30074998999992886, 30.84004644300006248 -26.30078823899992813, 30.84001839400008294 -26.30080098799993493, 30.83998014600007309 -26.30080863599994245, 30.83995974700007991 -26.30078058999993118, 30.83992659900007993 -26.30080098799993493, 30.83991895000008299 -26.30082903599992505, 30.83986030300007997 -26.30087493299993184, 30.83980420700004288 -26.30086473399995839, 30.83978125700008377 -26.30088513299995157, 30.83977360800008682 -26.30092338099990457, 30.83974301000006335 -26.30092083099992806, 30.83973791000005349 -26.30095652999995082, 30.83969456200009063 -26.30096672899992427, 30.83963846600005354 -26.3009871259999386, 30.83957726900007401 -26.30097182699995528, 30.83954157100004068 -26.30100242599991134, 30.83950842300004069 -26.3010508739999409, 30.83945487500005811 -26.30104067399992118, 30.83940897800005132 -26.30105342299992799, 30.83934778100007179 -26.30106872299995757, 30.83930443400004151 -26.30110187099995755, 30.8392712850000521 -26.30113501999994696, 30.83923813800004154 -26.30115541699990445, 30.83920244000006505 -26.30116561599993474, 30.83916929100007565 -26.30119366599990371, 30.83914634300003854 -26.301237012999934, 30.83914379300006203 -26.30126761199994689, 30.83912594400004537 -26.30129820999991352, 30.83909534500008931 -26.30132880899992642, 30.83907749800005149 -26.30136705599994684, 30.83905454800003554 -26.3013721559999567, 30.83903669900007571 -26.30138490499990667, 30.83901630000008254 -26.30143080199991346, 30.83900100100004238 -26.30148180099990896, 30.83901120000007268 -26.30152004799992937, 30.8389806020000492 -26.30155319599992936, 30.83895510300004617 -26.30158379399995283, 30.83895765300007952 -26.30162459199993918, 30.83892960400004313 -26.30163224099993613, 30.83893980300007343 -26.3016602909999051, 30.83894490400007271 -26.30168833699991637, 30.8389321550000659 -26.30172913599994899, 30.83890920700008564 -26.30175463399990576, 30.83888115700005983 -26.30178523299991866, 30.83884800900005985 -26.30179798199992547, 30.83883271000007653 -26.30182857999994894, 30.8387970120000432 -26.30185152999990805, 30.83880211200005306 -26.30188722699995196, 30.83879191200009018 -26.30193822399991177, 30.83878936300004625 -26.30197392199994511, 30.83876609900005406 -26.30202547399994728, 30.83873627000008355 -26.30203694799990899, 30.83873627000008355 -26.30207136699993953, 30.83870873300008952 -26.30209431299994094, 30.83867201900005739 -26.30210578599991322, 30.83862612700005457 -26.30212873299990406, 30.83862842000007731 -26.30218380399992384, 30.83865825100008351 -26.30221133899993902, 30.83863301100006993 -26.30225493699992967, 30.83858711800007768 -26.30232377599992333, 30.83858482300007609 -26.30239031999991539, 30.83858482300007609 -26.30244768599993677, 30.83857105600003479 -26.30251881999993202, 30.83853893100007326 -26.30258765699994683, 30.8385343420000595 -26.30269091599990361, 30.83853663600007167 -26.30272992599992676, 30.83851827900008402 -26.30274828199992498, 30.83848386000005348 -26.30278040599995393, 30.83849762800008421 -26.30280105999992202, 30.83850221700004113 -26.30288136999990911, 30.838442556000075 -26.30297774499990737, 30.83841961100006301 -26.30300298599991038, 30.83837142300006917 -26.30307411899991621, 30.83837830700008453 -26.30310624399993458, 30.83836453900005381 -26.30314066299990827, 30.83837830700008453 -26.30315901999995276, 30.83837371800007077 -26.30320032299994182, 30.83835306600008153 -26.30325080399995841, 30.83830335000004652 -26.30336515399994823, 30.83829723000008016 -26.30344470099993259, 30.83826969500006498 -26.30350283199993555, 30.83826969500006498 -26.30357014199995547, 30.83826663500008181 -26.30361297399991827, 30.83826051600004803 -26.30366192599990427, 30.83822380200007274 -26.30369252099990263, 30.83819320700007438 -26.30372617599994101, 30.83818708700005118 -26.30377818699992076, 30.83814119500004836 -26.30381796099993608, 30.83810754200004567 -26.30386079299995572, 30.83811977900006696 -26.30390668599994797, 30.83807388500008528 -26.30397399499992162, 30.83798966100005146 -26.30403908399995316, 30.83791135000006989 -26.30412783099990293, 30.83789586200003896 -26.30418634399995881, 30.83784767500003454 -26.30422592699994766, 30.83777711500005125 -26.30426722999993672, 30.83777539400006162 -26.30429304399990542, 30.83775130000003628 -26.30433090599990464, 30.83771516000007296 -26.30437220899995054, 30.83768418200008909 -26.30439458299991884, 30.83765664700007392 -26.30442555899992385, 30.83762739000007969 -26.30444793199990272, 30.83759985500006451 -26.30448751299991272, 30.83759641400007467 -26.30452537499991195, 30.83757748200008564 -26.30455291099991655, 30.83756027200007566 -26.30457528299990599, 30.83752929400003495 -26.30459937699993134, 30.83748799200003532 -26.30462519199994631, 30.83747422400006144 -26.30464756299994633, 30.83745529300006183 -26.30468714699992461, 30.83745012900004667 -26.30470779799992442, 30.83747594500005107 -26.30472328699994478, 30.83745873500004109 -26.30474221799994439, 30.83745529300006183 -26.30476975299990272, 30.83746561900005645 -26.30479384599993864, 30.83746561900005645 -26.3048248239999225, 30.83745012900004667 -26.3048523599999271, 30.83742947900003628 -26.30489538499995206, 30.83743464100007259 -26.3049143149999054, 30.83741054800003667 -26.30495045499992557, 30.83741226900008314 -26.30497110699991481, 30.83742087400008813 -26.30499692099994036, 30.83738645400006817 -26.30504338699995515, 30.83736924600003704 -26.3050795279999079, 30.83740022200004205 -26.30510534199993344, 30.83739678000006279 -26.30518278599993209, 30.83740882700004704 -26.30526195099992037, 30.83742775800004665 -26.30529464799991501, 30.83745873500004109 -26.30531185899991442, 30.83748627100004569 -26.30533595199995034, 30.83750175900007662 -26.30538069799990808, 30.8375155270000505 -26.30541167499990252, 30.83753617900003974 -26.30542200099995398, 30.83753101600007085 -26.30544781499992268, 30.83751724900008639 -26.30548567699992191, 30.83753101600007085 -26.30551665399991634, 30.83751036400008161 -26.30554074799994169, 30.83751208500007124 -26.30558377199992037, 30.83749831700004052 -26.3056113089999144, 30.83752069000007623 -26.30565777299995034, 30.83748627100004569 -26.3057162869999388, 30.83753617900003974 -26.30574382199995398, 30.83755510900004992 -26.30575758999992786, 30.83756027200007566 -26.30578684699992209, 30.8375430630000551 -26.30579372999994803, 30.83753790000008621 -26.30581610399991632, 30.83753101600007085 -26.30591936199994052, 30.83750003800008699 -26.30595206099991401, 30.83748885300008169 -26.30600675399995225, 30.83745981100008748 -26.30603676399994129, 30.83746077900008231 -26.3060677399999463, 30.83748982100007652 -26.30610549599992964, 30.83749659500006146 -26.30613647299992408, 30.83749950100008164 -26.30615389599995524, 30.8375053090000506 -26.3061839069999337, 30.83751014900008158 -26.30622262899993302, 30.83747723500005122 -26.30623134199993274, 30.83748207600007163 -26.30628070999995316, 30.83749175700006617 -26.30632911399993645, 30.837492725000061 -26.30637654799994607, 30.83747917200008715 -26.30644043899991402, 30.83748498000005611 -26.30647432099993921, 30.83745981100008748 -26.3064946499999337, 30.83746852300004093 -26.30652659499992296, 30.83745787500004099 -26.30656822099990677, 30.83741528100006235 -26.30661468699992156, 30.83737752700005785 -26.30663791999995738, 30.83737462300007337 -26.30667276999992055, 30.83735332600008405 -26.30672020399993016, 30.83733977300005336 -26.30676376599990363, 30.8373136360000899 -26.30681507299993882, 30.83729137100004891 -26.30682765699992842, 30.83727685100006966 -26.30684701799992808, 30.83724780900007545 -26.30689735699991161, 30.83722651200008613 -26.30694672699991088, 30.83721973500007607 -26.30697189599993635, 30.83722748000008096 -26.30701352199992016, 30.83724587300008579 -26.30703869099994563, 30.83725942500007022 -26.30708806199993433, 30.83728749800008018 -26.30712097499991842, 30.83729137100004891 -26.30715388899994878, 30.83731847700005346 -26.30718389799994839, 30.83732912400006398 -26.30722455599993737, 30.83729814700006955 -26.30727005399995733, 30.83730105100005403 -26.30730780799990498, 30.83730298700004369 -26.30735330599992494, 30.83732912400006398 -26.30738621899990903, 30.83733977300005336 -26.3074230069999544, 30.83732234700005392 -26.30744139799992354, 30.83732718800007433 -26.30749076899991223, 30.83734945300005847 -26.30752658599993765, 30.83736978100006354 -26.30755853099992692, 30.83741043900005252 -26.30758757299992112, 30.83743173700008811 -26.30761855099990498, 30.83745400100008283 -26.30764952799995626, 30.83745496900007765 -26.30766501699991977, 30.83747239500007709 -26.30769308999992973, 30.83748982100007652 -26.3077201969999237, 30.83750918100008676 -26.30773858799994969, 30.83751208500007124 -26.30777440599990769, 30.83753338300004998 -26.30778215099991257, 30.83753725300005044 -26.30782764899993253, 30.83754209500006027 -26.30786733899992669, 30.83753531900003964 -26.30790315599995211, 30.8375430630000551 -26.30795639899992011, 30.83754983900007574 -26.30797188799994046, 30.83755274300006022 -26.30801641799990875, 30.83757307300004413 -26.3080406189999394, 30.83757887900003425 -26.30806578899995429, 30.83758565700009058 -26.30809579699990763, 30.83760598600008507 -26.30812967899993282, 30.83760017700006983 -26.3081974409999475, 30.8375827510000704 -26.30826133299990488, 30.8375556470000447 -26.30830295899994553, 30.83749369100007698 -26.30838524299991832, 30.8374675550000461 -26.30842009299993833, 30.83746077900008231 -26.30845494099992266, 30.83748691700003519 -26.30851302499991107, 30.83750046900007646 -26.30857304399995655, 30.83749756300005629 -26.30864467899993997, 30.83750821300003508 -26.30870857099995419, 30.83752370200005544 -26.30877246099993272, 30.83752079800007095 -26.3088131189999217, 30.83752563800004509 -26.30883247999992136, 30.83752176600006578 -26.30885861799993108, 30.8375053090000506 -26.30890121199990972, 30.83753435100004481 -26.30892541299994036, 30.83754209500006027 -26.30900091999990309, 30.83754887100008091 -26.30905416299992794, 30.83752951000008125 -26.30907545999991726, 30.83754209500006027 -26.30908417199992755, 30.83755371100005505 -26.3091112779999321, 30.8375304790000655 -26.30913063799994234, 30.83757113600006505 -26.30915290299992648, 30.83759243300005437 -26.30918388099991034, 30.83759630500009052 -26.30923131499991996, 30.83757694500008029 -26.30926035599992474, 30.83755661500003953 -26.30929036599991377, 30.83757404100003896 -26.30931166299990309, 30.83757694500008029 -26.30934263999995437, 30.83755661500003953 -26.30937264999994341, 30.83754887100008091 -26.30942105199994785, 30.83753338300004998 -26.30942976399995814, 30.83753144700006033 -26.3095110799999361, 30.83751014900008158 -26.30952753699995128, 30.83753435100004481 -26.30955173799992508, 30.83752854200008642 -26.30961272499990855, 30.83751305300006607 -26.30963595799994437, 30.83748691700003519 -26.30963595799994437, 30.83747529900006157 -26.3096495099999288, 30.83747239500007709 -26.309682425999938, 30.83748304400006646 -26.30970662599992238, 30.83751692500004538 -26.30970565799992755, 30.83752660600003992 -26.30971533799993267, 30.83755758300003436 -26.30973760299991682, 30.83756048700007568 -26.30976954999994177, 30.83754790300008608 -26.30979762199990546, 30.83755467900004987 -26.30983924799994611, 30.83754693500003441 -26.30987506599990411, 30.83755080700007056 -26.30990700999990395, 30.83755855100008603 -26.30993992599991316, 30.83757113600006505 -26.30996606199994403, 30.83759049700006472 -26.30999607099994364, 30.8375827510000704 -26.31001930499991204, 30.83758662500008541 -26.31004544199993234, 30.83757404100003896 -26.31006286699994234, 30.83758178300007557 -26.31010739699991063, 30.83760308100005432 -26.31016838399995095, 30.83763405900003818 -26.31017806399995607, 30.83765148400004819 -26.31021484999990889, 30.83766310100008923 -26.31022549799990884, 30.83767762100006848 -26.31023808299994471, 30.83768536500008395 -26.31026421999990816, 30.83768536500008395 -26.31030487799995399, 30.83768826900006843 -26.31033585599993785, 30.83769407800008366 -26.31034456799994814, 30.83769214200003717 -26.31038038599990614, 30.837674717000084 -26.31041039599995202, 30.837674717000084 -26.31044040499995162, 30.83766890900005819 -26.31046750999990991, 30.8376456750000898 -26.31047815799990985, 30.83762631500007956 -26.31045782999990479, 30.83759824100008018 -26.31044137299994645, 30.83755080700007056 -26.31047428599993054, 30.8375198290000867 -26.31051784799990401, 30.83753241500005515 -26.31056044199993948, 30.83751111700007641 -26.31057980299993915, 30.8375053090000506 -26.31064078999992262, 30.83750918100008676 -26.31067563999994263, 30.83749562700006663 -26.31069596899993712, 30.83748207600007163 -26.31072984999991604, 30.83745981100008748 -26.31076566799993088, 30.8374375460000465 -26.310775347999936, 30.83741818500004683 -26.31079083699995635, 30.83738527100007332 -26.31081697399991981, 30.83734267700003784 -26.31082084699994539, 30.83732815600006916 -26.31084988799995017, 30.83723425700003418 -26.31087892899995495, 30.83718585400004031 -26.31091765099995428, 30.83714616500003558 -26.31097670199994809, 30.83713551500005678 -26.31103188099990575, 30.83713067500008265 -26.31107156999991048, 30.83711615400005712 -26.31109189899990497, 30.83712680300004649 -26.31110738799992532, 30.83712583500005167 -26.3111238449999405, 30.83710647500004143 -26.31115578999992977, 30.83708614500005751 -26.31119644799991875, 30.83709098500008849 -26.31122839399995428, 30.83709195300008332 -26.31128163599993286, 30.8370822730000782 -26.31130583699990666, 30.83706968800004233 -26.31132810299993707, 30.83706387900008394 -26.31135327099991628, 30.83710647500004143 -26.31137263299990536, 30.83711615400005712 -26.31138618499994664, 30.83712389900006201 -26.31139876999992566, 30.83712486700005684 -26.3114171629999305, 30.83710840900005223 -26.31145491699993499, 30.83710840900005223 -26.31147427899992408, 30.8371200270000827 -26.31150138299994978, 30.83712680300004649 -26.3115468809999129, 30.8371200270000827 -26.31157592199991768, 30.8371200270000827 -26.31160012299994833, 30.83715778000004093 -26.3116281969999477, 30.83715874800003576 -26.31165530199990599, 30.83716746100003547 -26.31168434299991077, 30.83717230100006645 -26.31172112899992044, 30.83717617300004576 -26.31176953199991431, 30.83718488600004548 -26.31178114699991966, 30.83718295000005583 -26.31182374099995513, 30.83717230100006645 -26.311872143999949, 30.83718295000005583 -26.31191861099995322, 30.8371326110000723 -26.31196798099995249, 30.8371326110000723 -26.31199314899993169, 30.83712293100006718 -26.31201928699994141, 30.83711518600006229 -26.31204929699993045, 30.83709292100007815 -26.31208608299994012, 30.8370561360000579 -26.31213158099990324, 30.8370145100000741 -26.31217127099995423, 30.83698546800007989 -26.31220515299992257, 30.8369506190000493 -26.31223225699994828, 30.83692835300007573 -26.31224484299991673, 30.83691673700008096 -26.31228549999991628, 30.83689447100005054 -26.31230582899991077, 30.83690802400008124 -26.31234067899993079, 30.83688672700003508 -26.31236100799992528, 30.83689060100005008 -26.31236875199994074, 30.83689737500003503 -26.31240069699993001, 30.83689543900004537 -26.31243361099990352, 30.83691480100003446 -26.31245297199990318, 30.83691189700004998 -26.31247814099992866, 30.83690318400005026 -26.31252363899994862, 30.83693319500008556 -26.31254203199995345, 30.83692351300004475 -26.31257784999991145, 30.83694190600004958 -26.31259914699995761, 30.8369757890000642 -26.31264754899990521, 30.83698353100004397 -26.31269207899993035, 30.83698740400006955 -26.31272112099992455, 30.83697385300007454 -26.3127491939999345, 30.83695836300006476 -26.31280534099994384, 30.83694190600004958 -</t>
+  </si>
+  <si>
+    <t>26.31284115799991241, 30.83699030800005403 -26.31284793499992247, 30.83697772500005385 -26.31288181599995823, 30.83697772500005385 -26.31292731399992135, 30.83703580700006341 -26.3129302189999521, 30.83705419900007882 -26.31293118699994693, 30.83707646400006297 -26.31290795299992169, 30.83710357100005695 -26.31291666599992141, 30.83711325000007264 -26.31294473899993136, 30.83712777100004132 -26.31296893999990516, 30.83713648300005161 -26.31297087599995166, 30.83716455700005099 -26.31296119599994654, 30.83718017500007136 -26.3129711469999279, 30.83721908900008657 -26.31301006099994311, 30.83725313800005097 -26.31298087599992641, 30.83727746000005254 -26.31302951799995071, 30.83726286700004948 -26.31307815999991817, 30.83732123900006172 -26.31312193999991678, 30.83737474600007999 -26.31318517499994414, 30.83736988200007545 -26.31328246099991475, 30.83740879600009066 -26.31333596799993302, 30.83746230300005209 -26.31337001799994368, 30.83750608200006127 -26.31337488199994823, 30.83756931600004236 -26.31342352499990511, 30.83766660300005924 -26.31347216799991884, 30.83774929400004794 -26.31351594599993859, 30.8378417180000497 -26.31355486099994323, 30.83793413800003691 -26.31359863899990614, 30.83791954500009069 -26.31369105999993963, 30.83793413800003691 -26.31372997599993369, 30.83794873000005055 -26.31377375199991775, 30.83793413800003691 -26.31381266699992239, 30.83790008800008309 -26.31384671799992248, 30.83790495200008763 -26.31388076699994372, 30.83792927400008921 -26.31390995199990357, 30.83795359500004452 -26.31396345899992184, 30.83798278100005064 -26.31404128899993111, 30.8380168310000613 -26.31414343899990627, 30.8380168310000613 -26.3141823539999109, 30.83803142500005379 -26.31430882399990878, 30.83803142500005379 -26.31438665299992863, 30.83807497100008277 -26.31447746899993945, 30.83807846800004882 -26.31450019999994083, 30.83809595500008527 -26.31455440399992085, 30.83808896000005006 -26.31461734999993496, 30.83807497100008277 -26.31464532599994754, 30.83809070800003838 -26.31466106299990315, 30.83809070800003838 -26.31468379399990454, 30.83810644500005083 -26.31469778199993925, 30.83813267200008568 -26.31472400999990668, 30.838162397000076 -26.31476072799995336, 30.83818163100005449 -26.31476947099992003, 30.83821135500005539 -26.31479919599991035, 30.83825506800008043 -26.31483940999993365, 30.83830402700004925 -26.3148796259999358, 30.83833724900006246 -26.31490935199991554, 30.8384054390000415 -26.3150072689999206, 30.83845789600007947 -26.31507895799995822, 30.83845803700006627 -26.31510377799992284)))</t>
+  </si>
+  <si>
+    <t>Mafumulo SP</t>
+  </si>
+  <si>
+    <t>Mafumulo</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.79894036500007815 -26.40313298799992481, 30.79890590600007272 -26.40318122999991601, 30.79874010300005693 -26.40334703399992122, 30.79879056400005766 -26.40352725599990436, 30.79850941800003739 -26.40372189599992225, 30.79815422200005059 -26.4038568289999489, 30.79731873200006476 -26.40418777099995395, 30.79649409100005641 -26.40458381499990992, 30.79425742700004776 -26.40560933999995541, 30.79377793900005145 -26.40507299999995894, 30.79365104200007863 -26.40492865499993513, 30.79356697100007523 -26.40484934299990982, 30.7931275870000718 -26.40432588699991356, 30.79295944700004384 -26.40416567899995925, 30.79268027100005156 -26.40399119399995698, 30.79264220100003513 -26.40390871099992864, 30.79262951000004023 -26.403802432999953, 30.79261840800006667 -26.40368346599990446, 30.79261523600007422 -26.40361049999995657, 30.79261364900008857 -26.40354863599992541, 30.79264220100003513 -26.40348994599992238, 30.79268978800007517 -26.40340746299995089, 30.79273420200007649 -26.40331228899992766, 30.7928198580000867 -26.40307911399992236, 30.7928753770000867 -26.40298076699991725, 30.79297848100003421 -26.40287607499993783, 30.79306889600007935 -26.402815799999928, 30.79317676000005122 -26.40276821299994481, 30.79322943800008261 -26.40275451699994846, 30.79325559800008705 -26.40274771499991857, 30.79338348900006395 -26.40233359299992344, 30.79342703600008235 -26.40208240599991996, 30.79342155900008038 -26.40199340199990274, 30.79342210900006194 -26.40184566199991423, 30.79340102100007925 -26.40158809199994039, 30.79339238900007558 -26.40150131799993005, 30.79352653100005455 -26.40147163199992519, 30.79356050200004802 -26.40142775299995037, 30.79358173300005319 -26.401392365999925, 30.79361570600008235 -26.40133999399995446, 30.79363976800004821 -26.40131451499991044, 30.79366241500008528 -26.40128762199992707, 30.79368930900005807 -26.40125223499995855, 30.7937275260000547 -26.4012196789999507, 30.79375795900006096 -26.40122193499990999, 30.79380175000005693 -26.40122193499990999, 30.79384076400003778 -26.40121954699992557, 30.79384474500005808 -26.40123547099994994, 30.79385589100007792 -26.40123387799991406, 30.79388455400004432 -26.40122830399991471, 30.79390286700004253 -26.40122193499990999, 30.79392038300005652 -26.40122352799994587, 30.79393153000006578 -26.40122750899990933, 30.7939466580000385 -26.40123706299993955, 30.79396815600006221 -26.40123785899993436, 30.79399363400005996 -26.40124900599994362, 30.79400478000007979 -26.40124422899992851, 30.79401115000007394 -26.40122910199994521, 30.79403662800007169 -26.40122750899990933, 30.79404299800006584 -26.40121636199995692, 30.79407007000008889 -26.40119565999992801, 30.79407803100008323 -26.40117575599992961, 30.79409793600007106 -26.40117336699995576, 30.79410828600003924 -26.40116381299992554, 30.79414650400008213 -26.40113753799994356, 30.79416481600003408 -26.40112161399991919, 30.79419427500005213 -26.40111604099990927, 30.79419029400008867 -26.40109693199991625, 30.7942038310000612 -26.40108737799994287, 30.79423886400007859 -26.4010618989999557, 30.79429380000004812 -26.4010427909999521, 30.79430096600003708 -26.40102607099993293, 30.79430892800007769 -26.40100218499992479, 30.79433042500005513 -26.40096874399995386, 30.79434077600006958 -26.40095680099994979, 30.79435266000007232 -26.4009557249999034, 30.79438096900008759 -26.4009557249999034, 30.79442060200005926 -26.40094062699995447, 30.79442815100009057 -26.40092364099990618, 30.79442815100009057 -26.40089721899994402, 30.79443758800005071 -26.40088589599992019, 30.79444891100007453 -26.40085569899991924, 30.79446657500005813 -26.40082622599993556, 30.79446737100005294 -26.40077606399995602, 30.79448727500005134 -26.4007696949999513, 30.79449921900004483 -26.4007338659999391, 30.79450399700004937 -26.40068768599991245, 30.79451036600005409 -26.40065026499991063, 30.7945191240000895 -26.40061682499992912, 30.79453266000007261 -26.40060328899994602, 30.79453186300008838 -26.40058099599991692, 30.79452549400008365 -26.40055073999991464, 30.79454221400004599 -26.40048943399995096, 30.7945605270000442 -26.40043927199991458, 30.79460352100005593 -26.40043767899993554, 30.79460989100005008 -26.40042095899991637, 30.79461307600007558 -26.40039229699993939, 30.7946186490000855 -26.40035328199991227, 30.79463457300005302 -26.40033178599992425, 30.79462661100006926 -26.40030789999991612, 30.79463298100006341 -26.40026012799995669, 30.79467438400007495 -26.40022987299994384, 30.79468632600008959 -26.40020996799995601, 30.79469747300004201 -26.40017811999990727, 30.7947189700000763 -26.40014786399990498, 30.7947484290000375 -26.40011840499994378, 30.79475081800006819 -26.40009531499993045, 30.79477151900005083 -26.40007779899991647, 30.7947834620000549 -26.40007859499991127, 30.79480575600007342 -26.40004833899990899, 30.79483123400007116 -26.4000204719999374, 30.79484476900006484 -26.40001012199991237, 30.79485113900005899 -26.39999180899991416, 30.79485910200008902 -26.39997110799993152, 30.79487661700005674 -26.39996234999995295, 30.79488247200004025 -26.3999447989999112, 30.79489063100004387 -26.39992276899994295, 30.79489144700005454 -26.39990481799992494, 30.79491266200005839 -26.39989339399994606, 30.79493469400006234 -26.39989584199992123, 30.79495672200005174 -26.3998729959999423, 30.7949673300000768 -26.3998550449999243, 30.79497630600008051 -26.39982567099991684, 30.79498609700004863 -26.39978813699991633, 30.79499425700004167 -26.39977018599995517, 30.79499670500007369 -26.39973183699993342, 30.79500731200005248 -26.39968287999994345, 30.79502607900008115 -26.39960781199994244, 30.79504484500006356 -26.3995963899999424, 30.79504403000004231 -26.39957435899992788, 30.79502607900008115 -26.39954253699994524, 30.79503179000005275 -26.39950255599995899, 30.79504495200006886 -26.39949133799990477, 30.79507862800005569 -26.399446333999947, 30.79509384600004296 -26.39943111599990289, 30.79508775900006867 -26.39938241899994864, 30.79506188800007749 -26.39937481099991601, 30.79505580200003578 -26.39934741899992332, 30.79505580200003578 -26.39932154999991099, 30.7950679760000412 -26.39930176799992978, 30.79508623700007774 -26.39928198499995915, 30.79509232400005203 -26.39925459399995589, 30.79508928000007018 -26.39923480999993899, 30.79504819300007057 -26.39919828899991217, 30.79505275800005393 -26.39918307099992489, 30.79507406300007233 -26.39917089699991948, 30.79508928000007018 -26.39914807099995642, 30.7951060210000378 -26.3991328529999123, 30.79514558500005705 -26.39913437499990323, 30.79516689000007545 -26.39912372299994558, 30.79519732500006057 -26.39912980999991987, 30.7952338460000874 -26.39916785299993762, 30.79526428100007251 -26.39919067999994695, 30.79529319500005613 -26.39918611499990675, 30.7953099340000449 -26.39917241899991041, 30.79531450000007453 -26.39914959399993677, 30.79532058600005939 -26.39911611499991295, 30.79530384600008119 -26.39909480999995139, 30.79527493400007643 -26.39906437499990943, 30.79526580300006344 -26.39903393999992431, 30.79526580300006344 -26.39901111299991499, 30.79529623800004856 -26.39896850299993503, 30.79532363000004125 -26.39893350299990971, 30.79533276000006481 -26.39890154699992308, 30.79532515100004275 -26.39886654699995461, 30.79535863000006657 -26.39886502399991741, 30.79541036900008066 -26.39886350299991591, 30.79543167400004222 -26.39884828599991806, 30.79544689100004007 -26.39881785199992237, 30.79547732500003576 -26.39881328599994958, 30.79548797900008594 -26.39880111199994417, 30.79548797900008594 -26.39877067699995905, 30.79550928300005808 -26.39875850299995363, 30.79555037000005768 -26.39875850299995363, 30.79563254500004632 -26.39875850299995363, 30.79563711100007595 -26.3987295899999026, 30.7956538490000753 -26.39870371899991142, 30.79567819700008613 -26.39865958899991938, 30.79567819700008613 -26.39863523999991912, 30.79566602300008071 -26.39859111099991651, 30.79567667500003836 -26.39855611099994803, 30.79569950200004769 -26.39854393699994262, 30.79572385000005852 -26.39854241499995169, 30.79576341600005662 -26.39855915399994046, 30.79578776200008861 -26.39855611099994803, 30.79582885000007764 -26.39853937099991299, 30.79589409500005104 -26.39851673499993012, 30.79593746500006546 -26.39849162599995225, 30.79596828000006781 -26.39845167999993691, 30.79600708500004203 -26.39843456099993091, 30.79604703100005736 -26.39842542999991792, 30.79611322800008111 -26.39841287599995212, 30.7961280640000723 -26.39839803999990409, 30.79615887900007465 -26.39836722299992289, 30.79618969500006642 -26.39833640699993111, 30.79622393400006786 -26.3983409729999039, 30.79623991300007901 -26.39835923299995102, 30.79625132600006054 -26.39837407099992106, 30.79629469600007496 -26.39837407099992106, 30.79633007600006067 -26.39835923299995102, 30.79635746800005336 -26.3983466799999178, 30.79638371800007235 -26.39832956099991179, 30.79641453200008527 -26.39830331099994964, 30.79645219700006464 -26.39829303799990612, 30.79651382700006934 -26.39828847299992276, 30.79654121900006203 -26.39827363599994214, 30.79656290400004082 -26.39826222299990377, 30.79658002300004682 -26.39826222299990377, 30.79661442600007604 -26.39827229999991687, 30.79666469200003576 -26.39844534499991369, 30.79699057900006665 -26.39953509299994039, 30.79734218000004375 -26.40056336099991086, 30.79783545000003642 -26.40200594499992803, 30.79803318800009038 -26.40247925799991435, 30.79808109000003924 -26.40254457899993668, 30.7981442330000732 -26.40260227899995016, 30.79824874600006979 -26.40267848599995659, 30.79838047600003392 -26.40276557999993656, 30.79848281300007784 -26.40281130499994333, 30.79865155600003845 -26.40292779299994663, 30.79875607100007073 -26.40300508899991883, 30.79894036500007815 -26.40313298799992481)))</t>
+  </si>
+  <si>
+    <t>Fernie SP</t>
+  </si>
+  <si>
+    <t>Fernie</t>
   </si>
 </sst>
 </file>
@@ -487,8 +892,150 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -533,7 +1080,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -554,6 +1101,77 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -574,6 +1192,77 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -903,10 +1592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -2375,6 +3064,2121 @@
       </c>
       <c r="R29">
         <v>59101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" t="s">
+        <v>10</v>
+      </c>
+      <c r="L32" t="s">
+        <v>11</v>
+      </c>
+      <c r="M32" t="s">
+        <v>12</v>
+      </c>
+      <c r="N32" t="s">
+        <v>13</v>
+      </c>
+      <c r="O32" t="s">
+        <v>14</v>
+      </c>
+      <c r="P32" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>16</v>
+      </c>
+      <c r="R32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33">
+        <v>70008</v>
+      </c>
+      <c r="D33">
+        <v>8720085</v>
+      </c>
+      <c r="E33">
+        <v>872036002</v>
+      </c>
+      <c r="F33" t="s">
+        <v>142</v>
+      </c>
+      <c r="G33">
+        <v>872036</v>
+      </c>
+      <c r="H33" t="s">
+        <v>143</v>
+      </c>
+      <c r="I33" t="s">
+        <v>144</v>
+      </c>
+      <c r="J33">
+        <v>872</v>
+      </c>
+      <c r="K33" t="s">
+        <v>145</v>
+      </c>
+      <c r="L33" t="s">
+        <v>146</v>
+      </c>
+      <c r="M33">
+        <v>831</v>
+      </c>
+      <c r="N33" t="s">
+        <v>147</v>
+      </c>
+      <c r="O33" t="s">
+        <v>36</v>
+      </c>
+      <c r="P33">
+        <v>8</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>37</v>
+      </c>
+      <c r="R33">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34">
+        <v>72189</v>
+      </c>
+      <c r="D34">
+        <v>8720162</v>
+      </c>
+      <c r="E34">
+        <v>872046001</v>
+      </c>
+      <c r="F34" t="s">
+        <v>150</v>
+      </c>
+      <c r="G34">
+        <v>872046</v>
+      </c>
+      <c r="H34" t="s">
+        <v>151</v>
+      </c>
+      <c r="I34" t="s">
+        <v>144</v>
+      </c>
+      <c r="J34">
+        <v>872</v>
+      </c>
+      <c r="K34" t="s">
+        <v>145</v>
+      </c>
+      <c r="L34" t="s">
+        <v>146</v>
+      </c>
+      <c r="M34">
+        <v>831</v>
+      </c>
+      <c r="N34" t="s">
+        <v>147</v>
+      </c>
+      <c r="O34" t="s">
+        <v>36</v>
+      </c>
+      <c r="P34">
+        <v>8</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>37</v>
+      </c>
+      <c r="R34">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" t="s">
+        <v>152</v>
+      </c>
+      <c r="B35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35">
+        <v>71939</v>
+      </c>
+      <c r="D35">
+        <v>8720252</v>
+      </c>
+      <c r="E35">
+        <v>872022002</v>
+      </c>
+      <c r="F35" t="s">
+        <v>154</v>
+      </c>
+      <c r="G35">
+        <v>872022</v>
+      </c>
+      <c r="H35" t="s">
+        <v>155</v>
+      </c>
+      <c r="I35" t="s">
+        <v>144</v>
+      </c>
+      <c r="J35">
+        <v>872</v>
+      </c>
+      <c r="K35" t="s">
+        <v>145</v>
+      </c>
+      <c r="L35" t="s">
+        <v>146</v>
+      </c>
+      <c r="M35">
+        <v>831</v>
+      </c>
+      <c r="N35" t="s">
+        <v>147</v>
+      </c>
+      <c r="O35" t="s">
+        <v>36</v>
+      </c>
+      <c r="P35">
+        <v>8</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>37</v>
+      </c>
+      <c r="R35">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" t="s">
+        <v>156</v>
+      </c>
+      <c r="B36" t="s">
+        <v>157</v>
+      </c>
+      <c r="C36">
+        <v>83602</v>
+      </c>
+      <c r="D36">
+        <v>9840150</v>
+      </c>
+      <c r="E36">
+        <v>984062001</v>
+      </c>
+      <c r="F36" t="s">
+        <v>158</v>
+      </c>
+      <c r="G36">
+        <v>984062</v>
+      </c>
+      <c r="H36" t="s">
+        <v>159</v>
+      </c>
+      <c r="I36" t="s">
+        <v>160</v>
+      </c>
+      <c r="J36">
+        <v>984</v>
+      </c>
+      <c r="K36" t="s">
+        <v>161</v>
+      </c>
+      <c r="L36" t="s">
+        <v>162</v>
+      </c>
+      <c r="M36">
+        <v>947</v>
+      </c>
+      <c r="N36" t="s">
+        <v>163</v>
+      </c>
+      <c r="O36" t="s">
+        <v>26</v>
+      </c>
+      <c r="P36">
+        <v>9</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>27</v>
+      </c>
+      <c r="R36">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37">
+        <v>72068</v>
+      </c>
+      <c r="D37">
+        <v>8720421</v>
+      </c>
+      <c r="E37">
+        <v>872031001</v>
+      </c>
+      <c r="F37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G37">
+        <v>872031</v>
+      </c>
+      <c r="H37" t="s">
+        <v>167</v>
+      </c>
+      <c r="I37" t="s">
+        <v>144</v>
+      </c>
+      <c r="J37">
+        <v>872</v>
+      </c>
+      <c r="K37" t="s">
+        <v>145</v>
+      </c>
+      <c r="L37" t="s">
+        <v>146</v>
+      </c>
+      <c r="M37">
+        <v>831</v>
+      </c>
+      <c r="N37" t="s">
+        <v>147</v>
+      </c>
+      <c r="O37" t="s">
+        <v>36</v>
+      </c>
+      <c r="P37">
+        <v>8</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>37</v>
+      </c>
+      <c r="R37">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" t="s">
+        <v>186</v>
+      </c>
+      <c r="B38" t="s">
+        <v>187</v>
+      </c>
+      <c r="C38">
+        <v>83665</v>
+      </c>
+      <c r="D38">
+        <v>9840387</v>
+      </c>
+      <c r="E38">
+        <v>984073001</v>
+      </c>
+      <c r="F38" t="s">
+        <v>188</v>
+      </c>
+      <c r="G38">
+        <v>984073</v>
+      </c>
+      <c r="H38" t="s">
+        <v>189</v>
+      </c>
+      <c r="I38" t="s">
+        <v>160</v>
+      </c>
+      <c r="J38">
+        <v>984</v>
+      </c>
+      <c r="K38" t="s">
+        <v>161</v>
+      </c>
+      <c r="L38" t="s">
+        <v>162</v>
+      </c>
+      <c r="M38">
+        <v>947</v>
+      </c>
+      <c r="N38" t="s">
+        <v>163</v>
+      </c>
+      <c r="O38" t="s">
+        <v>26</v>
+      </c>
+      <c r="P38">
+        <v>9</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>27</v>
+      </c>
+      <c r="R38">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39" t="s">
+        <v>169</v>
+      </c>
+      <c r="C39">
+        <v>71913</v>
+      </c>
+      <c r="D39">
+        <v>8720147</v>
+      </c>
+      <c r="E39">
+        <v>872019001</v>
+      </c>
+      <c r="F39" t="s">
+        <v>170</v>
+      </c>
+      <c r="G39">
+        <v>872019</v>
+      </c>
+      <c r="H39" t="s">
+        <v>171</v>
+      </c>
+      <c r="I39" t="s">
+        <v>144</v>
+      </c>
+      <c r="J39">
+        <v>872</v>
+      </c>
+      <c r="K39" t="s">
+        <v>145</v>
+      </c>
+      <c r="L39" t="s">
+        <v>146</v>
+      </c>
+      <c r="M39">
+        <v>831</v>
+      </c>
+      <c r="N39" t="s">
+        <v>147</v>
+      </c>
+      <c r="O39" t="s">
+        <v>36</v>
+      </c>
+      <c r="P39">
+        <v>8</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>37</v>
+      </c>
+      <c r="R39">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" t="s">
+        <v>172</v>
+      </c>
+      <c r="B40" t="s">
+        <v>173</v>
+      </c>
+      <c r="C40">
+        <v>83182</v>
+      </c>
+      <c r="D40">
+        <v>9830174</v>
+      </c>
+      <c r="E40">
+        <v>983063001</v>
+      </c>
+      <c r="F40" t="s">
+        <v>174</v>
+      </c>
+      <c r="G40">
+        <v>983063</v>
+      </c>
+      <c r="H40" t="s">
+        <v>175</v>
+      </c>
+      <c r="I40" t="s">
+        <v>176</v>
+      </c>
+      <c r="J40">
+        <v>983</v>
+      </c>
+      <c r="K40" t="s">
+        <v>177</v>
+      </c>
+      <c r="L40" t="s">
+        <v>162</v>
+      </c>
+      <c r="M40">
+        <v>947</v>
+      </c>
+      <c r="N40" t="s">
+        <v>163</v>
+      </c>
+      <c r="O40" t="s">
+        <v>26</v>
+      </c>
+      <c r="P40">
+        <v>9</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>27</v>
+      </c>
+      <c r="R40">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41">
+        <v>72200</v>
+      </c>
+      <c r="D41">
+        <v>8720329</v>
+      </c>
+      <c r="E41">
+        <v>872049001</v>
+      </c>
+      <c r="F41" t="s">
+        <v>180</v>
+      </c>
+      <c r="G41">
+        <v>872049</v>
+      </c>
+      <c r="H41" t="s">
+        <v>181</v>
+      </c>
+      <c r="I41" t="s">
+        <v>144</v>
+      </c>
+      <c r="J41">
+        <v>872</v>
+      </c>
+      <c r="K41" t="s">
+        <v>145</v>
+      </c>
+      <c r="L41" t="s">
+        <v>146</v>
+      </c>
+      <c r="M41">
+        <v>831</v>
+      </c>
+      <c r="N41" t="s">
+        <v>147</v>
+      </c>
+      <c r="O41" t="s">
+        <v>36</v>
+      </c>
+      <c r="P41">
+        <v>8</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>37</v>
+      </c>
+      <c r="R41">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42" t="s">
+        <v>183</v>
+      </c>
+      <c r="C42">
+        <v>83544</v>
+      </c>
+      <c r="D42">
+        <v>9840271</v>
+      </c>
+      <c r="E42">
+        <v>984051001</v>
+      </c>
+      <c r="F42" t="s">
+        <v>184</v>
+      </c>
+      <c r="G42">
+        <v>984051</v>
+      </c>
+      <c r="H42" t="s">
+        <v>185</v>
+      </c>
+      <c r="I42" t="s">
+        <v>160</v>
+      </c>
+      <c r="J42">
+        <v>984</v>
+      </c>
+      <c r="K42" t="s">
+        <v>161</v>
+      </c>
+      <c r="L42" t="s">
+        <v>162</v>
+      </c>
+      <c r="M42">
+        <v>947</v>
+      </c>
+      <c r="N42" t="s">
+        <v>163</v>
+      </c>
+      <c r="O42" t="s">
+        <v>26</v>
+      </c>
+      <c r="P42">
+        <v>9</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>27</v>
+      </c>
+      <c r="R42">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43" t="s">
+        <v>226</v>
+      </c>
+      <c r="C43">
+        <v>71277</v>
+      </c>
+      <c r="D43">
+        <v>8710387</v>
+      </c>
+      <c r="E43">
+        <v>871006001</v>
+      </c>
+      <c r="F43" t="s">
+        <v>227</v>
+      </c>
+      <c r="G43">
+        <v>871006</v>
+      </c>
+      <c r="H43" t="s">
+        <v>228</v>
+      </c>
+      <c r="I43" t="s">
+        <v>229</v>
+      </c>
+      <c r="J43">
+        <v>871</v>
+      </c>
+      <c r="K43" t="s">
+        <v>230</v>
+      </c>
+      <c r="L43" t="s">
+        <v>146</v>
+      </c>
+      <c r="M43">
+        <v>831</v>
+      </c>
+      <c r="N43" t="s">
+        <v>147</v>
+      </c>
+      <c r="O43" t="s">
+        <v>36</v>
+      </c>
+      <c r="P43">
+        <v>8</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>37</v>
+      </c>
+      <c r="R43">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
+      <c r="A44" t="s">
+        <v>231</v>
+      </c>
+      <c r="C44">
+        <v>72147</v>
+      </c>
+      <c r="D44">
+        <v>8720386</v>
+      </c>
+      <c r="E44">
+        <v>872040001</v>
+      </c>
+      <c r="F44" t="s">
+        <v>232</v>
+      </c>
+      <c r="G44">
+        <v>872040</v>
+      </c>
+      <c r="H44" t="s">
+        <v>233</v>
+      </c>
+      <c r="I44" t="s">
+        <v>144</v>
+      </c>
+      <c r="J44">
+        <v>872</v>
+      </c>
+      <c r="K44" t="s">
+        <v>145</v>
+      </c>
+      <c r="L44" t="s">
+        <v>146</v>
+      </c>
+      <c r="M44">
+        <v>831</v>
+      </c>
+      <c r="N44" t="s">
+        <v>147</v>
+      </c>
+      <c r="O44" t="s">
+        <v>36</v>
+      </c>
+      <c r="P44">
+        <v>8</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>37</v>
+      </c>
+      <c r="R44">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" t="s">
+        <v>8</v>
+      </c>
+      <c r="I48" t="s">
+        <v>9</v>
+      </c>
+      <c r="J48" t="s">
+        <v>10</v>
+      </c>
+      <c r="K48" t="s">
+        <v>11</v>
+      </c>
+      <c r="L48" t="s">
+        <v>12</v>
+      </c>
+      <c r="M48" t="s">
+        <v>13</v>
+      </c>
+      <c r="N48" t="s">
+        <v>14</v>
+      </c>
+      <c r="O48" t="s">
+        <v>15</v>
+      </c>
+      <c r="P48" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
+      <c r="A49" t="s">
+        <v>190</v>
+      </c>
+      <c r="B49">
+        <v>71790</v>
+      </c>
+      <c r="C49">
+        <v>8720191</v>
+      </c>
+      <c r="D49">
+        <v>872002001</v>
+      </c>
+      <c r="E49" t="s">
+        <v>191</v>
+      </c>
+      <c r="F49">
+        <v>872002</v>
+      </c>
+      <c r="G49" t="s">
+        <v>192</v>
+      </c>
+      <c r="H49" t="s">
+        <v>144</v>
+      </c>
+      <c r="I49">
+        <v>872</v>
+      </c>
+      <c r="J49" t="s">
+        <v>145</v>
+      </c>
+      <c r="K49" t="s">
+        <v>146</v>
+      </c>
+      <c r="L49">
+        <v>831</v>
+      </c>
+      <c r="M49" t="s">
+        <v>147</v>
+      </c>
+      <c r="N49" t="s">
+        <v>36</v>
+      </c>
+      <c r="O49">
+        <v>8</v>
+      </c>
+      <c r="P49" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q49">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17">
+      <c r="A50" t="s">
+        <v>193</v>
+      </c>
+      <c r="B50">
+        <v>71822</v>
+      </c>
+      <c r="C50">
+        <v>8720201</v>
+      </c>
+      <c r="D50">
+        <v>872007001</v>
+      </c>
+      <c r="E50" t="s">
+        <v>194</v>
+      </c>
+      <c r="F50">
+        <v>872007</v>
+      </c>
+      <c r="G50" t="s">
+        <v>195</v>
+      </c>
+      <c r="H50" t="s">
+        <v>144</v>
+      </c>
+      <c r="I50">
+        <v>872</v>
+      </c>
+      <c r="J50" t="s">
+        <v>145</v>
+      </c>
+      <c r="K50" t="s">
+        <v>146</v>
+      </c>
+      <c r="L50">
+        <v>831</v>
+      </c>
+      <c r="M50" t="s">
+        <v>147</v>
+      </c>
+      <c r="N50" t="s">
+        <v>36</v>
+      </c>
+      <c r="O50">
+        <v>8</v>
+      </c>
+      <c r="P50" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q50">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
+      <c r="A51" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51">
+        <v>71849</v>
+      </c>
+      <c r="C51">
+        <v>8720368</v>
+      </c>
+      <c r="D51">
+        <v>872008001</v>
+      </c>
+      <c r="E51" t="s">
+        <v>197</v>
+      </c>
+      <c r="F51">
+        <v>872008</v>
+      </c>
+      <c r="G51" t="s">
+        <v>198</v>
+      </c>
+      <c r="H51" t="s">
+        <v>144</v>
+      </c>
+      <c r="I51">
+        <v>872</v>
+      </c>
+      <c r="J51" t="s">
+        <v>145</v>
+      </c>
+      <c r="K51" t="s">
+        <v>146</v>
+      </c>
+      <c r="L51">
+        <v>831</v>
+      </c>
+      <c r="M51" t="s">
+        <v>147</v>
+      </c>
+      <c r="N51" t="s">
+        <v>36</v>
+      </c>
+      <c r="O51">
+        <v>8</v>
+      </c>
+      <c r="P51" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q51">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17">
+      <c r="A52" t="s">
+        <v>199</v>
+      </c>
+      <c r="B52">
+        <v>71864</v>
+      </c>
+      <c r="C52">
+        <v>8720167</v>
+      </c>
+      <c r="D52">
+        <v>872011001</v>
+      </c>
+      <c r="E52" t="s">
+        <v>200</v>
+      </c>
+      <c r="F52">
+        <v>872011</v>
+      </c>
+      <c r="G52" t="s">
+        <v>201</v>
+      </c>
+      <c r="H52" t="s">
+        <v>144</v>
+      </c>
+      <c r="I52">
+        <v>872</v>
+      </c>
+      <c r="J52" t="s">
+        <v>145</v>
+      </c>
+      <c r="K52" t="s">
+        <v>146</v>
+      </c>
+      <c r="L52">
+        <v>831</v>
+      </c>
+      <c r="M52" t="s">
+        <v>147</v>
+      </c>
+      <c r="N52" t="s">
+        <v>36</v>
+      </c>
+      <c r="O52">
+        <v>8</v>
+      </c>
+      <c r="P52" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q52">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
+      <c r="A53" t="s">
+        <v>202</v>
+      </c>
+      <c r="B53">
+        <v>71881</v>
+      </c>
+      <c r="C53">
+        <v>8720008</v>
+      </c>
+      <c r="D53">
+        <v>872013001</v>
+      </c>
+      <c r="E53" t="s">
+        <v>203</v>
+      </c>
+      <c r="F53">
+        <v>872013</v>
+      </c>
+      <c r="G53" t="s">
+        <v>204</v>
+      </c>
+      <c r="H53" t="s">
+        <v>144</v>
+      </c>
+      <c r="I53">
+        <v>872</v>
+      </c>
+      <c r="J53" t="s">
+        <v>145</v>
+      </c>
+      <c r="K53" t="s">
+        <v>146</v>
+      </c>
+      <c r="L53">
+        <v>831</v>
+      </c>
+      <c r="M53" t="s">
+        <v>147</v>
+      </c>
+      <c r="N53" t="s">
+        <v>36</v>
+      </c>
+      <c r="O53">
+        <v>8</v>
+      </c>
+      <c r="P53" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q53">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
+      <c r="A54" t="s">
+        <v>205</v>
+      </c>
+      <c r="B54">
+        <v>83063</v>
+      </c>
+      <c r="C54">
+        <v>9830088</v>
+      </c>
+      <c r="D54">
+        <v>983035001</v>
+      </c>
+      <c r="E54" t="s">
+        <v>206</v>
+      </c>
+      <c r="F54">
+        <v>983035</v>
+      </c>
+      <c r="G54" t="s">
+        <v>207</v>
+      </c>
+      <c r="H54" t="s">
+        <v>176</v>
+      </c>
+      <c r="I54">
+        <v>983</v>
+      </c>
+      <c r="J54" t="s">
+        <v>177</v>
+      </c>
+      <c r="K54" t="s">
+        <v>162</v>
+      </c>
+      <c r="L54">
+        <v>947</v>
+      </c>
+      <c r="M54" t="s">
+        <v>163</v>
+      </c>
+      <c r="N54" t="s">
+        <v>26</v>
+      </c>
+      <c r="O54">
+        <v>9</v>
+      </c>
+      <c r="P54" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q54">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
+      <c r="A55" t="s">
+        <v>208</v>
+      </c>
+      <c r="B55">
+        <v>83094</v>
+      </c>
+      <c r="C55">
+        <v>9830171</v>
+      </c>
+      <c r="D55">
+        <v>983042001</v>
+      </c>
+      <c r="E55" t="s">
+        <v>209</v>
+      </c>
+      <c r="F55">
+        <v>983042</v>
+      </c>
+      <c r="G55" t="s">
+        <v>210</v>
+      </c>
+      <c r="H55" t="s">
+        <v>176</v>
+      </c>
+      <c r="I55">
+        <v>983</v>
+      </c>
+      <c r="J55" t="s">
+        <v>177</v>
+      </c>
+      <c r="K55" t="s">
+        <v>162</v>
+      </c>
+      <c r="L55">
+        <v>947</v>
+      </c>
+      <c r="M55" t="s">
+        <v>163</v>
+      </c>
+      <c r="N55" t="s">
+        <v>26</v>
+      </c>
+      <c r="O55">
+        <v>9</v>
+      </c>
+      <c r="P55" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q55">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17">
+      <c r="A56" t="s">
+        <v>211</v>
+      </c>
+      <c r="B56">
+        <v>83098</v>
+      </c>
+      <c r="C56">
+        <v>9830094</v>
+      </c>
+      <c r="D56">
+        <v>983043001</v>
+      </c>
+      <c r="E56" t="s">
+        <v>212</v>
+      </c>
+      <c r="F56">
+        <v>983043</v>
+      </c>
+      <c r="G56" t="s">
+        <v>213</v>
+      </c>
+      <c r="H56" t="s">
+        <v>176</v>
+      </c>
+      <c r="I56">
+        <v>983</v>
+      </c>
+      <c r="J56" t="s">
+        <v>177</v>
+      </c>
+      <c r="K56" t="s">
+        <v>162</v>
+      </c>
+      <c r="L56">
+        <v>947</v>
+      </c>
+      <c r="M56" t="s">
+        <v>163</v>
+      </c>
+      <c r="N56" t="s">
+        <v>26</v>
+      </c>
+      <c r="O56">
+        <v>9</v>
+      </c>
+      <c r="P56" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q56">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
+      <c r="A57" t="s">
+        <v>214</v>
+      </c>
+      <c r="B57">
+        <v>83115</v>
+      </c>
+      <c r="C57">
+        <v>9830073</v>
+      </c>
+      <c r="D57">
+        <v>983048001</v>
+      </c>
+      <c r="E57" t="s">
+        <v>215</v>
+      </c>
+      <c r="F57">
+        <v>983048</v>
+      </c>
+      <c r="G57" t="s">
+        <v>216</v>
+      </c>
+      <c r="H57" t="s">
+        <v>176</v>
+      </c>
+      <c r="I57">
+        <v>983</v>
+      </c>
+      <c r="J57" t="s">
+        <v>177</v>
+      </c>
+      <c r="K57" t="s">
+        <v>162</v>
+      </c>
+      <c r="L57">
+        <v>947</v>
+      </c>
+      <c r="M57" t="s">
+        <v>163</v>
+      </c>
+      <c r="N57" t="s">
+        <v>26</v>
+      </c>
+      <c r="O57">
+        <v>9</v>
+      </c>
+      <c r="P57" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q57">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
+      <c r="A58" t="s">
+        <v>217</v>
+      </c>
+      <c r="B58">
+        <v>83122</v>
+      </c>
+      <c r="C58">
+        <v>9830191</v>
+      </c>
+      <c r="D58">
+        <v>983051001</v>
+      </c>
+      <c r="E58" t="s">
+        <v>218</v>
+      </c>
+      <c r="F58">
+        <v>983051</v>
+      </c>
+      <c r="G58" t="s">
+        <v>219</v>
+      </c>
+      <c r="H58" t="s">
+        <v>176</v>
+      </c>
+      <c r="I58">
+        <v>983</v>
+      </c>
+      <c r="J58" t="s">
+        <v>177</v>
+      </c>
+      <c r="K58" t="s">
+        <v>162</v>
+      </c>
+      <c r="L58">
+        <v>947</v>
+      </c>
+      <c r="M58" t="s">
+        <v>163</v>
+      </c>
+      <c r="N58" t="s">
+        <v>26</v>
+      </c>
+      <c r="O58">
+        <v>9</v>
+      </c>
+      <c r="P58" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q58">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17">
+      <c r="A59" t="s">
+        <v>220</v>
+      </c>
+      <c r="B59">
+        <v>83172</v>
+      </c>
+      <c r="C59">
+        <v>9830151</v>
+      </c>
+      <c r="D59">
+        <v>983061001</v>
+      </c>
+      <c r="E59" t="s">
+        <v>221</v>
+      </c>
+      <c r="F59">
+        <v>983061</v>
+      </c>
+      <c r="G59" t="s">
+        <v>222</v>
+      </c>
+      <c r="H59" t="s">
+        <v>176</v>
+      </c>
+      <c r="I59">
+        <v>983</v>
+      </c>
+      <c r="J59" t="s">
+        <v>177</v>
+      </c>
+      <c r="K59" t="s">
+        <v>162</v>
+      </c>
+      <c r="L59">
+        <v>947</v>
+      </c>
+      <c r="M59" t="s">
+        <v>163</v>
+      </c>
+      <c r="N59" t="s">
+        <v>26</v>
+      </c>
+      <c r="O59">
+        <v>9</v>
+      </c>
+      <c r="P59" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q59">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17">
+      <c r="A60" t="s">
+        <v>223</v>
+      </c>
+      <c r="B60">
+        <v>83175</v>
+      </c>
+      <c r="C60">
+        <v>9830124</v>
+      </c>
+      <c r="D60">
+        <v>983062001</v>
+      </c>
+      <c r="E60" t="s">
+        <v>224</v>
+      </c>
+      <c r="F60">
+        <v>983062</v>
+      </c>
+      <c r="G60" t="s">
+        <v>225</v>
+      </c>
+      <c r="H60" t="s">
+        <v>176</v>
+      </c>
+      <c r="I60">
+        <v>983</v>
+      </c>
+      <c r="J60" t="s">
+        <v>177</v>
+      </c>
+      <c r="K60" t="s">
+        <v>162</v>
+      </c>
+      <c r="L60">
+        <v>947</v>
+      </c>
+      <c r="M60" t="s">
+        <v>163</v>
+      </c>
+      <c r="N60" t="s">
+        <v>26</v>
+      </c>
+      <c r="O60">
+        <v>9</v>
+      </c>
+      <c r="P60" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q60">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63" t="s">
+        <v>6</v>
+      </c>
+      <c r="G63" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" t="s">
+        <v>8</v>
+      </c>
+      <c r="I63" t="s">
+        <v>9</v>
+      </c>
+      <c r="J63" t="s">
+        <v>10</v>
+      </c>
+      <c r="K63" t="s">
+        <v>11</v>
+      </c>
+      <c r="L63" t="s">
+        <v>12</v>
+      </c>
+      <c r="M63" t="s">
+        <v>13</v>
+      </c>
+      <c r="N63" t="s">
+        <v>14</v>
+      </c>
+      <c r="O63" t="s">
+        <v>15</v>
+      </c>
+      <c r="P63" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="A64" t="s">
+        <v>234</v>
+      </c>
+      <c r="B64">
+        <v>68334</v>
+      </c>
+      <c r="C64">
+        <v>8600069</v>
+      </c>
+      <c r="D64">
+        <v>860008001</v>
+      </c>
+      <c r="E64" t="s">
+        <v>235</v>
+      </c>
+      <c r="F64">
+        <v>860008</v>
+      </c>
+      <c r="G64" t="s">
+        <v>236</v>
+      </c>
+      <c r="H64" t="s">
+        <v>237</v>
+      </c>
+      <c r="I64">
+        <v>860</v>
+      </c>
+      <c r="J64" t="s">
+        <v>238</v>
+      </c>
+      <c r="K64" t="s">
+        <v>239</v>
+      </c>
+      <c r="L64">
+        <v>830</v>
+      </c>
+      <c r="M64" t="s">
+        <v>240</v>
+      </c>
+      <c r="N64" t="s">
+        <v>36</v>
+      </c>
+      <c r="O64">
+        <v>8</v>
+      </c>
+      <c r="P64" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q64">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
+      <c r="A65" t="s">
+        <v>241</v>
+      </c>
+      <c r="B65">
+        <v>68356</v>
+      </c>
+      <c r="C65">
+        <v>8600025</v>
+      </c>
+      <c r="D65">
+        <v>860009002</v>
+      </c>
+      <c r="E65" t="s">
+        <v>242</v>
+      </c>
+      <c r="F65">
+        <v>860009</v>
+      </c>
+      <c r="G65" t="s">
+        <v>243</v>
+      </c>
+      <c r="H65" t="s">
+        <v>237</v>
+      </c>
+      <c r="I65">
+        <v>860</v>
+      </c>
+      <c r="J65" t="s">
+        <v>238</v>
+      </c>
+      <c r="K65" t="s">
+        <v>239</v>
+      </c>
+      <c r="L65">
+        <v>830</v>
+      </c>
+      <c r="M65" t="s">
+        <v>240</v>
+      </c>
+      <c r="N65" t="s">
+        <v>36</v>
+      </c>
+      <c r="O65">
+        <v>8</v>
+      </c>
+      <c r="P65" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q65">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
+      <c r="A66" t="s">
+        <v>244</v>
+      </c>
+      <c r="B66">
+        <v>68407</v>
+      </c>
+      <c r="C66">
+        <v>8600045</v>
+      </c>
+      <c r="D66">
+        <v>860012001</v>
+      </c>
+      <c r="E66" t="s">
+        <v>245</v>
+      </c>
+      <c r="F66">
+        <v>860012</v>
+      </c>
+      <c r="G66" t="s">
+        <v>246</v>
+      </c>
+      <c r="H66" t="s">
+        <v>237</v>
+      </c>
+      <c r="I66">
+        <v>860</v>
+      </c>
+      <c r="J66" t="s">
+        <v>238</v>
+      </c>
+      <c r="K66" t="s">
+        <v>239</v>
+      </c>
+      <c r="L66">
+        <v>830</v>
+      </c>
+      <c r="M66" t="s">
+        <v>240</v>
+      </c>
+      <c r="N66" t="s">
+        <v>36</v>
+      </c>
+      <c r="O66">
+        <v>8</v>
+      </c>
+      <c r="P66" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q66">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
+      <c r="A67" t="s">
+        <v>247</v>
+      </c>
+      <c r="B67">
+        <v>68481</v>
+      </c>
+      <c r="C67">
+        <v>8600137</v>
+      </c>
+      <c r="D67">
+        <v>860021001</v>
+      </c>
+      <c r="E67" t="s">
+        <v>248</v>
+      </c>
+      <c r="F67">
+        <v>860021</v>
+      </c>
+      <c r="G67" t="s">
+        <v>249</v>
+      </c>
+      <c r="H67" t="s">
+        <v>237</v>
+      </c>
+      <c r="I67">
+        <v>860</v>
+      </c>
+      <c r="J67" t="s">
+        <v>238</v>
+      </c>
+      <c r="K67" t="s">
+        <v>239</v>
+      </c>
+      <c r="L67">
+        <v>830</v>
+      </c>
+      <c r="M67" t="s">
+        <v>240</v>
+      </c>
+      <c r="N67" t="s">
+        <v>36</v>
+      </c>
+      <c r="O67">
+        <v>8</v>
+      </c>
+      <c r="P67" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q67">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17">
+      <c r="A68" t="s">
+        <v>250</v>
+      </c>
+      <c r="B68">
+        <v>68482</v>
+      </c>
+      <c r="C68">
+        <v>8600180</v>
+      </c>
+      <c r="D68">
+        <v>860022001</v>
+      </c>
+      <c r="E68" t="s">
+        <v>251</v>
+      </c>
+      <c r="F68">
+        <v>860022</v>
+      </c>
+      <c r="G68" t="s">
+        <v>252</v>
+      </c>
+      <c r="H68" t="s">
+        <v>237</v>
+      </c>
+      <c r="I68">
+        <v>860</v>
+      </c>
+      <c r="J68" t="s">
+        <v>238</v>
+      </c>
+      <c r="K68" t="s">
+        <v>239</v>
+      </c>
+      <c r="L68">
+        <v>830</v>
+      </c>
+      <c r="M68" t="s">
+        <v>240</v>
+      </c>
+      <c r="N68" t="s">
+        <v>36</v>
+      </c>
+      <c r="O68">
+        <v>8</v>
+      </c>
+      <c r="P68" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q68">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17">
+      <c r="A69" t="s">
+        <v>253</v>
+      </c>
+      <c r="B69">
+        <v>68492</v>
+      </c>
+      <c r="C69">
+        <v>8600013</v>
+      </c>
+      <c r="D69">
+        <v>860026001</v>
+      </c>
+      <c r="E69" t="s">
+        <v>254</v>
+      </c>
+      <c r="F69">
+        <v>860026</v>
+      </c>
+      <c r="G69" t="s">
+        <v>255</v>
+      </c>
+      <c r="H69" t="s">
+        <v>237</v>
+      </c>
+      <c r="I69">
+        <v>860</v>
+      </c>
+      <c r="J69" t="s">
+        <v>238</v>
+      </c>
+      <c r="K69" t="s">
+        <v>239</v>
+      </c>
+      <c r="L69">
+        <v>830</v>
+      </c>
+      <c r="M69" t="s">
+        <v>240</v>
+      </c>
+      <c r="N69" t="s">
+        <v>36</v>
+      </c>
+      <c r="O69">
+        <v>8</v>
+      </c>
+      <c r="P69" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q69">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17">
+      <c r="A70" t="s">
+        <v>256</v>
+      </c>
+      <c r="B70">
+        <v>68506</v>
+      </c>
+      <c r="C70">
+        <v>8600303</v>
+      </c>
+      <c r="D70">
+        <v>860031001</v>
+      </c>
+      <c r="E70" t="s">
+        <v>257</v>
+      </c>
+      <c r="F70">
+        <v>860031</v>
+      </c>
+      <c r="G70" t="s">
+        <v>258</v>
+      </c>
+      <c r="H70" t="s">
+        <v>237</v>
+      </c>
+      <c r="I70">
+        <v>860</v>
+      </c>
+      <c r="J70" t="s">
+        <v>238</v>
+      </c>
+      <c r="K70" t="s">
+        <v>239</v>
+      </c>
+      <c r="L70">
+        <v>830</v>
+      </c>
+      <c r="M70" t="s">
+        <v>240</v>
+      </c>
+      <c r="N70" t="s">
+        <v>36</v>
+      </c>
+      <c r="O70">
+        <v>8</v>
+      </c>
+      <c r="P70" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q70">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17">
+      <c r="A71" t="s">
+        <v>259</v>
+      </c>
+      <c r="B71">
+        <v>68518</v>
+      </c>
+      <c r="C71">
+        <v>8600067</v>
+      </c>
+      <c r="D71">
+        <v>860035001</v>
+      </c>
+      <c r="E71" t="s">
+        <v>260</v>
+      </c>
+      <c r="F71">
+        <v>860035</v>
+      </c>
+      <c r="G71" t="s">
+        <v>261</v>
+      </c>
+      <c r="H71" t="s">
+        <v>237</v>
+      </c>
+      <c r="I71">
+        <v>860</v>
+      </c>
+      <c r="J71" t="s">
+        <v>238</v>
+      </c>
+      <c r="K71" t="s">
+        <v>239</v>
+      </c>
+      <c r="L71">
+        <v>830</v>
+      </c>
+      <c r="M71" t="s">
+        <v>240</v>
+      </c>
+      <c r="N71" t="s">
+        <v>36</v>
+      </c>
+      <c r="O71">
+        <v>8</v>
+      </c>
+      <c r="P71" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q71">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17">
+      <c r="A72" t="s">
+        <v>262</v>
+      </c>
+      <c r="B72">
+        <v>68550</v>
+      </c>
+      <c r="C72">
+        <v>8600220</v>
+      </c>
+      <c r="D72">
+        <v>860038001</v>
+      </c>
+      <c r="E72" t="s">
+        <v>263</v>
+      </c>
+      <c r="F72">
+        <v>860038</v>
+      </c>
+      <c r="G72" t="s">
+        <v>264</v>
+      </c>
+      <c r="H72" t="s">
+        <v>237</v>
+      </c>
+      <c r="I72">
+        <v>860</v>
+      </c>
+      <c r="J72" t="s">
+        <v>238</v>
+      </c>
+      <c r="K72" t="s">
+        <v>239</v>
+      </c>
+      <c r="L72">
+        <v>830</v>
+      </c>
+      <c r="M72" t="s">
+        <v>240</v>
+      </c>
+      <c r="N72" t="s">
+        <v>36</v>
+      </c>
+      <c r="O72">
+        <v>8</v>
+      </c>
+      <c r="P72" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q72">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17">
+      <c r="A73" t="s">
+        <v>265</v>
+      </c>
+      <c r="B73">
+        <v>68553</v>
+      </c>
+      <c r="C73">
+        <v>8600231</v>
+      </c>
+      <c r="D73">
+        <v>860039001</v>
+      </c>
+      <c r="E73" t="s">
+        <v>266</v>
+      </c>
+      <c r="F73">
+        <v>860039</v>
+      </c>
+      <c r="G73" t="s">
+        <v>267</v>
+      </c>
+      <c r="H73" t="s">
+        <v>237</v>
+      </c>
+      <c r="I73">
+        <v>860</v>
+      </c>
+      <c r="J73" t="s">
+        <v>238</v>
+      </c>
+      <c r="K73" t="s">
+        <v>239</v>
+      </c>
+      <c r="L73">
+        <v>830</v>
+      </c>
+      <c r="M73" t="s">
+        <v>240</v>
+      </c>
+      <c r="N73" t="s">
+        <v>36</v>
+      </c>
+      <c r="O73">
+        <v>8</v>
+      </c>
+      <c r="P73" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q73">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17">
+      <c r="A74" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17">
+      <c r="A75" t="s">
+        <v>269</v>
+      </c>
+      <c r="B75">
+        <v>68557</v>
+      </c>
+      <c r="C75">
+        <v>8600079</v>
+      </c>
+      <c r="D75">
+        <v>860041001</v>
+      </c>
+      <c r="E75" t="s">
+        <v>270</v>
+      </c>
+      <c r="F75">
+        <v>860041</v>
+      </c>
+      <c r="G75" t="s">
+        <v>271</v>
+      </c>
+      <c r="H75" t="s">
+        <v>237</v>
+      </c>
+      <c r="I75">
+        <v>860</v>
+      </c>
+      <c r="J75" t="s">
+        <v>238</v>
+      </c>
+      <c r="K75" t="s">
+        <v>239</v>
+      </c>
+      <c r="L75">
+        <v>830</v>
+      </c>
+      <c r="M75" t="s">
+        <v>240</v>
+      </c>
+      <c r="N75" t="s">
+        <v>36</v>
+      </c>
+      <c r="O75">
+        <v>8</v>
+      </c>
+      <c r="P75" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q75">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17">
+      <c r="A76" t="s">
+        <v>272</v>
+      </c>
+      <c r="B76">
+        <v>68611</v>
+      </c>
+      <c r="C76">
+        <v>8600211</v>
+      </c>
+      <c r="D76">
+        <v>860050001</v>
+      </c>
+      <c r="E76" t="s">
+        <v>273</v>
+      </c>
+      <c r="F76">
+        <v>860050</v>
+      </c>
+      <c r="G76" t="s">
+        <v>274</v>
+      </c>
+      <c r="H76" t="s">
+        <v>237</v>
+      </c>
+      <c r="I76">
+        <v>860</v>
+      </c>
+      <c r="J76" t="s">
+        <v>238</v>
+      </c>
+      <c r="K76" t="s">
+        <v>239</v>
+      </c>
+      <c r="L76">
+        <v>830</v>
+      </c>
+      <c r="M76" t="s">
+        <v>240</v>
+      </c>
+      <c r="N76" t="s">
+        <v>36</v>
+      </c>
+      <c r="O76">
+        <v>8</v>
+      </c>
+      <c r="P76" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q76">
+        <v>59104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added in new map graphics, map files, rewrite Excel sampled_villages
</commit_message>
<xml_diff>
--- a/sampling/hea_selected_villages.xlsx
+++ b/sampling/hea_selected_villages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="-1260" windowWidth="24720" windowHeight="15180" tabRatio="500"/>
+    <workbookView xWindow="360" yWindow="0" windowWidth="24720" windowHeight="17040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="275">
   <si>
     <t>wkt_geom</t>
   </si>
@@ -439,6 +439,411 @@
   </si>
   <si>
     <t>Buyisonto</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.4907964320000815 -25.15075875199994471, 28.4897451270000488 -25.15089239299993551, 28.48823289800003522 -25.15108462399990685, 28.48670032100005756 -25.15142532099991968, 28.48676020900006733 -25.15084141799991713, 28.48687998300004764 -25.15016768599992147, 28.48699976000006018 -25.14925440399991885, 28.48707461500004001 -25.14864055799995768, 28.48713824700007535 -25.14842159399995936, 28.48725053600009005 -25.14716395799990778, 28.48725287200005596 -25.14714579299993602, 28.4873515970000426 -25.14637793699995427, 28.48744142700007842 -25.1455694569999082, 28.48750880100004679 -25.14494063799992318, 28.48760986000008089 -25.14446902599991063, 28.48765477500006682 -25.1440423289999444, 28.48769969200003516 -25.14332367999992357, 28.48760986000008089 -25.14322261799992475, 28.48772215000008146 -25.14291943999996093, 28.48800209800004168 -25.14285950899994759, 28.48836573000005146 -25.14284652199996017, 28.48859949200004849 -25.14285950899994759, 28.48884624100008978 -25.14279457499992532, 28.48920987300004981 -25.14276860099994337, 28.48956051800007927 -25.14278158799993079, 28.48972934600004692 -25.14279457499992532, 28.49001505600006112 -25.14272964099990304, 28.49021239500007141 -25.14270390099994756, 28.49043575300003894 -25.14382362299994256, 28.49066288000005542 -25.14529020899993483, 28.49079266600006122 -25.14601701199995887, 28.49099383500004024 -25.14734083299993017, 28.49109117600005092 -25.14798976399992725, 28.49066936900004521 -25.14804167799991674, 28.49068234700007451 -25.14841156999995064, 28.49071479400004137 -25.14963805099995753, 28.4907964320000815 -25.15075875199994471)))</t>
+  </si>
+  <si>
+    <t>demog_sas.49096</t>
+  </si>
+  <si>
+    <t>Phaphamang</t>
+  </si>
+  <si>
+    <t>Phake</t>
+  </si>
+  <si>
+    <t>MP316</t>
+  </si>
+  <si>
+    <t>Dr JS Moroka</t>
+  </si>
+  <si>
+    <t>DC31</t>
+  </si>
+  <si>
+    <t>Nkangala</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.96872778700003437 -25.19659764199991514, 28.96856567300005736 -25.2003533939999329, 28.96853268900008516 -25.20130988899995828, 28.96586858300008771 -25.20125330599995905, 28.96330493000004935 -25.20126177499992082, 28.96331370100006097 -25.2002808289999507, 28.96340245200007857 -25.19684911499990676, 28.96342217500006555 -25.19641521999994893, 28.96342181400007121 -25.19640081999995118, 28.96335034300005518 -25.19640135999992481, 28.96334766700005048 -25.19635528799994972, 28.96337971200006223 -25.19613453399995606, 28.96346624000005576 -25.19504432899992707, 28.96349463700005344 -25.19504543699991927, 28.96742689100005563 -25.19519326499994349, 28.96798864300006926 -25.19541500999989836, 28.96798864300006926 -25.19597676099994032, 28.968772135000048 -25.19603589099995133, 28.96872778700003437 -25.19659764199991514)))</t>
+  </si>
+  <si>
+    <t>demog_sas.51255</t>
+  </si>
+  <si>
+    <t>Pieterskraal B</t>
+  </si>
+  <si>
+    <t>Pieterskraal</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.76231299900007699 -25.11305114999993293, 28.76224775000008549 -25.1130664619999493, 28.76159308300004014 -25.11328004299992145, 28.76143102700007148 -25.11333291299990833, 28.76035944000005529 -25.11362832199995765, 28.75937473900006225 -25.11387739399992824, 28.75900982100006331 -25.11401061799995205, 28.75881288000005043 -25.11412646499991652, 28.75848271500007058 -25.1142365199999027, 28.75825681300005954 -25.11423072799993506, 28.75768916300006239 -25.11414384299990843, 28.75664483600008126 -25.11398859299992736, 28.75664490600007994 -25.11398821699992823, 28.75673867400007921 -25.11348659499992664, 28.75717577100004974 -25.11082030199991877, 28.75732875500006003 -25.11040505899995878, 28.75761001300008957 -25.10794201299995976, 28.75968908200007945 -25.1076731989999189, 28.75977650100008987 -25.10784803799992915, 28.7598639210000897 -25.10832884499990314, 28.75992948500004331 -25.10843811899991707, 28.7603447280000637 -25.10843811899991707, 28.76047585700007758 -25.10902820099994415, 28.76120367100008934 -25.1088841539999521, 28.76134069500005452 -25.10930808299992023, 28.76158104700004969 -25.11022769199990989, 28.7616849340000762 -25.11059959399995023, 28.76186934700007214 -25.11139625899994243, 28.76231299900007699 -25.11305114999993293)))</t>
+  </si>
+  <si>
+    <t>demog_sas.51005</t>
+  </si>
+  <si>
+    <t>Loding SP</t>
+  </si>
+  <si>
+    <t>Loding</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.12677272800004857 -25.24929171499991654, 29.12662827000008292 -25.24986793199991908, 29.12610481000007212 -25.25173231399992346, 29.12569394200005135 -25.25164336399990361, 29.12308680500007085 -25.25107282699991984, 29.12275459400007094 -25.2522355659999107, 29.12133290600008095 -25.25196162699996094, 29.12129995100008273 -25.24915369099994678, 29.12128938600005768 -25.24809264999993275, 29.121288679000088 -25.24802159999995865, 29.12670920800007934 -25.24927583499993133, 29.12677272800004857 -25.24929171499991654)))</t>
+  </si>
+  <si>
+    <t>demog_sas.60340</t>
+  </si>
+  <si>
+    <t>Phukukane SP</t>
+  </si>
+  <si>
+    <t>Phukukane</t>
+  </si>
+  <si>
+    <t>LIM472</t>
+  </si>
+  <si>
+    <t>Elias Motsoaledi</t>
+  </si>
+  <si>
+    <t>DC47</t>
+  </si>
+  <si>
+    <t>Greater Sekhukhune</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.91806747200007521 -25.12076359899992894, 28.91808162500007029 -25.12081454999989916, 28.91772697000004655 -25.12112283699991977, 28.91728336900007434 -25.1214723409999614, 28.91704006000009031 -25.12163454599993528, 28.9170359140000528 -25.1216373099999295, 28.91688009500006729 -25.12174118899991981, 28.91661124800004146 -25.12191594099994063, 28.91644769000004089 -25.12203139299992927, 28.91638272500006224 -25.12207725099995059, 28.91601977800008072 -25.1222923319999154, 28.91580469800004494 -25.12241331299992453, 28.91515061800004105 -25.12274785199992166, 28.91317865400003484 -25.12001743999991632, 28.91379718400008869 -25.11965924399993355, 28.91305655500007887 -25.11859772599990492, 28.91258487800007515 -25.11796567999994068, 28.91233960700003536 -25.11764376199994331, 28.9135146940000709 -25.11701236599992626, 28.91499196800004157 -25.11618656099994951, 28.91447813400003497 -25.11545251199993345, 28.91605633900007888 -25.1145808289999195, 28.91735927600007017 -25.11392018599991971, 28.91802909500006535 -25.113543985999911, 28.91841447100006235 -25.11312190599994665, 28.91856128100004852 -25.11291086699992547, 28.9188181980000536 -25.11286498899994513, 28.91960730100003829 -25.11283746299994846, 28.9201094820000435 -25.11277380599995013, 28.92009038500004081 -25.11283203199991476, 28.91984749400006294 -25.11354100599993089, 28.91949957300005281 -25.11440096399991617, 28.91924355300005445 -25.11509024399992995, 28.91920416600004273 -25.11512963099994522, 28.919112263000045 -25.11528061599994999, 28.91907943800003977 -25.11539877899992135, 28.91902692300004674 -25.1155891499999484, 28.91901379400007954 -25.11574670199991033, 28.91901379400007954 -25.11578608799993617, 28.91875121100008528 -25.11657383699991897, 28.91836390300005633 -25.11774233199992068, 28.91829825400003529 -25.11782766999990102, 28.91825230300008798 -25.11798521999992317, 28.91821291600007626 -25.1181427699999027, 28.91819978800004165 -25.11824780299992099, 28.91751050800008116 -25.1200727529999277, 28.91771400900006483 -25.12033533599992907, 28.91784530000006725 -25.12045349899995017, 28.91797659200005555 -25.12062417699991101, 28.91804880200004391 -25.12069638699995622, 28.91806747200007521 -25.12076359899992894)))</t>
+  </si>
+  <si>
+    <t>demog_sas.51128</t>
+  </si>
+  <si>
+    <t>Allemansdrift C</t>
+  </si>
+  <si>
+    <t>Allemansdrift</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.54302568500008874 -25.10442044199993106, 28.54294102100004693 -25.10452049999992141, 28.54235606100008127 -25.10525939599995127, 28.54247151200008048 -25.1053286679999168, 28.54205588500008162 -25.10566732699993153, 28.54165564900006302 -25.1059982909999313, 28.54115535600004705 -25.10637543499990443, 28.54087057400005278 -25.10656015899991189, 28.54052421800008688 -25.10676027699992119, 28.54023943500004634 -25.10687572899990982, 28.53995465200006265 -25.10698348399995439, 28.53965447600006655 -25.10706814899992878, 28.53943896500004485 -25.10712202799993165, 28.53912339500004691 -25.10717590499990237, 28.53882321900004726 -25.10720669199992017, 28.53848455900003955 -25.10722978299992292, 28.53804584000004851 -25.10722978299992292, 28.53763536300004944 -25.10717953699991867, 28.53728709400008157 -25.10710068499992076, 28.53680740400005433 -25.10699554699993996, 28.53645256300006849 -25.10690355099995941, 28.53534204600003932 -25.10669327599993039, 28.53457979700004898 -25.10652242699995895, 28.53374526600003946 -25.10634500899993427, 28.53310786900004814 -25.10623329799994963, 28.53263475000005656 -25.1061478739999302, 28.53199078100004726 -25.10607559199991101, 28.53137309700008473 -25.10602959399994916, 28.53081455200004157 -25.105990166999959, 28.53016401200005703 -25.10594416999990131, 28.52917268200008039 -25.10587844599990248, 28.52916973800006417 -25.10576367299995937, 28.52915037400003939 -25.10513431199990464, 28.52979910000004793 -25.10520208999992064, 28.52977973500008702 -25.10391431899995496, 28.52970227700006944 -25.10321718099993049, 28.53022512900008678 -25.10330432299992154, 28.53051560300008305 -25.10317845099990564, 28.53062211100007062 -25.10293638899992175, 28.53080607800006874 -25.10174544399990282, 28.53112560100003847 -25.10174544399990282, 28.53109655300005087 -25.1011741779999511, 28.53318796900003917 -25.1011257649999493, 28.53305241500004286 -25.10052544999990687, 28.53308146100004805 -25.10051576899991232, 28.53304273200006946 -25.09988640699992857, 28.53306845500003774 -25.09955974099995046, 28.53314458100004458 -25.09959803799995726, 28.53348721400004706 -25.09983909799990442, 28.53384436600003937 -25.10007166299993742, 28.53391092500004333 -25.10011416399993323, 28.53418906100006325 -25.10029176899990944, 28.53443408400005055 -25.10044542699995773, 28.53489601000006815 -25.10073213899994471, 28.53537286400006678 -25.10016135999995868, 28.53600190200006281 -25.09946862099991449, 28.53648761500005193 -25.0989112449999574, 28.53664683300008065 -25.09870850999993763, 28.54115392100004911 -25.10178217799995082, 28.54109539600005974 -25.10185742599992409, 28.54097392100004527 -25.10195388999994748, 28.54259466300004533 -25.10326591899990945, 28.54254848100003983 -25.1033351899999353, 28.54246670300005562 -25.10351919199990789, 28.5422502290000466 -25.10402573999990139, 28.54302568500008874 -25.10442044199993106)))</t>
+  </si>
+  <si>
+    <t>demog_sas.50977</t>
+  </si>
+  <si>
+    <t>Mmamethlake SP</t>
+  </si>
+  <si>
+    <t>Mmamethlake</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.10432595100008157 -25.04480215299992096, 29.10471700400006512 -25.04543385299990277, 29.10492757000008623 -25.04594522899992626, 29.10522837900003879 -25.04624603799993565, 29.10573975500005517 -25.04666716999992104, 29.10625113200006808 -25.04702814199992744, 29.10679258800007929 -25.04732895099994039, 29.10715355800005 -25.04759967899991935, 29.10769501500004708 -25.04793056899995918, 29.10823647200004416 -25.04838178299991114, 29.10883809000006295 -25.04892323999990822, 29.10841695700008813 -25.04913380699991876, 29.10805598800004645 -25.04943461499993518, 29.10772509600008107 -25.04991591099991766, 29.10766493400006993 -25.05051753099991174, 29.10754461100004065 -25.05105898599992997, 29.10736412400007112 -25.05169068499992946, 29.10718364000007696 -25.0518711709999593, 29.10709339700008513 -25.05214189899993116, 29.10688283000007459 -25.05262319499991008, 29.1065820210000652 -25.05304432699995232, 29.10634137300008106 -25.05349554099990428, 29.105829998000047 -25.05439796899991833, 29.10558117900006891 -25.05481341999990264, 29.10533145500005148 -25.05514676299992516, 29.10258087800008298 -25.05374645899991037, 29.10058736700005966 -25.05225089399993976, 29.09937169400006951 -25.05080789899994897, 29.09962866500006839 -25.0504520919999436, 29.09919379200004741 -25.04973059399992508, 29.0993222750000804 -25.04947362399991917, 29.09836357500006443 -25.04877189499995893, 29.0985711290000495 -25.04839631999993443, 29.09842619300007982 -25.04825138399991147, 29.09870124400003988 -25.04790130399993586, 29.0989671770000804 -25.0475595099999282, 29.09923044300006723 -25.04723548999993099, 29.09911347300004536 -25.04705167999992454, 29.09917365800004063 -25.0467818379999585, 29.0994456230000651 -25.04644080399992845, 29.09957081200008133 -25.04625949599994783, 29.09969622600004868 -25.04579764299996114, 29.1001215030000786 -25.04557487799991122, 29.10060753500004793 -25.04567613499995105, 29.10089105500008699 -25.04561538099994777, 29.10157960100008268 -25.04523060499991516, 29.10175083400008944 -25.04508098799993476, 29.1020098470000903 -25.04499033399991959, 29.10226886000004143 -25.04500760099995205, 29.10279120200004854 -25.04504645299994081, 29.10310608300005697 -25.04517239399990558, 29.10334147000008898 -25.04525085599993517, 29.1033739930000479 -25.04519510299991225, 29.10345934200006468 -25.04510513499991475, 29.10352098100008789 -25.0449783689999208, 29.10357913000007102 -25.0447969419999481, 29.10358654200007678 -25.04476050399995657, 29.10359657500004005 -25.04464575299994067, 29.10361983500007454 -25.04455852799992499, 29.10363495400008915 -25.04445851099995934, 29.10364363600007209 -25.04440550199990412, 29.10367100700005594 -25.04430266799994342, 29.10368728900004953 -25.04423405299991146, 29.10367682300005754 -25.0441793919999327, 29.10364309400006277 -25.04408751499994423, 29.10362681300006571 -25.04401773599994385, 29.10360833400005731 -25.04380559699990272, 29.10357071700007836 -25.04364454299991749, 29.1035642330000428 -25.04356999299994868, 29.10358172100006868 -25.04334267099994804, 29.10390481900003934 -25.04380948199991508, 29.10432595100008157 -25.04480215299992096)))</t>
+  </si>
+  <si>
+    <t>demog_sas.62471</t>
+  </si>
+  <si>
+    <t>Matlala Ramoshebo SP</t>
+  </si>
+  <si>
+    <t>Matlala Ramoshebo</t>
+  </si>
+  <si>
+    <t>LIM471</t>
+  </si>
+  <si>
+    <t>Ephraim Mogale</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.82293753200008268 -25.27798374999991893, 28.8233697670000879 -25.27811120399991651, 28.82375180100007128 -25.27822958299992706, 28.82422391200003986 -25.27839364399994793, 28.82353269500003989 -25.2803762289999554, 28.82330956300006264 -25.28094800699994948, 28.82302915900004336 -25.28174045299994077, 28.82384405200008359 -25.28198637199994891, 28.82382748800006311 -25.28206919399992003, 28.82363975800006983 -25.2826544709999439, 28.82351828500003776 -25.28297471699994503, 28.82348515600006067 -25.28311827599992512, 28.82339681200005188 -25.2833060059999184, 28.82330294700005524 -25.28357655899992906, 28.82307660900005075 -25.28411738999994895, 28.82285203700007514 -25.2849230489999286, 28.82274990600006959 -25.28526657999992722, 28.82274062100004031 -25.28542441999991652, 28.82270348300005125 -25.28562867999994523, 28.82266598900008958 -25.28567148399991993, 28.82248344200008106 -25.28577144999991688, 28.82196622700007538 -25.28563236699994832, 28.82157070800008114 -25.28551066899990474, 28.82158809300005586 -25.28545851299992364, 28.82120561400006409 -25.28534550799992076, 28.82080575000009048 -25.2852368509999188, 28.82035373000007894 -25.28510211199994728, 28.82034068800004434 -25.28505864899995004, 28.82030157300004802 -25.28501083699995888, 28.82026680200004876 -25.28494998799993709, 28.82043196300008958 -25.28446754399993424, 28.81962354100005186 -25.2842241469999216, 28.81910632600005329 -25.28406333299994913, 28.81859345600008737 -25.28391990399995848, 28.81846741100008913 -25.28385905399994726, 28.8188107730000489 -25.28288981699995475, 28.81860214800007824 -25.28287242999994078, 28.81828486500006292 -25.28277681299994128, 28.81798931200006564 -25.28271596299993007, 28.81796092000007548 -25.28270260499994038, 28.8177769760000615 -25.28263600499991526, 28.8179831200000649 -25.28209051799990448, 28.81837637800003904 -25.28112640099993769, 28.81850957600005358 -25.2807965719999288, 28.81885526400003528 -25.27990222799991216, 28.81916289300005118 -25.27907448399992063, 28.81940709400004152 -25.27847508299993251, 28.81966715100008969 -25.27778370799995855, 28.81983523700006344 -25.27738727999991752, 28.82025069600007683 -25.27636290799995678, 28.82120420000006789 -25.27721605599992927, 28.82161420200003477 -25.27754849099994772, 28.8216640690000645 -25.27758173299991995, 28.82182474500007174 -25.27764267899993555, 28.82244965800003911 -25.27782602399992129, 28.82274021900008165 -25.27792556799994372, 28.82293753200008268 -25.27798374999991893)))</t>
+  </si>
+  <si>
+    <t>demog_sas.51268</t>
+  </si>
+  <si>
+    <t>Kameelpoort SP</t>
+  </si>
+  <si>
+    <t>Kameelpoort</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.15858167100003939 -25.19794360599991023, 29.15849683700008654 -25.19801475699995663, 29.15832966600004283 -25.19820978999990757, 29.1582553670000415 -25.19828408799992303, 29.1582553670000415 -25.19867415299995983, 29.15839467700004661 -25.19994650799992542, 29.15852469800006475 -25.20097739499993494, 29.15864813100006359 -25.20176735999990569, 29.1583622530000639 -25.20198322799990365, 29.15781869400007054 -25.20227803999995686, 29.15770813800008909 -25.20170684099991831, 29.15575501000006398 -25.20213984599990908, 29.15436958400004741 -25.20247135699991858, 29.15436164100004035 -25.20196140899992088, 29.15433279700004832 -25.20083069899993689, 29.15433856600003537 -25.20018457999992734, 29.15430972000007159 -25.20005189499994458, 29.15320063400008976 -25.19919698099994321, 29.1538627030000761 -25.19855650099992772, 29.15462450700004737 -25.19790134999993469, 29.15524918700004164 -25.19728428999991721, 29.15613288000008652 -25.19652248399995997, 29.15697751800007964 -25.19572079299990719, 29.15746283000004269 -25.19625434099992844, 29.15830177200007611 -25.19721034399992732, 29.15844809900005075 -25.19744446699991158, 29.15858167100003939 -25.19794360599991023)))</t>
+  </si>
+  <si>
+    <t>demog_sas.61945</t>
+  </si>
+  <si>
+    <t>Mpheleng SP</t>
+  </si>
+  <si>
+    <t>Mpheleng</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.26194776200008718 -25.32509195699992688, 29.26199131300006684 -25.32548501299993049, 29.26243375200004948 -25.32571508199992749, 29.26294698200007716 -25.3260336389999452, 29.26338942100005625 -25.3260336389999452, 29.26386725500004005 -25.32622831199995517, 29.26415041500007774 -25.32652916999996151, 29.26438048300008177 -25.32690081899994539, 29.26453976200008356 -25.32734325699993505, 29.26473483600005565 -25.32736985799994045, 29.26409309800004976 -25.32915665599995236, 29.26381325700004155 -25.3294098469999085, 29.2635200890000533 -25.32975631699991936, 29.26342680900006243 -25.33006280999995852, 29.26340015700003505 -25.33043593099995761, 29.26321359600007099 -25.33103559299991048, 29.26306701300006807 -25.3315019949999396, 29.2629204280000863 -25.33184846599993989, 29.2629470800000604 -25.3322882169999275, 29.2629470800000604 -25.33248810399993189, 29.26272054200006778 -25.33267466599994577, 29.26256063400006724 -25.33340758299993567, 29.26209423000005572 -25.33415382699990914, 29.26152122100006281 -25.33491339699992295, 29.26056176500008732 -25.33620599899996151, 29.2604609830000868 -25.3364609169999575, 29.26010868800005582 -25.33735201699994377, 29.25948237500006144 -25.33840475299990658, 29.25882941300005768 -25.33927092899995159, 29.2584562920000657 -25.34021706099991889, 29.25798988800005063 -25.34168289599995205, 29.2579075850000514 -25.34261174599992827, 29.25772730300008106 -25.34370376999993368, 29.25737476700004436 -25.34520508799994332, 29.25737872700005582 -25.34523296599991227, 29.25701027200005555 -25.34507665199992843, 29.25663015300006009 -25.34475501299993994, 29.25633775400007153 -25.34465267299992774, 29.25608360800003993 -25.34307014199992736, 29.25521911900005989 -25.34282314499995437, 29.25402904300005957 -25.34239651399991544, 29.25410763300004646 -25.34226178799992013, 29.2545965170000386 -25.34146854699991991, 29.25505779800005257 -25.34098420299994814, 29.25548448200004259 -25.34036147499995195, 29.25579584700005498 -25.33961189199993669, 29.2561187430000551 -25.33823958299990409, 29.25503473300005552 -25.33802047199992913, 29.25474643300004018 -25.33799740799992151, 29.25348944300003495 -25.33780136499990476, 29.25308582200005958 -25.33766298099993719, 29.25297050200003923 -25.33714404099992734, 29.25164003100007903 -25.33699676099990938, 29.25172207400004254 -25.33605782499995485, 29.25190439200008541 -25.33541971299990792, 29.25196132700006046 -25.33521673299992472, 29.25199006300004712 -25.33511428199994953, 29.25229545200005177 -25.33383165499992629, 29.25255441200004825 -25.3327620339999271, 29.25257640700004913 -25.33267118199995949, 29.25320474200004028 -25.33055064599994921, 29.25356204700005591 -25.32947186499990266, 29.25372008500005094 -25.32870915899991715, 29.2539330930000574 -25.32725933199992951, 29.25436598000004906 -25.32598128399990856, 29.25474389600003988 -25.32488188799993623, 29.25493430100004844 -25.32386058599990974, 29.25515916000006555 -25.32388200199994799, 29.25538401900007912 -25.32392483199992839, 29.25570524700004071 -25.32404261499993581, 29.25618708700005755 -25.32409615399990344, 29.25655114500005993 -25.32417110599993748, 29.25675458900008152 -25.32425676599990538, 29.25688308000007964 -25.32437454999995907, 29.25706510900004886 -25.32455657999992127, 29.25728996800006243 -25.32459940899991935, 29.25762190200003943 -25.32446020999992697, 29.25784676100005299 -25.32419251999990095, 29.25805020500007458 -25.32396766199991944, 29.25830718800006025 -25.32383916999992834, 29.25869266000006519 -25.32387129299991102, 29.25892822800005533 -25.32395695399992519, 29.25924945400004162 -25.32408544599991629, 29.25955997400006936 -25.32425676599990538, 29.2598490780000553 -25.32436384199991153, 29.26003110700008847 -25.32435313499991025, 29.26044870200007963 -25.32450303999991092, 29.26074851400005628 -25.32455657999992127, 29.26106974100008529 -25.32464223899996014, 29.26111257100006924 -25.32473860699991519, 29.26110186400006796 -25.32496346599992876, 29.26124106300005678 -25.32509195699992688, 29.2614980440000636 -25.32498488199991016, 29.26194776200008718 -25.32509195699992688)))</t>
+  </si>
+  <si>
+    <t>demog_sas.57452</t>
+  </si>
+  <si>
+    <t>Thabakhubedu SP</t>
+  </si>
+  <si>
+    <t>Thabakhubedu</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.86861646900007372 -24.95652935799995475, 28.86859281300007751 -24.9565361169999278, 28.8679349350000507 -24.95674490499993681, 28.86725736000005327 -24.95697732899992616, 28.86680827000003546 -24.95713096599990877, 28.86641039100004491 -24.95727278299995078, 28.86603986700004043 -24.95742909799992049, 28.865654030000087 -24.95759187299995574, 28.86482281900003954 -24.95790308499994126, 28.86414846600007422 -24.9581140539999069, 28.86413135000003649 -24.9581181289999563, 28.86374342500005241 -24.9582615689999443, 28.86320766800008641 -24.95839550799991002, 28.86292403300006981 -24.95846641699995416, 28.86215979100006734 -24.95858065999993869, 28.86102918700004238 -24.95871065899990526, 28.8602727840000739 -24.95881290599993463, 28.85973864300007108 -24.95893160499991836, 28.8589706400000523 -24.95917934699991747, 28.85753373000005695 -24.95967483299995138, 28.85706400800006577 -24.95984752599991907, 28.85584908000004134 -24.96029418899991015, 28.85462756200007561 -24.96068507599994746, 28.85461036600008811 -24.96069057899995869, 28.85460149000005003 -24.96069271399994705, 28.85408339800005706 -24.96084448199991357, 28.85316196800005173 -24.96109908799991217, 28.85280733800004782 -24.9611960819999581, 28.85219507100003966 -24.96137794199995597, 28.85197380600004635 -24.96147493499995562, 28.85164342500007706 -24.96166588999994929, 28.85133729100004985 -24.96191746499994224, 28.85122301000006928 -24.96203138399994259, 28.85117072900004587 -24.96153143799995178, 28.85106608400008099 -24.96043848099992601, 28.85091493000004448 -24.9594617959999141, 28.85087423500004888 -24.95916530299990654, 28.85082772700008036 -24.95901996299994607, 28.85075796300003503 -24.95887462299992876, 28.85041496100006952 -24.95828744899995399, 28.85001382300004025 -24.95775841199991874, 28.84954873500004169 -24.95729913699994995, 28.84955353800006606 -24.957168607999904, 28.84964466200005972 -24.95675587199991696, 28.84978938700004392 -24.95621984999991128, 28.84990195200003882 -24.95558198399993444, 28.84993947300006312 -24.95522820899992666, 28.85003059700005679 -24.95432233299993641, 28.85009491900007106 -24.95406504199991105, 28.8501270810000392 -24.95392567699991559, 28.8501860420000753 -24.95331461199992873, 28.85024500600007968 -24.95282683199991425, 28.85028788800008215 -24.95228544999991982, 28.85034685100004026 -24.95197455799990394, 28.85041117300005453 -24.95173334799994791, 28.85051837600008184 -24.95148677899993572, 28.85067382300007921 -24.95124556799993343, 28.85074350600007165 -24.95113836399991669, 28.8507649480000623 -24.951074040999913, 28.8507649480000623 -24.95095075599994061, 28.8507649480000623 -24.95069346599990467, 28.85078638800007411 -24.95044153599991432, 28.85082926900008715 -24.95017352499991148, 28.85096863500007203 -24.94967502399993009, 28.85104903800004195 -24.94930516999994552, 28.85104903800004195 -24.94919260499995062, 28.85100615700008575 -24.9490532389999089, 28.85087751100007836 -24.94889243299991222, 28.85079373000007763 -24.94870172199995295, 28.85116687700008242 -24.94862704699994538, 28.85194720900005905 -24.9485515309999073, 28.85253455800005895 -24.94848440599992045, 28.85282823100004634 -24.94841727999994418, 28.85347431300004928 -24.94826624799992487, 28.85447280400006775 -24.94804809099991871, 28.85481682100004264 -24.9479138399999556, 28.85512727500008623 -24.94778797999993003, 28.85532865200008246 -24.94776280799993629, 28.85560554400007049 -24.94764533799991568, 28.8558656560000486 -24.94756143199992948, 28.8563187520000497 -24.94748591599994825, 28.85681380200009016 -24.94740200899991578, 28.85725352100007512 -24.94731881999990719, 28.85743471200004251 -24.94728453899995202, 28.85765286900004867 -24.94720063399995524, 28.85811435700009042 -24.94708316299994522, 28.85882756300009078 -24.9469321309999259, 28.85925548800008755 -24.9468146609999053, 28.8599938680000605 -24.94654615999991165, 28.8604050110000685 -24.94635317399990981, 28.86095040500003961 -24.94611823499991488, 28.86149580000005699 -24.94583295199993245, 28.86184820700003684 -24.94567352999990817, 28.8622425700000349 -24.94546376299990698, 28.86251107100008539 -24.94533790299993825, 28.86276279100007969 -24.9451952609999239, 28.8629389950000359 -24.94512813599993706, 28.8632830110000782 -24.94503583699992078, 28.86386196900008372 -24.94486802499994837, 28.86431506600007424 -24.94473377399992842, 28.86451644200008104 -24.94468342999994093, 28.86456678600006853 -24.94480928999990965, 28.8646758650000379 -24.94506100999990394, 28.86486045900005593 -24.9454469809999182, 28.86499470900008646 -24.94574065599994128, 28.86510378900004525 -24.94604271899993364, 28.86517930500008333 -24.94639512799994918, 28.86527999300005831 -24.94674753499992903, 28.86536390000009078 -24.94699925699995902, 28.86554010400004699 -24.94725097699995331, 28.86562401100007946 -24.9473432739999339, 28.86570581100005484 -24.94754607299995541, 28.86578211500005864 -24.94794032299995479, 28.86594744800004264 -24.9485507739999548, 28.86606190600008404 -24.94897045899995192, 28.86630279500008101 -24.94886778799991589, 28.86679262100005872 -24.94873199499994598, 28.86737459200008971 -24.94860105099991188, 28.86748570800006064 -24.94857425299994702, 28.86764998300003526 -24.94896045899992032, 28.86788263300007884 -24.94961963599990895, 28.86803773300005105 -24.95004616199992142, 28.8679380260000471 -24.95019572299992205, 28.86777738600005705 -24.95046714799991605, 28.86772753300004979 -24.95056685499992, 28.8676776790000531 -24.95070533799992063, 28.86772199300008879 -24.95094352799992521, 28.86781062300008216 -24.95115402099992252, 28.8681872950000411 -24.95152515399990989, 28.86835333600004105 -24.95166483999992124, 28.86780348800004958 -24.9520333499999083, 28.86764919600005896 -24.95217661999993197, 28.86764919600005896 -24.95230886799993186, 28.86779246600008264 -24.95267255499993553, 28.86795777700007193 -24.95312440699990475, 28.86812309000004007 -24.95354319699993084, 28.86818921400004001 -24.95391790299993318, 28.86825596600004928 -24.95447133499993697, 28.86828737300004377 -24.95477285299995174, 28.86825596600004928 -24.95502411699993672, 28.86828109100008533 -24.95519372099994371, 28.86843185100008213 -24.95568368799990822, 28.86861646900007372 -24.95652935799995475)))</t>
+  </si>
+  <si>
+    <t>Lefiswane SP</t>
+  </si>
+  <si>
+    <t>Lefiswane</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.71032430100007105 -25.02230495799994969, 28.71043479000007892 -25.02240181999991364, 28.71061720900007685 -25.0224914829999534, 28.71077180100007809 -25.02258732999990798, 28.71095112800009019 -25.02272646199992323, 28.71124794400003566 -25.0229830859999538, 28.71151075100004846 -25.02320260599992707, 28.71191269000007651 -25.02354580099995474, 28.71207655800003522 -25.02366019899994853, 28.71194051800006264 -25.02385189299991453, 28.71152002600007336 -25.02449808799991615, 28.7113252400000647 -25.0247578019999537, 28.71127205000004778 -25.02486549999991894, 28.7114134480000871 -25.02506741099995224, 28.71022163600008525 -25.02565151699991475, 28.7099148330000844 -25.0257990189999191, 28.7097319320000679 -25.0259465189999446, 28.70946052900006862 -25.02617072099991447, 28.70907702500005598 -25.02630642299993724, 28.70854012000006605 -25.02650112499992474, 28.70797371500003692 -25.02679612799994402, 28.70776131300004863 -25.02690822899995737, 28.70756027500004848 -25.0270636849999164, 28.70700921900004232 -25.02657703899990338, 28.70664399700007152 -25.02621181499995373, 28.70618078700005071 -25.02571297499991942, 28.70589573500006964 -25.02543683099992222, 28.70566261100003658 -25.0251934069999038, 28.70522891800004572 -25.02503851699992765, 28.70473327000007657 -25.02494558299991922, 28.70395882000008214 -25.02448091199994451, 28.70337023600006887 -25.02423308799990309, 28.70321534500004645 -25.02479069299994308, 28.70309143300005417 -25.02541025399995078, 28.70290556600008358 -25.02602981399991222, 28.70302947800007587 -25.02649448399995435, 28.70271969800006673 -25.02664937499991993, 28.70225502700003517 -25.02708306599993193, 28.70191426800005274 -25.02754773799995291, 28.70138764200004289 -25.02791947399992978, 28.70123275100007731 -25.02819827799993391, 28.7009849270000359 -25.02850805699995362, 28.70086101400005418 -25.02878685999991148, 28.70089199300008431 -25.0290966389999312, 28.70102553000003809 -25.03045156899992207, 28.7004636110000888 -25.02978429099994173, 28.69991638900006592 -25.02914189899991015, 28.69929779100004907 -25.02828537799990727, 28.69901228300005869 -25.02757160999993857, 28.69856022900006565 -25.02638199699993038, 28.69801300800008903 -25.02535892899993542, 28.69777508500004615 -25.02464516399993499, 28.697735132000048 -25.02452529999993658, 28.69734682500006784 -25.02336037999992868, 28.69706507900008319 -25.02252257299994653, 28.69748919300008083 -25.02235800699992296, 28.69816359100008185 -25.0221041149999337, 28.69901253900007987 -25.02169947599992383, 28.69935370500007821 -25.02155666299995573, 28.69963933200006068 -25.02151699199993118, 28.70001223400004164 -25.02155666299995573, 28.7001074430000358 -25.02150905799993552, 28.70028604100008351 -25.02106164299993907, 28.70037154500005272 -25.02087204599990855, 28.70048307300004353 -25.02074192999992874, 28.70070984600005204 -25.02061924899993528, 28.70088244500004748 -25.02059689899994055, 28.70112899700006892 -25.02057034799992152, 28.70139451400007147 -25.02058551999994052, 28.70191417000006595 -25.02061586499991108, 28.70239210100004357 -25.02065758899993853, 28.70258175700007541 -25.02068414099994698, 28.70267658400007349 -25.02054000199990469, 28.70279417000006106 -25.02026310499991268, 28.70296486000006553 -25.01995586499992896, 28.70304451500004461 -25.01986103799993089, 28.703222791000087 -25.01970551999994541, 28.70322658400004912 -25.01956896899991989, 28.70321899800006804 -25.01930345099992792, 28.70324175700005753 -25.01921620799993207, 28.70337451500006409 -25.01904551899991702, 28.70346554900004321 -25.01893551899991053, 28.7035755510000854 -25.01874965699994391, 28.70379555100004154 -25.01840069199994332, 28.70381451500009007 -25.01824138099993888, 28.70380692900005215 -25.01813138099993239, 28.70387141200006909 -25.01810862299993232, 28.70431520500005718 -25.01811241599995128, 28.70480451500003483 -25.0180744849999428, 28.70485003300007065 -25.01802896699990697, 28.70486899800005176 -25.01789620799991098, 28.70489555100004964 -25.01775207199995066, 28.70492968800004974 -25.01771034699993379, 28.70506244800003515 -25.01764207199994416, 28.70527995700007295 -25.01752928299993073, 28.70529779500003542 -25.01755338599991774, 28.70553065400008563 -25.0178444589999458, 28.70588962800007948 -25.01830931599994301, 28.70626627400008601 -25.01879706099992973, 28.70661556200008135 -25.01924689899993837, 28.70719770600004495 -25.01999839599994857, 28.70788040400003638 -25.02090865799993935, 28.70824027500003695 -25.02140083599994114, 28.70946807300003911 -25.02295675199991365, 28.70960037800006148 -25.0228985379999358, 28.70983852800003433 -25.02268155599995225, 28.71032430100007105 -25.02230495799994969)))</t>
+  </si>
+  <si>
+    <t>Seabe SP</t>
+  </si>
+  <si>
+    <t>Seabe</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.78537674100005006 -25.00490883299994493, 28.78736398400008056 -25.0056503409999209, 28.78752140700004247 -25.0057685639999363, 28.78722448100006659 -25.00693226699991101, 28.78712670200008006 -25.0075189419999333, 28.78691908000007516 -25.00947652499991136, 28.7868922710000561 -25.00968028099993035, 28.78662247600004775 -25.01173070999993797, 28.7862957970000366 -25.01338293099991006, 28.7859291800000392 -25.01353568799993354, 28.78531814900009067 -25.01387175499991145, 28.78434050300006675 -25.0139023069999098, 28.78259906900007081 -25.01393285899990815, 28.78140756100003728 -25.01381065199990417, 28.77994109100006881 -25.01368844599994645, 28.77929951000004394 -25.0137189979999448, 28.77847462000005407 -25.013993960999926, 28.77725256100006845 -25.01442168099993069, 28.77624436300004618 -25.01484940299991422, 28.77523616500008075 -25.01515491699990434, 28.77465568600007373 -25.01539932899993346, 28.77401410500004886 -25.01549098299994967, 28.77315866500003949 -25.01576594699992029, 28.7723337740000602 -25.01573539599991136, 28.77117281900007129 -25.01570484299992359, 28.77059234100005369 -25.01588815199994542, 28.77013406900005066 -25.01604090899991206, 28.76878980300006106 -25.01646862999990617, 28.76828416000006428 -25.01688425399993321, 28.76827287700007219 -25.01680244899995387, 28.76818833700008327 -25.01618953899992448, 28.76799669200005383 -25.014225167999939, 28.76775713500006759 -25.01147025899990695, 28.76770922400004338 -25.01072763299993085, 28.76770922400004338 -25.01000895999993645, 28.76770922400004338 -25.00921842199994671, 28.76756549000003815 -25.00840392699990389, 28.76746966600006772 -25.00766129899994894, 28.76737384300008671 -25.00689471599991975, 28.76723010900008148 -25.00612813399993684, 28.76715824200005045 -25.00557715099995448, 28.76691868500006422 -25.00440331999993759, 28.76679890600007639 -25.00356487099992364, 28.76687077300005058 -25.0026785079999172, 28.76694264000008161 -25.00215148199993109, 28.76741311200004247 -25.0021619509999482, 28.77094942100006847 -25.00273072799990359, 28.77421370500007924 -25.0032624109999233, 28.77604368300006854 -25.0035344349999491, 28.77940688600006069 -25.00404138799990506, 28.78201584100008859 -25.00446178799995778, 28.78437750200004075 -25.00480799999991177, 28.78537674100005006 -25.00490883299994493)))</t>
+  </si>
+  <si>
+    <t>Marapyane SP</t>
+  </si>
+  <si>
+    <t>Marapyane</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.86548924600003829 -25.05253057699991359, 28.86415399300005902 -25.05222689199990782, 28.86201178300007086 -25.05175262099993461, 28.86222361100004719 -25.05095560399990973, 28.86284793300006868 -25.04860655199991015, 28.8632114900000829 -25.04729396199991243, 28.86355144200007317 -25.0459860969999113, 28.86369791100008797 -25.0454295119999415, 28.86701806300004591 -25.0461327949999486, 28.86715322000003425 -25.04620037399990906, 28.86717011500007857 -25.04631863599990993, 28.8664943290000906 -25.0486838889999035, 28.86635917100005599 -25.0493089919999079, 28.86591991000005919 -25.05086330099993575, 28.86571717400005355 -25.05167424599994774, 28.86570203200005835 -25.05173985499993705, 28.86561580600005072 -25.05211350599995512, 28.86548924600003829 -25.05253057699991359)))</t>
+  </si>
+  <si>
+    <t>Koedoespoort SP</t>
+  </si>
+  <si>
+    <t>Koedoespoort</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.77373281300003782 -25.05518785499992873, 28.77262985100009018 -25.05512468899991063, 28.7722897310000576 -25.05574176399994712, 28.77190050500007601 -25.05652878399990868, 28.77155276200005574 -25.0572894709999332, 28.77040086400006658 -25.05697794999991856, 28.77034290600005306 -25.05750680999994984, 28.77024872700008018 -25.05748507599992081, 28.7701545460000716 -25.05745609899992132, 28.770125566000047 -25.0575357899999176, 28.77002414300005739 -25.05760823599990772, 28.76996618500004388 -25.05765894799992566, 28.76984302600004639 -25.05774588399992808, 28.76971986700004891 -25.0578038419999416, 28.76953150800005687 -25.05782557499992436, 28.76937212400008548 -25.05789077799994402, 28.76924172200006069 -25.05794873499991127, 28.76913305200008608 -25.0579849569999169, 28.76909682700005533 -25.05809362699994836, 28.76902438200005463 -25.05820229599993354, 28.76894469100005836 -25.05831096599990815, 28.76882153100007145 -25.05836167799992609, 28.76870561800006953 -25.05844136999991179, 28.76858245800008262 -25.05851381499991248, 28.7685027690000652 -25.05870217699992963, 28.76843756600004554 -25.05885431399991603, 28.76843756600004554 -25.05904267499994376, 28.76856796800007032 -25.05926001299991412, 28.76861143600007154 -25.0594483759999207, 28.76865490500006217 -25.05958602299995164, 28.7687563310000769 -25.05976713699993752, 28.76879255200003627 -25.05994101099992122, 28.76883602100008375 -25.06007141399993543, 28.76903887100007751 -25.06019457299993292, 28.76911131700006763 -25.06022355299995752, 28.76925621100008357 -25.06050609299995813, 28.76937212400008548 -25.06066547499995067, 28.76945181500008175 -25.06075965599995925, 28.76765514400005941 -25.06178839499995092, 28.76697414900007743 -25.06218685099992172, 28.76683649900007822 -25.06228102999995144, 28.76420120200003794 -25.06377499999990732, 28.76405162700007168 -25.0625862629999574, 28.76392928300003859 -25.06255567599993128, 28.76338637200007042 -25.06234157099993354, 28.76310344800003804 -25.06222687299992913, 28.76287405000005037 -25.06220393299992111, 28.76269053000004305 -25.06211217299994587, 28.76248407100007398 -25.06208923299993785, 28.7613523730000793 -25.06195159399993599, 28.76109238600008666 -25.06172219599994833, 28.7609929820000616 -25.06153102999991233, 28.76086299000007784 -25.06140103799992858, 28.76084005000006982 -25.06091165499992712, 28.76082475500004421 -25.06059814499991489, 28.76076358400007393 -25.0592217529999175, 28.76006774200004656 -25.05903823399995645, 28.75813314800006992 -25.05843415199990432, 28.75831666700008782 -25.05779948199995033, 28.75866841200007684 -25.05693541499994126, 28.75893604200007303 -25.05693541499994126, 28.75907368200006431 -25.0569583559999387, 28.75922661300006666 -25.05695070899992061, 28.7594483650000825 -25.05690482899990457, 28.75967011800008777 -25.0569583559999387, 28.75989951700006486 -25.05705011499992452, 28.76012891500005253 -25.057118935999938, 28.76019008800005849 -25.05717245999994702, 28.76025890700003629 -25.05682071699993685, 28.76053418500004 -25.05688953599991464, 28.76056477200006611 -25.05643838599991113, 28.76072535200006541 -25.05641544599990311, 28.76096239500003549 -25.05642309199993178, 28.7609776900000611 -25.05631603999995605, 28.76107709400008616 -25.05628545299992993, 28.76108474100004742 -25.05606370199990351, 28.76122238000004927 -25.05603311499993424, 28.76142119300004651 -25.05603311499993424, 28.76235408000007965 -25.05624721999993199, 28.76263700400005519 -25.05609428799994021, 28.76274405600008777 -25.05601017599991565, 28.76285875600007103 -25.05588782999990372, 28.76296580800004676 -25.05577312999992046, 28.76259877100005724 -25.05562784399995735, 28.76263700400005519 -25.05555902499992271, 28.76286640300008912 -25.05487847699993154, 28.76319520600003443 -25.05492435699994758, 28.76332519900006446 -25.05479436399991755, 28.76338637200007042 -25.05435850699990397, 28.76328696700005594 -25.05430497999992667, 28.76276699600003894 -25.05421322099994086, 28.76288934200005087 -25.05381559699992522, 28.76285111000004235 -25.05364737199994352, 28.7629046350000408 -25.05341797399995585, 28.76307286300004762 -25.05266860399990492, 28.76267523600006371 -25.05259978499992712, 28.76269053000004305 -25.05238567999992938, 28.762728763000041 -25.05207216999991715, 28.76269817600007173 -25.05188864999990983, 28.76297345500006486 -25.0518962959999385, 28.76326402600005849 -25.05190394399994602, 28.76330226000004586 -25.05159807699993735, 28.76398280600005819 -25.04962525299993104, 28.76373811600007002 -25.04957172599995374, 28.7638986950000799 -25.04890647099995249, 28.76402104100003498 -25.04879941799993048, 28.76411280000007764 -25.0487153049999165, 28.76402868700006366 -25.04844002799995906, 28.76397516100007579 -25.04823356899993314, 28.76388340200008997 -25.04805769699993334, 28.76376105600007804 -25.0476983039999368, 28.76458689100007859 -25.0473389149999548, 28.76450277800006461 -25.04720892199992477, 28.76428867300006686 -25.04705598999993299, 28.76415103400006501 -25.04691835099993114, 28.76399045400006571 -25.04674247899993134, 28.76386046300007138 -25.0466965989999153, 28.76378399700007549 -25.04666601299993545, 28.76360047900004702 -25.04649778899994317, 28.76342460400007894 -25.04636779499992372, 28.76283581500007358 -25.04653602099995169, 28.76161235700004681 -25.04668895299994347, 28.76104650800004947 -25.04683423799991715, 28.76085534300005975 -25.04692599699990296, 28.76043477900003609 -25.04708657699995911, 28.7600295080000592 -25.04729303599992818, 28.75967776500004902 -25.04750714099992592, 28.75954777200007584 -25.04759125399993991, 28.75941013300007398 -25.04767536599990763, 28.75923426000008476 -25.04777477199991154, 28.75900486200004025 -25.0479506449999576, 28.75889781000006451 -25.04805004999991525, 28.75878311000008125 -25.04810357699994938, 28.75868370400007734 -25.04804240399994342, 28.75836254800003644 -25.04775183299994978, 28.75846960000006902 -25.04763713299990968, 28.75882134400006862 -25.04732362199990803, 28.75898956900005032 -25.04719362899993484, 28.7591272090000416 -25.04710951699991028, 28.75947895100006235 -25.04681894499992723, 28.75984599000008757 -25.04668130599992537, 28.75975423100004491 -25.04636014899995189, 28.75941778000003524 -25.0453125619999355, 28.75992245700007288 -25.04522080299994968, 28.75984599000008757 -25.04505257699992171, 28.75968541300005654 -25.04489199799991184, 28.75950953900007789 -25.04454789999994091, 28.75979246300005343 -25.04440261499991038, 28.76004480200003854 -25.04436438399994813, 28.76017479400007915 -25.04453260699995099, 28.76043477900003609 -25.04513669099992512, 28.76192586900003789 -25.04488435199994001, 28.76229290600008426 -25.04485376599990332, 28.76233878500005403 -25.04493787799992788, 28.7625528910000412 -25.0449608179999359, 28.76286640300008912 -25.04499140499990517, 28.76404397900006416 -25.04486141399991084, 28.76418926800005238 -25.04530491599990683, 28.76490804800005208 -25.04528197599995565, 28.76477805500007889 -25.04483082499990587, 28.7647321770000417 -25.04467024699994226, 28.76552742600006241 -25.04461671999990813, 28.76569564900006526 -25.04454025399991224, 28.76565741700005674 -25.04436438399994813, 28.76649089700003969 -25.04399734499992292, 28.76710255400007554 -25.04384576699993659, 28.76746450900003538 -25.04369064299993397, 28.76820293900004799 -25.04278208699992092, 28.77373281300003782 -25.05518785499992873)))</t>
+  </si>
+  <si>
+    <t>Ramantsho SP</t>
+  </si>
+  <si>
+    <t>Ramantsho</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.93193390900006534 -24.90181914599992297, 28.93067053800007216 -24.90209379199990281, 28.93019448400008287 -24.90075717899992469, 28.93019552400005523 -24.90072556199993414, 28.93032139000007419 -24.90070149999991145, 28.93051203900006385 -24.90067373499994119, 28.93067307300003677 -24.90065707599995903, 28.93096552500009011 -24.90061080299994956, 28.93123021200005951 -24.90056082599994625, 28.93127215900005922 -24.90055067699995561, 28.93120152000005874 -24.89991492999990896, 28.93098180300006561 -24.89923747099993534, 28.93078039600004558 -24.89872479899992186, 28.93050575000006575 -24.8981022669999561, 28.9325198210000849 -24.89762621299990997, 28.93376488400008384 -24.8972417089999567, 28.93453389300003664 -24.89705861099992035, 28.93403953000006368 -24.89585016799992445, 28.93440572500009011 -24.89570368999994798, 28.93494947600004252 -24.89553613999993331, 28.93496502600004305 -24.89581414299993867, 28.93566561600005116 -24.89995806599995376, 28.93530290200004629 -24.9000614089999317, 28.93484515900007636 -24.90018957599994565, 28.93469959600008679 -24.90021489299994073, 28.93449978900008546 -24.90028062099992212, 28.93402245200007883 -24.90040214099991545, 28.93352685700006077 -24.90057408199993461, 28.93359503300007418 -24.90073478099992599, 28.9337584630000606 -24.90118763499992838, 28.93281277700003784 -24.90154449799990743, 28.93193390900006534 -24.90181914599992297)))</t>
+  </si>
+  <si>
+    <t>Malebitsa SP</t>
+  </si>
+  <si>
+    <t>Malebitsa</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.00121006200004103 -24.93710336699990648, 28.99993528100003459 -24.93785426599993116, 28.9999605650000376 -24.93789219199993568, 29.00012099900004614 -24.93817260299994132, 29.00037471700005653 -24.93856414299995095, 29.00055012800004306 -24.93884605299990653, 29.0006253040000388 -24.93899013999993031, 29.00074363600003835 -24.93921845299990991, 29.00088842000008071 -24.93944676499995694, 29.00133300700008476 -24.94010345499992809, 29.00008442100005368 -24.94082542599994667, 28.99974327600006063 -24.9402462279999213, 28.99925731000007545 -24.93939925799992352, 28.99871580400008497 -24.93860782599995218, 28.99820206800006872 -24.93767754799995373, 28.99767444600007593 -24.93678892199994834, 28.99721625000006497 -24.93602525999995123, 28.99680116900003668 -24.93529619799994634, 28.99638777300003767 -24.9346623229999409, 28.9984134170000516 -24.93342213299990817, 28.9990970680000828 -24.93483320799992953, 28.99969080200008875 -24.93455380399990418, 29.00014483400008203 -24.93537455399990677, 29.0006337920000874 -24.93631754199992656, 29.00121006200004103 -24.93710336699990648)))</t>
+  </si>
+  <si>
+    <t>Uitvlugt SP</t>
+  </si>
+  <si>
+    <t>Uitvlugt</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.05217366900006937 -24.92307301799991137, 29.05189981100005525 -24.92297052699990445, 29.05135814800007665 -24.92292128499991577, 29.05108731700005364 -24.92287204199993766, 29.0506277250000835 -24.92287204199993766, 29.05057027600008723 -24.92292128499991577, 29.05006964800008973 -24.92283921399990732, 29.04968392000006361 -24.92273252299992237, 29.04901915200008489 -24.92260121199990408, 29.04807534700006499 -24.92240424399994936, 29.04782913700006475 -24.92291307699991876, 29.04767320400003427 -24.92315928799990843, 29.04749265000003788 -24.92325777199994263, 29.04732851000005667 -24.92333163499995408, 29.04709050700006401 -24.92338908399995034, 29.04638470500003677 -24.92352039599995805, 29.04616311500006987 -24.92355322399993156, 29.04569531600003529 -24.92355322399993156, 29.04517827400007945 -24.92353680999991639, 29.04487461500008294 -24.92341370499991626, 29.04450530000008257 -24.92329880699992373, 29.04400467300007449 -24.92320032299994637, 29.04364356400003544 -24.92303618299990831, 29.04330707800005484 -24.92301156099995296, 29.04311011000004328 -24.92300335399994538, 29.0429213490000393 -24.92305259599993406, 29.04175595500004192 -24.92387329699994325, 29.04161643600008347 -24.92377481299990905, 29.04150153600005524 -24.92358605199990507, 29.0414030530000673 -24.92343011999992086, 29.04120608500005574 -24.92312645999993492, 29.04120608500005574 -24.92301156099995296, 29.04118967000005114 -24.92274072999992995, 29.04105835900008969 -24.9225355549999108, 29.04086139200006755 -24.92260941899991167, 29.040467455000055 -24.92268328199992311, 29.03990117200004306 -24.92281459399993082, 29.03975344500008759 -24.92283921399990732, 29.03895736500004432 -24.92261762599991926, 29.03865370700003723 -24.92335625599991999, 29.03862908600007131 -24.92338908399995034, 29.03754576000005727 -24.92203492799990272, 29.03716003200008799 -24.92148505899990596, 29.0362408470000446 -24.92022938699994938, 29.03552199300008851 -24.91930375399994091, 29.0348884190000831 -24.91803660599993009, 29.03420415900006901 -24.91714960099994869, 29.03291166700006443 -24.91608519699991575, 29.03093756200007647 -24.91427673999993431, 29.03218298300004108 -24.91451624299992318, 29.03776685100007171 -24.91570007699993994, 29.04010714800006099 -24.91618592799994758, 29.0409419910000679 -24.9163501599999222, 29.04170156100008171 -24.91648017699992579, 29.04322754500003612 -24.91661703599993416, 29.0460742220000725 -24.91690444099992874, 29.04948886600004698 -24.91723290399994539, 29.04981048600006943 -24.91725343299992801, 29.05157597400005898 -24.91739713499993059, 29.0529582540000888 -24.91756820999995625, 29.05321828900008541 -24.91762979599991468, 29.05417938500005448 -24.91763966599995683, 29.05513293900008875 -24.9177985929999295, 29.05509320900006287 -24.91863295399991785, 29.05382180100008327 -24.92235447099994872, 29.05196766400007391 -24.92214257099993802, 29.05199850500008552 -24.92239381099994944, 29.05208199600008356 -24.92274741599993604, 29.05217366900006937 -24.92307301799991137)))</t>
+  </si>
+  <si>
+    <t>Rathoke SP</t>
+  </si>
+  <si>
+    <t>Rathoke</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.9671790450000799 -24.97541156099993032, 28.9672530730000517 -24.97526672599991571, 28.96761056400004009 -24.97462534299995696, 28.96756771400004027 -24.97461709399993879, 28.96615393800004767 -24.97419370599993727, 28.96590435300004174 -24.97475758199993834, 28.96514635300007967 -24.97450799799992183, 28.96563211100004764 -24.97323924099993064, 28.96694142800004101 -24.97110966899992945, 28.96694891400005645 -24.97108775799995328, 28.96796574100005728 -24.97145751199991537, 28.96872374100007619 -24.96984907499995643, 28.96896456400008901 -24.96937451199994484, 28.96935232500004531 -24.968610392999949, 28.96986074000005829 -24.96744566199993187, 28.97026747200004593 -24.96663219999993544, 28.97096076300005052 -24.96514393199993265, 28.97145069000004014 -24.96534729899991589, 28.97202381200008858 -24.96568932299993548, 28.9721809570000346 -24.96541200399991567, 28.97236583500006191 -24.96526410299992449, 28.97260617700004559 -24.96494056599993883, 28.97288349200005086 -24.96529183499990268, 28.97380788300006316 -24.96678934599992772, 28.97479285900004697 -24.96835969199992178, 28.97522969400006332 -24.96915145399992753, 28.97585764200005087 -24.97064396999991231, 28.97588661400004639 -24.97070958899990956, 28.9769224260000442 -24.97305565799990745, 28.97751397100006443 -24.97442986499993367, 28.9780782170000748 -24.97534903699994402, 28.9774490410000567 -24.9754763389999539, 28.97720737800005963 -24.97590596299994559, 28.97699256700008164 -24.97628188399994542, 28.97680460700007643 -24.97671150499991199, 28.97637498400007416 -24.97663095099994734, 28.97581110400005855 -24.97676520799990385, 28.97546203500007778 -24.97703372199993055, 28.97487130200005367 -24.97676520799990385, 28.97446853100007047 -24.97681891099995255, 28.97430742300008433 -24.97676520799990385, 28.97368984100006628 -24.9770068729999366, 28.97342132700003958 -24.9771679789999439, 28.97334077100003924 -24.97671150499991199, 28.97326021700007459 -24.97614762499995322, 28.97315281300006973 -24.97579855699990503, 28.97312595900007182 -24.97518097299990814, 28.97213245800008963 -24.97523467699994626, 28.97113895400008232 -24.97526152799991905, 28.97036026200004244 -24.97531522899993206, 28.96931305700007897 -24.97542263499991577, 28.96858806800008779 -24.97553004299993518, 28.9678899300000694 -24.97553004299993518, 28.9671790450000799 -24.97541156099993032)))</t>
+  </si>
+  <si>
+    <t>Doornlaagte SP</t>
+  </si>
+  <si>
+    <t>Doornlaagte</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.92104829300006941 -24.95122997599992232, 28.92105995200006419 -24.95128943699995716, 28.92122364100004006 -24.95212427699993896, 28.921264567000037 -24.9525065449999488, 28.9205595750000839 -24.95260144899992838, 28.92016640700006747 -24.95264212199992926, 28.91980035400007409 -24.95268279399994071, 28.91916314900004181 -24.95281836899994232, 28.91900045900007399 -24.95212693499991019, 28.91879709600004844 -24.95115079299995386, 28.91841748500007725 -24.95121858199991038, 28.91784807000004776 -24.95131348399991111, 28.91756336200006672 -24.95136771399995723, 28.9169261580000807 -24.95146261699994739, 28.91595001600006754 -24.95159819099990273, 28.91515012100006743 -24.9517337669999506, 28.91463493500003779 -24.95177443799991579, 28.91426754900004426 -24.95186597199995049, 28.91376760700006798 -24.94913933599991651, 28.91373883100004605 -24.94890712599993776, 28.9146891650000839 -24.94869687999994312, 28.91565175000005183 -24.94850707499995224, 28.91665500700008806 -24.94845284499990612, 28.91687192700004516 -24.948493517999907, 28.91702106000008143 -24.94850707499995224, 28.91772605100004512 -24.94838505699993902, 28.9188106540000831 -24.94823592499994902, 28.91927161000006663 -24.94820880899993654, 28.9204163960000642 -24.9480072049999535, 28.92104829300006941 -24.95122997599992232)))</t>
+  </si>
+  <si>
+    <t>Spitspunt SP</t>
+  </si>
+  <si>
+    <t>Spitspunt</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.06709276700007649 -24.97860764999995808, 29.06747347000003856 -24.97888587599993571, 29.06903475200005005 -24.98066822499993123, 29.07113373900006081 -24.98283853499992802, 29.07132582500008766 -24.98424455399992894, 29.06813942400003725 -24.98816491099995574, 29.06765371300008383 -24.98816390999991199, 29.06671772100008866 -24.98821761399995012, 29.06612299400006805 -24.98825173799991717, 29.066107655000053 -24.98825261799993314, 29.06628507200008471 -24.98611094699992918, 29.06544868000008819 -24.98619965499995033, 29.0648150490000603 -24.98627569099994616, 29.06457426900004748 -24.98627569099994616, 29.06371253100007834 -24.98638974499993992, 29.06361795800006576 -24.98642126999993707, 29.06356046100006552 -24.9864404349999063, 29.06344886200008659 -24.98638342199990348, 29.06239458000004561 -24.98584482199993317, 29.06154236700007232 -24.98542350099995701, 29.0587072070000545 -24.98402184199994736, 29.05815953500007254 -24.98374939499990433, 29.0571173300000396 -24.98323542999992242, 29.05566110000006574 -24.98250731599995333, 29.05501310100004275 -24.98219494599993595, 29.0563419960000715 -24.98030462999992096, 29.05663123800007952 -24.98046188799992251, 29.05739494500005549 -24.98087710699991248, 29.05822299100003647 -24.97979349099995261, 29.05875457600006939 -24.98004905999994207, 29.05960148800005527 -24.97866686499992284, 29.06205709100004242 -24.97868114299990339, 29.06228552000004584 -24.97868828099990424, 29.06295652700003984 -24.97865972699992199, 29.06337769300006357 -24.97872397199995476, 29.06403442300006645 -24.97880963299991208, 29.06493200000005572 -24.97876601899992011, 29.0670342410000444 -24.97856487699993977, 29.06709276700007649 -24.97860764999995808)))</t>
+  </si>
+  <si>
+    <t>Matlerekeng SP</t>
+  </si>
+  <si>
+    <t>Matlerekeng</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.94841527200009068 -24.97867287799994074, 28.95002420700006951 -24.97877511799993044, 28.95005111200003967 -24.97854373399991346, 28.95082060200007845 -24.97852758999994194, 28.95087441300006503 -24.97901188499992031, 28.95198290900003713 -24.97894193099995164, 28.95259096900008444 -24.97899574199993822, 28.95312369300006594 -24.97901188499992031, 28.95285464000005504 -24.97981904199991732, 28.95280083000005789 -24.97994818799992345, 28.95269859000006818 -24.98049167399994985, 28.95294611800005669 -24.98057777099995747, 28.9527282870000704 -24.98117751299992051, 28.95505011000005879 -24.98186922399992227, 28.95477567600005386 -24.98288624099990329, 28.95607789100006357 -24.98311224699995137, 28.95588119400008509 -24.98390927399992734, 28.95543813700004421 -24.98539955399991186, 28.95414924700008896 -24.98511760899992851, 28.95384819100007689 -24.98616737399993326, 28.95373492600003829 -24.9864424479999343, 28.95371272200003432 -24.98649636799990503, 28.95231251700005259 -24.98642146699995692, 28.95144092800006774 -24.98635265699994079, 28.94994683200008012 -24.986157976999948, 28.94817658700003449 -24.98598526999995784, 28.94714034700007232 -24.98581256299991082, 28.94619046100007154 -24.98572620799990318, 28.94511104200006457 -24.98568303299992976, 28.94415714500007653 -24.98572209399992516, 28.94313494900006845 -24.98573912999995628, 28.94210446300007789 -24.98577514799995924, 28.94105243500007418 -24.98589891599993962, 28.93967078200006426 -24.98602844599992068, 28.93824595100005581 -24.98602844599992068, 28.93556436800008669 -24.98646139799990351, 28.93444866200007937 -24.98646139799990351, 28.93460389000006217 -24.98587928999995711, 28.93437104700007012 -24.98585018599993646, 28.93381804400007695 -24.98563674599995466, 28.93344937700004493 -24.98559793799995532, 28.93319713100004265 -24.98553972799993517, 28.93287697100004152 -24.98545241199991551, 28.93262472500003923 -24.98544270999991568, 28.93218814500005465 -24.98545241199991551, 28.93182917800004361 -24.98553972799993517, 28.93165454500007172 -24.98571435999991763, 28.93150901900008876 -24.98585988599995744, 28.93044122900005277 -24.9858653299999105, 28.93052315100004535 -24.98536209099995631, 28.93052191800006767 -24.98535737699995707, 28.93040786300008449 -24.9853301029999102, 28.93046463300004234 -24.98484991599991645, 28.93082859700007248 -24.98446191699991914, 28.9310140420000721 -24.98409377099994799, 28.93108290000003535 -24.98395707199995286, 28.93140132700006006 -24.98396320899990997, 28.93103093000007675 -24.98178771899995354, 28.93088000600005216 -24.98131876299993337, 28.93149447800004737 -24.98094751999991558, 28.93312867200006622 -24.97948880899991764, 28.93441992200007462 -24.9802436989999137, 28.93689920200006327 -24.98147217199993975, 28.9369492440000613 -24.98134491799993384, 28.93726573100008181 -24.98054010299995298, 28.93832041700005675 -24.98101901899991617, 28.93864758500006928 -24.98058902599990461, 28.93948075400004427 -24.97955622699993228, 28.94020779500004892 -24.98021175699994956, 28.9404461690000403 -24.98043821199991044, 28.94092149800007974 -24.98087040499990508, 28.94103090600003725 -24.98058906899990461, 28.94155710900008671 -24.98054217999992943, 28.94157284500005289 -24.98050028899990593, 28.94168571700004122 -24.98019983799991905, 28.94183962500005691 -24.9795822769999063, 28.94198491500003456 -24.97906569599990689, 28.9427813100000435 -24.97910336299992196, 28.94405123800004276 -24.97805943799994566, 28.94622518400007039 -24.97653660199995329, 28.94774264000005815 -24.97817782199990688, 28.94841527200009068 -24.97867287799994074)))</t>
+  </si>
+  <si>
+    <t>Tshikanosi SP</t>
+  </si>
+  <si>
+    <t>Tshikanosi</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((28.94106264200007672 -25.29005731299992021, 28.94108456400005025 -25.29029056899992156, 28.94110253400003785 -25.29040070899992543, 28.94071808500007137 -25.29050245099995209, 28.94039016700008915 -25.2905844299999103, 28.9409921640000789 -25.29231491599995252, 28.94023397500006922 -25.29252154099992822, 28.94023964400008708 -25.29241385099993522, 28.94017123500003663 -25.29228615599993191, 28.93985655900007714 -25.29119619099992633, 28.93967869800007975 -25.29079030399992689, 28.93857864700004257 -25.29102245199993604, 28.93738038700007564 -25.29119032299990977, 28.93735150800006295 -25.29060431199991399, 28.93733752300005335 -25.29045247099992366, 28.93718383100008396 -25.29038670699992508, 28.93700632800005224 -25.2903151099999377, 28.936879541000053 -25.29027781999991475, 28.93677512800007889 -25.29018981399991617, 28.93649210400008087 -25.29023855299993784, 28.93644055700008266 -25.28988011399991365, 28.93628157300008752 -25.28863853499990455, 28.93626695800008974 -25.28854754599990429, 28.93704909100006262 -25.28844553699991593, 28.93749284400007582 -25.28839810099992746, 28.93804524000006495 -25.28832312299994101, 28.93916449500005683 -25.28816431399991416, 28.93955138700005136 -25.28810628099995483, 28.93991847000006601 -25.28807337299991786, 28.94010680100006994 -25.28804467899993824, 28.94074632900003508 -25.2879848139999126, 28.94078257300003543 -25.2883373709999546, 28.94079245800008948 -25.28879536299990605, 28.94080234300008669 -25.28893374899990931, 28.94083529200008797 -25.28905895599990572, 28.94083858600004078 -25.28936867699991353, 28.94088801100008368 -25.28958943599991471, 28.94100992200003475 -25.28994528599992009, 28.94106264200007672 -25.29005731299992021)))</t>
+  </si>
+  <si>
+    <t>Kwaggafontein A</t>
+  </si>
+  <si>
+    <t>Kwaggafontein</t>
+  </si>
+  <si>
+    <t>MP315</t>
+  </si>
+  <si>
+    <t>Thembisile</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((29.01062861500008694 -25.1597306699999308, 29.01040928100007932 -25.16079363999995167, 29.01101584100007358 -25.1612640339999416, 29.01157288600006723 -25.16168491199994151, 29.01333067300004132 -25.16304657799992128, 29.01395982100007132 -25.16352866599993376, 29.0135905510000498 -25.16424191499993412, 29.01341506800008574 -25.16458086099993352, 29.01322411600006035 -25.1649648629999092, 29.01211728000004086 -25.16719069899994565, 29.01139010100007454 -25.1686257519999117, 29.01101603800003659 -25.16936394799995469, 29.01017195900004708 -25.16869842399995605, 29.00933368300007942 -25.1680134919999432, 29.0080967150000788 -25.16705254199990804, 29.00676774000004343 -25.16596891699992966, 29.00611347700004217 -25.16547821899990822, 29.00557368700003735 -25.165190255999903, 29.0058940000000689 -25.16480587999990348, 29.00586502800007338 -25.16461273699991352, 29.00584467200008021 -25.1644770289999542, 29.00579534400003467 -25.16419750499994734, 29.00591044200007218 -25.1638850959999445, 29.00595397100005357 -25.16380473499992831, 29.00633794900005569 -25.16309585299995888, 29.00653338900008293 -25.16274504399990519, 29.00710227100006477 -25.16193789999994124, 29.00680187700004353 -25.16183341599992218, 29.00836914200004912 -25.15865970699991294, 29.01027597900008459 -25.15945639899990738, 29.01062861500008694 -25.1597306699999308)))</t>
+  </si>
+  <si>
+    <t>Waterval A</t>
+  </si>
+  <si>
+    <t>Waterval</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.84665479200003801 -25.98021166699993501, 30.84673372800006064 -25.98039118899993127, 30.84669938100006448 -25.98128421099994512, 30.84642460400004893 -25.98176506999993762, 30.84614982900006908 -25.98207419199991364, 30.84618417600006524 -25.98234896899992918, 30.84645895100004509 -25.98276113199995052, 30.8462185230000614 -25.98282982499995342, 30.8450507260000677 -25.98262374399990904, 30.84453552100006846 -25.98258939699991288, 30.84347076400007381 -25.98231462199993302, 30.84213123200004247 -25.98186810999993668, 30.84137559800007011 -25.98179941699993378, 30.84055127000004859 -25.98176506999993762, 30.83938347300005489 -25.98131855799994128, 30.83842175700004873 -25.98104378199991515, 30.83649832600008267 -25.98018510699995431, 30.83526183300006096 -25.97966990399993392, 30.8338879540000903 -25.97867383999994217, 30.83210960600007411 -25.97743333599993321, 30.83090898900007915 -25.97640841899993802, 30.83044045500008679 -25.9757934689999388, 30.83026821500004644 -25.97563558199993849, 30.83025500400003693 -25.97554310799995392, 30.83026064000006272 -25.97513172399993664, 30.83018737900005135 -25.97488376499995866, 30.83015920200006121 -25.97478796299992609, 30.8301704720000771 -25.97465271399994435, 30.83015920200006121 -25.97452873499992165, 30.8302268270000468 -25.97429768299991792, 30.83029445200008922 -25.97396519399995896, 30.83031135700008463 -25.97380740199992033, 30.83033523700004253 -25.9736665169999128, 30.83085799300005192 -25.9736665169999128, 30.83177656500004105 -25.97368905799993399, 30.83216540800003713 -25.97369469399990294, 30.83263314700008095 -25.97370032999992873, 30.83297850300004939 -25.97370548299994653, 30.83301072000006116 -25.97370596599995451, 30.8333375740000406 -25.97369469399990294, 30.83359116700006552 -25.97370596599995451, 30.83392365600008134 -25.97367215199994916, 30.83425051000006079 -25.97361579799991205, 30.8344590200000539 -25.97350872599992044, 30.83471825000003719 -25.97337347499990301, 30.8347464260000379 -25.97313678799991976, 30.83464498900008266 -25.9730015379999486, 30.83450973900005465 -25.97291700699992134, 30.83434631200003651 -25.97280993399994031, 30.8342392400000449 -25.9726915909999434, 30.83426741600004561 -25.97249998699993512, 30.83431250000006685 -25.97238727899991773, 30.83436885400004712 -25.97230838299992683, 30.83443647900008955 -25.97213932099992917, 30.83448719700004403 -25.97186882099992999, 30.83471261400006824 -25.97194771699992089, 30.834763333000069 -25.9716659459999164, 30.83459990600005085 -25.97151942499993993, 30.83441393700007893 -25.97142925899993315, 30.83428995800005623 -25.97135036299994226, 30.83420542700008582 -25.97127146699995137, 30.83403636500008815 -25.97120947799993473, 30.83395746900004042 -25.97115312399995446, 30.83393492700008665 -25.97103477999991128, 30.83385603100003891 -25.97092770799991968, 30.83372078200005717 -25.9708375419999129, 30.83361370800008672 -25.97069102099993643, 30.83354608400009056 -25.9705670409999243, 30.83351227100007463 -25.97040361499995242, 30.83351227100007463 -25.97033035399994105, 30.8333601150000618 -25.97016129199994339, 30.83305094000007784 -25.97003360099995461, 30.83292785500003674 -25.96982259799995063, 30.8330685230000654 -25.96945334399993044, 30.8335256960000379 -25.96945334399993044, 30.83414112100007287 -25.9697346799999309, 30.83435212400007686 -25.9697346799999309, 30.83480929600005993 -25.96978742999993983, 30.83514338400004817 -25.96982259799995063, 30.83542472000004864 -25.96985776499991516, 30.83554780600007916 -25.96955884399994829, 30.83560055700007752 -25.96899616899992225, 30.83553022200004534 -25.9687324169999556, 30.83545988800005944 -25.96836316199994599, 30.83524888500005545 -25.96797632399994882, 30.83498513200004254 -25.96758948499990538, 30.83421015300007184 -25.96688189499991495, 30.83442299000006415 -25.96680348099994262, 30.8350965080000492 -25.96580784699995093, 30.83755630900003553 -25.96478292999995574, 30.83940115800004378 -25.96440224699995269, 30.8399575430000823 -25.96481221299995923, 30.84189024400006929 -25.96469508099994528, 30.84314942700007123 -25.96443152999995618, 30.84420362900004875 -25.96431439599990654, 30.84552137900004709 -25.96405084599990687, 30.84683913000003486 -25.96387514599990709, 30.84798338300004161 -25.96382416699992746, 30.84836258700005374 -25.96398107899995011, 30.84863718100007191 -25.96392877399995314, 30.84899023400004126 -25.96399415499990937, 30.84936943800005338 -25.96430797899995468, 30.84991863000004741 -25.96430797899995468, 30.8505462780000812 -25.96496177899990698, 30.85180157300004566 -25.96510561499991354, 30.85262536100003672 -25.96510561499991354, 30.85374989700005699 -25.96484409499993262, 30.8539591130000872 -25.96453027099994415, 30.85440369800005556 -25.96459565099991096, 30.85493981200005464 -25.96481794299995727, 30.85550208000006478 -25.96511869099992964, 30.8558812840000769 -25.96530175499992765, 30.85636509600004729 -25.96541943799991259, 30.85683583300004784 -25.96543251499991811, 30.85721503500008112 -25.96531483199993318, 30.85776422700007515 -25.96521022299992865, 30.85814343100008728 -25.9652756029999523, 30.85835264600007122 -25.9656286539999428, 30.85861416700004156 -25.96594247799993127, 30.85887568700007932 -25.96604708599994638, 30.8591633590000356 -25.96612554199992928, 30.85946410600007539 -25.96615169399990464, 30.86002637500007495 -25.96615169399990464, 30.8603532740000901 -25.96611246599991318, 30.86047095800006446 -25.96649166999992531, 30.86009175500004176 -25.96687087399993743, 30.8612293660000887 -25.96738083699995059, 30.86159549400008473 -25.96745929399992292, 30.86204007800006366 -25.9679823339999416, 30.86243235800003504 -25.96816539799993961, 30.86354381700004978 -25.96887150099991004, 30.86409300900004382 -25.96876689299995178, 30.86478603800009068 -25.96843999399993663, 30.86523062100008019 -25.96841384199990443, 30.86583211700008178 -25.96925070599991159, 30.86615901700008635 -25.96976066899992475, 30.86638130900007582 -25.97020525299990368, 30.86689127200008897 -25.970610608999948, 30.86737508400005936 -25.97096366099992792, 30.86771506000008003 -25.97098981299990328, 30.86842116500008615 -25.97109442099991838, 30.86885267200005956 -25.97130363599995917, 30.86974184000007426 -25.97152592799994864, 30.87042179100006933 -25.97170899199994665, 30.87120635100006893 -25.97153900399990789, 30.87163785900008861 -25.97121210399990332, 30.87209551800003737 -25.97083289999994804, 30.87244857100006357 -25.97051907699994899, 30.87261855800005605 -25.97024448099995197, 30.87286700200007772 -25.97007449299991322, 30.87322005400005764 -25.96972143999994387, 30.87329851000004055 -25.96942069299990408, 30.87349465000005466 -25.96896303299990905, 30.87369079000006877 -25.96876689299995178, 30.87362541000004512 -25.96847922199992809, 30.87376924600005168 -25.96830923299995675, 30.87386077800005069 -25.96813924599990742, 30.87403076700007887 -25.9679954099999577, 30.8740569180000648 -25.96769466199992848, 30.87430536300007589 -25.96748544599995512, 30.87497223800005486 -25.96732853399993246, 30.87535144000008813 -25.9670800899999108, 30.87570449300005748 -25.9667270389999203, 30.87684210400004758 -25.96658320199992431, 30.8775482090000537 -25.96645244099994443, 30.87809740000005831 -25.96645244099994443, 30.87839814800008753 -25.96604708599994638, 30.87896360700005971 -25.96561870799990857, 30.87906122900005812 -25.96265690999990738, 30.87911817000008341 -25.96097718999993731, 30.87895542600006138 -25.96078956099995594, 30.87899591600006488 -25.96029357399993387, 30.87914545800003907 -25.96017220199991016, 30.87919918300008248 -25.9585873319999223, 30.87922575600003938 -25.95780342199992674, 30.87924390700004551 -25.95737839199995278, 30.8794822750000435 -25.95730183599994234, 30.87953535200006172 -25.95720326699995439, 30.87956947100008165 -25.95700233399992385, 30.87966804200004844 -25.95672936999994818, 30.87979315100005806 -25.95642228599990631, 30.8799637520000374 -25.95616069499993728, 30.88009644400005982 -25.95596734599990896, 30.88009644400005982 -25.95581569899991337, 30.88117757800006302 -25.95418373699993708, 30.88220979000004718 -25.95376925699991943, 30.88313211800004865 -25.9544870069999547, 30.88450971600008188 -25.95986128199990617, 30.88479442300007349 -25.96167441699992651, 30.8849192940000421 -25.96244362499993485, 30.88489045000005717 -25.96289560299993582, 30.88482179100003577 -25.96296189499992124, 30.88471998700003951 -25.96299977499995748, 30.88460871200004476 -25.96306133199993837, 30.88452111200007266 -25.96318917999991527, 30.8845353190000651 -25.9632886169999324, 30.8845353190000651 -25.9633549079999284, 30.88446429100008572 -25.96337621599991508, 30.88437432400007765 -25.96338095099991961, 30.88434354600008191 -25.96340936199993621, 30.88433407600007286 -25.96346855099994855, 30.88429382700007864 -25.96349459399993975, 30.88422990400005119 -25.96349695999992946, 30.88416361200006577 -25.96350406399994881, 30.88411389300006249 -25.96354194499991763, 30.88404286700006196 -25.96356325299990431, 30.88397894300004509 -25.96358692699993753, 30.88391502000007449 -25.96361533899994356, 30.88387713700006998 -25.96368163099992898, 30.88381558200006793 -25.96369110099993804, 30.88371140900005685 -25.96368399799990812, 30.88361197100005029 -25.96375029099993981, 30.88349122700003591 -25.96377396499991619, 30.88331366000005573 -25.96385209399994665, 30.88309111000006624 -25.96395863399993686, 30.88293485200006216 -25.96402492599992229, 30.88286856100006617 -25.96409831999994822, 30.88282594500003597 -25.96412672999991855, 30.88276912400004903 -25.96415750899990371, 30.88272887500005481 -25.9641456709999261, 30.88268389200004549 -25.96411489299993036, 30.88265784800006486 -25.96411725999990949, 30.88264601100007667 -25.96412909799994395, 30.8826223350000646 -25.96417644899992183, 30.88256551400007766 -25.96418118399992636, 30.8824873850000472 -25.96418118399992636, 30.88238558000006151 -25.96418591899993089, 30.88237137500004792 -25.96421432999994749, 30.88236190400004944 -25.96427115099993443, 30.8823263920000386 -25.964287724999906, 30.88229798000008941 -25.96435638299993798, 30.88227193700004136 -25.96441793899992945, 30.88220564600004536 -25.96443451199991159, 30.88211331100006873 -25.96443451199991159, 30.88201860800006671 -25.96444161499994152, 30.88186235100005206 -25.9644676569999433, 30.88181500000007418 -25.96451974399991514, 30.88174397300008422 -25.96454341999992721, 30.88170845900003769 -25.96460260899993955, 30.88170845900003769 -25.96466179699990562, 30.88170609300004799 -25.96475176399991369, 30.88164690300004622 -25.96487724499991145, 30.88157114300008743 -25.96489381699990417, 30.8815143200000648 -25.96488197999991598, 30.88146223400008239 -25.96487724499991145, 30.88142672100008213 -25.96488197999991598, 30.88140304400008063 -25.96493880099990292, 30.88141725100007307 -25.96498615199993765, 30.88143145600008665 -25.965028767999911, 30.88141014800004314 -25.96506191399993213, 30.88135806200006073 -25.96505244299993365, 30.88126336100003755 -25.96515661599994473, 30.88118049600006998 -25.9653720629999043, 30.88114261500004432 -25.96553779199990686, 30.88109999900007097 -25.96558750999992071, 30.88102660500004504 -25.96560408299990286, 30.88109526400006644 -25.96568457999995871, 30.88103134000004957 -25.96587161699994795, 30.88098398900007169 -25.96593554099990797, 30.88075330200007329 -25.96599374399994531, 30.88064014300005056 -25.96606696499992495, 30.88054029500005981 -25.96616681199992627, 30.88035391500005744 -25.96624668899994504, 30.88014090900009023 -25.96624668899994504, 30.88002109300003895 -25.96626000199995588, 30.87996784100005243 -25.96628662799992071, 30.87991459000005534 -25.96638647499992203, 30.87986133800006883 -25.96653291699993815, 30.87982140000008258 -25.96673260999995136, 30.87969492700005958 -25.9670920579999347, 30.87954182900006117 -25.96747147599995742, 30.87980142900005376 -25.96755800899995847, 30.88004106200008891 -25.96756466599993018, 30.88034726000006458 -25.96769113799990691, 30.88056026500004236 -25.96779764199993679, 30.88081321000004209 -25.9680173029999537, 30.88079989700008809 -25.96825693599993201, 30.88075330200007329 -25.96850322499994945, 30.88045376200005876 -25.96867629299993041, 30.88012094000004026 -25.96863635399995474, 30.8798813090000408 -25.96864966699990873, 30.87912912800004506 -25.96860972799993306, 30.87900265600006833 -25.96921546499993383, 30.87891612300006727 -25.96976794999994809, 30.87885621500004163 -25.97005417699995178, 30.87892943600007811 -25.9703204349999055, 30.87902262600005088 -25.97056672399992294, 30.87903593900006172 -25.97071316699992849, 30.87894940600006066 -25.97089288899991288, 30.8788096190000374 -25.97093948499991711, 30.87873639900004719 -25.97109258299991552, 30.87868980300004296 -25.97119242999991684, 30.87847679700007575 -25.97119908599995597, 30.87835032500004218 -25.97111255199990865, 30.8783103860000665 -25.97083963699992637, 30.87795093800008317 -25.97067322799995281, 30.87757152000006045 -25.97064660199993114, 30.87739246800003912 -25.97083302399994409, 30.8771750490000727 -25.97086596599990571, 30.87708281000004717 -25.97093843899995136, 30.87695104100004073 -25.97114926899990905, 30.87677974200005337 -25.97150504599994747, 30.87664797200005751 -25.97176858399990351, 30.87643714200004297 -25.97205188699990686, 30.87616042700005892 -25.97215071399995168, 30.8759232430000452 -25.97219683299994131, 30.87579147500008503 -25.97224954099993965, 30.87558064500007049 -25.97247354899991478, 30.87518533700006174 -25.9730533329999389, 30.87484273700005133 -25.97340910799994163, 30.87461873000006563 -25.97360676099992816, 30.87442766500004154 -25.97392300699993939, 30.87433542600007286 -25.97419313399990415, 30.87492179800005943 -25.97432490399995686, 30.8753698130000771 -25.97436443399993777, 30.87585735800007569 -25.97449620199995479, 30.8760484240000892 -25.97470044399995004, 30.87594300800003566 -25.97494421799990505, 30.87552793600008272 -25.97496398199990608, 30.87509968800003435 -25.97482562499993719, 30.87504697900004658 -25.97498374799994281, 30.87508651000007376 -25.97516822399995817, 30.87496132900008661 -25.97542517499994119, 30.87469779100007372 -25.97584683499991343, 30.87456602200006728 -25.97609719599995515, 30.8744671950000793 -25.97634755699994002, 30.87427613000005522 -25.97663744899995208, 30.87395329600008154 -25.97701299099992411, 30.87372270000008712 -25.97736876699991626, 30.87355799000005163 -25.97757300899991151, 30.87322856700006923 -25.97810008499993728, 30.87303750100005573 -25.97827797199994393, 30.87319562400006134 -25.97873257599991348, 30.87450013800008719 -25.97954954299990504, 30.87480470100007324 -25.97977381299995159, 30.8754966110000737 -25.97979178499991804, 30.87601283700007571 -25.97980276899994578, 30.87647414400004209 -25.97976981799990881, 30.87683660000004693 -25.97978080199993656, 30.87717708900004254 -25.97978080199993656, 30.87760544600007506 -25.97971490099990888, 30.87778118300008146 -25.97971490099990888, 30.87815462200006777 -25.97959408199994868, 30.8783852760000741 -25.97955014799993023, 30.87871478100004197 -25.97945129599992242, 30.87901133500008655 -25.97937441199991326, 30.87945067700007939 -25.97920965899993462, 30.87962641400008579 -25.97915474099994526, 30.87992296800007352 -25.97909982399994533, 30.88023050700007843 -25.97907785599994668, 30.88072476400003552 -25.97894605499993759, 30.88107623700005888 -25.97890211999992971, 30.88146066000007295 -25.97870441699990351, 30.88209694500005753 -25.979051492999929, 30.88196002700004783 -25.97928425399993557, 30.88182310800004871 -25.97973608499995635, 30.88180941700005633 -25.98006468999994922, 30.88183680100007678 -25.98051652099991315, 30.88189156700008198 -25.98095465899990586, 30.88168618900004958 -25.98129695699992681, 30.88157665500006033 -25.98152971799993338, 30.88104267200003505 -25.98176247999992938, 30.88045392300006142 -25.98196785599992609, 30.87991994100008242 -25.98213215899994566, 30.87934488300004432 -25.98213215899994566, 30.87838645300007556 -25.98203631699993821, 30.87775662800004284 -25.98210477499992521, 30.87727741300005846 -25.98199523999994653, 30.87697619100003976 -25.98194047399994133, 30.87608622200008313 -25.98161186899994846, 30.87564808300004415 -25.98132433999995783, 30.87518533700006174 -25.98103853399993568, 30.87380176100003837 -25.98083429199994043, 30.87349210400003585 -25.9808672339999589, 30.87343939700008377 -25.98085405799992031, 30.87336692400003813 -25.98057075399992755, 30.87292549800008601 -25.98063004999994519, 30.87275419800005238 -25.98056416599990825, 30.87261584100008349 -25.98046533899992028, 30.87231277200004342 -25.9803401569999437, 30.87214147200006664 -25.98016885899994577, 30.87191087600007222 -25.97997779399992169, 30.87178569600007449 -25.97978672899995445, 30.87170004600005768 -25.97964178299992, 30.87123848800007408 -25.9782263639999087, 30.87208181000005425 -25.97741817999991554, 30.87149616900006777 -25.97676226299995506, 30.87100423200007526 -25.97653971999994837, 30.87079340200006072 -25.97630546399994955, 30.87048886800005221 -25.97618833599995014, 30.87028975100008665 -25.97611805899992987, 30.87005549600007726 -25.9760126439999226, 30.86973925000006602 -25.97591894199990747, 30.86946985500003393 -25.97587209099992833, 30.86934101400004238 -25.97587209099992833, 30.86918874800005597 -25.97596579299994346, 30.86896620500004929 -25.97591894199990747, 30.86880222700006016 -25.97594236699995918, 30.86859139500006677 -25.9759775059999356, 30.86846255400007522 -25.97598921899992774, 30.8683454260000758 -25.97598921899992774, 30.86818144700004041 -25.97602435699991474, 30.86801746800006185 -25.97608292099994287, 30.86784177600003432 -25.97609463399993501, 30.86760752000003549 -25.97610634599993773, 30.86726784900008624 -25.97630546399994955, 30.86703359300008742 -25.97635231399993927, 30.86689304000003631 -25.97648115599992025, 30.86674077100008162 -25.97648115599992025, 30.86645966600008251 -25.97634060299992598, 30.86635425000008581 -25.97614148599990358, 30.86640110100006495 -25.97576667499993164, 30.86640110100006495 -25.97546214199991255, 30.86652994100006708 -25.97504048199994031, 30.86647137800008522 -25.97451340599991454, 30.86628397300006554 -25.97405660599991961, 30.86596772800004373 -25.97371693499991352, 30.86565148200008935 -25.97340068799991286, 30.86514783100005843 -25.97283847499994636, 30.86487843800006203 -25.97249880399994026, 30.86452705300007437 -25.97233482399991544, 30.86417566900007614 -25.97224112199995716, 30.86370656700006521 -25.9721131469999591, 30.86322476400005144 -25.97196489999993219, 30.86282943800006251 -25.9718042989999276, 30.86255765300006715 -25.97160663599993313, 30.86234763700008443 -25.97137191199993822, 30.86222409800006972 -25.9709642329999042, 30.86216232800006765 -25.97055655399992702, 30.86195231100003866 -25.97022299799994016, 30.86176700300006814 -25.96985238199994228, 30.86148286300004884 -25.9696423649999133, 30.86076633500005073 -25.96929645499994876, 30.86007451700004367 -25.96886406899994881, 30.8595433000000412 -25.96853051099992626, 30.85917268100007504 -25.9682957889999102, 30.85890089500009026 -25.96822166399994103, 30.85838203100007604 -25.96811047899990399, 30.85760373400006529 -25.9679622309999445, 30.85689956100003428 -25.96781398599995327, 30.85605949500006773 -25.96762867699993649, 30.85529355300008092 -25.9675421979999328, 30.85462644000006094 -25.96751749099991002, 30.85419405400006099 -25.96751749099991002, 30.85225449000006392 -25.96761632299995881, 30.85109322100004192 -25.96765338399995926, 30.8496972300000607 -25.96769044599994913, 30.84963546100004805 -25.9683699109999111, 30.84862244000004239 -25.96864169699995273, 30.84828888400005553 -25.96776456999992888, 30.84762177200008182 -25.96780163099992933, 30.84725115600008394 -25.96785104699995372, 30.84685583100008444 -25.96811047899990399, 30.84638638200004834 -25.96834520399994517, 30.84581810200006657 -25.9683946189999233, 30.84555866900007004 -25.96848109699993756, 30.84523746800005028 -25.96851815799993801, 30.8449656820000655 -25.96851815799993801, 30.84455800300008832 -25.96850580399990349, 30.84415682400003789 -25.96849668699991298, 30.84407149000008985 -25.96874913499993909, 30.84400644000004377 -25.96890091599993866, 30.84389079600003924 -25.96898764899992784, 30.84374624100007622 -25.96900933299991721, 30.84358723100007182 -25.96897319499993273, 30.8435149540000566 -25.96897319499993273, 30.84340653800006748 -25.96893705399992314, 30.84329089400006296 -25.96890091599993866, 30.84317421000008608 -25.96890722399990636, 30.84316201100006083 -25.96893819099994971, 30.8428037480000512 -25.9694941169999538, 30.84274158600004512 -25.96956586799990419, 30.84253198200008228 -25.96934903599992595, 30.84230792200008864 -25.96905992699993249, 30.84204772300006425 -25.96875636199990822, 30.8419648840000491 -25.96867670899990799, 30.84090124500005459 -25.96882700599991267, 30.84013530200007835 -25.96898760699991726, 30.83799807500008683 -25.96970413499991537, 30.83741744100007054 -25.97006239699993557, 30.83707153200003859 -25.97049478399992495, 30.83644354100005103 -25.97143024999991212, 30.83544790800004876 -25.97263086699990708, 30.83518435700005966 -25.97304083399990304, 30.83563684000006333 -25.97316565699992452, 30.83594853100004229 -25.97318072299992764, 30.83622681900004636 -25.9732045759999437, 30.83646535200006156 -25.97328408699991087, 30.83657666600004177 -25.97323638099993559, 30.83669593100006523 -25.97321252699993011, 30.83690265900008853 -25.97318867399991404, 30.8371173380000414 -25.973244331999922, 30.83737972300008323 -25.97336359699994546, 30.83757850000006329 -25.9734510599999453, 30.83791244500008588 -25.97353056999992305, 30.83819868300008693 -25.973586227999931, 30.83842926400006945 -25.97371344499993029, 30.83878706200005126 -25.97380885699993769, 30.83912100700007386 -25.97391221999993149, 30.83903354500006344 -25.9743018229999052, 30.83865189500005499 -25.97418255699994916, 30.83859623700004704 -25.97434952999992674, 30.8385803340000848 -25.97448469799991244, 30.83856443200005515 -25.97470732799990856, 30.83844516600004226 -25.97486634899991031, 30.83842926400006945 -25.97500946799993926, 30.83904149700003927 -25.97518439199990326, 30.83908125100003872 -25.97531956099993522, 30.83920051800004103 -25.97560579799994684, 30.83928797900006202 -25.97593974199992317, 30.83951856000004454 -25.97609876299992493, 30.83975709200007032 -25.976289589999908, 30.84011489000005213 -25.97640885599992089, 30.84031366700008903 -25.97655197499994983, 30.8401069380000763 -25.97684616499992671, 30.84000357500008249 -25.97723576699991099, 30.84004333000007136 -25.97741864099992881, 30.84013079200008178 -25.97772078199994894, 30.84013960700008283 -25.9778054029999339, 30.84017054700007066 -25.97810243299994681, 30.84036932400005071 -25.9781580899999085, 30.84067941700004667 -25.97821374799991645, 30.84088767000008602 -25.97825539899992009, 30.84099745800006076 -25.97827735599992138, 30.841267794000089 -25.97839662199993427, 30.8414506690000394 -25.97843637799991257, 30.8417925650000484 -25.97849998699990692, 30.84208675400003585 -25.97853974099990637, 30.84226167800005669 -25.97857949699994151, 30.84252406300004168 -25.9786351539999032, 30.84265128100008724 -25.9786987629999544, 30.84288186200006976 -25.97879417499990495, 30.84305678300006548 -25.97887368699991839, 30.8431919520000406 -25.97891344099991784, 30.84329531600008067 -25.97893729499992332, 30.84345433700008243 -25.97895319699995298, 30.84360540800008721 -25.97901680499995791, 30.84376442900008897 -25.97908041399995227, 30.84395525500008262 -25.97913607099991395, 30.84409042400005774 -25.9791837779999355, 30.84427329700008613 -25.97922353299992437, 30.84442436600005522 -25.97924738599994043, 30.84453568200007112 -25.97927123899995649, 30.8446867530000759 -25.97929509299990514, 30.84484577400007765 -25.97930304399994839, 30.84496504000009054 -25.97935074999992366, 30.84510020800007624 -25.97940640699994219, 30.84524332600005891 -25.97949386799990634, 30.84546595700004445 -25.97957337999991978, 30.84557727200007093 -25.9796210859999519, 30.84566473400008135 -25.97968469499994626, 30.84581580400003986 -25.97972444899994571, 30.84595892300006881 -25.97972444899994571, 30.84605433600006563 -25.97987551999995048, 30.84617360200007852 -25.98001068799993618, 30.84637237900005857 -25.98008224899990637, 30.84661886200007075 -25.98012995399994907, 30.84665479200003801 -25.98021166699993501)))</t>
+  </si>
+  <si>
+    <t>Mbejeka SP B</t>
+  </si>
+  <si>
+    <t>Mbejeka</t>
+  </si>
+  <si>
+    <t>MP301</t>
+  </si>
+  <si>
+    <t>Albert Luthuli</t>
+  </si>
+  <si>
+    <t>DC30</t>
+  </si>
+  <si>
+    <t>Gert Sibande</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.80497386800004733 -25.98257217499991611, 30.80330034500008196 -25.98302154699990751, 30.80347358200003782 -25.98313312299995914, 30.80360646000008273 -25.98332136799990622, 30.80340714100003652 -25.98370893099991008, 30.80336284800006297 -25.98386395599993648, 30.80341821500007882 -25.98412971399994831, 30.8034846550000907 -25.98425151899994034, 30.80409368200008657 -25.98460586299995612, 30.80478022300007979 -25.98522596399993745, 30.80458090500007984 -25.98542528299992682, 30.80510134600007177 -25.98590143199993463, 30.80479481400004715 -25.98629780899995012, 30.80445909900004153 -25.98673192499995821, 30.80361753300007877 -25.98785032099993941, 30.80320676100006949 -25.98842056999990291, 30.8031980300000896 -25.98843268999991096, 30.8026763090000486 -25.98915696299991396, 30.80233303700003944 -25.98933413499992184, 30.80197869400006994 -25.98945594099990331, 30.80108176100003448 -25.98962203899992573, 30.79911072500004821 -25.98978813799993759, 30.79805274200003851 -25.9898563759999206, 30.79714505400005464 -25.98996983599994337, 30.79669120800008386 -25.99015137499992534, 30.79725851400007741 -25.99055983399995284, 30.79789389600006189 -25.99085483299995758, 30.79848389400007136 -25.99114983199990547, 30.79880158400004575 -25.99121790899994267, 30.79905120000006491 -25.99126329299991767, 30.79923273700006803 -25.99128598499993359, 30.79964119800007438 -25.99158098399993833, 30.80009504200006631 -25.99173982899992552, 30.80043542500004605 -25.99192136699991806, 30.80098003800003426 -25.99210290499991061, 30.80138849900004061 -25.99230713499991907, 30.80202387900004624 -25.99267020999991473, 30.80124685800007001 -25.99372702299990578, 30.79976084000008996 -25.99397447799992733, 30.79832229900006269 -25.9932192429999418, 30.7963443040000584 -25.99246400899994569, 30.79570134900006906 -25.99188226299992266, 30.79500552700005755 -25.99112965199992686, 30.79483746200008909 -25.99109145499994611, 30.79460050900007673 -25.9912602119999292, 30.79440812700005381 -25.99139722699993627, 30.79391748000006146 -25.99176521099991533, 30.79205216100007192 -25.9931216769999196, 30.79134494000004452 -25.99360465699993483, 30.79023640300005127 -25.99441294799993329, 30.78999383500007525 -25.99456819199991742, 30.78940682000006746 -25.99499511199991275, 30.78878099400003521 -25.99549480299992865, 30.78848506100007398 -25.99576162799991152, 30.78804843800008939 -25.99620310199992446, 30.78728677400005154 -25.99548995099991089, 30.7873226270000373 -25.99525726299992812, 30.78739942000004248 -25.99454692299991621, 30.78730342800008657 -25.99324143199993387, 30.78730342800008657 -25.9924350999999092, 30.78701365400007717 -25.99194614099991441, 30.78674367600007145 -25.99156817299990507, 30.78633331100007808 -25.99115780599993286, 30.78602013500005796 -25.99066104899992524, 30.78572856000005231 -25.99011029499990855, 30.78518860600007656 -25.98952714399990782, 30.78430308000008608 -25.98884680099990874, 30.78351474600003712 -25.98791807899993955, 30.78402230300008569 -25.98752931199993554, 30.78465944900005979 -25.98678417499991156, 30.78618212200007065 -25.98530469799993625, 30.78676527300007137 -25.9844947669999442, 30.7870784470000558 -25.98409519999995609, 30.78745641500006514 -25.98342565699994111, 30.78767239700005121 -25.98309088499991049, 30.78790997700008347 -25.98263732299994899, 30.78834194100005561 -25.98250773399990976, 30.78861191800007191 -25.98269131799992238, 30.78892509200005634 -25.98286410399992974, 30.78911947600005306 -25.98301529099995832, 30.78927066300008164 -25.98314487999994071, 30.78954064000004109 -25.98333926399993743, 30.78968102900006443 -25.98359844199995905, 30.78983221600003617 -25.9838252229999398, 30.79067454500005852 -25.98381442399994512, 30.79164646400005267 -25.98363083899994308, 30.79201363300006733 -25.98351204999994479, 30.79268317600008231 -25.98337166099992146, 30.79351470700004256 -25.98335006299993211, 30.79454062000007752 -25.98325287099993375, 30.79572852100005775 -25.98311248299995668, 30.79674363500004119 -25.9830044919999068, 30.79738054000006287 -25.98296508499993251, 30.79761707200003684 -25.98288281499992536, 30.79785360100004254 -25.98273883899992143, 30.79817240400006995 -25.98268741899994438, 30.79847063700003673 -25.98264628399994081, 30.79869688400003724 -25.9826051479999478, 30.79897455000008222 -25.9825434449999193, 30.79920802600008756 -25.98240850699994553, 30.80037491000007321 -25.98211678599994912, 30.80164787400008208 -25.98222286599991548, 30.80297387800004572 -25.98219634599990968, 30.80361036000005015 -25.98232894699992812, 30.80411424200008241 -25.98214330599995492, 30.80497386800004733 -25.98257217499991611)))</t>
+  </si>
+  <si>
+    <t>Los-my-cherry</t>
+  </si>
+  <si>
+    <t>Tjakastad</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.77993673800006036 -26.01056232799993495, 30.7794849290000343 -26.010854674999905, 30.77881606300007888 -26.01120670899990728, 30.77765434800005551 -26.01173476099995696, 30.77691507400004411 -26.01219240699992952, 30.77603498900003842 -26.01272045899992236, 30.77511969800008274 -26.01328371499994319, 30.77438042600005019 -26.01398778399993716, 30.77427476000008255 -26.01428715799994507, 30.77426259900005334 -26.0143216109999571, 30.77401105200004849 -26.01457315799990511, 30.77380524000005835 -26.01493904499994869, 30.77369090100006588 -26.01523632799995767, 30.77348509000006516 -26.0153735359999132, 30.77348509000006516 -26.01557934699991392, 30.77295912700003555 -26.01585376199994926, 30.7724560330000827 -26.01592236599992702, 30.77188433500003839 -26.01592236599992702, 30.77119829700006903 -26.01589949799995338, 30.7709696170000484 -26.01603670699995519, 30.77032931500008317 -26.0158766299999229, 30.76996342800003958 -26.01603670699995519, 30.76932312600007435 -26.01612817699992775, 30.76900297500003489 -26.01585376199994926, 30.76875142800008689 -26.0150762519999148, 30.76843127700004743 -26.01461889399990923, 30.7683855410000433 -26.01381851599995798, 30.76843127700004743 -26.01301813799994989, 30.7685456160000399 -26.01176040299992565, 30.7685456160000399 -26.01139451699992833, 30.76856848500005981 -26.01093715699994391, 30.7685456160000399 -26.01054840199992668, 30.76840840900007379 -26.01009104399992111, 30.76822546600004671 -26.00954221299991787, 30.76804252200008705 -26.00903911899990817, 30.76756229600005099 -26.00892477899992627, 30.7669143120000399 -26.00857338499992011, 30.76633787800005848 -26.00880528299995831, 30.76643726400004653 -26.00901730499992937, 30.76627824800004873 -26.00926907999991045, 30.76571506600004113 -26.01015691799995011, 30.76537053200007676 -26.01026955399993312, 30.76501274700007116 -26.01044844699993064, 30.76495974100004105 -26.01038219099990556, 30.7637207420000891 -26.00945459799993387, 30.76378700000003619 -26.00934858799990934, 30.76385141400004386 -26.00927465099994151, 30.76439434800005301 -26.00857202899993581, 30.76469775100008519 -26.00818878199993378, 30.76492131300005894 -26.00759794099991495, 30.76474565800003802 -26.00737437999993062, 30.76445822300007649 -26.00686338299993849, 30.76401110000006156 -26.00638432299990654, 30.76372366500004318 -26.00609688699995559, 30.76340429100008578 -26.00555395099991074, 30.76302104200004806 -26.00529845299990939, 30.76241423300007227 -26.00462776899991013, 30.76211082900005067 -26.0041966159999447, 30.76182339400008914 -26.00365367999995669, 30.76072364500004142 -26.00334207399993147, 30.76076406500004623 -26.00308944499994368, 30.76076911700005212 -26.0030187079999564, 30.76077922200005332 -26.00263471199991727, 30.76070343400004958 -26.00237702999993417, 30.76054680400005736 -26.00221029499994074, 30.76032449100006261 -26.00210924299994986, 30.75998596700003418 -26.00200313799990681, 30.75978891700003715 -26.00190713999995751, 30.75958176100004948 -26.0018212459999063, 30.75944534100005967 -26.00180608799990978, 30.7593594470000653 -26.00175050899991902, 30.75925839500007442 -26.00162924699992573, 30.75909166000008099 -26.00147766999992882, 30.7589148190000401 -26.00135135499994021, 30.75875313700004199 -26.00124019799994812, 30.7586419800000499 -26.00115935699994907, 30.75852577000006249 -26.00110377899994774, 30.7584398750000787 -26.00102293699995926, 30.7584146130000704 -26.00091683299990564, 30.7587753750000843 -26.00081563199995571, 30.76000302900007455 -26.00031487799992647, 30.76071377600004553 -26.00010488499992789, 30.76131145000005063 -25.99987873799994986, 30.76231295700006285 -25.99965259199990442, 30.76286217000006218 -25.99958797899995488, 30.76357291700009 -25.99950721099992279, 30.76434827800005678 -25.99942644499992639, 30.76522055800006683 -25.99929721799992421, 30.76588284400008888 -25.99929721799992421, 30.76641590500008761 -25.99942644499992639, 30.76709434400004284 -25.99957182499991859, 30.76835430500005941 -25.99994335199994566, 30.76933965900008161 -26.00028257199994641, 30.77034727900007738 -26.00058139199995821, 30.77059711400005426 -26.00065548199995646, 30.7721408260000544 -25.99866817299994182, 30.7722792410000352 -25.99843033299993067, 30.77289652600006775 -25.99853793299990912, 30.77338174100003698 -25.99839340099993024, 30.77382566000005681 -25.99843469599994705, 30.77423861000005445 -25.99840372599993543, 30.77452767500005848 -25.99844501999990598, 30.77489932700007103 -25.99862052199995333, 30.77435217000004286 -25.99929156499990768, 30.77394954600003985 -25.99965289599992957, 30.77359853900009057 -26.00002454999992096, 30.77407343000004403 -26.00032393699990507, 30.77472382400003426 -26.00054073599994808, 30.77521936400006553 -26.00072656199995436, 30.77560134200007269 -26.00074720899993963, 30.77607623300008299 -26.00078850499994587, 30.7762104410000461 -26.00084012499991104, 30.77633432600003971 -26.00098465599995734, 30.77648918200003436 -26.0010775699999499, 30.77674727500004792 -26.0010878929999194, 30.77690213100004257 -26.00104659799990259, 30.77719119500005718 -26.00111886399992045, 30.77746993700003486 -26.00121177899995928, 30.77777964800003474 -26.00110854099995095, 30.77799644700007775 -26.00099497999991627, 30.77814097800006721 -26.00094336099994052, 30.77846101400007228 -26.00117048299995304, 30.77888428600005 -26.00125307299992983, 30.77936950100007607 -26.00141825199995083, 30.7796688890000496 -26.0014595469999108, 30.7799682780000694 -26.00137695699993401, 30.78030896000007033 -26.0010775699999499, 30.78068061500005115 -26.00080915299992057, 30.78067029100003538 -26.00064397299991015, 30.78061867200005963 -26.00050976399995761, 30.78070126200003642 -26.00034458499993661, 30.78083547000005638 -26.00017940599991562, 30.78092838400004894 -26.00000390299993569, 30.78096967900006575 -25.99985936999991054, 30.78096967900006575 -25.99967354199992542, 30.78093870800006471 -25.99948771599991915, 30.78084579300008272 -25.99936383099992554, 30.78077352800005428 -25.99921929899994666, 30.78077352800005428 -25.99904379599990989, 30.78074255700005324 -25.99893023599992148, 30.78076320400003851 -25.99884764499995526, 30.78072190900007854 -25.99868246499994484, 30.78079417600008583 -25.99836242999992919, 30.78115550700005087 -25.99806304199995566, 30.78152715900006342 -25.99820757399993454, 30.7817852530000664 -25.99819724999991877, 30.78218787800005884 -25.99813530799991668, 30.78236338300007446 -25.99835210599991342, 30.78238403000005974 -25.99862052199995333, 30.78239435300008608 -25.99901282299992999, 30.78242532300004086 -25.99948771599991915, 30.78233241100008399 -25.9999109879999537, 30.78256985600006601 -25.99997293099994522, 30.78270406500007539 -26.00021037599992724, 30.78282794900007957 -26.00089174199990794, 30.78255953200005024 -26.00200670499992839, 30.78223949700003459 -26.00200670499992839, 30.78171298700004854 -26.00191379199992525, 30.78107291600008466 -26.00205832299991471, 30.78076320400003851 -26.00219253199992409, 30.78056705400007331 -26.00228544599991665, 30.7808148230000711 -26.00278098399991222, 30.78087676500007319 -26.00298745799995004, 30.78100064900007737 -26.00323522799993725, 30.7811245350000604 -26.00337975999991613, 30.78133101000008764 -26.00364817699994546, 30.78156845500006966 -26.0038856229999169, 30.78172331100006431 -26.00423662799994418, 30.78190913800006001 -26.00436051399992721, 30.78211561200004098 -26.00461860699994077, 30.78236338300007446 -26.00483540499993751, 30.78242532300004086 -26.00515544099994258, 30.78227046800003563 -26.00536191499992356, 30.78209496500005571 -26.00552709499993398, 30.78204334600007996 -26.00567162699991286, 30.78237370500005454 -26.00609489999993684, 30.78244597200006183 -26.00639428799991038, 30.78224982100005036 -26.00680723799990801, 30.78174395800004959 -26.00710662499994896, 30.78104194500008362 -26.0070240339999259, 30.78080450000004475 -26.00743698399992354, 30.78063932000003433 -26.0075092499999414, 30.78056705400007331 -26.00776734299995496, 30.78041219800007866 -26.00802543699995795, 30.7803399320000608 -26.00822158699992315, 30.78029863600005456 -26.00839709099994934, 30.78027799000005871 -26.00860356399994089, 30.78022637100008296 -26.00886165799994387, 30.78005086700005677 -26.00901651399993852, 30.77992698200006316 -26.00932622599992783, 30.77971018400006642 -26.00960496599992666, 30.77946241500006863 -26.00981143999990763, 30.77961727100006328 -26.01020374299992, 30.77993673800006036 -26.01056232799993495)))</t>
+  </si>
+  <si>
+    <t>Malahleka SP</t>
+  </si>
+  <si>
+    <t>Malahleka</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((31.00833302600005936 -26.07266262899992171, 31.00751054300008036 -26.0731025629999067, 31.00718928800006324 -26.07334350299993275, 31.00705293900006154 -26.07402524699995183, 31.00698850300005915 -26.07434742299994923, 31.00670740700007855 -26.07539149999990968, 31.00598458500007837 -26.07619463499992207, 31.00544921100004103 -26.07667902099990442, 31.00542760500007944 -26.07677470699991318, 31.00541039700004831 -26.07682878799994342, 31.00530030600003784 -26.0768278139999552, 31.0051709480000568 -26.07683629799993241, 31.00503310700008797 -26.07682145099994386, 31.00488042200004202 -26.07678964399991628, 31.00449022600008675 -26.07671117999990429, 31.00365894000003664 -26.07652032299995426, 31.00354654500006291 -26.0764863929999251, 31.00349989300008247 -26.07644822099990733, 31.00344263500005582 -26.07638248199992859, 31.00315210900004104 -26.07570388099992442, 31.00265588300004538 -26.07465204999994057, 31.00264290600006234 -26.07462617799990312, 31.00203208300007418 -26.07486154099990472, 31.00167532200003961 -26.07501721899990343, 31.00042989700006046 -26.07548425299995642, 30.99979421400007595 -26.07572425699993346, 30.99957366900008537 -26.07582155499994769, 30.999430966000034 -26.07589290599992182, 30.997955690000083 -26.07641088499991611, 30.99819008300005407 -26.07595381999993833, 30.99848298700004534 -26.07534360199991852, 30.99869046100008063 -26.07483102099990901, 30.99884141400008275 -26.07444062699994447, 30.99904438700008313 -26.07391569499992556, 30.99931288200008339 -26.07325665999991315, 30.99955789900008085 -26.07275641799992627, 30.99960578600007466 -26.07265864699991198, 30.99984987300007333 -26.07204843099992786, 31.000093960000072 -26.07159686999995074, 31.00031363800007966 -26.07104767499993159, 31.00053331500004106 -26.07060831899991626, 31.00075299400003814 -26.07027880199990477, 31.0009726720000458 -26.06990046799995753, 31.00122896200008427 -26.06961976699994921, 31.00150966300003574 -26.06924143299994512, 31.00185138400007645 -26.06888750699994262, 31.00226633200009019 -26.0685579889999417, 31.00255923600008146 -26.06869223799992596, 31.0027667100000599 -26.06888750699994262, 31.00303520500006016 -26.0691560029999323, 31.00315724900008263 -26.06935127199994895, 31.00341354000005367 -26.06959535899994762, 31.00375526100003754 -26.06988826299993889, 31.00409698200007824 -26.07009573699991734, 31.00420682300006092 -26.07026659699994298, 31.00436547900005735 -26.07048627399990437, 31.00463397500004703 -26.07075477099994032, 31.00491467300008708 -26.07091342699993675, 31.00515876000008575 -26.0710720839999226, 31.00530521200005296 -26.07121853599994665, 31.00548827800008667 -26.07130396599990263, 31.00570795500004806 -26.0714260099999251, 31.00595204200004673 -26.0711453099999062, 31.00629376300008744 -26.07115751299994599, 31.00678193700008478 -26.07115751299994599, 31.00711145400003943 -26.07115751299994599, 31.00739215500004775 -26.07109649199992418, 31.0079901670000595 -26.07096224499991877, 31.0082220500000858 -26.07116971799990779, 31.00838070600008223 -26.07126735399992867, 31.00860038500007931 -26.07153584999991836, 31.00877124400005869 -26.07182875199993077, 31.00863699700005327 -26.07209724899990988, 31.00830748000004178 -26.072573216999956, 31.00833302600005936 -26.07266262899992171)))</t>
+  </si>
+  <si>
+    <t>Nhlaba SP</t>
+  </si>
+  <si>
+    <t>Nhlaba</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.90629029100006164 -26.08175850099991067, 30.90638714700008904 -26.08209750199995369, 30.90675843500008568 -26.08214593099995682, 30.90719429300008869 -26.08246878899990406, 30.90704900800005817 -26.08293693399991753, 30.90650014800007739 -26.08306607699995538, 30.9053862850000769 -26.08324364899993952, 30.90524100000004637 -26.08343736499995202, 30.90514414300008639 -26.08367950799993196, 30.90485924800003659 -26.08378924599992388, 30.90488931800007322 -26.08415008099990473, 30.9049344230000429 -26.08445077399994716, 30.90506973400005108 -26.08479657299994869, 30.90519001200004823 -26.08506719799993334, 30.90523511600008533 -26.08542803199992477, 30.90522008200008486 -26.08578886499992677, 30.90524181300008877 -26.085998932999928, 30.90541337000007616 -26.08605611799993085, 30.90571174100006147 -26.08626124899990373, 30.90586092700004883 -26.08639178599992192, 30.90615929800003414 -26.08639178599992192, 30.90653226200004156 -26.08642908299992769, 30.90668144800008577 -26.08655961999994588, 30.90681198500004712 -26.08689528799993695, 30.90701711500008741 -26.08739878899990572, 30.90705441200003634 -26.08792093899995734, 30.90703576400005659 -26.08814471799990997, 30.9072222460000603 -26.088349846999904, 30.9072222460000603 -26.08855497799993373, 30.9072222460000603 -26.08872281199995768, 30.90737143200004766 -26.08887199799994505, 30.90755791400005137 -26.08903983199991217, 30.90765115500005322 -26.08922631299992645, 30.90783763700005693 -26.08945009199993592, 30.90791223000007903 -26.08959927899991271, 30.9081919530000846 -26.08967387099994539, 30.90839708300006805 -26.08967387099994539, 30.90882599200006098 -26.08982305499995391, 30.90914301100008288 -26.09014007599995466, 30.90946003100003736 -26.09043844699993997, 30.91000082900006873 -26.09043844699993997, 30.91041109000008191 -26.09041979899990338, 30.91072810900004697 -26.09041979899990338, 30.91093323900008727 -26.09043844699993997, 30.91186564900004896 -26.09066222699993887, 30.91235050300008425 -26.0908673559999329, 30.91270481900005507 -26.09092330099991841, 30.91315237500003832 -26.09116572799990763, 30.91369317400005912 -26.09140815399990743, 30.91447639900007971 -26.09114707899993846, 30.91477477100005444 -26.09148274699992953, 30.91507314100005033 -26.09198624799995514, 30.91494260400008898 -26.09235921299995198, 30.91486801100006687 -26.09263893599995754, 30.91468153000005259 -26.0929559549999226, 30.91464423300004682 -26.09347810499991738, 30.91477477100005444 -26.09377647599990269, 30.91492395600005239 -26.09398160599994299, 30.91520367900005795 -26.09433592299990323, 30.9156139390000817 -26.09482077599994909, 30.91643446000006179 -26.09538022199990337, 30.91714309200006028 -26.0956972419999147, 30.91768389000003481 -26.0958837239999184, 30.91807550300006824 -26.09599561299995685, 30.9184671150000554 -26.0961261499999182, 30.91902656100006652 -26.09638722499994401, 30.91938087600004792 -26.09670424599994476, 30.91934358200006727 -26.0970958569999425, 30.91910115400008863 -26.09769259999990254, 30.91878413500006673 -26.09825204599991366, 30.91867224500003886 -26.09858771399990474, 30.91850441000008232 -26.0989420299999324, 30.91820604000008643 -26.09933364299990899, 30.91794496500006062 -26.09972525399990673, 30.91757200100005321 -26.10011686599995073, 30.9173855190000495 -26.10034064499990336, 30.91708714800006419 -26.10067631299995128, 30.9167141850000462 -26.10104927699995869, 30.91667688700005101 -26.10151548199991112, 30.91652770100006364 -26.10190709499994455, 30.91635986800008595 -26.10237329999995382, 30.9160614970000438 -26.10278355999992073, 30.91578177200005939 -26.10315652499991756, 30.91565123700007689 -26.10352948899992498, 30.91552069800007985 -26.10388380499995264, 30.91531556800003955 -26.10423812099992347, 30.91511043800005609 -26.10448054699992326, 30.91484936300008712 -26.10459243699995113, 30.91443910200007394 -26.10455513999994537, 30.91376776700008122 -26.10442460299992717, 30.91335750600006804 -26.10442460299992717, 30.91290994900003852 -26.10433136199992532, 30.91261157800005321 -26.10448054699992326, 30.91242509600004951 -26.10500269699991804, 30.91201483500003633 -26.10558079199995518, 30.91151133400006756 -26.10539430899990521, 30.91151133400006756 -26.10479756699993459, 30.91126890700007834 -26.10477891799990857, 30.91095188800005644 -26.10470432599993273, 30.91028055200007429 -26.10399569499992367, 30.90998218100008899 -26.10386515599992663, 30.90957192000007581 -26.10367867399992292, 30.90904977100007045 -26.10351084099994523, 30.90847167600009016 -26.10326841399995601, 30.90809871200008274 -26.10306328399991571, 30.90781898900007718 -26.10306328399991571, 30.90705244100007576 -26.10209393799993904, 30.9057672270000694 -26.10103223799995931, 30.90520843800004513 -26.0999984769999287, 30.90442613200008282 -26.0990764749999471, 30.90294533900004126 -26.09742804399991201, 30.90224685200007571 -26.0965060419999304, 30.90149248700004136 -26.09443852099991545, 30.901162753000051 -26.09323499399994262, 30.90109257900007833 -26.09324749999990445, 30.90088115400004654 -26.09324749999990445, 30.90076275500007341 -26.09329824199994619, 30.90066127000005736 -26.0933828119999589, 30.90055132900005219 -26.09356886699993083, 30.9002553330000751 -26.09328978499991081, 30.89991705100004538 -26.09285001999995757, 30.89964642600006073 -26.09253710899992029, 30.89955339800008005 -26.09258785199995145, 30.89932505900003434 -26.09262167799994359, 30.89907134800006361 -26.09270624899994573, 30.89880072300007896 -26.09243562399990424, 30.89872460900005535 -26.09228339799994956, 30.89870769500004144 -26.09204660199992531, 30.89882609400007141 -26.09188591699995641, 30.89896140600006902 -26.09168294799991372, 30.89897832000008293 -26.09150535199995602, 30.89891066400008413 -26.09141232299992907, 30.89861466800005019 -26.09091335799990929, 30.89834404300006554 -26.09046513499993125, 30.89835250000004407 -26.09036365099990462, 30.89850472700004502 -26.09021142499994994, 30.8987499800000478 -26.08994925699994383, 30.8988768360000563 -26.0897547439999471, 30.89908826200007752 -26.08949257599994098, 30.89939271500008999 -26.08918812299992851, 30.89944345700007489 -26.08904435399995236, 30.89947728500004587 -26.08879064299992478, 30.89943500000003951 -26.08849464599995827, 30.89928277300003856 -26.08804642499995907, 30.89885992200004239 -26.08752208699991115, 30.89835250000004407 -26.08685398199992278, 30.89768171400004348 -26.08591354399993634, 30.89737249600005953 -26.08550125199991498, 30.89683136500008231 -26.08529510699992215, 30.89629023400004826 -26.08529510699992215, 30.89551719000007779 -26.08526933999991115, 30.89529234700006555 -26.08500361599993767, 30.89523374000003741 -26.08493435399992677, 30.89446069600006695 -26.08467667399992251, 30.89358457900004851 -26.08465090499993266, 30.89219309900005328 -26.0839551639999172, 30.89059547400006522 -26.08302751099995476, 30.88964205200005608 -26.08449629599994068, 30.88822701300006202 -26.0836843869999484, 30.88800340900007768 -26.08406558599995151, 30.88782468900006961 -26.08452231399991206, 30.88754668100006029 -26.08495918499994559, 30.88716938400006029 -26.0854556269999307, 30.88679208600007087 -26.08585278299995025, 30.88631550000008019 -26.08624993799992353, 30.88554104900003949 -26.08664709399994308, 30.8851041780000628 -26.08690524299993285, 30.88478645400005007 -26.08704424699993751, 30.88438929900007679 -26.0870839619999515, 30.88391271200003985 -26.0870839619999515, 30.88331698100006406 -26.08700453199992353, 30.88260210200007805 -26.08682581199991546, 30.88222480500007805 -26.08674638099995491, 30.88180779300006407 -26.08684566999994559, 30.88180779300006407 -26.08559463299991421, 30.88196665500004201 -26.08489961099991206, 30.88284039600006281 -26.08511804599993411, 30.88345598500006872 -26.08531662399991546, 30.88452830400007088 -26.08515776199993752, 30.88542190200007553 -26.08501875699994343, 30.88583891500007894 -26.08478046499993752, 30.88603749100008145 -26.08442302499992138, 30.88620013400003472 -26.08423793499991916, 30.88635752600004025 -26.08409711099994865, 30.88654805300006956 -26.08397285399991006, 30.88673858000004202 -26.08387344799990615, 30.88687112100006971 -26.08369120499992277, 30.88697052600008419 -26.08362493499993207, 30.88704508100005341 -26.08345925899993745, 30.8871444860000679 -26.08335985399992296, 30.88743441800005485 -26.08328529999994316, 30.88760009400004947 -26.08318589499992868, 30.88775748700004442 -26.08312790799993763, 30.88803913500004228 -26.08301193499994497, 30.88813025600006767 -26.0829705159999321, 30.88850686200004247 -26.08294864699990967, 30.88971935700004678 -26.08251214799992113, 30.89023472000008042 -26.0811206679999259, 30.89080161900005805 -26.08063107399993896, 30.89152312700008451 -26.08039915999995628, 30.89209002600006215 -26.07960034799992854, 30.89270846200008691 -26.0798322609999218, 30.89312075200007257 -26.08032185499990874, 30.8933268970000654 -26.08078568199994152, 30.89355881100004808 -26.08114643699991575, 30.89379072400004134 -26.08153295899995783, 30.89430608600008554 -26.08184217699994178, 30.89479568200005133 -26.08189371299994264, 30.89549142200007736 -26.0815071909999574, 30.89657368400008863 -26.08070837799994024, 30.89626446700003726 -26.08034762499994486, 30.89623869800004741 -26.07985802899992223, 30.89624007000008987 -26.07985713699991948, 30.89617924400005222 -26.07971759299994119, 30.8959646310000835 -26.07905944799995268, 30.89577863400006663 -26.07868745199994009, 30.89570709600008058 -26.07853007099993192, 30.89575002000003678 -26.07808653799992271, 30.89583586400004833 -26.07768592899992655, 30.89585017100006326 -26.0774570089999429, 30.89595032300007915 -26.07714224399995828, 30.89557832900004541 -26.07662717399995245, 30.89527787100007572 -26.07622656399991001, 30.89500602900005788 -26.07574010899992345, 30.89477710900007423 -26.07528226899995616, 30.89467695600006891 -26.07482442899993202, 30.89473418600005061 -26.07452397099990549, 30.8950775660000545 -26.07423782199992957, 30.89530648600003815 -26.074023208999904, 30.89552109900006371 -26.07379428999990978, 30.89553791700006968 -26.07377054399995586, 30.89553795000006176 -26.07377049999990959, 30.89564968100006581 -26.0736127589999569, 30.89576432600006228 -26.07345090899991646, 30.89613632100008545 -26.07315045199993619, 30.89647970100008934 -26.07289291699993328, 30.89678015900005903 -26.07270691899992698, 30.89723799900008316 -26.07249230699994769, 30.89739538100008076 -26.0722633869999072, 30.89773876100008465 -26.07192000699990331, 30.89798198900007264 -26.07159093399991434, 30.89819660200004137 -26.07137632199993504, 30.89836829100005389 -26.07111878699993213, 30.89845413600005486 -26.07086125199992921, 30.89852567300005148 -26.07054648699994459, 30.8986258260000568 -26.07030325999994602, 30.89869770100006008 -26.07000218299992866, 30.89876898600005006 -26.06990238399993132, 30.89882601300007536 -26.06975981399995135, 30.89891155500004061 -26.0695459609999034, 30.89901135300004853 -26.06944616199990605, 30.89919669300007854 -26.06934636399995497, 30.89926797900005795 -26.06901845499993442, 30.89928223500004378 -26.06867628799994918, 30.89882601300007536 -26.06816303799990919, 30.89875472800008538 -26.06787789899993868, 30.89875472800008538 -26.06756424699995023, 30.89875472800008538 -26.06739316299990605, 30.89862641600007009 -26.06713653899993233, 30.89834127700004274 -26.06693694099993763, 30.89794208300008904 -26.06659477499994182, 30.8977424870000732 -26.06618132399995602, 30.89758566000006113 -26.06579638699992074, 30.89741457600007379 -26.06546847699991076, 30.89750011800003904 -26.06526887899991607, 30.89758566000006113 -26.06514056799994705, 30.89768545800006905 -26.06494096999995236, 30.89777100000003429 -26.06476988599990818, 30.89802762500005429 -26.06455603299991708, 30.89809890900005485 -26.06447049199994126, 30.89824147900003481 -26.06424238199991805, 30.89839830400006804 -26.06411406899991334, 30.89856938800005537 -26.06391447099991865, 30.89884027000005062 -26.06375764499995284, 30.89895432500009065 -26.06367210299993076, 30.89903986700005589 -26.06350102099992228, 30.89912540900007798 -26.06332993699993494, 30.89931075000004057 -26.06321588099990549, 30.89946757400008437 -26.06311608299995441, 30.89965291500004696 -26.06291648599994915, 30.89980974200005903 -26.06268837499993651, 30.89995231100004958 -26.06260283299991443, 30.90008062300006486 -26.06253154799992444, 30.90013765100007959 -26.0623889789999339, 30.9002659640000843 -26.06214661099994601, 30.90040853300007484 -26.06190424299995811, 30.90044909100004134 -26.06186996899992891, 30.90075476700008039 -26.06247000199994091, 30.90104042700005493 -26.06284587199991165, 30.90113063600006171 -26.06298118399990926, 30.90128098300004922 -26.06323677399990402, 30.90140126100004636 -26.06347732999995515, 30.90164181600005122 -26.06376298999992969, 30.90180719800008546 -26.0640636839999047, 30.90195754600006239 -26.06430423999995583, 30.90212292800003979 -26.06463500399991062, 30.90239355300008128 -26.06517625399993676, 30.90255893600004811 -26.06547694799991177, 30.90275438600008329 -26.0656723999999258, 30.90291976800006069 -26.06592798999992056, 30.90305508100004772 -26.06627378899992209, 30.90326556600007279 -26.06649930999992648, 30.90356626100003723 -26.06670979599994098, 30.903716609000071 -26.06693531699994537, 30.90407744100008358 -26.06716083699990349, 30.9044683450000548 -26.06725104599991027, 30.90463372700008904 -26.06755174099993155, 30.90479910900006644 -26.06797271199991428, 30.90463372700008904 -26.06846885899994959, 30.90448338000004469 -26.06881465799995112, 30.90475400500008618 -26.06934087299993053, 30.90461869100005288 -26.06973177599991232, 30.90449841600008085 -26.0702279219999582, 30.90460365800004183 -26.07069399899995688, 30.90454351900007168 -26.07119014499994591, 30.90424282300006098 -26.0715960829999176, 30.90422778900006051 -26.07192684699992924, 30.90422778900006051 -26.07239292399992792, 30.90400226900004554 -26.07281389499991064, 30.9035061230000565 -26.07321983299993917, 30.90319039300004533 -26.07361073599992096, 30.90323549700008243 -26.0741519859999471, 30.90307819800005973 -26.07462388499993722, 30.90335227900004611 -26.07505918899994413, 30.90362670800004707 -26.0754143329999124, 30.90404642500004684 -26.07567262099991012, 30.90411099600004263 -26.07601162199995315, 30.90401413800003638 -26.07636676599992143, 30.90419171000007736 -26.07667348099994342, 30.90464371200005189 -26.07686719699995592, 30.90504728500008014 -26.07704476899994006, 30.90525714400007473 -26.07733534099992312, 30.9052732860000674 -26.07765819899992721, 30.90606429000007438 -26.07775505699993346, 30.90638714700008904 -26.07781962899991868, 30.90625800400005119 -26.07820705899990799, 30.90601586100007125 -26.07841691699991316, 30.90556385900003988 -26.0795146349999527, 30.90599971700004289 -26.07991820799992411, 30.90606959400008691 -26.08058203999991065, 30.90609657500004914 -26.08083835399992267, 30.90625800400005119 -26.08120964199991931, 30.90630643300005431 -26.08151635699994131, 30.90629029100006164 -26.08175850099991067)))</t>
+  </si>
+  <si>
+    <t>Enkhaba SP</t>
+  </si>
+  <si>
+    <t>Enkhaba</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.99379133300004696 -26.12878301899991129, 30.99380235400008132 -26.12878301899991129, 30.9940008750000402 -26.12878301899991129, 30.99423545800004831 -26.12882739899993112, 30.99445102100008853 -26.12894152099994471, 30.99471730300007266 -26.12916976399992564, 30.99492018700004792 -26.12925852499995472, 30.99510404900007643 -26.1293029049999177, 30.99536399300006906 -26.12942970699992884, 30.9954907930000445 -26.12946140699995112, 30.99566831700008152 -26.12945506699992393, 30.99592826000008472 -26.12941702799992072, 30.99602336100008415 -26.12961990799993828, 30.99643546600003674 -26.12977207199992336, 30.99649252700004354 -26.1301080939999224, 30.9964176870000756 -26.13012221599990426, 30.99615650300006564 -26.13017149699993524, 30.99616284300003599 -26.13028561799990257, 30.99585217900005318 -26.13038071899995884, 30.99594728000005261 -26.13086256499991578, 30.99604109700004528 -26.13134337799994, 30.99623617700007117 -26.1319645919999175, 30.99592563500004871 -26.13206662699991512, 30.99588127200007648 -26.13196015499994473, 30.99577480100003868 -26.13158306899993022, 30.99513153600008764 -26.13168066799994449, 30.99487866700007999 -26.13171172199992043, 30.99463023400005568 -26.13176495799990562, 30.99430638300003693 -26.13183593899992729, 30.99395591600006128 -26.13191135599993231, 30.99364981000007901 -26.1319645919999175, 30.99341024900007824 -26.1319912099999101, 30.99313519800006134 -26.13203557299993918, 30.99289120100007722 -26.13207549899993865, 30.99262945900005661 -26.13212429899994049, 30.99229539400005251 -26.13218130199993539, 30.99172478600007707 -26.1322066629999199, 30.99160432500008255 -26.1321559419999403, 30.99143314300005159 -26.13205449999992425, 30.99121124000004102 -26.13208620099993595, 30.99106541700007256 -26.13208620099993595, 30.99088155600009031 -26.13209254199995257, 30.99067867300004764 -26.13207352099993841, 30.99046944900004519 -26.13207352099993841, 30.99032362800005558 -26.13210522099990385, 30.99019682700009071 -26.13216228099992122, 30.99001296400007277 -26.13217496199990819, 30.98984812300005842 -26.13219398199993293, 30.98965792000007013 -26.13227006299990762, 30.98942967700008921 -26.13232078399994407, 30.98933457600008978 -26.13206083999995144, 30.98930287500007807 -26.13185161699993841, 30.98929019500008053 -26.13166141499993955, 30.98926483500008544 -26.13145853299994315, 30.98929653400006146 -26.1313380709999592, 30.98929653400006146 -26.13119224899992332, 30.98927117600004522 -26.13100838699995165, 30.9892458150000607 -26.13060262199991257, 30.9891950940000811 -26.13007005499991919, 30.98917607400005636 -26.12961356899995735, 30.98911901200006014 -26.12887811999991072, 30.98911270000007789 -26.12851825899991809, 30.98951843800006145 -26.12855477499994095, 30.9898417820000418 -26.12858647599995265, 30.99019048700006351 -26.12861817599991809, 30.99038702900008957 -26.12861817599991809, 30.9906469730000822 -26.12863085699990506, 30.99095129600004839 -26.12860549599992055, 30.99128732100007255 -26.128592815999923, 30.99175648700008878 -26.12864353799994888, 30.99216225200007102 -26.12866889599990827, 30.99266945800007989 -26.12869425699994963, 30.99301816300004475 -26.12869425699994963, 30.99334150800007137 -26.12871961799993414, 30.9937219120000691 -26.12878301899991129, 30.99379133300004696 -26.12878301899991129)))</t>
+  </si>
+  <si>
+    <t>Kalwerskraal SP</t>
+  </si>
+  <si>
+    <t>Kalwerskraal</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.90188827300005414 -26.16524254199993038, 30.90224995200009062 -26.16588243899991539, 30.90250747600003933 -26.16639748199992255, 30.90276499800006604 -26.16654055099991183, 30.90322281300007035 -26.16634025499990912, 30.90356617600008349 -26.16611134599992283, 30.9043037740000841 -26.16597149699992997, 30.90631011700008912 -26.16612011399990934, 30.90730991100008396 -26.16653894699993543, 30.90779039600005262 -26.16687305499993954, 30.90780582600007165 -26.16705821199991533, 30.90794469400003663 -26.16724336999993739, 30.90796012500004508 -26.16742852699991317, 30.90800641400005588 -26.16759825399992678, 30.90805270100008784 -26.16778341199994884, 30.90808356200005846 -26.16799942899990583, 30.90811442300008594 -26.16809200799991686, 30.90820700000006127 -26.16812286699990864, 30.9082532900000615 -26.1683543139999415, 30.90831500900003448 -26.16850861199992551, 30.90842301800006453 -26.16855490199992573, 30.90866989400007014 -26.16852404199994453, 30.90883962200007318 -26.16864747999994734, 30.90904020900006799 -26.16872462899993934, 30.90931794600004423 -26.16878634799991232, 30.90951853100006019 -26.16878634799991232, 30.90978083900006368 -26.16877091899993957, 30.91007400500006952 -26.16881720799995037, 30.9102283020000641 -26.16889435699994237, 30.91045974900004012 -26.16886349699990433, 30.91058318800008919 -26.16892521599993415, 30.91096893200005979 -26.16904865499992638, 30.91113866000006283 -26.16903322499990736, 30.91132381700003862 -26.16914123299994799, 30.91152440600006912 -26.1692492419999212, 30.91163241300006348 -26.16931096099995102, 30.91180214100006651 -26.16940353999990521, 30.91207987700005333 -26.16931096099995102, 30.91215702600004533 -26.16921838299992942, 30.91231132400008619 -26.1692492419999212, 30.91255819900004553 -26.16926467199994022, 30.91263534900008381 -26.16923381199995902, 30.91274335800005701 -26.169295530999932, 30.91285468300003458 -26.16955529099993782, 30.91211576700004571 -26.17096595299994988, 30.91226410600006602 -26.17382150799994633, 30.91222702100003517 -26.17452612499994302, 30.91193034100007253 -26.1759353589999364, 30.91222702100003517 -26.1765287209999542, 30.91311706400006187 -26.17830880699995078, 30.91287934000007454 -26.17822018899994418, 30.91250608300003933 -26.17809772699990845, 30.91236600700005965 -26.17805411099993762, 30.91206153100006304 -26.17795429599993895, 30.91186777300003996 -26.17788887199992587, 30.91169666300004337 -26.17784273899991376, 30.91146432300007518 -26.17776892699993141, 30.91112629400004153 -26.1776573689999168, 30.91098454100006165 -26.17761039799995615, 30.91073542400005181 -26.1775315529999375, 30.91035713600007284 -26.17740573599991194, 30.91021118900005149 -26.17735624799991001, 30.9099763310000526 -26.17728159699993284, 30.90965591800005541 -26.17717674999994415, 30.90946970900006363 -26.17711635699993167, 30.90920968900007892 -26.17703164199991761, 30.90892801900008635 -26.17694578499992986, 30.9088854990000641 -26.17716518699995731, 30.90870609000006652 -26.17767317699991736, 30.90863553600007663 -26.17787072799990256, 30.9085932030000663 -26.17792918699990423, 30.9084722530000704 -26.17809851699990986, 30.90835735100006332 -26.1782275309999477, 30.90827873300008832 -26.17832025899991777, 30.90820616300004531 -26.17846136699995441, 30.90813762500005168 -26.17856618999991269, 30.9080993240000339 -26.17860045899993793, 30.90805296000007729 -26.17870931399994561, 30.90804288100008534 -26.17878994799991688, 30.90811141800008954 -26.17888469199994006, 30.90817189500006634 -26.17907821199992213, 30.90813762500005168 -26.17932212799991021, 30.90812222000005249 -26.17958820599994851, 30.90799956500006829 -26.17999000699995804, 30.90794458300007364 -26.18076823199993441, 30.90788114000008591 -26.18097124899992423, 30.90768235400008734 -26.18133498499992129, 30.90736091300004773 -26.18157606599993414, 30.90719173300004741 -26.1816521969999485, 30.90681953900008239 -26.18171563799995738, 30.90634160500007965 -26.18173255699991842, 30.90589750900005583 -26.18166065599990588, 30.90563951000007137 -26.18163950799993245, 30.90529692100005832 -26.18158875399990393, 30.90501777500008984 -26.18150839399993401, 30.9046328910000625 -26.18158029499994655, 30.90390964800008078 -26.18180445799993095, 30.90364319000008209 -26.18170294999993075, 30.90300030600008085 -26.18153799999993225, 30.90295221700006323 -26.18175700799992001, 30.90291865700004337 -26.18196955399992021, 30.90287391100008563 -26.18243659499995601, 30.90284035200005519 -26.18250371499993889, 30.90270890700008977 -26.18255125899992208, 30.90253831200004697 -26.18272744799992324, 30.90210762800006705 -26.18311058999995566, 30.90184474200003706 -26.1834322049999173, 30.90163219700008312 -26.18372585299994171, 30.90151473800005988 -26.18377339599993547, 30.90146999100005587 -26.18386288899995407, 30.90143922700008261 -26.1840139069999509, 30.90136371800008419 -26.18413695999993251, 30.90127981800003454 -26.18427679299992406, 30.90118193500006782 -26.18437187999995786, 30.9010225260000766 -26.18448374599995532, 30.90089108300009002 -26.18457883199994285, 30.90080159100006085 -26.18463196799990556, 30.90067574100004322 -26.18469908799994528, 30.90055475800005524 -26.18474591199992574, 30.90046603500007905 -26.18481534699992608, 30.90038502700008394 -26.18501593699994601, 30.90017672100003665 -26.18524738899992599, 30.9000841410000362 -26.18523581699992064, 30.899937555000065 -26.18515095099991186, 30.89969067400005542 -26.18504679799991663, 30.89950551300006509 -26.18510851899992531, 30.89938593000005085 -26.18509308999995255, 30.89932806800004528 -26.18502365399990595, 30.89921234300004471 -26.18498507799995423, 30.8990966160000653 -26.18506608599994934, 30.89898474900007841 -26.18515095099991186, 30.89889602500005594 -26.18512780599991174, 30.89877258500007429 -26.18514323599993077, 30.89868386200004124 -26.18518952799990984, 30.89864528700007895 -26.18527439199993978, 30.89860671100007039 -26.18538625999991609, 30.89856042100007016 -26.18543254999991632, 30.89851027300005626 -26.18542869299994891, 30.89839840600006937 -26.18544026499995425, 30.89832125500004167 -26.18550584399991976, 30.89835597300003656 -26.18555213299993056, 30.89839454800005569 -26.1856987189999586, 30.89834825800005547 -26.18582601699995394, 30.89828653800003622 -26.18590702499994904, 30.89816695600006824 -26.18596102999993036, 30.89803580000005923 -26.18599960399990323, 30.89791235800004188 -26.18609604199991736, 30.89791235800004188 -26.18618090899991557, 30.89786606800004165 -26.18636221199994907, 30.89770791000006511 -26.18650108599990745, 30.89690336300003537 -26.18650108599990745, 30.89632068700007039 -26.18681184599995504, 30.89577685700004395 -26.18754990199994381, 30.89534956100004592 -26.18867640699994581, 30.89348499900006573 -26.18747221199993191, 30.89290232400009018 -26.18665646599993124, 30.89197004300007166 -26.18552995999993982, 30.89191465900006506 -26.18553158899993605, 30.89064931200005049 -26.18556880499994577, 30.88948396000006369 -26.18545227099991735, 30.88897897500004319 -26.18498612899992395, 30.88827976400006037 -26.18479190399995105, 30.8873086380000359 -26.1845199889999094, 30.88765824300008944 -26.18401500199991006, 30.88793015900006367 -26.18347117299992988, 30.88835745400007227 -26.18288849699990806, 30.88866821400006302 -26.18226697799991598, 30.88894012900004782 -26.18152892099993778, 30.88870705900006897 -26.18129585099995893, 30.88882359500007624 -26.18098508999992191, 30.88874590500006434 -26.18063548499992521, 30.88851283400003922 -26.18024703499992256, 30.88870705900006897 -26.17970320399990669, 30.88913435500006699 -26.17904283799992982, 30.88925089000008484 -26.17826593699993509, 30.88919685300004403 -26.17783947499992792, 30.88919685300004403 -26.17747891399994842, 30.88934531900008551 -26.17688504899990676, 30.88930290000007517 -26.17673658299992212, 30.88913322500008007 -26.1765669069999376, 30.88906959600006985 -26.1762487649999116, 30.88900596800004905 -26.17588820599991095, 30.88904838700005939 -26.17561248199990587, 30.88913322500008007 -26.17537917699991112, 30.88930290000007517 -26.17493377899995721, 30.88938773800003901 -26.17440354199993635, 30.88936653000007482 -26.17425507599995171, 30.88932411000007505 -26.17385209599990503, 30.88949378500007015 -26.17355516399993576, 30.88966346100005467 -26.17338548799995124, 30.8898119270000393 -26.17304613599992535, 30.89000281300008055 -26.17306734599992524, 30.89017248800007565 -26.17289766999994072, 30.89032095500004971 -26.17257952799991472, 30.89032095500004971 -26.1722401769999351, 30.89053304900005514 -26.17177356899992446, 30.89103345500006981 -26.17154791499990552, 30.89123374900003682 -26.17143346099993551, 30.8917201790000604 -26.17137623399992208, 30.89192047200003799 -26.17137623399992208, 30.89226383500005113 -26.17137623399992208, 30.89252135700007784 -26.17123316699991165, 30.89286471900004472 -26.17097564499994178, 30.89320808200005786 -26.17080396399995834, 30.89340837600008172 -26.17080396399995834, 30.89375173800004859 -26.17097564499994178, 30.89409510100006173 -26.17080396399995834, 30.89446707600006903 -26.17066089599995848, 30.89495350600003576 -26.17046060199993462, 30.89529686800005948 -26.17023169299994834, 30.89569745800008604 -26.16988833099992462, 30.89581191200005605 -26.16957358299993075, 30.89604082000005292 -26.16911576699993702, 30.89647002300006307 -26.16877240399992388, 30.89675615800007336 -26.16840042799992716, 30.89707090700005665 -26.16831458699994073, 30.89738565600003994 -26.16794261199993343, 30.89761456300004738 -26.16762786299995014, 30.89815822000008438 -26.16702697899995655, 30.89875910400007797 -26.16679807099990285, 30.89913108000007469 -26.16668361699993284, 30.89958889600006842 -26.16654055099991183, 30.89987503100007871 -26.16622580099993911, 30.90024700700007543 -26.1659682789999124, 30.90044730200008871 -26.16582521199995881, 30.90070482300006915 -26.16539600999993809, 30.90107679900006588 -26.16551046299991867, 30.90159184300006245 -26.16522432699991896, 30.90187163800004555 -26.16522432699991896, 30.90187797900006217 -26.16522432699991896, 30.90188827300005414 -26.16524254199993038)))</t>
+  </si>
+  <si>
+    <t>Etjelembube SP</t>
+  </si>
+  <si>
+    <t>Etjelembube</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.84473656700004085 -26.21491252299995267, 30.84462361300006705 -26.21523020599994425, 30.84559784300006413 -26.21635268899990479, 30.84621909100007997 -26.21710806999993792, 30.84584493000005523 -26.21734809799994537, 30.84489187900004481 -26.21783521199995448, 30.84568255900006761 -26.21888003999993089, 30.84528015900008313 -26.2191130079999084, 30.84528015900008313 -26.21926125999993928, 30.84498365500007822 -26.21936715499992943, 30.84452477800004999 -26.21939539299995658, 30.84420003500008534 -26.21953658599994696, 30.84453183800007992 -26.2201225349999163, 30.84410120000006827 -26.22030608599993684, 30.84413649800006851 -26.22041904099995691, 30.84426357100005589 -26.22080026199995473, 30.84432710800007271 -26.22115324299994654, 30.84446721600005503 -26.22144046599993317, 30.84434759600003417 -26.22144412699992699, 30.84430580300005431 -26.22145031899992773, 30.84428258500008724 -26.22146270099995036, 30.84427175000007537 -26.2215261659999328, 30.84425472300006277 -26.22155712399995764, 30.84422531300003811 -26.22156950699991285, 30.84419280600008051 -26.221606655999949, 30.84416339700004528 -26.22159427199994752, 30.84414791700004344 -26.22157105499991303, 30.84413398700007747 -26.22157260299991322, 30.84412160400006542 -26.22155093099991063, 30.84410302900005263 -26.22151378299992075, 30.84405659300006164 -26.22152152199993225, 30.84401634600004627 -26.22152771399993298, 30.84399932000007993 -26.22152771399993298, 30.84398229400005675 -26.22148591999990686, 30.84395288500007837 -26.22147508499995183, 30.84391573400006337 -26.2214781809999522, 30.8438847770000848 -26.22149985099991909, 30.84388322800003834 -26.22154009599995561, 30.84385846200007109 -26.22153080899994393, 30.8438151210000342 -26.22151687699994227, 30.84377797200005489 -26.22152461799993262, 30.84373308300007466 -26.22156950699991285, 30.84372069900007318 -26.22159117699993658, 30.84373463100007484 -26.22160975199994937, 30.84376404100004265 -26.22161749099990402, 30.84377797200005489 -26.2216391629999066, 30.84377023200005397 -26.22166392799994128, 30.8437671360000536 -26.22170726899992133, 30.8437284390000741 -26.22173048799993467, 30.84372689100007392 -26.22178311599992639, 30.84370522100005019 -26.22183419599991794, 30.84367581100008238 -26.22185896199994204, 30.8436309220000453 -26.22186979899993275, 30.8436185390000901 -26.22189920799991114, 30.8435829370000647 -26.22193480999993653, 30.84353185700007316 -26.22195183599990287, 30.84349470700004758 -26.22196731399992586, 30.84346684400009053 -26.221956478999914, 30.84344207900005586 -26.22191933099992411, 30.84341112100008786 -26.22188837299995612, 30.84337087600005134 -26.22185896199994204, 30.84337087600005134 -26.22181252599995105, 30.84331979500007037 -26.2218078819999505, 30.84327181200006862 -26.22182490799991683, 30.84324704300007625 -26.22181562299994084, 30.84324085300005436 -26.22184193599991886, 30.84319751200007431 -26.2218899209999563, 30.84314797900003668 -26.22188527699995575, 30.84310154200005627 -26.22191778299992393, 30.8430504610000753 -26.22191623499992374, 30.84299938100008376 -26.22192087799993487, 30.84295139600004632 -26.22191778299992393, 30.84289567300004364 -26.22194719399993801, 30.84285387900007436 -26.22197041099991566, 30.84282601700004989 -26.22194719399993801, 30.84277184100005798 -26.22191313799993395, 30.84275326700003461 -26.22190539999991188, 30.84269289900004196 -26.22190075599991133, 30.84266348900007415 -26.22187444199994388, 30.84263098300004913 -26.22183883999991849, 30.84258454600006871 -26.22183419599991794, 30.84252727400007643 -26.22185122299993054, 30.8424746460000847 -26.22186360599994259, 30.84244214000005968 -26.22185896199994204, 30.84242046900004652 -26.22184348399991904, 30.84241892100004634 -26.22182800499990663, 30.84237867600006666 -26.22183883999991849, 30.84236319700005424 -26.22186670199994296, 30.84232759600007512 -26.22188218099995538, 30.84227651500003731 -26.22188682499995593, 30.84218364300005533 -26.22189765999991096, 30.84215578000004143 -26.22192552199993543, 30.84208612400004768 -26.22193016599993598, 30.84206755000008116 -26.22191468699992356, 30.84204897500006837 -26.22188837299995612, 30.84201337300004298 -26.22188218099995538, 30.8419824160000644 -26.22189920799991114, 30.84194526600003883 -26.22191468699992356, 30.84191121200007046 -26.22191313799993395, 30.8418694190000906 -26.22194409699994821, 30.84182143600008885 -26.22195338399990305, 30.8417440410000836 -26.22195493199990324, 30.84168831500005581 -26.22195802899994987, 30.84165581100006648 -26.22197041099991566, 30.84161711300004072 -26.22198743799992826, 30.84162330400005203 -26.22206947599994464, 30.84158151100007217 -26.22209733799991227, 30.84154900500004715 -26.22210817399991356, 30.84150102100005597 -26.22213139199993748, 30.84147315900008834 -26.22217163699991715, 30.84143668500007607 -26.22221150399991529, 30.84136579300007952 -26.22224123199993073, 30.84133606400007466 -26.22227782199990997, 30.84133606400007466 -26.2223349909999115, 30.84130405000007613 -26.22235785999993141, 30.8412697470000694 -26.22237844099993254, 30.84121029100003852 -26.22237844099993254, 30.8411805620000905 -26.22235557299995889, 30.84115083300008564 -26.22231669699993972, 30.84109594800008836 -26.22228925699994306, 30.84102505900006008 -26.22229382899990924, 30.84101362400008384 -26.22232584499994346, 30.84097932300005596 -26.22236929399991823, 30.8409107170000425 -26.22241731699995171, 30.84086955400005081 -26.22240130999995245, 30.84082610500007604 -26.22240130999995245, 30.84075064000006705 -26.22236471999991636, 30.84074855800008663 -26.22236457199994675, 30.84068661000003431 -26.22236014599991449, 30.84062029200003963 -26.22236700699994572, 30.84054711400005999 -26.22238758899993627, 30.84049420900004179 -26.22240806799993607, 30.84048300400007747 -26.22237628899995343, 30.84044604200005324 -26.22236298199993598, 30.84038838100008206 -26.22234228399992162, 30.84032037100007528 -26.22227575199991634, 30.84021687700004577 -26.2222254829999315, 30.84015921600007459 -26.22218408599991335, 30.84012668900004428 -26.22214712399994596, 30.84011265900005583 -26.22212496899993539, 30.84010699800006705 -26.22200302699991425, 30.84015596800009007 -26.2218634629999201, 30.84022452600004272 -26.22168716999993876, 30.8402637020000725 -26.22155005399991978, 30.84026125400004048 -26.22148149699995656, 30.84023432000003595 -26.22144721699993397, 30.84019269700007726 -26.22141048999992563, 30.84009965300003842 -26.2213835559999211, 30.83954384200006871 -26.22121950599995444, 30.83924512500004766 -26.22115584499994156, 30.83901006800005007 -26.22120726399992918, 30.83885211300008677 -26.22127850499992974, 30.83875217400003521 -26.22132312099995488, 30.83863174300006449 -26.22136464799990563, 30.83852377100004105 -26.22140825299993594, 30.83832859300008522 -26.22147262099991849, 30.83810018900004479 -26.22152868299991724, 30.83612502300007918 -26.22223075899995592, 30.83605070400005843 -26.22226059699994494, 30.83540817100004006 -26.22252040399990847, 30.83532994900008362 -26.22254554599993526, 30.83528804400003764 -26.22254833999994617, 30.83522937900005445 -26.2225176099999544, 30.83500031500005889 -26.22203148299990971, 30.8349969980000651 -26.22202592999991566, 30.83469776900005854 -26.22129758699992408, 30.83452184800006535 -26.22088491499994234, 30.83429331500008175 -26.22033413499991639, 30.83416284700007282 -26.22003909699992619, 30.83441929300005313 -26.21995293599991328, 30.83445555200006538 -26.21993206099995177, 30.83448302000005015 -26.21991008499992404, 30.83450609300007272 -26.21988811199992142, 30.83452916700008473 -26.21985734699995874, 30.83455993000006856 -26.21982658199993921, 30.83458410300005426 -26.21981010099995046, 30.83463354600007733 -26.21976944799990861, 30.8346807920000856 -26.21974966999994194, 30.83472584000008965 -26.21973428999990574, 30.83476099900008194 -26.21971341299990854, 30.83479506000008996 -26.21967935199995736, 30.83482252800007473 -26.21965298199995686, 30.8348337590000483 -26.21961437299995623, 30.83483455800006823 -26.219598666999957, 30.83484333300003755 -26.21956883099994684, 30.83485649700008935 -26.21953987299991695, 30.83488984300004176 -26.21948809799994251, 30.83492143300009047 -26.2194328139999584, 30.8349477590000447 -26.21939420299992207, 30.83496969800006582 -26.21936348899993163, 30.83499163600004067 -26.2193222449999439, 30.83501357400007237 -26.21927398099995798, 30.83502410500005908 -26.21922834999992347, 30.83502761500005818 -26.21918183999991925, 30.83502147200005084 -26.21912304399995719, 30.83501620700008061 -26.21905020999992075, 30.83501971700007971 -26.21899843599993574, 30.83502586100007647 -26.21896157999992738, 30.8350074300000756 -26.21891945799990253, 30.83499602400007689 -26.21888611199995012, 30.83498812600004158 -26.21884750099991379, 30.8349837380000622 -26.21880625699992606, 30.83513830700007929 -26.21877450099992757, 30.83516122400004633 -26.21872866699993665, 30.83522997600005056 -26.21870116599990297, 30.83532164600006809 -26.21871033299993314, 30.83532622900008846 -26.21865533099992263, 30.83532622900008846 -26.2185911629999282, 30.83535831300008567 -26.21853616099991768, 30.83541789800005972 -26.21848574299991697, 30.83550498400006745 -26.21842157499992254, 30.83551873400006116 -26.21838490699991553, 30.83556915200006188 -26.21836198899995907, 30.8356470720000857 -26.21831157099995835, 30.83577082500005417 -26.21829323699995484, 30.83580290900005139 -26.21825656999993726, 30.83587624500006541 -26.21827490399994076, 30.83600458300008995 -26.21833448899991481, 30.83604583300007107 -26.21836198899995907, 30.83611000100006549 -26.21834365599994499, 30.83620625400004656 -26.2183161549999113, 30.83626125600005707 -26.21835282299991832, 30.83624484600005644 -26.21836940999992294, 30.83624484600005644 -26.2183992309999212, 30.83627918500008036 -26.21842724199990471, 30.83632255900005248 -26.21843808699992451, 30.83637225700005047 -26.21844169999991436, 30.83638852300003919 -26.21842453199991496, 30.83638129400003436 -26.21841188199994122, 30.83641292100008968 -26.21839832599994224, 30.83644454800008816 -26.2183992309999212, 30.8364715870000623 -26.21841613199995891, 30.83649515100006511 -26.21843085799991968, 30.83652677900005301 -26.21843718299993498, 30.83665780300003689 -26.2184335689999557, 30.83671382800008587 -26.2184543519999238, 30.83676804600008836 -26.21847242599994843, 30.83680870800003504 -26.21846248499991816, 30.83683491500005402 -26.21845796799993877, 30.83685027600006379 -26.21842995399993015, 30.83686563700007355 -26.21842633999995087, 30.83688913100007767 -26.21838838699994767, 30.83693250600003921 -26.21841820699995651, 30.83695600000004333 -26.21841820699995651, 30.83695690300004344 -26.21839380899990601, 30.83699666300003628 -26.21838657999995803, 30.83701563800008216 -26.21838206199993238, 30.83704365100004452 -26.21833959199994979, 30.8371032910000622 -26.21835675999994919, 30.83713491800006068 -26.21838025499994274, 30.83716654500005916 -26.21839019499992673, 30.83721805100003621 -26.21837392899993802, 30.83725419600006035 -26.21839109699993742, 30.83728130500009001 -26.21838838699994767, 30.83734004200005074 -26.21836850799991225, 30.83735992100008616 -26.21840284499995732, 30.83737076400007027 -26.21844169999991436, 30.8373987760000432 -26.21845977399993899, 30.83745299400004569 -26.21845344799993427, 30.83751263300007395 -26.21842633999995087, 30.83755781500008197 -26.2184091709999052, 30.83752347700004748 -26.21838477299991155, 30.83755871800008208 -26.21836308599995391, 30.83761112900003809 -26.21838477299991155, 30.83763552600004232 -26.21839380899990601, 30.83767257400006656 -26.21838386799993259, 30.83769335800008093 -26.21840284499995732, 30.8377403470000786 -26.21841820699995651, 30.8377990830000499 -26.21842182299991464, 30.83784155300008933 -26.2183956159999525, 30.83788312000007181 -26.21839832599994224, 30.8379228780000858 -26.21837212199994838, 30.83797619300008819 -26.21837392899993802, 30.83804215800006432 -26.21842091799993568, 30.83809908600005656 -26.21842091799993568, 30.8381225810000501 -26.21842362899991485, 30.83814697900004376 -26.21844169999991436, 30.83816234000005352 -26.21843266499990932, 30.83821475100006637 -26.21843628099992429, 30.83829969100008839 -26.21840826699991567, 30.83832837800008519 -26.21837674899995818, 30.83835817900006759 -26.21840790399994603, 30.83841236200004232 -26.21840790399994603, 30.83846654500007389 -26.21844041399992875, 30.83849499100006142 -26.21845260499992492, 30.83853156500003934 -26.21841332199994667, 30.83857355700007474 -26.21843364099993323, 30.83862909500004434 -26.21840248699993481, 30.83865889600008359 -26.218416030999947, 30.83869953200007785 -26.21839300299990327, 30.83874829800004136 -26.21841467699994155, 30.83879706300007228 -26.21840790399994603, 30.83883363600006078 -26.21841332199994667, 30.83890407300003744 -26.21838487499991288, 30.83892710200007059 -26.2183591389999151, 30.83894064800006163 -26.21833475699992277, 30.83896909400004915 -26.2183076649999407, 30.83899347700008775 -26.21826973799994676, 30.83901515000007976 -26.21822774499992192, 30.83901921400007495 -26.21818710699994881, 30.83901921400007495 -26.21814917799991917, 30.83903682300007176 -26.21811260599992011, 30.83907068800004936 -26.21808822299993835, 30.83913977100007742 -26.21808551399993803, 30.83918582600006175 -26.21809228799992297, 30.83923594600008755 -26.21804487699995434, 30.83928471100006163 -26.21809093099994925, 30.8393185750000498 -26.21808822299993835, 30.83935921300007976 -26.21806248699994057, 30.83939443200006281 -26.21802455799991094, 30.83946893400008094 -26.21800830299991958, 30.83959115800007567 -26.21796594999995023, 30.83966845700007298 -26.21791864299990493, 30.8396873670000673 -26.21784300399991707, 30.83974724700004799 -26.21780518599990728, 30.83980397600004153 -26.21776736499992921, 30.83988276700006281 -26.21778312299994695, 30.83994264600005408 -26.21783354899991991, 30.84004189000006591 -26.21785193399995251, 30.84006172400006562 -26.21782328399990547, 30.84010800300006849 -26.21776818999995839, 30.84011241000007431 -26.21772411499995314, 30.84013224400007402 -26.21766902199993865, 30.84017191000003777 -26.21763816899994026, 30.84019835600008719 -26.21759409399993501, 30.84022920900008558 -26.21755442599993557, 30.84027769200008606 -26.21756103799992843, 30.84029311800009054 -26.21752798099993242, 30.84035261800005401 -26.21747509199991555, 30.84037686000004896 -26.21744203499991954, 30.84039008300004525 -26.21741118299991058, 30.84044958400005498 -26.21739355299990848, 30.84043195400005288 -26.21734727399990561, 30.8404870480000568 -26.21726573499995538, 30.84049145600005204 -26.21722827099995357, 30.84049806600006605 -26.2171996219999528, 30.84054875200007473 -26.2171819919999507, 30.84054214200006072 -26.21715554699994755, 30.84056858600007445 -26.21713571399993725, 30.8405575680000652 -26.21710706499993648, 30.84058842000007417 -26.2170762119999381, 30.84059723600006464 -26.21705637799993838, 30.84063249600006884 -26.21703874799993628, 30.84068979200003469 -26.21700128499992388, 30.84076472000003832 -26.21696161699992444, 30.84084709400008251 -26.21693513299993583, 30.8409354060000851 -26.21686285199990607, 30.84096692300005316 -26.21676830399991331, 30.84094486000003599 -26.21669581499992319, 30.84089128300007587 -26.21663908699991907, 30.84087867700003471 -26.21657920699993838, 30.84096692300005316 -26.21655399399992348, 30.84100474100006295 -26.21650356799995052, 30.84098583100006863 -26.2164342319999264, 30.84103625700004159 -26.21640271599994776, 30.84109613800006855 -26.21634598799994365, 30.84107092500005365 -26.21631131999993158, 30.84105795700008912 -26.21628392699994947, 30.8410760950000622 -26.21625445299991952, 30.84107496100006074 -26.2161943729999507, 30.84112030400007143 -26.21618643799990878, 30.84113163900008203 -26.21617283399990583, 30.84116904900008649 -26.21619550699995216, 30.84121552600004179 -26.21614789699992798, 30.84125520100008089 -26.2161082209999563, 30.84132888400006323 -26.21604360699990366, 30.84135949100004837 -26.21599712999994836, 30.84136969400003636 -26.21597332499993627, 30.84143544100004419 -26.2159563209999078, 30.84148191800005634 -26.21592457999992121, 30.84152272700004005 -26.21590077499990912, 30.84157940600005077 -26.21583502699991186, 30.84164175300008992 -26.21576247799993098, 30.84169163100006017 -26.21574207299994441, 30.84176078000007237 -26.21575907699991603, 30.84179025300005605 -26.21576134399992952, 30.84179025300005605 -26.21570806599993375, 30.84179252000006954 -26.21568086099995298, 30.8418582680000668 -26.21563324999993938, 30.84189114300005485 -26.21562758099992152, 30.84190247800006546 -26.21561737899992295, 30.84190361100007749 -26.2155992419999393, 30.84193081700004768 -26.21561964599993644, 30.84194328700004917 -26.21559697399993638, 30.8419704930000762 -26.21557203599991226, 30.84201470300007486 -26.21552669199991215, 30.84206798100007063 -26.21546434399994041, 30.84209518700004082 -26.21538159299990411, 30.84209632100004228 -26.21536458999992192, 30.84213826300003802 -26.21535552099993538, 30.84214960000008432 -26.21530790999992178, 30.84216887000008001 -26.21529430699990826, 30.84221194600007721 -26.21528523899991114, 30.84223688500003391 -26.21524556299993947, 30.84225502300006383 -26.21523195999992595, 30.84231850300005817 -26.21525122999992163, 30.84234457600007318 -26.21524782999995296, 30.84240125500008389 -26.21523876199995584, 30.84251066700005595 -26.21520914199993513, 30.84255634600003759 -26.21521182899994074, 30.84258590300004244 -26.21519301999995832, 30.84263964400008717 -26.21514733999993041, 30.84267457500004639 -26.21510703499990314, 30.84271219400005748 -26.21508553999990454, 30.84275249800003849 -26.21507479099994953, 30.84276055900005531 -26.21504792099995029, 30.84275518600009036 -26.21501836399994545, 30.84288147500006971 -26.21503717299992786, 30.84291640600008577 -26.21498074499993436, 30.84292715500004078 -26.21490282199994226, 30.84306150500003696 -26.21490550899994787, 30.84318510700006755 -26.21495387499993512, 30.84327915300008272 -26.21499686599992174, 30.84331677100004754 -26.21501836399994545, 30.84337051100004601 -26.21491894399991907, 30.84342693800005009 -26.21484908199994379, 30.84349411400006602 -26.21483295999991014, 30.84353173300007711 -26.21483295999991014, 30.84355322900006513 -26.21488132599995424, 30.8435908470000868 -26.21491357099995412, 30.84364189900009023 -26.21491625699991346, 30.84369295300007252 -26.21491357099995412, 30.84373325900008922 -26.21491625699991346, 30.84376012900008845 -26.21485982999990938, 30.8438058080000701 -26.21478996699994468, 30.84383536500007494 -26.21476309699994545, 30.84387298300003977 -26.21476309699994545, 30.8439240370000789 -26.21472547899992378, 30.84399389900005417 -26.21472816699991881, 30.84406376100008629 -26.21476309699994545, 30.84407719700004691 -26.21481952399994952, 30.8440745100000413 -26.21485445599995501, 30.84411481400007915 -26.21488669999990861, 30.84414974600008463 -26.21488401199991358, 30.84417392900007826 -26.21488132599995424, 30.8442169210000543 -26.21488669999990861, 30.84427603600005341 -26.21487595199994303, 30.84439426400007278 -26.21489744799993105, 30.84442919600007826 -26.21489744799993105, 30.84446681400004309 -26.21494312699991269, 30.84452592800005277 -26.21494850099992391, 30.84457160600004499 -26.2149458139999183, 30.84461191300005112 -26.2149296919999415, 30.84464415600007214 -26.21490550899994787, 30.84470058300007622 -26.21489207399991983, 30.84473656700004085 -26.21491252299995267)))</t>
+  </si>
+  <si>
+    <t>Dundonald SP</t>
+  </si>
+  <si>
+    <t>Dundonald</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.87756874300004029 -26.23403556199991726, 30.87756322100005946 -26.23410949799995251, 30.87754129300003569 -26.23416431999993392, 30.87750017700005856 -26.23419995499995139, 30.87745906000003515 -26.23421640099991237, 30.8773960140000554 -26.23425751799993577, 30.87730281600005355 -26.23430685799991124, 30.87722332400005598 -26.2343973139999207, 30.87713835000005247 -26.234487771999909, 30.87708900900008757 -26.23456726399990657, 30.87702322300003743 -26.23457822899990788, 30.8770149990000391 -26.23462208599994483, 30.87693276600003855 -26.23470980199994074, 30.8768889070000796 -26.2347509189999073, 30.87686423800005286 -26.2348084809999591, 30.87679571000006717 -26.23484685799991212, 30.87700951700009 -26.23504695899993067, 30.87747002400004703 -26.23556777099992132, 30.87772220700009029 -26.23577335399994581, 30.87803469400006406 -26.23608035999990307, 30.87835594600005606 -26.23641268999995191, 30.87831968800009008 -26.23645584699994515, 30.87876594100004013 -26.23672426899992161, 30.8790075210000623 -26.23689874399991595, 30.87899242200006711 -26.23697256099995911, 30.87894880400006059 -26.23702624499992453, 30.8789337050000654 -26.23705811999991511, 30.87912663500003418 -26.23720071999991887, 30.87973058500006118 -26.23773420999992823, 30.880202003000079 -26.23822743699992088, 30.8802590000000805 -26.23827730999994401, 30.88023989500004518 -26.23829314199991813, 30.87966299900006106 -26.23876992999993263, 30.87964075300004652 -26.23879525799992507, 30.87976722800004836 -26.23886692699994683, 30.87983046500005457 -26.23890346399991813, 30.87989651200007302 -26.23899902299990572, 30.879963966000048 -26.23914517099990462, 30.88000331400007781 -26.23927867199995489, 30.88003001300006645 -26.23938406899992515, 30.88011573600005022 -26.23959907499994415, 30.88015789400003541 -26.23973398099991527, 30.88021270000007235 -26.23984640299994453, 30.88025204700005588 -26.24002908899990416, 30.88030966400003763 -26.24028203899990785, 30.88034058000005189 -26.24037759599991659, 30.88038695400007327 -26.24043802399995684, 30.88044035400008624 -26.24056309299993472, 30.88045721800006049 -26.24059962999990603, 30.88047127000004366 -26.24066567699992447, 30.88049234900006468 -26.24073313199994573, 30.88052607500003433 -26.2408343119999472, 30.88052024800003892 -26.24094352299994171, 30.88048713300008785 -26.24095456199995624, 30.88039330600008725 -26.24098767699990731, 30.88024980600005165 -26.24104838899995684, 30.88024980600005165 -26.24113669699994489, 30.88022220900006687 -26.24124156199991376, 30.88017253500004244 -26.24131331199993156, 30.88006215200005045 -26.24137402299993482, 30.87999592000005578 -26.24139609999991762, 30.87989105600007633 -26.24146233199991229, 30.87979722900007573 -26.24155063799992149, 30.8796923630000606 -26.24161134999991418, 30.87968684400004804 -26.24172725299990816, 30.87965924800005268 -26.24183211999991272, 30.87965924800005268 -26.24190386999993052, 30.87961509400008708 -26.24196458099993379, 30.87955990200003953 -26.24201977399991392, 30.87946055500003695 -26.24206392699994694, 30.87936672900008261 -26.24206944699994892, 30.87930601700008992 -26.2421135999999251, 30.87920115200006421 -26.24212463899993963, 30.8791238830000907 -26.24214671599992244, 30.8790521330000729 -26.24219086999994488, 30.87896382400003858 -26.24219638899995743, 30.87891967000007298 -26.24216879299990524, 30.87877617100008365 -26.24221846599994024, 30.87861059400006525 -26.24229021599995804, 30.87841742100005149 -26.24236196699990842, 30.87826288300004762 -26.24245027299991762, 30.87814594200006013 -26.24251187699991306, 30.8779817070000604 -26.24218540599991911, 30.87753564100006543 -26.24190289799992115, 30.8769706250000695 -26.24147170199995571, 30.87582572400003755 -26.24074312699991651, 30.87496698100005688 -26.24006846999992604, 30.87460370800005194 -26.23967652999994016, 30.87412910200004035 -26.23939607999994905, 30.8733740440000588 -26.23887832599990588, 30.87246797500006323 -26.2384468649999576, 30.87179921000006289 -26.23829585399994357, 30.87146954300004609 -26.23823245699992412, 30.87152796800006627 -26.23808155399990483, 30.87157913600003667 -26.23782270399993877, 30.87160923500005083 -26.23774444699995456, 30.87166341300007844 -26.23767822999991495, 30.87168749100004561 -26.23762405199994419, 30.87170555100004776 -26.23753676599994833, 30.87176875900007644 -26.23738326199992343, 30.87175972900007537 -26.2373200539999516, 30.87176875900007644 -26.23725383699991198, 30.87178681800008917 -26.23716053099991541, 30.87180487700004505 -26.23709732299994357, 30.87186206500007302 -26.23698896899992405, 30.87188915400008682 -26.23693779999990738, 30.87191323200005399 -26.23682041499995421, 30.87191022300004306 -26.23675720699992553, 30.87196139200005973 -26.23671506999994563, 30.87199149000008447 -26.23668496899995262, 30.87200653900003999 -26.23664885299990601, 30.87203964800005451 -26.23661273299995855, 30.87206372700006796 -26.23654049599991822, 30.87210887500003764 -26.23645922899993366, 30.87211489500003836 -26.23640806199995268, 30.87212392500003943 -26.236344853999924, 30.87217509200007726 -26.23621542799992312, 30.87220519000004515 -26.23614620199992942, 30.87221422100003565 -26.23607697499994629, 30.87223529100003816 -26.2359625989999472, 30.87225635900006182 -26.23584822399993755, 30.87231354700008978 -26.23573685799993882, 30.87237073400007148 -26.23566161099995497, 30.87239481300008492 -26.23559840499990514, 30.87239481300008492 -26.2355081079999195, 30.87240986300008672 -26.23546596899990391, 30.87244297100005497 -26.23541179099993315, 30.87246705000006841 -26.23536062399995217, 30.87250015900008293 -26.23526731699990933, 30.8725392870000519 -26.23521313999992799, 30.87267172200006371 -26.23511381299994127, 30.87269580100007715 -26.2350807059999056, 30.87271687000009024 -26.23505361599995922, 30.87274997900004792 -26.23503254799993556, 30.87278007800006208 -26.23500846799993269, 30.87281318600008717 -26.23497535899991817, 30.87286435400005757 -26.23493622999990293, 30.87293358200008697 -26.23483389499995155, 30.87358371500005205 -26.23427706699993678, 30.87423986900006412 -26.23372023999991143, 30.87598860800005696 -26.23389481299994941, 30.87679224600003636 -26.23394598099991981, 30.87702099600005567 -26.23395500999993146, 30.87711430300004167 -26.23393093099991802, 30.87716547100006892 -26.23391889199990601, 30.87729188600008001 -26.23391889199990601, 30.87732198400004791 -26.2339519999999311, 30.8773821810000868 -26.23397607899994455, 30.87748752800007424 -26.23397908899994491, 30.87753869600004464 -26.23401520799990294, 30.87756874300004029 -26.23403556199991726)))</t>
+  </si>
+  <si>
+    <t>Holeka SP</t>
+  </si>
+  <si>
+    <t>Holeka</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.93164914200008297 -26.24740325199991275, 30.93142817400007516 -26.24788938399990457, 30.93160494900007507 -26.24853018999993992, 30.93192975500005559 -26.24909318799990388, 30.93184570300007863 -26.2493033199999104, 30.93172166400006518 -26.24945654399994055, 30.93160492300006581 -26.24954409999992322, 30.93134955000004993 -26.24953680399994482, 30.9312765860000809 -26.24963165599990589, 30.93129847500006235 -26.24977758399995764, 30.93140062400004808 -26.24987973299994337, 30.93121821500005808 -26.25014969799991604, 30.93110147300006929 -26.25037588599991523, 30.93099932400008356 -26.25041966599991383, 30.9305980240000622 -26.25033210799995231, 30.93021131600005447 -26.25031021899991401, 30.92990486900004043 -26.25041966599991383, 30.9296494960000814 -26.25041966599991383, 30.92924089800004595 -26.25031751599993868, 30.92913875000004964 -26.2504488499999411, 30.92900011800008997 -26.25036129399995843, 30.92887608200004479 -26.25033210799995231, 30.928708264000079 -26.25025184799994804, 30.92858422600005497 -26.25021536599990668, 30.92845289100006312 -26.25017158799994377, 30.92828507400008675 -26.25017888499991159, 30.92810266600008617 -26.25011321699992095, 30.92804429400007393 -26.25025184799994804, 30.92795673800003442 -26.25038318399992932, 30.92781810700006417 -26.25049262799990402, 30.9277378470000599 -26.25055099899992683, 30.92757732700005135 -26.25060207399991441, 30.92751895600008538 -26.25057288799990829, 30.92746788100004096 -26.25065314799991256, 30.92740221400003975 -26.25072611199993844, 30.92738032500005829 -26.25085744799991971, 30.92730736100008926 -26.25091581799995311, 30.92721250900007135 -26.25103985599992029, 30.92716873000006217 -26.25109093099990787, 30.9270592850000412 -26.25112011599992456, 30.92700821000005362 -26.25116389399994432, 30.92697172900005853 -26.25118578199993635, 30.92690606100006789 -26.25128063599993311, 30.92682580100006362 -26.2513900819999435, 30.92670905900007483 -26.25152141599994593, 30.92663609500004895 -26.25160897299991802, 30.92661420700005692 -26.25171112199990375, 30.92657042800004774 -26.25176219699994817, 30.92645368700004838 -26.25184245699995245, 30.92633694500005959 -26.25194460599993818, 30.92630775900005347 -26.25201756999990721, 30.92627857300004734 -26.25210512599994672, 30.92613994100008767 -26.25222916399991391, 30.92608157100005428 -26.25246264799994833, 30.92603779300003453 -26.25257938999993712, 30.92599401500007161 -26.25272531699994261, 30.92599401500007161 -26.252834762999953, 30.92600131100005001 -26.2529952829999047, 30.92597942300005798 -26.25316309899994849, 30.92592105100004574 -26.2534914359999334, 30.9262202010000351 -26.25371762299994316, 30.92645368700004838 -26.25414081299993541, 30.92668717000003653 -26.25433781499992847, 30.92693524700007401 -26.25453481699992153, 30.92701550700007829 -26.25491422899995086, 30.92732925000007072 -26.25506745199993475, 30.92743869600008111 -26.25519878499994775, 30.92749706700004708 -26.25532282499995063, 30.9275554380000699 -26.25552712299992209, 30.92780351400006111 -26.25590653399990515, 30.92759921600008965 -26.25599409099993409, 30.92742410300007805 -26.25608164699991676, 30.92710306300006096 -26.25612542499993651, 30.92674554100005935 -26.25614001799993957, 30.92666528100005507 -26.25622027799994385, 30.92648287200006507 -26.2563516129999357, 30.92619831300004307 -26.25649024399990594, 30.92589186600008588 -26.25655591099990716, 30.92561460400008855 -26.2565340219999257, 30.92545408400008 -26.25643916899991837, 30.92541030500007082 -26.25616190699992103, 30.92492874500004518 -26.2560597579999353, 30.92467685500008656 -26.25603877299994338, 30.92453927100007149 -26.25599454999991167, 30.92441642800008594 -26.2559306709999305, 30.92421496600007913 -26.25579799999991337, 30.92402333300003647 -26.25581274299992174, 30.92380712900006756 -26.2558323969999492, 30.923630236000065 -26.2558323969999492, 30.92344351400004143 -26.25578325999993012, 30.92332558600008952 -26.25577834699993218, 30.92306024500004469 -26.25566533099993194, 30.92291774800008852 -26.25577343299994482, 30.92278507800006082 -26.25591592999995783, 30.92269171800006688 -26.25609773799993718, 30.92262292600008777 -26.2562500619999355, 30.92259344400008558 -26.25642204199994012, 30.92259344400008558 -26.25663333299991109, 30.92245586100005994 -26.25675617399991779, 30.92233793100007233 -26.256849534999958, 30.92215121000003819 -26.25691832599994768, 30.92201362500009054 -26.25692815399992242, 30.92185638700004802 -26.25698220499992885, 30.92174828600008141 -26.25710996099991235, 30.92162544300003901 -26.25720332199995255, 30.92152716900005771 -26.25735073199990666, 30.92146329100006596 -26.25745391999993217, 30.92139450000007628 -26.2575964179999346, 30.92131588000006559 -26.25771434699993279, 30.92122252000007165 -26.25781262099991409, 30.92108984900005453 -26.25791089499995223, 30.92103088500005015 -26.25802390999990621, 30.92094735200004152 -26.25805830599995261, 30.92082450900005597 -26.25811235699995905, 30.92076807900008362 -26.25816173299995171, 30.92072937400007504 -26.2580706049999435, 30.92070268600008376 -26.25798787399992307, 30.92069201000003886 -26.25792115499990587, 30.92070001700005832 -26.25787845499991136, 30.92071336100008239 -26.25780106199994179, 30.92072403600008101 -26.25775035499992782, 30.92072136700005558 -26.25770765499993331, 30.92069468000005372 -26.25764894299993557, 30.92068400500005509 -26.25759023099993783, 30.9206893420000597 -26.25749415599995018, 30.9206759990000819 -26.2574060859999463, 30.92067866700006107 -26.25732602499994073, 30.92065998700007867 -26.2572352879999471, 30.92066265500005784 -26.25719792499995719, 30.92065464800003838 -26.25708850699993491, 30.92065464800003838 -26.25701111299991908, 30.92065198000005921 -26.25693105099992408, 30.92065731800005324 -26.25684298199990963, 30.92068400500005509 -26.25677626299994927, 30.9206893420000597 -26.25661880899991729, 30.92069201000003886 -26.25654141399991204, 30.92069468000005372 -26.25642132099994797, 30.92071336100008239 -26.25637328199991316, 30.92074538600007827 -26.25631723999993028, 30.92076406700005009 -26.25626386499993714, 30.92077741100007415 -26.25615711499995086, 30.92079876100007141 -26.25613042699990274, 30.92080142900005058 -26.2560930649999591, 30.92078808600007278 -26.25600499599994464, 30.92077741100007415 -26.25587689699995053, 30.92080142900005058 -26.25578082199990604, 30.9207960930000354 -26.25571143599995594, 30.92079342300007738 -26.25550060399990571, 30.92078808600007278 -26.25538584799994624, 30.92079342300007738 -26.25529244099993775, 30.9208121040000492 -26.25522038599990537, 30.9207960930000354 -26.25516700999992281, 30.9207560610000769 -26.25508961699995325, 30.92074538600007827 -26.25502823599993008, 30.92074538600007827 -26.25495617999990827, 30.92077207400006955 -26.25488945999995849, 30.9208121040000492 -26.2548307499999396, 30.92084146100006592 -26.25476402999993297, 30.92084946700003911 -26.25468129899991254, 30.920881492000035 -26.25461991799994621, 30.92088416100006043 -26.2544758059999026, 30.92087615500008724 -26.25437706199994636, 30.92087615500008724 -26.25433169399991584, 30.92083345500003588 -26.25421426899993094, 30.92082811600005243 -26.25415555499995435, 30.92083345500003588 -26.25407015699994417, 30.92083612300007189 -26.2540141129999256, 30.92082544800007327 -26.25396073899992189, 30.92080943600007004 -26.25388334499990606, 30.92078363800004581 -26.25377792799991994, 30.92076584600005162 -26.25363559599992413, 30.92068756300005816 -26.25349326299993891, 30.92068756300005816 -26.25343277099995021, 30.92070535500005235 -26.25325841299991225, 30.92071247200004791 -26.25309472999992977, 30.92074805500004686 -26.25303779699993356, 30.92076940600009038 -26.25293460599993978, 30.92078008100008901 -26.25287411399995108, 30.92079787100004751 -26.25277803999995285, 30.92074805500004686 -26.25270687299990868, 30.92074449700004379 -26.25263570599992136, 30.920755171000053 -26.25257521499992208, 30.92075161300004993 -26.25250404799993476, 30.92076228800004856 -26.25243288199993685, 30.92077652100005025 -26.2523510399999509, 30.92080854600004614 -26.25216600699991432, 30.92077296300004718 -26.25211619099991367, 30.92066766600004257 -26.25201756999990721, 30.92092304000004788 -26.2519737919999443, 30.92120759600004476 -26.25185704999995551, 30.92124408000006497 -26.25156519499995511, 30.92117841200007433 -26.25145574999993414, 30.9212367830000403 -26.25126604199994063, 30.92131704300004458 -26.25106174599994802, 30.92117111500004967 -26.2509304099999099, 30.92139730300004885 -26.25080637199994271, 30.92157241500007103 -26.25072611199993844, 30.92165997200004313 -26.2505582959999515, 30.92200290000005225 -26.25034669999990911, 30.92212694000005513 -26.25034669999990911, 30.92228016400008528 -26.25022995799992032, 30.92254283300007955 -26.24998188399990795, 30.92284928000003674 -26.24980676999990692, 30.92327246900003956 -26.2495076179999387, 30.92349136000007093 -26.24940546899995297, 30.92347676800005729 -26.24927413499995055, 30.92335272900004384 -26.24924494899994443, 30.92311194900008786 -26.24920117099992467, 30.92306817100006811 -26.24904794699995136, 30.92300250400006689 -26.24892390899992733, 30.92292954000004102 -26.24882905599992, 30.92282009500007689 -26.24869042499994976, 30.92273253800004795 -26.24860286899991024, 30.9226814640000498 -26.24842775599995548, 30.92264498200006528 -26.24827453199992533, 30.92242609100003392 -26.24820156899994572, 30.9223896090000494 -26.24816508699990436, 30.92238231200008158 -26.24787323199990396, 30.92250635100003819 -26.24762515499992332, 30.92298061500008544 -26.24784404499990842, 30.92323598800004447 -26.24753759899994066, 30.92368106600008559 -26.24761785899994493, 30.92387806800007866 -26.24756678299991108, 30.92406047700006866 -26.2473114119999309, 30.92417721900005745 -26.24729681899992784, 30.92421370100004197 -26.24693199999995841, 30.92437928300006433 -26.24667405599990389, 30.9247770280000509 -26.24654147599994758, 30.92552832000006902 -26.24627631299995301, 30.92557251300007692 -26.24598905499993862, 30.9259481600000754 -26.24598905499993862, 30.92641219400007913 -26.24601115199993728, 30.92665525800003934 -26.24594486099994128, 30.92687622600004715 -26.2457680869999308, 30.92705300000005764 -26.24543663499991908, 30.92716348500005097 -26.2451272789999166, 30.92811364900006765 -26.24472953599990888, 30.92877655400008052 -26.24649728099990398, 30.9298813960000416 -26.2462984109999411, 30.93045591300005981 -26.24671825099994749, 30.93094204300007277 -26.2470718009999473, 30.93164914200008297 -26.24740325199991275)))</t>
+  </si>
+  <si>
+    <t>Betty's Goed SP</t>
+  </si>
+  <si>
+    <t>Betty's Goed</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.83845803700006627 -26.31510377799992284, 30.83798540600008664 -26.31484120599992593, 30.83756697800004076 -26.31460874499992997, 30.83737216400004399 -26.3145005149999065, 30.83459715700007564 -26.31478203899990831, 30.83310911000006627 -26.31510377799992284, 30.83154062700003806 -26.31590812699994331, 30.83073627800007444 -26.31639073899992809, 30.83034480100008068 -26.31640077599990946, 30.82916779500004623 -26.31643095499993024, 30.82788083600007667 -26.31582769299990332, 30.8269558340000458 -26.31522442999994382, 30.82659387600006085 -26.31506355999994184, 30.82582974400008879 -26.31433964499990452, 30.82530691700003445 -26.31425920999993195, 30.8250253940000789 -26.31377660199990487, 30.82438191400007099 -26.31321355599993694, 30.82369821700007151 -26.31289181599993299, 30.82333625900008656 -26.31224833599992508, 30.82265256200008707 -26.31192659499993169, 30.82176777700004777 -26.31132333399995105, 30.82104386200006729 -26.31096137599990925, 30.81987755500006188 -26.31035811399993918, 30.81935472800006437 -26.30999615599995423, 30.81911768800006257 -26.30980901899994251, 30.81904021100007185 -26.3093575329999112, 30.81892108800008145 -26.30876687699992544, 30.81910473800007821 -26.30778410599992867, 30.8192040060000636 -26.30741680899990342, 30.81927845900008833 -26.30685097199994971, 30.81945714400006864 -26.30662265099994102, 30.81954152300005489 -26.30623053599993, 30.81985422200006042 -26.30517331299995476, 30.82050940300007369 -26.30459258499990938, 30.82134326900006727 -26.30395725999994738, 30.82189421600008927 -26.30334674999994604, 30.82259903100003839 -26.30252281099990341, 30.82463254000003872 -26.30014980299995386, 30.82494877300007374 -26.2996024769999508, 30.82497309900008986 -26.29865377699991313, 30.82407764200007705 -26.29812013199995135, 30.82323837200004846 -26.29735715899994375, 30.82285052900004985 -26.29693752399992945, 30.82260256100005336 -26.29668955799991181, 30.82236731200003987 -26.29631442999993851, 30.82220200100005059 -26.2961046129999545, 30.82219564300004322 -26.29592658599995048, 30.82204940600007603 -26.29576127399991492, 30.82183958900003518 -26.29564047099995605, 30.82182687300007728 -26.29508731599992188, 30.82180144000005839 -26.29464860599995291, 30.82189681200003406 -26.29450872799992567, 30.82178236600003629 -26.29409544999992931, 30.82183999600005109 -26.29396578199992973, 30.82185866300005728 -26.29392378199992208, 30.82202397500003599 -26.29384112699995057, 30.82208755500005282 -26.29379026199995906, 30.82246268300008296 -26.29382841099993584, 30.82260256100005336 -26.29379026199995906, 30.82266649300004246 -26.29375558199990337, 30.82276440700007925 -26.29359079999994719, 30.82283127400006606 -26.2933949729999199, 30.82291963600005147 -26.29331377699992345, 30.82315606100007699 -26.29272868299995025, 30.82323487100006787 -26.29264270999993869, 30.82331845500004874 -26.29260211199994046, 30.82338054600006672 -26.29253285599992296, 30.82351667000006046 -26.2925161389999289, 30.82366473400008999 -26.2924349409999536, 30.82388921900007972 -26.29237285199991447, 30.82416863200006674 -26.29235135699991588, 30.82440744500007668 -26.29231553599993276, 30.82457939100004296 -26.29229881999992813, 30.82472984300005692 -26.29225583299995606, 30.82489005200005749 -26.29223402299993495, 30.8250141360000498 -26.29227068499994857, 30.82503951700005018 -26.29234400799992954, 30.82510437900003808 -26.29238348899991706, 30.82531024700006128 -26.29241450999995777, 30.82545689200009065 -26.29241450999995777, 30.82566840000004049 -26.29244271099992147, 30.82599271100008309 -26.29252731399992626, 30.82613371600007213 -26.29256961499993395, 30.82643546800005652 -26.29257525599990686, 30.82674567700007628 -26.2926034569999274, 30.82692616500008853 -26.29243707199992741, 30.82711511200005816 -26.29224530399994819, 30.82738866100004316 -26.29195765399992979, 30.82757196800008614 -26.29176870699990332, 30.82765375100007077 -26.2915910399999575, 30.82770451300007153 -26.29130902999992259, 30.82774117400003888 -26.29111726299993279, 30.82777501500004291 -26.29095087599995395, 30.82783987800007708 -26.29085217399995145, 30.82789628100005075 -26.29061246499992421, 30.82792730100004519 -26.29047145999993518, 30.82800062300003674 -26.29022893199993405, 30.82801190400004998 -26.29014714799990315, 30.82797524300008263 -26.29002588399993101, 30.82795268200004557 -26.28985667799992143, 30.82792448100008187 -26.28962542999994412, 30.8279131990000792 -26.28946468399993819, 30.82791038000004846 -26.2893321389999528, 30.82795268200004557 -26.28916011399991248, 30.8279865230000496 -26.28898244799995609, 30.82801754400009031 -26.28874273799993944, 30.82804960000004257 -26.28853425699992385, 30.82802422600008185 -26.28841302499995436, 30.82802986500007592 -26.28832280599993965, 30.82802140600006169 -26.28827769699995542, 30.82796502000007877 -26.28820721199991794, 30.82789171600006739 -26.28806624399993552, 30.82780149700005268 -26.2878858059999061, 30.82769718100007594 -26.2877758509999353, 30.82755057500008888 -26.28768563199992059, 30.82742934200007312 -26.28756721899992499, 30.82738141400005816 -26.28748545799993508, 30.82736167800004523 -26.28733321299995396, 30.82737859400003799 -26.2871443159999103, 30.8273842330000889 -26.28690467199993464, 30.82737231600003724 -26.28677473799990594, 30.82839343400007692 -26.28615318699991121, 30.82904526000004353 -26.28590248499995141, 30.83049933200004489 -26.28545122099990294, 30.83260522900008027 -26.28444841199990378, 30.83486154900003839 -26.28344560399995089, 30.83646604200004049 -26.28259321699994189, 30.8371425320000867 -26.2822972529999106, 30.8381226110000739 -26.28377596799992943, 30.8382920960000888 -26.28370064099993897, 30.83839567000006809 -26.283681809999905, 30.83862165000005007 -26.283681809999905, 30.83893237200004478 -26.28381363199991938, 30.83917718400005015 -26.28395486899995603, 30.83935608500007675 -26.28403019499995708, 30.83981746000006297 -26.28432208599991782, 30.83966948100004402 -26.28636061299994253, 30.83981851300006838 -26.28646316799995475, 30.83989421600006153 -26.28654968499995448, 30.84025109900005646 -26.28671190599993679, 30.84041331900004934 -26.28678760699995109, 30.84092160600005172 -26.28707960299993829, 30.84126767600008634 -26.28716612099992744, 30.84150559800008295 -26.2875770759999341, 30.84159211500008269 -26.28775011099992298, 30.84158866600006377 -26.28780299599992532, 30.84161020100003725 -26.28784128099994177, 30.84161020100003725 -26.28789392299995598, 30.84164609500004417 -26.28800878099991678, 30.84163891600007901 -26.28804706499994381, 30.84162695200006965 -26.28808295899995073, 30.84164130900006739 -26.28810449499991364, 30.84169873700005837 -26.28812124499995662, 30.84176573700005974 -26.28816670899993824, 30.84182077300005176 -26.28820738599995366, 30.84189016600004152 -26.28824088699991535, 30.84186863000007861 -26.28832224499990389, 30.84184709500004828 -26.28839163699990422, 30.84180402300006563 -26.28841077999993558, 30.84178009500004691 -26.28844427999990785, 30.84182316700008641 -26.28856870799995704, 30.84181120200008763 -26.28871706499995753, 30.84170352300003515 -26.28888456499993254, 30.84164609500004417 -26.28904010299993388, 30.8416054160000499 -26.28914777999995067, 30.84160063000007312 -26.28924588699993592, 30.84158866600006377 -26.2893033149999269, 30.84158866600006377 -26.28936792399991873, 30.84161020100003725 -26.28942535199990971, 30.84161977300004764 -26.28945645899995043, 30.84165088000008836 -26.28945885299992824, 30.84165805900005353 -26.28948995799993327, 30.84162695200006965 -26.2895234589999518, 30.84161738000005926 -26.28955217299994729, 30.84164609500004417 -26.28959524499992995, 30.84163891600007901 -26.28965745799990827, 30.84163413000004539 -26.28970770899991294, 30.84164609500004417 -26.28974599499991882, 30.84167481000008593 -26.28976992299993753, 30.8417154870000445 -26.28978906599991205, 30.8417322380000769 -26.28982735199991794, 30.84171309400005612 -26.28991110199990544, 30.84170591600008038 -26.29005467299992915, 30.8416484880000894 -26.29015517299990279, 30.8416484880000894 -26.29032745799992199, 30.84166284500008715 -26.29071031599994512, 30.84171788000008974 -26.29099506599993674, 30.84169873700005837 -26.29105728099995076, 30.84165327300007675 -26.29108838699994521, 30.8416939510000816 -26.29118649499991989, 30.84170591600008038 -26.29122238799993738, 30.84165805900005353 -26.29124392299991086, 30.84166045200004191 -26.29129178099992714, 30.84163652300009062 -26.2913133149999112, 30.84165566700005456 -26.29138510299992504, 30.84169155900008263 -26.29144731599990337, 30.84168438000006063 -26.29149995799991757, 30.84166762900008507 -26.29153585199992449, 30.84165327300007675 -26.29155499499995585, 30.84167959500007328 -26.29159328099990489, 30.8416891660000374 -26.29167463699991458, 30.84164609500004417 -26.29170335199995634, 30.84161020100003725 -26.29173924599990642, 30.84166762900008507 -26.29181581499994991, 30.84174180900004103 -26.29187324499991973, 30.84180402300006563 -26.29194024499992111, 30.84188538000006474 -26.29198570899990273, 30.84189973800005191 -26.29203117299994119, 30.84191648700004862 -26.2920527089999041, 30.84194759500007876 -26.2920527089999041, 30.84196434400007547 -26.29207185199993546, 30.84194998700007773 -26.29211492299992869, 30.84190691700007392 -26.29216517299994393, 30.84195716600004289 -26.2921795309999311, 30.84194520100004411 -26.29223935199991047, 30.84191170200006127 -26.2922824229999037, 30.84189734500006352 -26.29234224499992933, 30.84188059400008797 -26.29236378099994909, 30.84183752300003789 -26.29238053099993522, 30.84183991600008312 -26.29247863799992047, 30.84182555900008538 -26.29253606599991144, 30.8418542720000346 -26.29268681599995716, 30.84188538000006474 -26.29280645899990532, 30.84190930900007288 -26.29289978099990321, 30.84190213000005087 -26.2929548159999058, 30.8419547730000545 -26.29302660199994079, 30.8419547730000545 -26.29308642499995585, 30.84194280900004514 -26.29314624499994579, 30.84194280900004514 -26.29317256599995289, 30.84196673700006386 -26.29318931599993903, 30.84193802200007894 -26.29328503099992531, 30.84191409500004966 -26.29338792399994418, 30.84192606000004844 -26.29344774499992354, 30.84196434400007547 -26.2935434589999204, 30.84200262900003509 -26.29361045899992178, 30.84207202300007111 -26.2936989949999429, 30.84211509500005377 -26.29375163799994652, 30.84212705900006313 -26.29379470899993976, 30.84210552200005395 -26.29382581499993421, 30.84208398800006989 -26.29386170899994113, 30.84208877300005724 -26.29391435199994476, 30.84210073900004545 -26.29396938799993677, 30.84208637900007943 -26.29401724499990678, 30.84205527300008498 -26.29404595899995911, 30.84197630900007425 -26.29412970899994662, 30.84193563000007998 -26.29418235199995024, 30.84190691700007392 -26.29423738799994226, 30.84190930900007288 -26.29431874499994137, 30.84192127300008224 -26.29439531699995314, 30.84190213000005087 -26.29443120799993494, 30.84190213000005087 -26.29453649499993162, 30.84191648700004862 -26.29463460199991687, 30.84191648700004862 -26.29467767499994579, 30.84191648700004862 -26.29470878099994025, 30.84187341600005539 -26.29472313799993799, 30.84185188000003564 -26.2947614249999333, 30.84183991600008312 -26.29482124499992324, 30.84186384500003442 -26.29487149499993848, 30.84184231000006093 -26.29489542399994662, 30.8418447020000599 -26.29499353099993186, 30.84190452300003926 -26.29504617399993549, 30.84190691700007392 -26.29509881699993912, 30.84188777300005313 -26.29524238799990599, 30.84187580900004377 -26.29531656699992936, 30.84187341600005539 -26.29535963699993317, 30.84183034500006215 -26.29543860199993333, 30.84183512900006008 -26.29548885299993799, 30.84183034500006215 -26.29553192399993122, 30.84181359500007602 -26.29560131699992098, 30.84183752300003789 -26.29562285199995131, 30.84183752300003789 -26.29566113799995719, 30.84180402300006563 -26.29569463699994003, 30.84174420200008626 -26.29572335199992494, 30.84167959500007328 -26.29576642499995387, 30.84158148700004176 -26.29584060199994155, 30.8415479870000695 -26.29589324499994518, 30.84151209500004143 -26.29595306599992455, 30.84147859500006916 -26.29601288799995018, 30.84145705900004941 -26.29604638799992244, 30.84145466600006102 -26.29608228099993994, 30.84147380900003554 -26.29611099499993543, 30.84151448700004039 -26.29614449499990769, 30.8415288450000844 -26.29617560199994841, 30.84155038000005788 -26.29619235199993454, 30.84159823700008474 -26.29621628099994268, 30.84160780900003829 -26.2962713169999347, 30.84158627300007538 -26.29630720899990592, 30.84155277300004627 -26.29635028099994543, 30.84153841600004853 -26.29638856699995131, 30.84153602300006014 -26.29648428099994817, 30.84151209500004143 -26.29653453099990656, 30.84150970200005304 -26.29657042399992406, 30.84148816700007956 -26.29665895999994518, 30.84149295200006691 -26.29672595899995713, 30.84152405900005078 -26.29680492399995728, 30.84154320200008215 -26.29686953099991342, 30.8415479870000695 -26.29691978099992866, 30.84153363000007175 -26.2969437099999368, 30.84150932000005696 -26.29706633199992893, 30.84154830900007482 -26.29712664199990968, 30.84157125900003393 -26.29719038799993314, 30.84157890700004145 -26.29725923299992019, 30.84155851000008397 -26.29731533099993612, 30.8415202610000847 -26.29732043099994598, 30.84146167000005789 -26.2973066819999417, 30.84146105300004592 -26.29730979099991828, 30.8414228210000374 -26.29730463299995336, 30.84141316700004154 -26.29729238299995586, 30.84138001800005213 -26.29730003199995281, 30.84134687000005215 -26.29732043099994598, 30.84130607300005522 -26.2973663289999422, 30.84128567400006204 -26.29741732499991258, 30.84123212600007946 -26.29743517499991867, 30.84122702800004845 -26.2974759719999156, 30.84121172900006513 -26.29751166999994894, 30.84121172900006513 -26.29754481899993834, 30.84122447800007194 -26.29759836499994208, 30.84124232500005292 -26.29765956199992161, 30.84127292400006581 -26.29772840799995492, 30.84128567400006204 -26.29777685499993822, 30.84127802400007567 -26.29779725499992082, 30.84121427900004164 -26.29784570199990412, 30.84118367900003932 -26.29789414899994426, 30.84118113000005224 -26.29793494799992004, 30.8411556310000492 -26.29797319499994046, 30.84116328100003557 -26.29801399199993739, 30.84114798100006283 -26.29810578699994039, 30.84110208400005604 -26.29814913499990325, 30.84106638500009012 -26.29821033199993963, 30.84107403400008707 -26.29825877899992292, 30.84107148600008941 -26.29829447799994568, 30.84110208400005604 -26.29833782299994027, 30.84106893600005606 -26.29838882199993577, 30.84106128500008026 -26.29843726899991907, 30.8410587370000826 -26.29848061599994935, 30.8410587370000826 -26.29851886399995919, 30.84103833700004316 -26.29855456199993569, 30.84104088700007651 -26.29857751099990537, 30.84100518900004317 -26.29860810899992885, 30.84102303800005984 -26.2986489069999152, 30.84101028900005304 -26.29867950399994925, 30.84102558800003635 -26.29872030299992502, 30.84098989000005986 -26.29880189899995457, 30.84095674200005988 -26.29885289599991438, 30.84092104400008338 -26.29889624299994466, 30.84086749800007965 -26.29896253999993405, 30.8408445480000637 -26.29901098799990677, 30.84079355100004705 -26.2990415839999514, 30.84080375100006677 -26.29908493299990369, 30.84082924900008038 -26.29912573099994688, 30.84084709800004021 -26.29917417799993018, 30.84090574500004323 -26.29917672899995296, 30.84094654300008642 -26.29919712599991044, 30.84096694100009017 -26.29923537499990971, 30.8409363430000667 -26.2992914709999468, 30.84090064500009021 -26.29933736899994301, 30.84087514600008717 -26.29940366499994298, 30.84083944900004326 -26.2994750609999528, 30.8407961010000804 -26.29950565999990886, 30.84075020400007361 -26.29950310999993235, 30.84072470500007057 -26.29953370799995582, 30.84067370800005392 -26.29955155599992622, 30.84066860800004406 -26.29958980499992549, 30.84063546000004408 -26.29958470499991563, 30.8406150610000509 -26.29960000399995579, 30.84058446300008427 -26.29960765399994216, 30.84052836500006833 -26.29962550299995883, 30.84047991900007446 -26.29962040299994896, 30.84044677000008505 -26.29962040299994896, 30.84045697000004793 -26.29967139999990877, 30.84044932000006156 -26.29969689899991181, 30.84045442000007142 -26.29973514599993223, 30.84038812400007146 -26.2998218419999148, 30.84031672900005105 -26.30001053099994124, 30.84029122900005859 -26.30011252599990712, 30.84025808100005861 -26.30013547499993365, 30.84024278200007529 -26.30020432099991012, 30.84021983300004877 -26.30029101599990327, 30.84017903400007299 -26.30038281099990627, 30.84017903400007299 -26.3004542069999161, 30.84015608600003588 -26.30050265399995624, 30.84016118700003517 -26.30054345199994259, 30.84017903400007299 -26.30057659999994257, 30.84013058800007911 -26.30059699999992517, 30.84009744000007913 -26.30062249799993879, 30.84009234000006927 -26.30067349499995544, 30.84009489000004578 -26.30071429199995237, 30.84005154200008292 -26.30074998999992886, 30.84004644300006248 -26.30078823899992813, 30.84001839400008294 -26.30080098799993493, 30.83998014600007309 -26.30080863599994245, 30.83995974700007991 -26.30078058999993118, 30.83992659900007993 -26.30080098799993493, 30.83991895000008299 -26.30082903599992505, 30.83986030300007997 -26.30087493299993184, 30.83980420700004288 -26.30086473399995839, 30.83978125700008377 -26.30088513299995157, 30.83977360800008682 -26.30092338099990457, 30.83974301000006335 -26.30092083099992806, 30.83973791000005349 -26.30095652999995082, 30.83969456200009063 -26.30096672899992427, 30.83963846600005354 -26.3009871259999386, 30.83957726900007401 -26.30097182699995528, 30.83954157100004068 -26.30100242599991134, 30.83950842300004069 -26.3010508739999409, 30.83945487500005811 -26.30104067399992118, 30.83940897800005132 -26.30105342299992799, 30.83934778100007179 -26.30106872299995757, 30.83930443400004151 -26.30110187099995755, 30.8392712850000521 -26.30113501999994696, 30.83923813800004154 -26.30115541699990445, 30.83920244000006505 -26.30116561599993474, 30.83916929100007565 -26.30119366599990371, 30.83914634300003854 -26.301237012999934, 30.83914379300006203 -26.30126761199994689, 30.83912594400004537 -26.30129820999991352, 30.83909534500008931 -26.30132880899992642, 30.83907749800005149 -26.30136705599994684, 30.83905454800003554 -26.3013721559999567, 30.83903669900007571 -26.30138490499990667, 30.83901630000008254 -26.30143080199991346, 30.83900100100004238 -26.30148180099990896, 30.83901120000007268 -26.30152004799992937, 30.8389806020000492 -26.30155319599992936, 30.83895510300004617 -26.30158379399995283, 30.83895765300007952 -26.30162459199993918, 30.83892960400004313 -26.30163224099993613, 30.83893980300007343 -26.3016602909999051, 30.83894490400007271 -26.30168833699991637, 30.8389321550000659 -26.30172913599994899, 30.83890920700008564 -26.30175463399990576, 30.83888115700005983 -26.30178523299991866, 30.83884800900005985 -26.30179798199992547, 30.83883271000007653 -26.30182857999994894, 30.8387970120000432 -26.30185152999990805, 30.83880211200005306 -26.30188722699995196, 30.83879191200009018 -26.30193822399991177, 30.83878936300004625 -26.30197392199994511, 30.83876609900005406 -26.30202547399994728, 30.83873627000008355 -26.30203694799990899, 30.83873627000008355 -26.30207136699993953, 30.83870873300008952 -26.30209431299994094, 30.83867201900005739 -26.30210578599991322, 30.83862612700005457 -26.30212873299990406, 30.83862842000007731 -26.30218380399992384, 30.83865825100008351 -26.30221133899993902, 30.83863301100006993 -26.30225493699992967, 30.83858711800007768 -26.30232377599992333, 30.83858482300007609 -26.30239031999991539, 30.83858482300007609 -26.30244768599993677, 30.83857105600003479 -26.30251881999993202, 30.83853893100007326 -26.30258765699994683, 30.8385343420000595 -26.30269091599990361, 30.83853663600007167 -26.30272992599992676, 30.83851827900008402 -26.30274828199992498, 30.83848386000005348 -26.30278040599995393, 30.83849762800008421 -26.30280105999992202, 30.83850221700004113 -26.30288136999990911, 30.838442556000075 -26.30297774499990737, 30.83841961100006301 -26.30300298599991038, 30.83837142300006917 -26.30307411899991621, 30.83837830700008453 -26.30310624399993458, 30.83836453900005381 -26.30314066299990827, 30.83837830700008453 -26.30315901999995276, 30.83837371800007077 -26.30320032299994182, 30.83835306600008153 -26.30325080399995841, 30.83830335000004652 -26.30336515399994823, 30.83829723000008016 -26.30344470099993259, 30.83826969500006498 -26.30350283199993555, 30.83826969500006498 -26.30357014199995547, 30.83826663500008181 -26.30361297399991827, 30.83826051600004803 -26.30366192599990427, 30.83822380200007274 -26.30369252099990263, 30.83819320700007438 -26.30372617599994101, 30.83818708700005118 -26.30377818699992076, 30.83814119500004836 -26.30381796099993608, 30.83810754200004567 -26.30386079299995572, 30.83811977900006696 -26.30390668599994797, 30.83807388500008528 -26.30397399499992162, 30.83798966100005146 -26.30403908399995316, 30.83791135000006989 -26.30412783099990293, 30.83789586200003896 -26.30418634399995881, 30.83784767500003454 -26.30422592699994766, 30.83777711500005125 -26.30426722999993672, 30.83777539400006162 -26.30429304399990542, 30.83775130000003628 -26.30433090599990464, 30.83771516000007296 -26.30437220899995054, 30.83768418200008909 -26.30439458299991884, 30.83765664700007392 -26.30442555899992385, 30.83762739000007969 -26.30444793199990272, 30.83759985500006451 -26.30448751299991272, 30.83759641400007467 -26.30452537499991195, 30.83757748200008564 -26.30455291099991655, 30.83756027200007566 -26.30457528299990599, 30.83752929400003495 -26.30459937699993134, 30.83748799200003532 -26.30462519199994631, 30.83747422400006144 -26.30464756299994633, 30.83745529300006183 -26.30468714699992461, 30.83745012900004667 -26.30470779799992442, 30.83747594500005107 -26.30472328699994478, 30.83745873500004109 -26.30474221799994439, 30.83745529300006183 -26.30476975299990272, 30.83746561900005645 -26.30479384599993864, 30.83746561900005645 -26.3048248239999225, 30.83745012900004667 -26.3048523599999271, 30.83742947900003628 -26.30489538499995206, 30.83743464100007259 -26.3049143149999054, 30.83741054800003667 -26.30495045499992557, 30.83741226900008314 -26.30497110699991481, 30.83742087400008813 -26.30499692099994036, 30.83738645400006817 -26.30504338699995515, 30.83736924600003704 -26.3050795279999079, 30.83740022200004205 -26.30510534199993344, 30.83739678000006279 -26.30518278599993209, 30.83740882700004704 -26.30526195099992037, 30.83742775800004665 -26.30529464799991501, 30.83745873500004109 -26.30531185899991442, 30.83748627100004569 -26.30533595199995034, 30.83750175900007662 -26.30538069799990808, 30.8375155270000505 -26.30541167499990252, 30.83753617900003974 -26.30542200099995398, 30.83753101600007085 -26.30544781499992268, 30.83751724900008639 -26.30548567699992191, 30.83753101600007085 -26.30551665399991634, 30.83751036400008161 -26.30554074799994169, 30.83751208500007124 -26.30558377199992037, 30.83749831700004052 -26.3056113089999144, 30.83752069000007623 -26.30565777299995034, 30.83748627100004569 -26.3057162869999388, 30.83753617900003974 -26.30574382199995398, 30.83755510900004992 -26.30575758999992786, 30.83756027200007566 -26.30578684699992209, 30.8375430630000551 -26.30579372999994803, 30.83753790000008621 -26.30581610399991632, 30.83753101600007085 -26.30591936199994052, 30.83750003800008699 -26.30595206099991401, 30.83748885300008169 -26.30600675399995225, 30.83745981100008748 -26.30603676399994129, 30.83746077900008231 -26.3060677399999463, 30.83748982100007652 -26.30610549599992964, 30.83749659500006146 -26.30613647299992408, 30.83749950100008164 -26.30615389599995524, 30.8375053090000506 -26.3061839069999337, 30.83751014900008158 -26.30622262899993302, 30.83747723500005122 -26.30623134199993274, 30.83748207600007163 -26.30628070999995316, 30.83749175700006617 -26.30632911399993645, 30.837492725000061 -26.30637654799994607, 30.83747917200008715 -26.30644043899991402, 30.83748498000005611 -26.30647432099993921, 30.83745981100008748 -26.3064946499999337, 30.83746852300004093 -26.30652659499992296, 30.83745787500004099 -26.30656822099990677, 30.83741528100006235 -26.30661468699992156, 30.83737752700005785 -26.30663791999995738, 30.83737462300007337 -26.30667276999992055, 30.83735332600008405 -26.30672020399993016, 30.83733977300005336 -26.30676376599990363, 30.8373136360000899 -26.30681507299993882, 30.83729137100004891 -26.30682765699992842, 30.83727685100006966 -26.30684701799992808, 30.83724780900007545 -26.30689735699991161, 30.83722651200008613 -26.30694672699991088, 30.83721973500007607 -26.30697189599993635, 30.83722748000008096 -26.30701352199992016, 30.83724587300008579 -26.30703869099994563, 30.83725942500007022 -26.30708806199993433, 30.83728749800008018 -26.30712097499991842, 30.83729137100004891 -26.30715388899994878, 30.83731847700005346 -26.30718389799994839, 30.83732912400006398 -26.30722455599993737, 30.83729814700006955 -26.30727005399995733, 30.83730105100005403 -26.30730780799990498, 30.83730298700004369 -26.30735330599992494, 30.83732912400006398 -26.30738621899990903, 30.83733977300005336 -26.3074230069999544, 30.83732234700005392 -26.30744139799992354, 30.83732718800007433 -26.30749076899991223, 30.83734945300005847 -26.30752658599993765, 30.83736978100006354 -26.30755853099992692, 30.83741043900005252 -26.30758757299992112, 30.83743173700008811 -26.30761855099990498, 30.83745400100008283 -26.30764952799995626, 30.83745496900007765 -26.30766501699991977, 30.83747239500007709 -26.30769308999992973, 30.83748982100007652 -26.3077201969999237, 30.83750918100008676 -26.30773858799994969, 30.83751208500007124 -26.30777440599990769, 30.83753338300004998 -26.30778215099991257, 30.83753725300005044 -26.30782764899993253, 30.83754209500006027 -26.30786733899992669, 30.83753531900003964 -26.30790315599995211, 30.8375430630000551 -26.30795639899992011, 30.83754983900007574 -26.30797188799994046, 30.83755274300006022 -26.30801641799990875, 30.83757307300004413 -26.3080406189999394, 30.83757887900003425 -26.30806578899995429, 30.83758565700009058 -26.30809579699990763, 30.83760598600008507 -26.30812967899993282, 30.83760017700006983 -26.3081974409999475, 30.8375827510000704 -26.30826133299990488, 30.8375556470000447 -26.30830295899994553, 30.83749369100007698 -26.30838524299991832, 30.8374675550000461 -26.30842009299993833, 30.83746077900008231 -26.30845494099992266, 30.83748691700003519 -26.30851302499991107, 30.83750046900007646 -26.30857304399995655, 30.83749756300005629 -26.30864467899993997, 30.83750821300003508 -26.30870857099995419, 30.83752370200005544 -26.30877246099993272, 30.83752079800007095 -26.3088131189999217, 30.83752563800004509 -26.30883247999992136, 30.83752176600006578 -26.30885861799993108, 30.8375053090000506 -26.30890121199990972, 30.83753435100004481 -26.30892541299994036, 30.83754209500006027 -26.30900091999990309, 30.83754887100008091 -26.30905416299992794, 30.83752951000008125 -26.30907545999991726, 30.83754209500006027 -26.30908417199992755, 30.83755371100005505 -26.3091112779999321, 30.8375304790000655 -26.30913063799994234, 30.83757113600006505 -26.30915290299992648, 30.83759243300005437 -26.30918388099991034, 30.83759630500009052 -26.30923131499991996, 30.83757694500008029 -26.30926035599992474, 30.83755661500003953 -26.30929036599991377, 30.83757404100003896 -26.30931166299990309, 30.83757694500008029 -26.30934263999995437, 30.83755661500003953 -26.30937264999994341, 30.83754887100008091 -26.30942105199994785, 30.83753338300004998 -26.30942976399995814, 30.83753144700006033 -26.3095110799999361, 30.83751014900008158 -26.30952753699995128, 30.83753435100004481 -26.30955173799992508, 30.83752854200008642 -26.30961272499990855, 30.83751305300006607 -26.30963595799994437, 30.83748691700003519 -26.30963595799994437, 30.83747529900006157 -26.3096495099999288, 30.83747239500007709 -26.309682425999938, 30.83748304400006646 -26.30970662599992238, 30.83751692500004538 -26.30970565799992755, 30.83752660600003992 -26.30971533799993267, 30.83755758300003436 -26.30973760299991682, 30.83756048700007568 -26.30976954999994177, 30.83754790300008608 -26.30979762199990546, 30.83755467900004987 -26.30983924799994611, 30.83754693500003441 -26.30987506599990411, 30.83755080700007056 -26.30990700999990395, 30.83755855100008603 -26.30993992599991316, 30.83757113600006505 -26.30996606199994403, 30.83759049700006472 -26.30999607099994364, 30.8375827510000704 -26.31001930499991204, 30.83758662500008541 -26.31004544199993234, 30.83757404100003896 -26.31006286699994234, 30.83758178300007557 -26.31010739699991063, 30.83760308100005432 -26.31016838399995095, 30.83763405900003818 -26.31017806399995607, 30.83765148400004819 -26.31021484999990889, 30.83766310100008923 -26.31022549799990884, 30.83767762100006848 -26.31023808299994471, 30.83768536500008395 -26.31026421999990816, 30.83768536500008395 -26.31030487799995399, 30.83768826900006843 -26.31033585599993785, 30.83769407800008366 -26.31034456799994814, 30.83769214200003717 -26.31038038599990614, 30.837674717000084 -26.31041039599995202, 30.837674717000084 -26.31044040499995162, 30.83766890900005819 -26.31046750999990991, 30.8376456750000898 -26.31047815799990985, 30.83762631500007956 -26.31045782999990479, 30.83759824100008018 -26.31044137299994645, 30.83755080700007056 -26.31047428599993054, 30.8375198290000867 -26.31051784799990401, 30.83753241500005515 -26.31056044199993948, 30.83751111700007641 -26.31057980299993915, 30.8375053090000506 -26.31064078999992262, 30.83750918100008676 -26.31067563999994263, 30.83749562700006663 -26.31069596899993712, 30.83748207600007163 -26.31072984999991604, 30.83745981100008748 -26.31076566799993088, 30.8374375460000465 -26.310775347999936, 30.83741818500004683 -26.31079083699995635, 30.83738527100007332 -26.31081697399991981, 30.83734267700003784 -26.31082084699994539, 30.83732815600006916 -26.31084988799995017, 30.83723425700003418 -26.31087892899995495, 30.83718585400004031 -26.31091765099995428, 30.83714616500003558 -26.31097670199994809, 30.83713551500005678 -26.31103188099990575, 30.83713067500008265 -26.31107156999991048, 30.83711615400005712 -26.31109189899990497, 30.83712680300004649 -26.31110738799992532, 30.83712583500005167 -26.3111238449999405, 30.83710647500004143 -26.31115578999992977, 30.83708614500005751 -26.31119644799991875, 30.83709098500008849 -26.31122839399995428, 30.83709195300008332 -26.31128163599993286, 30.8370822730000782 -26.31130583699990666, 30.83706968800004233 -26.31132810299993707, 30.83706387900008394 -26.31135327099991628, 30.83710647500004143 -26.31137263299990536, 30.83711615400005712 -26.31138618499994664, 30.83712389900006201 -26.31139876999992566, 30.83712486700005684 -26.3114171629999305, 30.83710840900005223 -26.31145491699993499, 30.83710840900005223 -26.31147427899992408, 30.8371200270000827 -26.31150138299994978, 30.83712680300004649 -26.3115468809999129, 30.8371200270000827 -26.31157592199991768, 30.8371200270000827 -26.31160012299994833, 30.83715778000004093 -26.3116281969999477, 30.83715874800003576 -26.31165530199990599, 30.83716746100003547 -26.31168434299991077, 30.83717230100006645 -26.31172112899992044, 30.83717617300004576 -26.31176953199991431, 30.83718488600004548 -26.31178114699991966, 30.83718295000005583 -26.31182374099995513, 30.83717230100006645 -26.311872143999949, 30.83718295000005583 -26.31191861099995322, 30.8371326110000723 -26.31196798099995249, 30.8371326110000723 -26.31199314899993169, 30.83712293100006718 -26.31201928699994141, 30.83711518600006229 -26.31204929699993045, 30.83709292100007815 -26.31208608299994012, 30.8370561360000579 -26.31213158099990324, 30.8370145100000741 -26.31217127099995423, 30.83698546800007989 -26.31220515299992257, 30.8369506190000493 -26.31223225699994828, 30.83692835300007573 -26.31224484299991673, 30.83691673700008096 -26.31228549999991628, 30.83689447100005054 -26.31230582899991077, 30.83690802400008124 -26.31234067899993079, 30.83688672700003508 -26.31236100799992528, 30.83689060100005008 -26.31236875199994074, 30.83689737500003503 -26.31240069699993001, 30.83689543900004537 -26.31243361099990352, 30.83691480100003446 -26.31245297199990318, 30.83691189700004998 -26.31247814099992866, 30.83690318400005026 -26.31252363899994862, 30.83693319500008556 -26.31254203199995345, 30.83692351300004475 -26.31257784999991145, 30.83694190600004958 -26.31259914699995761, 30.8369757890000642 -26.31264754899990521, 30.83698353100004397 -26.31269207899993035, 30.83698740400006955 -26.31272112099992455, 30.83697385300007454 -26.3127491939999345, 30.83695836300006476 -26.31280534099994384, 30.83694190600004958 -</t>
+  </si>
+  <si>
+    <t>26.31284115799991241, 30.83699030800005403 -26.31284793499992247, 30.83697772500005385 -26.31288181599995823, 30.83697772500005385 -26.31292731399992135, 30.83703580700006341 -26.3129302189999521, 30.83705419900007882 -26.31293118699994693, 30.83707646400006297 -26.31290795299992169, 30.83710357100005695 -26.31291666599992141, 30.83711325000007264 -26.31294473899993136, 30.83712777100004132 -26.31296893999990516, 30.83713648300005161 -26.31297087599995166, 30.83716455700005099 -26.31296119599994654, 30.83718017500007136 -26.3129711469999279, 30.83721908900008657 -26.31301006099994311, 30.83725313800005097 -26.31298087599992641, 30.83727746000005254 -26.31302951799995071, 30.83726286700004948 -26.31307815999991817, 30.83732123900006172 -26.31312193999991678, 30.83737474600007999 -26.31318517499994414, 30.83736988200007545 -26.31328246099991475, 30.83740879600009066 -26.31333596799993302, 30.83746230300005209 -26.31337001799994368, 30.83750608200006127 -26.31337488199994823, 30.83756931600004236 -26.31342352499990511, 30.83766660300005924 -26.31347216799991884, 30.83774929400004794 -26.31351594599993859, 30.8378417180000497 -26.31355486099994323, 30.83793413800003691 -26.31359863899990614, 30.83791954500009069 -26.31369105999993963, 30.83793413800003691 -26.31372997599993369, 30.83794873000005055 -26.31377375199991775, 30.83793413800003691 -26.31381266699992239, 30.83790008800008309 -26.31384671799992248, 30.83790495200008763 -26.31388076699994372, 30.83792927400008921 -26.31390995199990357, 30.83795359500004452 -26.31396345899992184, 30.83798278100005064 -26.31404128899993111, 30.8380168310000613 -26.31414343899990627, 30.8380168310000613 -26.3141823539999109, 30.83803142500005379 -26.31430882399990878, 30.83803142500005379 -26.31438665299992863, 30.83807497100008277 -26.31447746899993945, 30.83807846800004882 -26.31450019999994083, 30.83809595500008527 -26.31455440399992085, 30.83808896000005006 -26.31461734999993496, 30.83807497100008277 -26.31464532599994754, 30.83809070800003838 -26.31466106299990315, 30.83809070800003838 -26.31468379399990454, 30.83810644500005083 -26.31469778199993925, 30.83813267200008568 -26.31472400999990668, 30.838162397000076 -26.31476072799995336, 30.83818163100005449 -26.31476947099992003, 30.83821135500005539 -26.31479919599991035, 30.83825506800008043 -26.31483940999993365, 30.83830402700004925 -26.3148796259999358, 30.83833724900006246 -26.31490935199991554, 30.8384054390000415 -26.3150072689999206, 30.83845789600007947 -26.31507895799995822, 30.83845803700006627 -26.31510377799992284)))</t>
+  </si>
+  <si>
+    <t>Mafumulo SP</t>
+  </si>
+  <si>
+    <t>Mafumulo</t>
+  </si>
+  <si>
+    <t>MultiPolygon (((30.79894036500007815 -26.40313298799992481, 30.79890590600007272 -26.40318122999991601, 30.79874010300005693 -26.40334703399992122, 30.79879056400005766 -26.40352725599990436, 30.79850941800003739 -26.40372189599992225, 30.79815422200005059 -26.4038568289999489, 30.79731873200006476 -26.40418777099995395, 30.79649409100005641 -26.40458381499990992, 30.79425742700004776 -26.40560933999995541, 30.79377793900005145 -26.40507299999995894, 30.79365104200007863 -26.40492865499993513, 30.79356697100007523 -26.40484934299990982, 30.7931275870000718 -26.40432588699991356, 30.79295944700004384 -26.40416567899995925, 30.79268027100005156 -26.40399119399995698, 30.79264220100003513 -26.40390871099992864, 30.79262951000004023 -26.403802432999953, 30.79261840800006667 -26.40368346599990446, 30.79261523600007422 -26.40361049999995657, 30.79261364900008857 -26.40354863599992541, 30.79264220100003513 -26.40348994599992238, 30.79268978800007517 -26.40340746299995089, 30.79273420200007649 -26.40331228899992766, 30.7928198580000867 -26.40307911399992236, 30.7928753770000867 -26.40298076699991725, 30.79297848100003421 -26.40287607499993783, 30.79306889600007935 -26.402815799999928, 30.79317676000005122 -26.40276821299994481, 30.79322943800008261 -26.40275451699994846, 30.79325559800008705 -26.40274771499991857, 30.79338348900006395 -26.40233359299992344, 30.79342703600008235 -26.40208240599991996, 30.79342155900008038 -26.40199340199990274, 30.79342210900006194 -26.40184566199991423, 30.79340102100007925 -26.40158809199994039, 30.79339238900007558 -26.40150131799993005, 30.79352653100005455 -26.40147163199992519, 30.79356050200004802 -26.40142775299995037, 30.79358173300005319 -26.401392365999925, 30.79361570600008235 -26.40133999399995446, 30.79363976800004821 -26.40131451499991044, 30.79366241500008528 -26.40128762199992707, 30.79368930900005807 -26.40125223499995855, 30.7937275260000547 -26.4012196789999507, 30.79375795900006096 -26.40122193499990999, 30.79380175000005693 -26.40122193499990999, 30.79384076400003778 -26.40121954699992557, 30.79384474500005808 -26.40123547099994994, 30.79385589100007792 -26.40123387799991406, 30.79388455400004432 -26.40122830399991471, 30.79390286700004253 -26.40122193499990999, 30.79392038300005652 -26.40122352799994587, 30.79393153000006578 -26.40122750899990933, 30.7939466580000385 -26.40123706299993955, 30.79396815600006221 -26.40123785899993436, 30.79399363400005996 -26.40124900599994362, 30.79400478000007979 -26.40124422899992851, 30.79401115000007394 -26.40122910199994521, 30.79403662800007169 -26.40122750899990933, 30.79404299800006584 -26.40121636199995692, 30.79407007000008889 -26.40119565999992801, 30.79407803100008323 -26.40117575599992961, 30.79409793600007106 -26.40117336699995576, 30.79410828600003924 -26.40116381299992554, 30.79414650400008213 -26.40113753799994356, 30.79416481600003408 -26.40112161399991919, 30.79419427500005213 -26.40111604099990927, 30.79419029400008867 -26.40109693199991625, 30.7942038310000612 -26.40108737799994287, 30.79423886400007859 -26.4010618989999557, 30.79429380000004812 -26.4010427909999521, 30.79430096600003708 -26.40102607099993293, 30.79430892800007769 -26.40100218499992479, 30.79433042500005513 -26.40096874399995386, 30.79434077600006958 -26.40095680099994979, 30.79435266000007232 -26.4009557249999034, 30.79438096900008759 -26.4009557249999034, 30.79442060200005926 -26.40094062699995447, 30.79442815100009057 -26.40092364099990618, 30.79442815100009057 -26.40089721899994402, 30.79443758800005071 -26.40088589599992019, 30.79444891100007453 -26.40085569899991924, 30.79446657500005813 -26.40082622599993556, 30.79446737100005294 -26.40077606399995602, 30.79448727500005134 -26.4007696949999513, 30.79449921900004483 -26.4007338659999391, 30.79450399700004937 -26.40068768599991245, 30.79451036600005409 -26.40065026499991063, 30.7945191240000895 -26.40061682499992912, 30.79453266000007261 -26.40060328899994602, 30.79453186300008838 -26.40058099599991692, 30.79452549400008365 -26.40055073999991464, 30.79454221400004599 -26.40048943399995096, 30.7945605270000442 -26.40043927199991458, 30.79460352100005593 -26.40043767899993554, 30.79460989100005008 -26.40042095899991637, 30.79461307600007558 -26.40039229699993939, 30.7946186490000855 -26.40035328199991227, 30.79463457300005302 -26.40033178599992425, 30.79462661100006926 -26.40030789999991612, 30.79463298100006341 -26.40026012799995669, 30.79467438400007495 -26.40022987299994384, 30.79468632600008959 -26.40020996799995601, 30.79469747300004201 -26.40017811999990727, 30.7947189700000763 -26.40014786399990498, 30.7947484290000375 -26.40011840499994378, 30.79475081800006819 -26.40009531499993045, 30.79477151900005083 -26.40007779899991647, 30.7947834620000549 -26.40007859499991127, 30.79480575600007342 -26.40004833899990899, 30.79483123400007116 -26.4000204719999374, 30.79484476900006484 -26.40001012199991237, 30.79485113900005899 -26.39999180899991416, 30.79485910200008902 -26.39997110799993152, 30.79487661700005674 -26.39996234999995295, 30.79488247200004025 -26.3999447989999112, 30.79489063100004387 -26.39992276899994295, 30.79489144700005454 -26.39990481799992494, 30.79491266200005839 -26.39989339399994606, 30.79493469400006234 -26.39989584199992123, 30.79495672200005174 -26.3998729959999423, 30.7949673300000768 -26.3998550449999243, 30.79497630600008051 -26.39982567099991684, 30.79498609700004863 -26.39978813699991633, 30.79499425700004167 -26.39977018599995517, 30.79499670500007369 -26.39973183699993342, 30.79500731200005248 -26.39968287999994345, 30.79502607900008115 -26.39960781199994244, 30.79504484500006356 -26.3995963899999424, 30.79504403000004231 -26.39957435899992788, 30.79502607900008115 -26.39954253699994524, 30.79503179000005275 -26.39950255599995899, 30.79504495200006886 -26.39949133799990477, 30.79507862800005569 -26.399446333999947, 30.79509384600004296 -26.39943111599990289, 30.79508775900006867 -26.39938241899994864, 30.79506188800007749 -26.39937481099991601, 30.79505580200003578 -26.39934741899992332, 30.79505580200003578 -26.39932154999991099, 30.7950679760000412 -26.39930176799992978, 30.79508623700007774 -26.39928198499995915, 30.79509232400005203 -26.39925459399995589, 30.79508928000007018 -26.39923480999993899, 30.79504819300007057 -26.39919828899991217, 30.79505275800005393 -26.39918307099992489, 30.79507406300007233 -26.39917089699991948, 30.79508928000007018 -26.39914807099995642, 30.7951060210000378 -26.3991328529999123, 30.79514558500005705 -26.39913437499990323, 30.79516689000007545 -26.39912372299994558, 30.79519732500006057 -26.39912980999991987, 30.7952338460000874 -26.39916785299993762, 30.79526428100007251 -26.39919067999994695, 30.79529319500005613 -26.39918611499990675, 30.7953099340000449 -26.39917241899991041, 30.79531450000007453 -26.39914959399993677, 30.79532058600005939 -26.39911611499991295, 30.79530384600008119 -26.39909480999995139, 30.79527493400007643 -26.39906437499990943, 30.79526580300006344 -26.39903393999992431, 30.79526580300006344 -26.39901111299991499, 30.79529623800004856 -26.39896850299993503, 30.79532363000004125 -26.39893350299990971, 30.79533276000006481 -26.39890154699992308, 30.79532515100004275 -26.39886654699995461, 30.79535863000006657 -26.39886502399991741, 30.79541036900008066 -26.39886350299991591, 30.79543167400004222 -26.39884828599991806, 30.79544689100004007 -26.39881785199992237, 30.79547732500003576 -26.39881328599994958, 30.79548797900008594 -26.39880111199994417, 30.79548797900008594 -26.39877067699995905, 30.79550928300005808 -26.39875850299995363, 30.79555037000005768 -26.39875850299995363, 30.79563254500004632 -26.39875850299995363, 30.79563711100007595 -26.3987295899999026, 30.7956538490000753 -26.39870371899991142, 30.79567819700008613 -26.39865958899991938, 30.79567819700008613 -26.39863523999991912, 30.79566602300008071 -26.39859111099991651, 30.79567667500003836 -26.39855611099994803, 30.79569950200004769 -26.39854393699994262, 30.79572385000005852 -26.39854241499995169, 30.79576341600005662 -26.39855915399994046, 30.79578776200008861 -26.39855611099994803, 30.79582885000007764 -26.39853937099991299, 30.79589409500005104 -26.39851673499993012, 30.79593746500006546 -26.39849162599995225, 30.79596828000006781 -26.39845167999993691, 30.79600708500004203 -26.39843456099993091, 30.79604703100005736 -26.39842542999991792, 30.79611322800008111 -26.39841287599995212, 30.7961280640000723 -26.39839803999990409, 30.79615887900007465 -26.39836722299992289, 30.79618969500006642 -26.39833640699993111, 30.79622393400006786 -26.3983409729999039, 30.79623991300007901 -26.39835923299995102, 30.79625132600006054 -26.39837407099992106, 30.79629469600007496 -26.39837407099992106, 30.79633007600006067 -26.39835923299995102, 30.79635746800005336 -26.3983466799999178, 30.79638371800007235 -26.39832956099991179, 30.79641453200008527 -26.39830331099994964, 30.79645219700006464 -26.39829303799990612, 30.79651382700006934 -26.39828847299992276, 30.79654121900006203 -26.39827363599994214, 30.79656290400004082 -26.39826222299990377, 30.79658002300004682 -26.39826222299990377, 30.79661442600007604 -26.39827229999991687, 30.79666469200003576 -26.39844534499991369, 30.79699057900006665 -26.39953509299994039, 30.79734218000004375 -26.40056336099991086, 30.79783545000003642 -26.40200594499992803, 30.79803318800009038 -26.40247925799991435, 30.79808109000003924 -26.40254457899993668, 30.7981442330000732 -26.40260227899995016, 30.79824874600006979 -26.40267848599995659, 30.79838047600003392 -26.40276557999993656, 30.79848281300007784 -26.40281130499994333, 30.79865155600003845 -26.40292779299994663, 30.79875607100007073 -26.40300508899991883, 30.79894036500007815 -26.40313298799992481)))</t>
+  </si>
+  <si>
+    <t>Fernie SP</t>
+  </si>
+  <si>
+    <t>Fernie</t>
   </si>
 </sst>
 </file>
@@ -487,8 +892,150 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -533,7 +1080,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -554,6 +1101,77 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -574,6 +1192,77 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -903,10 +1592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -2375,6 +3064,2121 @@
       </c>
       <c r="R29">
         <v>59101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" t="s">
+        <v>10</v>
+      </c>
+      <c r="L32" t="s">
+        <v>11</v>
+      </c>
+      <c r="M32" t="s">
+        <v>12</v>
+      </c>
+      <c r="N32" t="s">
+        <v>13</v>
+      </c>
+      <c r="O32" t="s">
+        <v>14</v>
+      </c>
+      <c r="P32" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>16</v>
+      </c>
+      <c r="R32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33">
+        <v>70008</v>
+      </c>
+      <c r="D33">
+        <v>8720085</v>
+      </c>
+      <c r="E33">
+        <v>872036002</v>
+      </c>
+      <c r="F33" t="s">
+        <v>142</v>
+      </c>
+      <c r="G33">
+        <v>872036</v>
+      </c>
+      <c r="H33" t="s">
+        <v>143</v>
+      </c>
+      <c r="I33" t="s">
+        <v>144</v>
+      </c>
+      <c r="J33">
+        <v>872</v>
+      </c>
+      <c r="K33" t="s">
+        <v>145</v>
+      </c>
+      <c r="L33" t="s">
+        <v>146</v>
+      </c>
+      <c r="M33">
+        <v>831</v>
+      </c>
+      <c r="N33" t="s">
+        <v>147</v>
+      </c>
+      <c r="O33" t="s">
+        <v>36</v>
+      </c>
+      <c r="P33">
+        <v>8</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>37</v>
+      </c>
+      <c r="R33">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34">
+        <v>72189</v>
+      </c>
+      <c r="D34">
+        <v>8720162</v>
+      </c>
+      <c r="E34">
+        <v>872046001</v>
+      </c>
+      <c r="F34" t="s">
+        <v>150</v>
+      </c>
+      <c r="G34">
+        <v>872046</v>
+      </c>
+      <c r="H34" t="s">
+        <v>151</v>
+      </c>
+      <c r="I34" t="s">
+        <v>144</v>
+      </c>
+      <c r="J34">
+        <v>872</v>
+      </c>
+      <c r="K34" t="s">
+        <v>145</v>
+      </c>
+      <c r="L34" t="s">
+        <v>146</v>
+      </c>
+      <c r="M34">
+        <v>831</v>
+      </c>
+      <c r="N34" t="s">
+        <v>147</v>
+      </c>
+      <c r="O34" t="s">
+        <v>36</v>
+      </c>
+      <c r="P34">
+        <v>8</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>37</v>
+      </c>
+      <c r="R34">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" t="s">
+        <v>152</v>
+      </c>
+      <c r="B35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35">
+        <v>71939</v>
+      </c>
+      <c r="D35">
+        <v>8720252</v>
+      </c>
+      <c r="E35">
+        <v>872022002</v>
+      </c>
+      <c r="F35" t="s">
+        <v>154</v>
+      </c>
+      <c r="G35">
+        <v>872022</v>
+      </c>
+      <c r="H35" t="s">
+        <v>155</v>
+      </c>
+      <c r="I35" t="s">
+        <v>144</v>
+      </c>
+      <c r="J35">
+        <v>872</v>
+      </c>
+      <c r="K35" t="s">
+        <v>145</v>
+      </c>
+      <c r="L35" t="s">
+        <v>146</v>
+      </c>
+      <c r="M35">
+        <v>831</v>
+      </c>
+      <c r="N35" t="s">
+        <v>147</v>
+      </c>
+      <c r="O35" t="s">
+        <v>36</v>
+      </c>
+      <c r="P35">
+        <v>8</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>37</v>
+      </c>
+      <c r="R35">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" t="s">
+        <v>156</v>
+      </c>
+      <c r="B36" t="s">
+        <v>157</v>
+      </c>
+      <c r="C36">
+        <v>83602</v>
+      </c>
+      <c r="D36">
+        <v>9840150</v>
+      </c>
+      <c r="E36">
+        <v>984062001</v>
+      </c>
+      <c r="F36" t="s">
+        <v>158</v>
+      </c>
+      <c r="G36">
+        <v>984062</v>
+      </c>
+      <c r="H36" t="s">
+        <v>159</v>
+      </c>
+      <c r="I36" t="s">
+        <v>160</v>
+      </c>
+      <c r="J36">
+        <v>984</v>
+      </c>
+      <c r="K36" t="s">
+        <v>161</v>
+      </c>
+      <c r="L36" t="s">
+        <v>162</v>
+      </c>
+      <c r="M36">
+        <v>947</v>
+      </c>
+      <c r="N36" t="s">
+        <v>163</v>
+      </c>
+      <c r="O36" t="s">
+        <v>26</v>
+      </c>
+      <c r="P36">
+        <v>9</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>27</v>
+      </c>
+      <c r="R36">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37">
+        <v>72068</v>
+      </c>
+      <c r="D37">
+        <v>8720421</v>
+      </c>
+      <c r="E37">
+        <v>872031001</v>
+      </c>
+      <c r="F37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G37">
+        <v>872031</v>
+      </c>
+      <c r="H37" t="s">
+        <v>167</v>
+      </c>
+      <c r="I37" t="s">
+        <v>144</v>
+      </c>
+      <c r="J37">
+        <v>872</v>
+      </c>
+      <c r="K37" t="s">
+        <v>145</v>
+      </c>
+      <c r="L37" t="s">
+        <v>146</v>
+      </c>
+      <c r="M37">
+        <v>831</v>
+      </c>
+      <c r="N37" t="s">
+        <v>147</v>
+      </c>
+      <c r="O37" t="s">
+        <v>36</v>
+      </c>
+      <c r="P37">
+        <v>8</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>37</v>
+      </c>
+      <c r="R37">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" t="s">
+        <v>186</v>
+      </c>
+      <c r="B38" t="s">
+        <v>187</v>
+      </c>
+      <c r="C38">
+        <v>83665</v>
+      </c>
+      <c r="D38">
+        <v>9840387</v>
+      </c>
+      <c r="E38">
+        <v>984073001</v>
+      </c>
+      <c r="F38" t="s">
+        <v>188</v>
+      </c>
+      <c r="G38">
+        <v>984073</v>
+      </c>
+      <c r="H38" t="s">
+        <v>189</v>
+      </c>
+      <c r="I38" t="s">
+        <v>160</v>
+      </c>
+      <c r="J38">
+        <v>984</v>
+      </c>
+      <c r="K38" t="s">
+        <v>161</v>
+      </c>
+      <c r="L38" t="s">
+        <v>162</v>
+      </c>
+      <c r="M38">
+        <v>947</v>
+      </c>
+      <c r="N38" t="s">
+        <v>163</v>
+      </c>
+      <c r="O38" t="s">
+        <v>26</v>
+      </c>
+      <c r="P38">
+        <v>9</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>27</v>
+      </c>
+      <c r="R38">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39" t="s">
+        <v>169</v>
+      </c>
+      <c r="C39">
+        <v>71913</v>
+      </c>
+      <c r="D39">
+        <v>8720147</v>
+      </c>
+      <c r="E39">
+        <v>872019001</v>
+      </c>
+      <c r="F39" t="s">
+        <v>170</v>
+      </c>
+      <c r="G39">
+        <v>872019</v>
+      </c>
+      <c r="H39" t="s">
+        <v>171</v>
+      </c>
+      <c r="I39" t="s">
+        <v>144</v>
+      </c>
+      <c r="J39">
+        <v>872</v>
+      </c>
+      <c r="K39" t="s">
+        <v>145</v>
+      </c>
+      <c r="L39" t="s">
+        <v>146</v>
+      </c>
+      <c r="M39">
+        <v>831</v>
+      </c>
+      <c r="N39" t="s">
+        <v>147</v>
+      </c>
+      <c r="O39" t="s">
+        <v>36</v>
+      </c>
+      <c r="P39">
+        <v>8</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>37</v>
+      </c>
+      <c r="R39">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" t="s">
+        <v>172</v>
+      </c>
+      <c r="B40" t="s">
+        <v>173</v>
+      </c>
+      <c r="C40">
+        <v>83182</v>
+      </c>
+      <c r="D40">
+        <v>9830174</v>
+      </c>
+      <c r="E40">
+        <v>983063001</v>
+      </c>
+      <c r="F40" t="s">
+        <v>174</v>
+      </c>
+      <c r="G40">
+        <v>983063</v>
+      </c>
+      <c r="H40" t="s">
+        <v>175</v>
+      </c>
+      <c r="I40" t="s">
+        <v>176</v>
+      </c>
+      <c r="J40">
+        <v>983</v>
+      </c>
+      <c r="K40" t="s">
+        <v>177</v>
+      </c>
+      <c r="L40" t="s">
+        <v>162</v>
+      </c>
+      <c r="M40">
+        <v>947</v>
+      </c>
+      <c r="N40" t="s">
+        <v>163</v>
+      </c>
+      <c r="O40" t="s">
+        <v>26</v>
+      </c>
+      <c r="P40">
+        <v>9</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>27</v>
+      </c>
+      <c r="R40">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41">
+        <v>72200</v>
+      </c>
+      <c r="D41">
+        <v>8720329</v>
+      </c>
+      <c r="E41">
+        <v>872049001</v>
+      </c>
+      <c r="F41" t="s">
+        <v>180</v>
+      </c>
+      <c r="G41">
+        <v>872049</v>
+      </c>
+      <c r="H41" t="s">
+        <v>181</v>
+      </c>
+      <c r="I41" t="s">
+        <v>144</v>
+      </c>
+      <c r="J41">
+        <v>872</v>
+      </c>
+      <c r="K41" t="s">
+        <v>145</v>
+      </c>
+      <c r="L41" t="s">
+        <v>146</v>
+      </c>
+      <c r="M41">
+        <v>831</v>
+      </c>
+      <c r="N41" t="s">
+        <v>147</v>
+      </c>
+      <c r="O41" t="s">
+        <v>36</v>
+      </c>
+      <c r="P41">
+        <v>8</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>37</v>
+      </c>
+      <c r="R41">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42" t="s">
+        <v>183</v>
+      </c>
+      <c r="C42">
+        <v>83544</v>
+      </c>
+      <c r="D42">
+        <v>9840271</v>
+      </c>
+      <c r="E42">
+        <v>984051001</v>
+      </c>
+      <c r="F42" t="s">
+        <v>184</v>
+      </c>
+      <c r="G42">
+        <v>984051</v>
+      </c>
+      <c r="H42" t="s">
+        <v>185</v>
+      </c>
+      <c r="I42" t="s">
+        <v>160</v>
+      </c>
+      <c r="J42">
+        <v>984</v>
+      </c>
+      <c r="K42" t="s">
+        <v>161</v>
+      </c>
+      <c r="L42" t="s">
+        <v>162</v>
+      </c>
+      <c r="M42">
+        <v>947</v>
+      </c>
+      <c r="N42" t="s">
+        <v>163</v>
+      </c>
+      <c r="O42" t="s">
+        <v>26</v>
+      </c>
+      <c r="P42">
+        <v>9</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>27</v>
+      </c>
+      <c r="R42">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43" t="s">
+        <v>226</v>
+      </c>
+      <c r="C43">
+        <v>71277</v>
+      </c>
+      <c r="D43">
+        <v>8710387</v>
+      </c>
+      <c r="E43">
+        <v>871006001</v>
+      </c>
+      <c r="F43" t="s">
+        <v>227</v>
+      </c>
+      <c r="G43">
+        <v>871006</v>
+      </c>
+      <c r="H43" t="s">
+        <v>228</v>
+      </c>
+      <c r="I43" t="s">
+        <v>229</v>
+      </c>
+      <c r="J43">
+        <v>871</v>
+      </c>
+      <c r="K43" t="s">
+        <v>230</v>
+      </c>
+      <c r="L43" t="s">
+        <v>146</v>
+      </c>
+      <c r="M43">
+        <v>831</v>
+      </c>
+      <c r="N43" t="s">
+        <v>147</v>
+      </c>
+      <c r="O43" t="s">
+        <v>36</v>
+      </c>
+      <c r="P43">
+        <v>8</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>37</v>
+      </c>
+      <c r="R43">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
+      <c r="A44" t="s">
+        <v>231</v>
+      </c>
+      <c r="C44">
+        <v>72147</v>
+      </c>
+      <c r="D44">
+        <v>8720386</v>
+      </c>
+      <c r="E44">
+        <v>872040001</v>
+      </c>
+      <c r="F44" t="s">
+        <v>232</v>
+      </c>
+      <c r="G44">
+        <v>872040</v>
+      </c>
+      <c r="H44" t="s">
+        <v>233</v>
+      </c>
+      <c r="I44" t="s">
+        <v>144</v>
+      </c>
+      <c r="J44">
+        <v>872</v>
+      </c>
+      <c r="K44" t="s">
+        <v>145</v>
+      </c>
+      <c r="L44" t="s">
+        <v>146</v>
+      </c>
+      <c r="M44">
+        <v>831</v>
+      </c>
+      <c r="N44" t="s">
+        <v>147</v>
+      </c>
+      <c r="O44" t="s">
+        <v>36</v>
+      </c>
+      <c r="P44">
+        <v>8</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>37</v>
+      </c>
+      <c r="R44">
+        <v>59205</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" t="s">
+        <v>8</v>
+      </c>
+      <c r="I48" t="s">
+        <v>9</v>
+      </c>
+      <c r="J48" t="s">
+        <v>10</v>
+      </c>
+      <c r="K48" t="s">
+        <v>11</v>
+      </c>
+      <c r="L48" t="s">
+        <v>12</v>
+      </c>
+      <c r="M48" t="s">
+        <v>13</v>
+      </c>
+      <c r="N48" t="s">
+        <v>14</v>
+      </c>
+      <c r="O48" t="s">
+        <v>15</v>
+      </c>
+      <c r="P48" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
+      <c r="A49" t="s">
+        <v>190</v>
+      </c>
+      <c r="B49">
+        <v>71790</v>
+      </c>
+      <c r="C49">
+        <v>8720191</v>
+      </c>
+      <c r="D49">
+        <v>872002001</v>
+      </c>
+      <c r="E49" t="s">
+        <v>191</v>
+      </c>
+      <c r="F49">
+        <v>872002</v>
+      </c>
+      <c r="G49" t="s">
+        <v>192</v>
+      </c>
+      <c r="H49" t="s">
+        <v>144</v>
+      </c>
+      <c r="I49">
+        <v>872</v>
+      </c>
+      <c r="J49" t="s">
+        <v>145</v>
+      </c>
+      <c r="K49" t="s">
+        <v>146</v>
+      </c>
+      <c r="L49">
+        <v>831</v>
+      </c>
+      <c r="M49" t="s">
+        <v>147</v>
+      </c>
+      <c r="N49" t="s">
+        <v>36</v>
+      </c>
+      <c r="O49">
+        <v>8</v>
+      </c>
+      <c r="P49" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q49">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17">
+      <c r="A50" t="s">
+        <v>193</v>
+      </c>
+      <c r="B50">
+        <v>71822</v>
+      </c>
+      <c r="C50">
+        <v>8720201</v>
+      </c>
+      <c r="D50">
+        <v>872007001</v>
+      </c>
+      <c r="E50" t="s">
+        <v>194</v>
+      </c>
+      <c r="F50">
+        <v>872007</v>
+      </c>
+      <c r="G50" t="s">
+        <v>195</v>
+      </c>
+      <c r="H50" t="s">
+        <v>144</v>
+      </c>
+      <c r="I50">
+        <v>872</v>
+      </c>
+      <c r="J50" t="s">
+        <v>145</v>
+      </c>
+      <c r="K50" t="s">
+        <v>146</v>
+      </c>
+      <c r="L50">
+        <v>831</v>
+      </c>
+      <c r="M50" t="s">
+        <v>147</v>
+      </c>
+      <c r="N50" t="s">
+        <v>36</v>
+      </c>
+      <c r="O50">
+        <v>8</v>
+      </c>
+      <c r="P50" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q50">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
+      <c r="A51" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51">
+        <v>71849</v>
+      </c>
+      <c r="C51">
+        <v>8720368</v>
+      </c>
+      <c r="D51">
+        <v>872008001</v>
+      </c>
+      <c r="E51" t="s">
+        <v>197</v>
+      </c>
+      <c r="F51">
+        <v>872008</v>
+      </c>
+      <c r="G51" t="s">
+        <v>198</v>
+      </c>
+      <c r="H51" t="s">
+        <v>144</v>
+      </c>
+      <c r="I51">
+        <v>872</v>
+      </c>
+      <c r="J51" t="s">
+        <v>145</v>
+      </c>
+      <c r="K51" t="s">
+        <v>146</v>
+      </c>
+      <c r="L51">
+        <v>831</v>
+      </c>
+      <c r="M51" t="s">
+        <v>147</v>
+      </c>
+      <c r="N51" t="s">
+        <v>36</v>
+      </c>
+      <c r="O51">
+        <v>8</v>
+      </c>
+      <c r="P51" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q51">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17">
+      <c r="A52" t="s">
+        <v>199</v>
+      </c>
+      <c r="B52">
+        <v>71864</v>
+      </c>
+      <c r="C52">
+        <v>8720167</v>
+      </c>
+      <c r="D52">
+        <v>872011001</v>
+      </c>
+      <c r="E52" t="s">
+        <v>200</v>
+      </c>
+      <c r="F52">
+        <v>872011</v>
+      </c>
+      <c r="G52" t="s">
+        <v>201</v>
+      </c>
+      <c r="H52" t="s">
+        <v>144</v>
+      </c>
+      <c r="I52">
+        <v>872</v>
+      </c>
+      <c r="J52" t="s">
+        <v>145</v>
+      </c>
+      <c r="K52" t="s">
+        <v>146</v>
+      </c>
+      <c r="L52">
+        <v>831</v>
+      </c>
+      <c r="M52" t="s">
+        <v>147</v>
+      </c>
+      <c r="N52" t="s">
+        <v>36</v>
+      </c>
+      <c r="O52">
+        <v>8</v>
+      </c>
+      <c r="P52" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q52">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
+      <c r="A53" t="s">
+        <v>202</v>
+      </c>
+      <c r="B53">
+        <v>71881</v>
+      </c>
+      <c r="C53">
+        <v>8720008</v>
+      </c>
+      <c r="D53">
+        <v>872013001</v>
+      </c>
+      <c r="E53" t="s">
+        <v>203</v>
+      </c>
+      <c r="F53">
+        <v>872013</v>
+      </c>
+      <c r="G53" t="s">
+        <v>204</v>
+      </c>
+      <c r="H53" t="s">
+        <v>144</v>
+      </c>
+      <c r="I53">
+        <v>872</v>
+      </c>
+      <c r="J53" t="s">
+        <v>145</v>
+      </c>
+      <c r="K53" t="s">
+        <v>146</v>
+      </c>
+      <c r="L53">
+        <v>831</v>
+      </c>
+      <c r="M53" t="s">
+        <v>147</v>
+      </c>
+      <c r="N53" t="s">
+        <v>36</v>
+      </c>
+      <c r="O53">
+        <v>8</v>
+      </c>
+      <c r="P53" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q53">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
+      <c r="A54" t="s">
+        <v>205</v>
+      </c>
+      <c r="B54">
+        <v>83063</v>
+      </c>
+      <c r="C54">
+        <v>9830088</v>
+      </c>
+      <c r="D54">
+        <v>983035001</v>
+      </c>
+      <c r="E54" t="s">
+        <v>206</v>
+      </c>
+      <c r="F54">
+        <v>983035</v>
+      </c>
+      <c r="G54" t="s">
+        <v>207</v>
+      </c>
+      <c r="H54" t="s">
+        <v>176</v>
+      </c>
+      <c r="I54">
+        <v>983</v>
+      </c>
+      <c r="J54" t="s">
+        <v>177</v>
+      </c>
+      <c r="K54" t="s">
+        <v>162</v>
+      </c>
+      <c r="L54">
+        <v>947</v>
+      </c>
+      <c r="M54" t="s">
+        <v>163</v>
+      </c>
+      <c r="N54" t="s">
+        <v>26</v>
+      </c>
+      <c r="O54">
+        <v>9</v>
+      </c>
+      <c r="P54" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q54">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
+      <c r="A55" t="s">
+        <v>208</v>
+      </c>
+      <c r="B55">
+        <v>83094</v>
+      </c>
+      <c r="C55">
+        <v>9830171</v>
+      </c>
+      <c r="D55">
+        <v>983042001</v>
+      </c>
+      <c r="E55" t="s">
+        <v>209</v>
+      </c>
+      <c r="F55">
+        <v>983042</v>
+      </c>
+      <c r="G55" t="s">
+        <v>210</v>
+      </c>
+      <c r="H55" t="s">
+        <v>176</v>
+      </c>
+      <c r="I55">
+        <v>983</v>
+      </c>
+      <c r="J55" t="s">
+        <v>177</v>
+      </c>
+      <c r="K55" t="s">
+        <v>162</v>
+      </c>
+      <c r="L55">
+        <v>947</v>
+      </c>
+      <c r="M55" t="s">
+        <v>163</v>
+      </c>
+      <c r="N55" t="s">
+        <v>26</v>
+      </c>
+      <c r="O55">
+        <v>9</v>
+      </c>
+      <c r="P55" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q55">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17">
+      <c r="A56" t="s">
+        <v>211</v>
+      </c>
+      <c r="B56">
+        <v>83098</v>
+      </c>
+      <c r="C56">
+        <v>9830094</v>
+      </c>
+      <c r="D56">
+        <v>983043001</v>
+      </c>
+      <c r="E56" t="s">
+        <v>212</v>
+      </c>
+      <c r="F56">
+        <v>983043</v>
+      </c>
+      <c r="G56" t="s">
+        <v>213</v>
+      </c>
+      <c r="H56" t="s">
+        <v>176</v>
+      </c>
+      <c r="I56">
+        <v>983</v>
+      </c>
+      <c r="J56" t="s">
+        <v>177</v>
+      </c>
+      <c r="K56" t="s">
+        <v>162</v>
+      </c>
+      <c r="L56">
+        <v>947</v>
+      </c>
+      <c r="M56" t="s">
+        <v>163</v>
+      </c>
+      <c r="N56" t="s">
+        <v>26</v>
+      </c>
+      <c r="O56">
+        <v>9</v>
+      </c>
+      <c r="P56" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q56">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
+      <c r="A57" t="s">
+        <v>214</v>
+      </c>
+      <c r="B57">
+        <v>83115</v>
+      </c>
+      <c r="C57">
+        <v>9830073</v>
+      </c>
+      <c r="D57">
+        <v>983048001</v>
+      </c>
+      <c r="E57" t="s">
+        <v>215</v>
+      </c>
+      <c r="F57">
+        <v>983048</v>
+      </c>
+      <c r="G57" t="s">
+        <v>216</v>
+      </c>
+      <c r="H57" t="s">
+        <v>176</v>
+      </c>
+      <c r="I57">
+        <v>983</v>
+      </c>
+      <c r="J57" t="s">
+        <v>177</v>
+      </c>
+      <c r="K57" t="s">
+        <v>162</v>
+      </c>
+      <c r="L57">
+        <v>947</v>
+      </c>
+      <c r="M57" t="s">
+        <v>163</v>
+      </c>
+      <c r="N57" t="s">
+        <v>26</v>
+      </c>
+      <c r="O57">
+        <v>9</v>
+      </c>
+      <c r="P57" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q57">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
+      <c r="A58" t="s">
+        <v>217</v>
+      </c>
+      <c r="B58">
+        <v>83122</v>
+      </c>
+      <c r="C58">
+        <v>9830191</v>
+      </c>
+      <c r="D58">
+        <v>983051001</v>
+      </c>
+      <c r="E58" t="s">
+        <v>218</v>
+      </c>
+      <c r="F58">
+        <v>983051</v>
+      </c>
+      <c r="G58" t="s">
+        <v>219</v>
+      </c>
+      <c r="H58" t="s">
+        <v>176</v>
+      </c>
+      <c r="I58">
+        <v>983</v>
+      </c>
+      <c r="J58" t="s">
+        <v>177</v>
+      </c>
+      <c r="K58" t="s">
+        <v>162</v>
+      </c>
+      <c r="L58">
+        <v>947</v>
+      </c>
+      <c r="M58" t="s">
+        <v>163</v>
+      </c>
+      <c r="N58" t="s">
+        <v>26</v>
+      </c>
+      <c r="O58">
+        <v>9</v>
+      </c>
+      <c r="P58" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q58">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17">
+      <c r="A59" t="s">
+        <v>220</v>
+      </c>
+      <c r="B59">
+        <v>83172</v>
+      </c>
+      <c r="C59">
+        <v>9830151</v>
+      </c>
+      <c r="D59">
+        <v>983061001</v>
+      </c>
+      <c r="E59" t="s">
+        <v>221</v>
+      </c>
+      <c r="F59">
+        <v>983061</v>
+      </c>
+      <c r="G59" t="s">
+        <v>222</v>
+      </c>
+      <c r="H59" t="s">
+        <v>176</v>
+      </c>
+      <c r="I59">
+        <v>983</v>
+      </c>
+      <c r="J59" t="s">
+        <v>177</v>
+      </c>
+      <c r="K59" t="s">
+        <v>162</v>
+      </c>
+      <c r="L59">
+        <v>947</v>
+      </c>
+      <c r="M59" t="s">
+        <v>163</v>
+      </c>
+      <c r="N59" t="s">
+        <v>26</v>
+      </c>
+      <c r="O59">
+        <v>9</v>
+      </c>
+      <c r="P59" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q59">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17">
+      <c r="A60" t="s">
+        <v>223</v>
+      </c>
+      <c r="B60">
+        <v>83175</v>
+      </c>
+      <c r="C60">
+        <v>9830124</v>
+      </c>
+      <c r="D60">
+        <v>983062001</v>
+      </c>
+      <c r="E60" t="s">
+        <v>224</v>
+      </c>
+      <c r="F60">
+        <v>983062</v>
+      </c>
+      <c r="G60" t="s">
+        <v>225</v>
+      </c>
+      <c r="H60" t="s">
+        <v>176</v>
+      </c>
+      <c r="I60">
+        <v>983</v>
+      </c>
+      <c r="J60" t="s">
+        <v>177</v>
+      </c>
+      <c r="K60" t="s">
+        <v>162</v>
+      </c>
+      <c r="L60">
+        <v>947</v>
+      </c>
+      <c r="M60" t="s">
+        <v>163</v>
+      </c>
+      <c r="N60" t="s">
+        <v>26</v>
+      </c>
+      <c r="O60">
+        <v>9</v>
+      </c>
+      <c r="P60" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q60">
+        <v>59303</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63" t="s">
+        <v>6</v>
+      </c>
+      <c r="G63" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" t="s">
+        <v>8</v>
+      </c>
+      <c r="I63" t="s">
+        <v>9</v>
+      </c>
+      <c r="J63" t="s">
+        <v>10</v>
+      </c>
+      <c r="K63" t="s">
+        <v>11</v>
+      </c>
+      <c r="L63" t="s">
+        <v>12</v>
+      </c>
+      <c r="M63" t="s">
+        <v>13</v>
+      </c>
+      <c r="N63" t="s">
+        <v>14</v>
+      </c>
+      <c r="O63" t="s">
+        <v>15</v>
+      </c>
+      <c r="P63" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="A64" t="s">
+        <v>234</v>
+      </c>
+      <c r="B64">
+        <v>68334</v>
+      </c>
+      <c r="C64">
+        <v>8600069</v>
+      </c>
+      <c r="D64">
+        <v>860008001</v>
+      </c>
+      <c r="E64" t="s">
+        <v>235</v>
+      </c>
+      <c r="F64">
+        <v>860008</v>
+      </c>
+      <c r="G64" t="s">
+        <v>236</v>
+      </c>
+      <c r="H64" t="s">
+        <v>237</v>
+      </c>
+      <c r="I64">
+        <v>860</v>
+      </c>
+      <c r="J64" t="s">
+        <v>238</v>
+      </c>
+      <c r="K64" t="s">
+        <v>239</v>
+      </c>
+      <c r="L64">
+        <v>830</v>
+      </c>
+      <c r="M64" t="s">
+        <v>240</v>
+      </c>
+      <c r="N64" t="s">
+        <v>36</v>
+      </c>
+      <c r="O64">
+        <v>8</v>
+      </c>
+      <c r="P64" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q64">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
+      <c r="A65" t="s">
+        <v>241</v>
+      </c>
+      <c r="B65">
+        <v>68356</v>
+      </c>
+      <c r="C65">
+        <v>8600025</v>
+      </c>
+      <c r="D65">
+        <v>860009002</v>
+      </c>
+      <c r="E65" t="s">
+        <v>242</v>
+      </c>
+      <c r="F65">
+        <v>860009</v>
+      </c>
+      <c r="G65" t="s">
+        <v>243</v>
+      </c>
+      <c r="H65" t="s">
+        <v>237</v>
+      </c>
+      <c r="I65">
+        <v>860</v>
+      </c>
+      <c r="J65" t="s">
+        <v>238</v>
+      </c>
+      <c r="K65" t="s">
+        <v>239</v>
+      </c>
+      <c r="L65">
+        <v>830</v>
+      </c>
+      <c r="M65" t="s">
+        <v>240</v>
+      </c>
+      <c r="N65" t="s">
+        <v>36</v>
+      </c>
+      <c r="O65">
+        <v>8</v>
+      </c>
+      <c r="P65" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q65">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
+      <c r="A66" t="s">
+        <v>244</v>
+      </c>
+      <c r="B66">
+        <v>68407</v>
+      </c>
+      <c r="C66">
+        <v>8600045</v>
+      </c>
+      <c r="D66">
+        <v>860012001</v>
+      </c>
+      <c r="E66" t="s">
+        <v>245</v>
+      </c>
+      <c r="F66">
+        <v>860012</v>
+      </c>
+      <c r="G66" t="s">
+        <v>246</v>
+      </c>
+      <c r="H66" t="s">
+        <v>237</v>
+      </c>
+      <c r="I66">
+        <v>860</v>
+      </c>
+      <c r="J66" t="s">
+        <v>238</v>
+      </c>
+      <c r="K66" t="s">
+        <v>239</v>
+      </c>
+      <c r="L66">
+        <v>830</v>
+      </c>
+      <c r="M66" t="s">
+        <v>240</v>
+      </c>
+      <c r="N66" t="s">
+        <v>36</v>
+      </c>
+      <c r="O66">
+        <v>8</v>
+      </c>
+      <c r="P66" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q66">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
+      <c r="A67" t="s">
+        <v>247</v>
+      </c>
+      <c r="B67">
+        <v>68481</v>
+      </c>
+      <c r="C67">
+        <v>8600137</v>
+      </c>
+      <c r="D67">
+        <v>860021001</v>
+      </c>
+      <c r="E67" t="s">
+        <v>248</v>
+      </c>
+      <c r="F67">
+        <v>860021</v>
+      </c>
+      <c r="G67" t="s">
+        <v>249</v>
+      </c>
+      <c r="H67" t="s">
+        <v>237</v>
+      </c>
+      <c r="I67">
+        <v>860</v>
+      </c>
+      <c r="J67" t="s">
+        <v>238</v>
+      </c>
+      <c r="K67" t="s">
+        <v>239</v>
+      </c>
+      <c r="L67">
+        <v>830</v>
+      </c>
+      <c r="M67" t="s">
+        <v>240</v>
+      </c>
+      <c r="N67" t="s">
+        <v>36</v>
+      </c>
+      <c r="O67">
+        <v>8</v>
+      </c>
+      <c r="P67" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q67">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17">
+      <c r="A68" t="s">
+        <v>250</v>
+      </c>
+      <c r="B68">
+        <v>68482</v>
+      </c>
+      <c r="C68">
+        <v>8600180</v>
+      </c>
+      <c r="D68">
+        <v>860022001</v>
+      </c>
+      <c r="E68" t="s">
+        <v>251</v>
+      </c>
+      <c r="F68">
+        <v>860022</v>
+      </c>
+      <c r="G68" t="s">
+        <v>252</v>
+      </c>
+      <c r="H68" t="s">
+        <v>237</v>
+      </c>
+      <c r="I68">
+        <v>860</v>
+      </c>
+      <c r="J68" t="s">
+        <v>238</v>
+      </c>
+      <c r="K68" t="s">
+        <v>239</v>
+      </c>
+      <c r="L68">
+        <v>830</v>
+      </c>
+      <c r="M68" t="s">
+        <v>240</v>
+      </c>
+      <c r="N68" t="s">
+        <v>36</v>
+      </c>
+      <c r="O68">
+        <v>8</v>
+      </c>
+      <c r="P68" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q68">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17">
+      <c r="A69" t="s">
+        <v>253</v>
+      </c>
+      <c r="B69">
+        <v>68492</v>
+      </c>
+      <c r="C69">
+        <v>8600013</v>
+      </c>
+      <c r="D69">
+        <v>860026001</v>
+      </c>
+      <c r="E69" t="s">
+        <v>254</v>
+      </c>
+      <c r="F69">
+        <v>860026</v>
+      </c>
+      <c r="G69" t="s">
+        <v>255</v>
+      </c>
+      <c r="H69" t="s">
+        <v>237</v>
+      </c>
+      <c r="I69">
+        <v>860</v>
+      </c>
+      <c r="J69" t="s">
+        <v>238</v>
+      </c>
+      <c r="K69" t="s">
+        <v>239</v>
+      </c>
+      <c r="L69">
+        <v>830</v>
+      </c>
+      <c r="M69" t="s">
+        <v>240</v>
+      </c>
+      <c r="N69" t="s">
+        <v>36</v>
+      </c>
+      <c r="O69">
+        <v>8</v>
+      </c>
+      <c r="P69" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q69">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17">
+      <c r="A70" t="s">
+        <v>256</v>
+      </c>
+      <c r="B70">
+        <v>68506</v>
+      </c>
+      <c r="C70">
+        <v>8600303</v>
+      </c>
+      <c r="D70">
+        <v>860031001</v>
+      </c>
+      <c r="E70" t="s">
+        <v>257</v>
+      </c>
+      <c r="F70">
+        <v>860031</v>
+      </c>
+      <c r="G70" t="s">
+        <v>258</v>
+      </c>
+      <c r="H70" t="s">
+        <v>237</v>
+      </c>
+      <c r="I70">
+        <v>860</v>
+      </c>
+      <c r="J70" t="s">
+        <v>238</v>
+      </c>
+      <c r="K70" t="s">
+        <v>239</v>
+      </c>
+      <c r="L70">
+        <v>830</v>
+      </c>
+      <c r="M70" t="s">
+        <v>240</v>
+      </c>
+      <c r="N70" t="s">
+        <v>36</v>
+      </c>
+      <c r="O70">
+        <v>8</v>
+      </c>
+      <c r="P70" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q70">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17">
+      <c r="A71" t="s">
+        <v>259</v>
+      </c>
+      <c r="B71">
+        <v>68518</v>
+      </c>
+      <c r="C71">
+        <v>8600067</v>
+      </c>
+      <c r="D71">
+        <v>860035001</v>
+      </c>
+      <c r="E71" t="s">
+        <v>260</v>
+      </c>
+      <c r="F71">
+        <v>860035</v>
+      </c>
+      <c r="G71" t="s">
+        <v>261</v>
+      </c>
+      <c r="H71" t="s">
+        <v>237</v>
+      </c>
+      <c r="I71">
+        <v>860</v>
+      </c>
+      <c r="J71" t="s">
+        <v>238</v>
+      </c>
+      <c r="K71" t="s">
+        <v>239</v>
+      </c>
+      <c r="L71">
+        <v>830</v>
+      </c>
+      <c r="M71" t="s">
+        <v>240</v>
+      </c>
+      <c r="N71" t="s">
+        <v>36</v>
+      </c>
+      <c r="O71">
+        <v>8</v>
+      </c>
+      <c r="P71" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q71">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17">
+      <c r="A72" t="s">
+        <v>262</v>
+      </c>
+      <c r="B72">
+        <v>68550</v>
+      </c>
+      <c r="C72">
+        <v>8600220</v>
+      </c>
+      <c r="D72">
+        <v>860038001</v>
+      </c>
+      <c r="E72" t="s">
+        <v>263</v>
+      </c>
+      <c r="F72">
+        <v>860038</v>
+      </c>
+      <c r="G72" t="s">
+        <v>264</v>
+      </c>
+      <c r="H72" t="s">
+        <v>237</v>
+      </c>
+      <c r="I72">
+        <v>860</v>
+      </c>
+      <c r="J72" t="s">
+        <v>238</v>
+      </c>
+      <c r="K72" t="s">
+        <v>239</v>
+      </c>
+      <c r="L72">
+        <v>830</v>
+      </c>
+      <c r="M72" t="s">
+        <v>240</v>
+      </c>
+      <c r="N72" t="s">
+        <v>36</v>
+      </c>
+      <c r="O72">
+        <v>8</v>
+      </c>
+      <c r="P72" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q72">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17">
+      <c r="A73" t="s">
+        <v>265</v>
+      </c>
+      <c r="B73">
+        <v>68553</v>
+      </c>
+      <c r="C73">
+        <v>8600231</v>
+      </c>
+      <c r="D73">
+        <v>860039001</v>
+      </c>
+      <c r="E73" t="s">
+        <v>266</v>
+      </c>
+      <c r="F73">
+        <v>860039</v>
+      </c>
+      <c r="G73" t="s">
+        <v>267</v>
+      </c>
+      <c r="H73" t="s">
+        <v>237</v>
+      </c>
+      <c r="I73">
+        <v>860</v>
+      </c>
+      <c r="J73" t="s">
+        <v>238</v>
+      </c>
+      <c r="K73" t="s">
+        <v>239</v>
+      </c>
+      <c r="L73">
+        <v>830</v>
+      </c>
+      <c r="M73" t="s">
+        <v>240</v>
+      </c>
+      <c r="N73" t="s">
+        <v>36</v>
+      </c>
+      <c r="O73">
+        <v>8</v>
+      </c>
+      <c r="P73" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q73">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17">
+      <c r="A74" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17">
+      <c r="A75" t="s">
+        <v>269</v>
+      </c>
+      <c r="B75">
+        <v>68557</v>
+      </c>
+      <c r="C75">
+        <v>8600079</v>
+      </c>
+      <c r="D75">
+        <v>860041001</v>
+      </c>
+      <c r="E75" t="s">
+        <v>270</v>
+      </c>
+      <c r="F75">
+        <v>860041</v>
+      </c>
+      <c r="G75" t="s">
+        <v>271</v>
+      </c>
+      <c r="H75" t="s">
+        <v>237</v>
+      </c>
+      <c r="I75">
+        <v>860</v>
+      </c>
+      <c r="J75" t="s">
+        <v>238</v>
+      </c>
+      <c r="K75" t="s">
+        <v>239</v>
+      </c>
+      <c r="L75">
+        <v>830</v>
+      </c>
+      <c r="M75" t="s">
+        <v>240</v>
+      </c>
+      <c r="N75" t="s">
+        <v>36</v>
+      </c>
+      <c r="O75">
+        <v>8</v>
+      </c>
+      <c r="P75" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q75">
+        <v>59104</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17">
+      <c r="A76" t="s">
+        <v>272</v>
+      </c>
+      <c r="B76">
+        <v>68611</v>
+      </c>
+      <c r="C76">
+        <v>8600211</v>
+      </c>
+      <c r="D76">
+        <v>860050001</v>
+      </c>
+      <c r="E76" t="s">
+        <v>273</v>
+      </c>
+      <c r="F76">
+        <v>860050</v>
+      </c>
+      <c r="G76" t="s">
+        <v>274</v>
+      </c>
+      <c r="H76" t="s">
+        <v>237</v>
+      </c>
+      <c r="I76">
+        <v>860</v>
+      </c>
+      <c r="J76" t="s">
+        <v>238</v>
+      </c>
+      <c r="K76" t="s">
+        <v>239</v>
+      </c>
+      <c r="L76">
+        <v>830</v>
+      </c>
+      <c r="M76" t="s">
+        <v>240</v>
+      </c>
+      <c r="N76" t="s">
+        <v>36</v>
+      </c>
+      <c r="O76">
+        <v>8</v>
+      </c>
+      <c r="P76" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q76">
+        <v>59104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>